<commit_message>
aggiornamento dati nazionali al 02/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B864CDA-1983-4F18-BDE9-C0C9A1A4F348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394D8EE3-C703-4962-B97C-15A8B146CFC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -907,6 +907,9 @@
                 <c:pt idx="37">
                   <c:v>2937</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>2477</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1375,13 +1378,13 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>14</c:v>
@@ -1390,7 +1393,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>39</c:v>
@@ -1405,25 +1408,25 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>39</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>30</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>53</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>67</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>60</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>90</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>92</c:v>
@@ -1432,40 +1435,40 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>91</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>63</c:v>
-                </c:pt>
                 <c:pt idx="27">
-                  <c:v>80</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>97</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>123</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>115</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>149</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>183</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>140</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>139</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3124,8 +3127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AP6" sqref="AP6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AQ6" sqref="AQ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3469,7 +3472,9 @@
       <c r="AP5" s="7">
         <v>2937</v>
       </c>
-      <c r="AQ5" s="7"/>
+      <c r="AQ5" s="7">
+        <v>2477</v>
+      </c>
       <c r="AR5" s="7"/>
       <c r="AS5" s="7"/>
       <c r="AT5" s="7"/>
@@ -3500,7 +3505,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>80572</v>
+        <v>83049</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -3959,8 +3964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BG49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AM6" sqref="AM6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4184,13 +4189,13 @@
         <v>4</v>
       </c>
       <c r="I5" s="29">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J5" s="29">
         <v>13</v>
       </c>
       <c r="K5" s="29">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="L5" s="29">
         <v>14</v>
@@ -4199,7 +4204,7 @@
         <v>12</v>
       </c>
       <c r="N5" s="29">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="O5" s="29">
         <v>39</v>
@@ -4214,25 +4219,25 @@
         <v>23</v>
       </c>
       <c r="S5" s="29">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="T5" s="29">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="U5" s="29">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="V5" s="29">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="W5" s="29">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="X5" s="29">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="Y5" s="29">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="Z5" s="29">
         <v>92</v>
@@ -4241,40 +4246,40 @@
         <v>97</v>
       </c>
       <c r="AB5" s="29">
+        <v>99</v>
+      </c>
+      <c r="AC5" s="30">
+        <v>108</v>
+      </c>
+      <c r="AD5" s="30">
+        <v>77</v>
+      </c>
+      <c r="AE5" s="30">
         <v>91</v>
       </c>
-      <c r="AC5" s="30">
-        <v>73</v>
-      </c>
-      <c r="AD5" s="30">
-        <v>63</v>
-      </c>
-      <c r="AE5" s="30">
-        <v>63</v>
-      </c>
       <c r="AF5" s="30">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="AG5" s="30">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="AH5" s="30">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="AI5" s="30">
-        <v>115</v>
+        <v>170</v>
       </c>
       <c r="AJ5" s="30">
-        <v>149</v>
+        <v>193</v>
       </c>
       <c r="AK5" s="30">
-        <v>183</v>
+        <v>122</v>
       </c>
       <c r="AL5" s="30">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="AM5" s="30">
-        <v>139</v>
+        <v>225</v>
       </c>
       <c r="AN5" s="30"/>
       <c r="AO5" s="30"/>
@@ -4310,7 +4315,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BG5)</f>
-        <v>2018</v>
+        <v>2456</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4378,7 +4383,7 @@
       </c>
       <c r="Q48" s="15">
         <f>MAXA(G5:BL5)</f>
-        <v>183</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="16:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
aggiornamento dati nazionali e Campania al 02/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394D8EE3-C703-4962-B97C-15A8B146CFC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A168AF56-70E4-4C94-958C-37377A54F17E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1470,6 +1470,9 @@
                 <c:pt idx="34">
                   <c:v>225</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>221</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3127,7 +3130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AQ6" sqref="AQ6"/>
     </sheetView>
   </sheetViews>
@@ -3964,8 +3967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BG49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AN6" sqref="AN6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4281,7 +4284,9 @@
       <c r="AM5" s="30">
         <v>225</v>
       </c>
-      <c r="AN5" s="30"/>
+      <c r="AN5" s="30">
+        <v>221</v>
+      </c>
       <c r="AO5" s="30"/>
       <c r="AP5" s="30"/>
       <c r="AQ5" s="30"/>
@@ -4315,7 +4320,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BG5)</f>
-        <v>2456</v>
+        <v>2677</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>

</xml_diff>

<commit_message>
aggiornamento dati nazionali al 03/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A168AF56-70E4-4C94-958C-37377A54F17E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFB1D8F-447B-4D76-8336-9FAFB30C4C07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -660,10 +660,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Italia!$E$4:$AR$4</c:f>
+              <c:f>Italia!$E$4:$BJ$4</c:f>
               <c:numCache>
                 <c:formatCode>d/m;@</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>43885</c:v>
                 </c:pt>
@@ -783,16 +783,70 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43927</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43929</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43932</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43933</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43935</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43936</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43937</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>43939</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>43940</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43941</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>43942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Italia!$E$5:$AR$5</c:f>
+              <c:f>Italia!$E$5:$BJ$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>221</c:v>
                 </c:pt>
@@ -909,6 +963,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2477</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2339</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1241,10 +1298,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Campania!$E$4:$AO$4</c:f>
+              <c:f>Campania!$E$4:$BG$4</c:f>
               <c:numCache>
                 <c:formatCode>d/m;@</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>43888</c:v>
                 </c:pt>
@@ -1355,16 +1412,70 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43927</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43929</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43932</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43933</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43935</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43936</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43937</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43939</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43940</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43941</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>43942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Campania!$E$5:$AO$5</c:f>
+              <c:f>Campania!$E$5:$BG$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -3130,8 +3241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AQ6" sqref="AQ6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3478,7 +3589,9 @@
       <c r="AQ5" s="7">
         <v>2477</v>
       </c>
-      <c r="AR5" s="7"/>
+      <c r="AR5" s="7">
+        <v>2339</v>
+      </c>
       <c r="AS5" s="7"/>
       <c r="AT5" s="7"/>
       <c r="AU5" s="7"/>
@@ -3508,7 +3621,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>83049</v>
+        <v>85388</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -3967,8 +4080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BG49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AN6" sqref="AN6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4407,10 +4520,10 @@
     <mergeCell ref="G7:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="E5:BG5">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
       <formula>$Q$48</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>$Q$48</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
aggiornamento dati nazionali e Campania al 03/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFB1D8F-447B-4D76-8336-9FAFB30C4C07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE03AB8-F03B-465C-B03F-EB386F2AFB38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1584,6 +1584,9 @@
                 <c:pt idx="35">
                   <c:v>221</c:v>
                 </c:pt>
+                <c:pt idx="36">
+                  <c:v>151</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3241,7 +3244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -4080,8 +4083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BG49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AO6" sqref="AO6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4400,7 +4403,9 @@
       <c r="AN5" s="30">
         <v>221</v>
       </c>
-      <c r="AO5" s="30"/>
+      <c r="AO5" s="30">
+        <v>151</v>
+      </c>
       <c r="AP5" s="30"/>
       <c r="AQ5" s="30"/>
       <c r="AR5" s="30"/>
@@ -4433,7 +4438,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BG5)</f>
-        <v>2677</v>
+        <v>2828</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>

</xml_diff>

<commit_message>
aggiornamento dati nazionali al 04/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE03AB8-F03B-465C-B03F-EB386F2AFB38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AD137C-D61B-4CEA-B8A9-B04B4FBF8FE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -967,6 +967,9 @@
                 <c:pt idx="39">
                   <c:v>2339</c:v>
                 </c:pt>
+                <c:pt idx="40">
+                  <c:v>2886</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3244,8 +3247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AS6" sqref="AS6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3595,7 +3598,9 @@
       <c r="AR5" s="7">
         <v>2339</v>
       </c>
-      <c r="AS5" s="7"/>
+      <c r="AS5" s="7">
+        <v>2886</v>
+      </c>
       <c r="AT5" s="7"/>
       <c r="AU5" s="7"/>
       <c r="AV5" s="7"/>
@@ -3624,7 +3629,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>85388</v>
+        <v>88274</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4083,7 +4088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BG49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AO6" sqref="AO6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
aggiornamento dati nazionali e Campania al 04/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AD137C-D61B-4CEA-B8A9-B04B4FBF8FE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348F93AC-1914-4597-B052-146F5A94BAEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="5805" yWindow="1110" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1590,6 +1590,9 @@
                 <c:pt idx="36">
                   <c:v>151</c:v>
                 </c:pt>
+                <c:pt idx="37">
+                  <c:v>132</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3247,7 +3250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AS6" sqref="AS6"/>
     </sheetView>
   </sheetViews>
@@ -4088,8 +4091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BG49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AO6" sqref="AO6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AP6" sqref="AP6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4411,7 +4414,9 @@
       <c r="AO5" s="30">
         <v>151</v>
       </c>
-      <c r="AP5" s="30"/>
+      <c r="AP5" s="30">
+        <v>132</v>
+      </c>
       <c r="AQ5" s="30"/>
       <c r="AR5" s="30"/>
       <c r="AS5" s="30"/>
@@ -4443,7 +4448,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BG5)</f>
-        <v>2828</v>
+        <v>2960</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>

</xml_diff>

<commit_message>
aggiornamento dati nazionali al giorno 05/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348F93AC-1914-4597-B052-146F5A94BAEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A81F673-879D-4EAF-9DE7-FAB29404C0EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="5805" yWindow="1110" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -970,6 +970,9 @@
                 <c:pt idx="40">
                   <c:v>2886</c:v>
                 </c:pt>
+                <c:pt idx="41">
+                  <c:v>2972</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3250,8 +3253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AS6" sqref="AS6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AT6" sqref="AT6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3604,7 +3607,9 @@
       <c r="AS5" s="7">
         <v>2886</v>
       </c>
-      <c r="AT5" s="7"/>
+      <c r="AT5" s="7">
+        <v>2972</v>
+      </c>
       <c r="AU5" s="7"/>
       <c r="AV5" s="7"/>
       <c r="AW5" s="7"/>
@@ -3632,7 +3637,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>88274</v>
+        <v>91246</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4091,7 +4096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BG49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AP6" sqref="AP6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
aggiornamento dati nazionali e Campania al giorno 05/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A81F673-879D-4EAF-9DE7-FAB29404C0EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0792E26-9CA0-4E62-8037-4DE54BEA2752}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1596,6 +1596,9 @@
                 <c:pt idx="37">
                   <c:v>132</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>108</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3253,7 +3256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AT6" sqref="AT6"/>
     </sheetView>
   </sheetViews>
@@ -4096,8 +4099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BG49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AP6" sqref="AP6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AQ6" sqref="AQ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4422,7 +4425,9 @@
       <c r="AP5" s="30">
         <v>132</v>
       </c>
-      <c r="AQ5" s="30"/>
+      <c r="AQ5" s="30">
+        <v>108</v>
+      </c>
       <c r="AR5" s="30"/>
       <c r="AS5" s="30"/>
       <c r="AT5" s="30"/>
@@ -4453,7 +4458,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BG5)</f>
-        <v>2960</v>
+        <v>3068</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>

</xml_diff>

<commit_message>
aggiornamento dati nazionali al 06/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0792E26-9CA0-4E62-8037-4DE54BEA2752}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0057C9-0DC4-4828-9281-0176CE2CF4A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -973,6 +973,9 @@
                 <c:pt idx="41">
                   <c:v>2972</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>1941</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3256,8 +3259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT6" sqref="AT6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AU6" sqref="AU6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3613,7 +3616,9 @@
       <c r="AT5" s="7">
         <v>2972</v>
       </c>
-      <c r="AU5" s="7"/>
+      <c r="AU5" s="7">
+        <v>1941</v>
+      </c>
       <c r="AV5" s="7"/>
       <c r="AW5" s="7"/>
       <c r="AX5" s="7"/>
@@ -3640,7 +3645,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>91246</v>
+        <v>93187</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4099,7 +4104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BG49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AQ6" sqref="AQ6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
aggiornamento dati nazionali e Campania al giorno 06/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0057C9-0DC4-4828-9281-0176CE2CF4A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487FDEFB-447A-44FB-A963-7E25350FF224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1602,6 +1602,9 @@
                 <c:pt idx="38">
                   <c:v>108</c:v>
                 </c:pt>
+                <c:pt idx="39">
+                  <c:v>90</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3259,7 +3262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AU6" sqref="AU6"/>
     </sheetView>
   </sheetViews>
@@ -4104,8 +4107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BG49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AQ6" sqref="AQ6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AR6" sqref="AR6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4433,7 +4436,9 @@
       <c r="AQ5" s="30">
         <v>108</v>
       </c>
-      <c r="AR5" s="30"/>
+      <c r="AR5" s="30">
+        <v>90</v>
+      </c>
       <c r="AS5" s="30"/>
       <c r="AT5" s="30"/>
       <c r="AU5" s="30"/>
@@ -4463,7 +4468,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BG5)</f>
-        <v>3068</v>
+        <v>3158</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>

</xml_diff>

<commit_message>
aggiornamento dati nazionali al 07/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487FDEFB-447A-44FB-A963-7E25350FF224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3A4BF4-5884-4EF1-8D9A-1E30B52D1ADA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -976,6 +976,9 @@
                 <c:pt idx="42">
                   <c:v>1941</c:v>
                 </c:pt>
+                <c:pt idx="43">
+                  <c:v>880</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3262,8 +3265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AU6" sqref="AU6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AV6" sqref="AV6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3622,7 +3625,9 @@
       <c r="AU5" s="7">
         <v>1941</v>
       </c>
-      <c r="AV5" s="7"/>
+      <c r="AV5" s="7">
+        <v>880</v>
+      </c>
       <c r="AW5" s="7"/>
       <c r="AX5" s="7"/>
       <c r="AY5" s="7"/>
@@ -3648,7 +3653,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>93187</v>
+        <v>94067</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4105,10 +4110,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
-  <dimension ref="A2:BG49"/>
+  <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AR6" sqref="AR6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BH5" sqref="BH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4119,7 +4124,7 @@
     <col min="29" max="62" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:59" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:62" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Z2" s="32" t="s">
         <v>4</v>
       </c>
@@ -4138,8 +4143,8 @@
       <c r="AM2" s="32"/>
       <c r="AN2" s="32"/>
     </row>
-    <row r="3" spans="1:59" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:59" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:62" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:62" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="39" t="s">
         <v>2</v>
       </c>
@@ -4311,8 +4316,17 @@
       <c r="BG4" s="4">
         <v>43942</v>
       </c>
+      <c r="BH4" s="4">
+        <v>43943</v>
+      </c>
+      <c r="BI4" s="4">
+        <v>43944</v>
+      </c>
+      <c r="BJ4" s="4">
+        <v>43945</v>
+      </c>
     </row>
-    <row r="5" spans="1:59" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:62" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A5" s="35" t="s">
         <v>0</v>
       </c>
@@ -4454,11 +4468,14 @@
       <c r="BE5" s="30"/>
       <c r="BF5" s="30"/>
       <c r="BG5" s="30"/>
+      <c r="BH5" s="30"/>
+      <c r="BI5" s="30"/>
+      <c r="BJ5" s="30"/>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="AF6" s="11"/>
     </row>
-    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
         <v>1</v>
       </c>
@@ -4473,7 +4490,7 @@
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
     </row>
-    <row r="8" spans="1:59" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:62" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -4483,7 +4500,7 @@
       <c r="H8" s="37"/>
       <c r="I8" s="37"/>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="36" t="s">
         <v>3</v>
@@ -4491,7 +4508,7 @@
       <c r="D13" s="36"/>
       <c r="E13" s="36"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B14" s="16"/>
       <c r="C14" s="33" t="s">
         <v>6</v>
@@ -4501,7 +4518,7 @@
       <c r="F14" s="33"/>
       <c r="G14" s="33"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="31" t="s">
         <v>8</v>
@@ -4512,7 +4529,7 @@
       <c r="G15" s="31"/>
       <c r="H15" s="31"/>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B16" s="23"/>
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
@@ -4554,7 +4571,7 @@
     <mergeCell ref="B7:F8"/>
     <mergeCell ref="G7:I8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E5:BG5">
+  <conditionalFormatting sqref="E5:BJ5">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
       <formula>$Q$48</formula>
     </cfRule>

</xml_diff>

<commit_message>
aggiornamento dati nazionali e Campania al 07/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3A4BF4-5884-4EF1-8D9A-1E30B52D1ADA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6499B08-F644-4D15-B051-8B3748E5709F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1608,6 +1608,9 @@
                 <c:pt idx="39">
                   <c:v>90</c:v>
                 </c:pt>
+                <c:pt idx="40">
+                  <c:v>120</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3265,7 +3268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AV6" sqref="AV6"/>
     </sheetView>
   </sheetViews>
@@ -4112,8 +4115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BH5" sqref="BH5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AS6" sqref="AS6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4453,7 +4456,9 @@
       <c r="AR5" s="30">
         <v>90</v>
       </c>
-      <c r="AS5" s="30"/>
+      <c r="AS5" s="30">
+        <v>120</v>
+      </c>
       <c r="AT5" s="30"/>
       <c r="AU5" s="30"/>
       <c r="AV5" s="30"/>
@@ -4485,7 +4490,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BG5)</f>
-        <v>3158</v>
+        <v>3278</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>

</xml_diff>

<commit_message>
aggiornamento dati nazionali e Campania al 08/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6499B08-F644-4D15-B051-8B3748E5709F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539CF563-D7B4-4795-91CC-F5A2C9442B4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -979,6 +979,9 @@
                 <c:pt idx="43">
                   <c:v>880</c:v>
                 </c:pt>
+                <c:pt idx="44">
+                  <c:v>1195</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1610,6 +1613,9 @@
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3269,7 +3275,7 @@
   <dimension ref="A2:BJ55"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AV6" sqref="AV6"/>
+      <selection activeCell="AW6" sqref="AW6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3631,7 +3637,9 @@
       <c r="AV5" s="7">
         <v>880</v>
       </c>
-      <c r="AW5" s="7"/>
+      <c r="AW5" s="7">
+        <v>1195</v>
+      </c>
       <c r="AX5" s="7"/>
       <c r="AY5" s="7"/>
       <c r="AZ5" s="7"/>
@@ -3656,7 +3664,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>94067</v>
+        <v>95262</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4116,7 +4124,7 @@
   <dimension ref="A2:BJ49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AS6" sqref="AS6"/>
+      <selection activeCell="AT6" sqref="AT6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4459,7 +4467,9 @@
       <c r="AS5" s="30">
         <v>120</v>
       </c>
-      <c r="AT5" s="30"/>
+      <c r="AT5" s="30">
+        <v>76</v>
+      </c>
       <c r="AU5" s="30"/>
       <c r="AV5" s="30"/>
       <c r="AW5" s="30"/>
@@ -4490,7 +4500,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BG5)</f>
-        <v>3278</v>
+        <v>3354</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>

</xml_diff>

<commit_message>
aggiornamento dati nazionali al 09/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539CF563-D7B4-4795-91CC-F5A2C9442B4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FA8F2A-D7F7-4D0A-A39B-9BA9322B7D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -982,6 +982,9 @@
                 <c:pt idx="44">
                   <c:v>1195</c:v>
                 </c:pt>
+                <c:pt idx="45">
+                  <c:v>1615</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1313,10 +1316,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Campania!$E$4:$BG$4</c:f>
+              <c:f>Campania!$E$4:$BJ$4</c:f>
               <c:numCache>
                 <c:formatCode>d/m;@</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>43888</c:v>
                 </c:pt>
@@ -1481,16 +1484,25 @@
                 </c:pt>
                 <c:pt idx="54">
                   <c:v>43942</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>43945</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Campania!$E$5:$BG$5</c:f>
+              <c:f>Campania!$E$5:$BJ$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -3274,8 +3286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AW6" sqref="AW6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AX6" sqref="AX6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3640,7 +3652,9 @@
       <c r="AW5" s="7">
         <v>1195</v>
       </c>
-      <c r="AX5" s="7"/>
+      <c r="AX5" s="7">
+        <v>1615</v>
+      </c>
       <c r="AY5" s="7"/>
       <c r="AZ5" s="7"/>
       <c r="BA5" s="7"/>
@@ -3664,7 +3678,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>95262</v>
+        <v>96877</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4123,8 +4137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT6" sqref="AT6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
aggiornamento dati nazionali e Campania al 09/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FA8F2A-D7F7-4D0A-A39B-9BA9322B7D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE946E1C-AC1C-4B53-B2D5-E72242F7CF75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1629,6 +1629,9 @@
                 <c:pt idx="41">
                   <c:v>76</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>98</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3286,7 +3289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AX6" sqref="AX6"/>
     </sheetView>
   </sheetViews>
@@ -4137,8 +4140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AU6" sqref="AU6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4484,7 +4487,9 @@
       <c r="AT5" s="30">
         <v>76</v>
       </c>
-      <c r="AU5" s="30"/>
+      <c r="AU5" s="30">
+        <v>98</v>
+      </c>
       <c r="AV5" s="30"/>
       <c r="AW5" s="30"/>
       <c r="AX5" s="30"/>
@@ -4514,7 +4519,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BG5)</f>
-        <v>3354</v>
+        <v>3452</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>

</xml_diff>

<commit_message>
aggiornamento dati nazionali  al 10/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE946E1C-AC1C-4B53-B2D5-E72242F7CF75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8989F81B-1255-40DF-A544-78E42826868E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -985,6 +985,9 @@
                 <c:pt idx="45">
                   <c:v>1615</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>1396</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3289,8 +3292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AX6" sqref="AX6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AY6" sqref="AY6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3658,7 +3661,9 @@
       <c r="AX5" s="7">
         <v>1615</v>
       </c>
-      <c r="AY5" s="7"/>
+      <c r="AY5" s="7">
+        <v>1396</v>
+      </c>
       <c r="AZ5" s="7"/>
       <c r="BA5" s="7"/>
       <c r="BB5" s="7"/>
@@ -3681,7 +3686,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>96877</v>
+        <v>98273</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4140,7 +4145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AU6" sqref="AU6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
aggiornamento dati nazionali e Campania al 10/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8989F81B-1255-40DF-A544-78E42826868E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B479E58-A338-4EAB-A7F3-B42D52F6F0C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1635,6 +1635,9 @@
                 <c:pt idx="42">
                   <c:v>98</c:v>
                 </c:pt>
+                <c:pt idx="43">
+                  <c:v>75</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3292,7 +3295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AY6" sqref="AY6"/>
     </sheetView>
   </sheetViews>
@@ -4145,8 +4148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AU6" sqref="AU6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AV6" sqref="AV6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4495,7 +4498,9 @@
       <c r="AU5" s="30">
         <v>98</v>
       </c>
-      <c r="AV5" s="30"/>
+      <c r="AV5" s="30">
+        <v>75</v>
+      </c>
       <c r="AW5" s="30"/>
       <c r="AX5" s="30"/>
       <c r="AY5" s="30"/>
@@ -4524,7 +4529,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BG5)</f>
-        <v>3452</v>
+        <v>3527</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>

</xml_diff>

<commit_message>
aggiornamento dati nazionali al 11/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B479E58-A338-4EAB-A7F3-B42D52F6F0C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2515DF1E-6C8E-4D3A-8609-44728D89EE33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -69,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +222,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -321,7 +329,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -429,6 +437,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="20" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -987,6 +998,9 @@
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>1396</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3295,8 +3309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AY6" sqref="AY6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3667,7 +3681,9 @@
       <c r="AY5" s="7">
         <v>1396</v>
       </c>
-      <c r="AZ5" s="7"/>
+      <c r="AZ5" s="7">
+        <v>1996</v>
+      </c>
       <c r="BA5" s="7"/>
       <c r="BB5" s="7"/>
       <c r="BC5" s="7"/>
@@ -3687,13 +3703,13 @@
       <c r="D7" s="38"/>
       <c r="E7" s="38"/>
       <c r="F7" s="38"/>
-      <c r="G7" s="37">
+      <c r="G7" s="40">
         <f>SUM(E5:BJ5)</f>
-        <v>98273</v>
-      </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
+        <v>100269</v>
+      </c>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
     </row>
     <row r="8" spans="1:62" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="38"/>
@@ -3701,10 +3717,10 @@
       <c r="D8" s="38"/>
       <c r="E8" s="38"/>
       <c r="F8" s="38"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
@@ -4148,7 +4164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AV6" sqref="AV6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
aggiornamento dati nazionali e Campania al 12/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2515DF1E-6C8E-4D3A-8609-44728D89EE33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5E14B8-1347-4837-B72F-62A95792E9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -429,7 +429,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="20" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -438,7 +438,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="20" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1001,6 +1001,9 @@
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1984</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1651,6 +1654,12 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>66</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3309,8 +3318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BA6" sqref="BA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3684,7 +3693,9 @@
       <c r="AZ5" s="7">
         <v>1996</v>
       </c>
-      <c r="BA5" s="7"/>
+      <c r="BA5" s="7">
+        <v>1984</v>
+      </c>
       <c r="BB5" s="7"/>
       <c r="BC5" s="7"/>
       <c r="BD5" s="7"/>
@@ -3703,13 +3714,13 @@
       <c r="D7" s="38"/>
       <c r="E7" s="38"/>
       <c r="F7" s="38"/>
-      <c r="G7" s="40">
+      <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>100269</v>
-      </c>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
+        <v>102253</v>
+      </c>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
     </row>
     <row r="8" spans="1:62" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="38"/>
@@ -3717,10 +3728,10 @@
       <c r="D8" s="38"/>
       <c r="E8" s="38"/>
       <c r="F8" s="38"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
@@ -4164,8 +4175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AV6" sqref="AV6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AX6" sqref="AX6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4517,8 +4528,12 @@
       <c r="AV5" s="30">
         <v>75</v>
       </c>
-      <c r="AW5" s="30"/>
-      <c r="AX5" s="30"/>
+      <c r="AW5" s="30">
+        <v>87</v>
+      </c>
+      <c r="AX5" s="30">
+        <v>66</v>
+      </c>
       <c r="AY5" s="30"/>
       <c r="AZ5" s="30"/>
       <c r="BA5" s="30"/>
@@ -4543,12 +4558,12 @@
       <c r="D7" s="38"/>
       <c r="E7" s="38"/>
       <c r="F7" s="38"/>
-      <c r="G7" s="37">
+      <c r="G7" s="40">
         <f>SUM(E5:BG5)</f>
-        <v>3527</v>
-      </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+        <v>3680</v>
+      </c>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
     </row>
     <row r="8" spans="1:62" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="38"/>
@@ -4556,9 +4571,9 @@
       <c r="D8" s="38"/>
       <c r="E8" s="38"/>
       <c r="F8" s="38"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>

</xml_diff>

<commit_message>
aggiornamento dati nazionali al 13/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5E14B8-1347-4837-B72F-62A95792E9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ED7693-95DC-4FDA-B4E3-799F4E783E33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1005,6 +1005,9 @@
                 <c:pt idx="48">
                   <c:v>1984</c:v>
                 </c:pt>
+                <c:pt idx="49">
+                  <c:v>1363</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3318,8 +3321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BA6" sqref="BA6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BB6" sqref="BB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3696,7 +3699,9 @@
       <c r="BA5" s="7">
         <v>1984</v>
       </c>
-      <c r="BB5" s="7"/>
+      <c r="BB5" s="7">
+        <v>1363</v>
+      </c>
       <c r="BC5" s="7"/>
       <c r="BD5" s="7"/>
       <c r="BE5" s="7"/>
@@ -3716,7 +3721,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>102253</v>
+        <v>103616</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4175,7 +4180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AX6" sqref="AX6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
aggiornamento dati nazionali e Campania al 13/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ED7693-95DC-4FDA-B4E3-799F4E783E33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B76DCEC-0401-4D07-9DDB-FE6E4321EBF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1664,6 +1664,9 @@
                 <c:pt idx="45">
                   <c:v>66</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>99</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3321,7 +3324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="BB6" sqref="BB6"/>
     </sheetView>
   </sheetViews>
@@ -4180,8 +4183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AX6" sqref="AX6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AY6" sqref="AY6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4539,7 +4542,9 @@
       <c r="AX5" s="30">
         <v>66</v>
       </c>
-      <c r="AY5" s="30"/>
+      <c r="AY5" s="30">
+        <v>99</v>
+      </c>
       <c r="AZ5" s="30"/>
       <c r="BA5" s="30"/>
       <c r="BB5" s="30"/>
@@ -4565,7 +4570,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="40">
         <f>SUM(E5:BG5)</f>
-        <v>3680</v>
+        <v>3779</v>
       </c>
       <c r="H7" s="40"/>
       <c r="I7" s="40"/>

</xml_diff>

<commit_message>
aggiornamento dati nazionali al 14/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B76DCEC-0401-4D07-9DDB-FE6E4321EBF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67C4CCB-9A55-44C8-8BD2-31B9F146CACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1008,6 +1008,9 @@
                 <c:pt idx="49">
                   <c:v>1363</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>675</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3324,8 +3327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BB6" sqref="BB6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BC6" sqref="BC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3705,7 +3708,9 @@
       <c r="BB5" s="7">
         <v>1363</v>
       </c>
-      <c r="BC5" s="7"/>
+      <c r="BC5" s="7">
+        <v>675</v>
+      </c>
       <c r="BD5" s="7"/>
       <c r="BE5" s="7"/>
       <c r="BF5" s="7"/>
@@ -3724,7 +3729,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>103616</v>
+        <v>104291</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4183,7 +4188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AY6" sqref="AY6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
aggiornamento dati nazionali e Campania al 14/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67C4CCB-9A55-44C8-8BD2-31B9F146CACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6257FC8-143D-4F90-89AA-8DCE390FBA2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1670,6 +1670,9 @@
                 <c:pt idx="46">
                   <c:v>99</c:v>
                 </c:pt>
+                <c:pt idx="47">
+                  <c:v>38</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3327,7 +3330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="BC6" sqref="BC6"/>
     </sheetView>
   </sheetViews>
@@ -4188,8 +4191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AY6" sqref="AY6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AZ6" sqref="AZ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4550,7 +4553,9 @@
       <c r="AY5" s="30">
         <v>99</v>
       </c>
-      <c r="AZ5" s="30"/>
+      <c r="AZ5" s="30">
+        <v>38</v>
+      </c>
       <c r="BA5" s="30"/>
       <c r="BB5" s="30"/>
       <c r="BC5" s="30"/>
@@ -4575,7 +4580,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="40">
         <f>SUM(E5:BG5)</f>
-        <v>3779</v>
+        <v>3817</v>
       </c>
       <c r="H7" s="40"/>
       <c r="I7" s="40"/>

</xml_diff>

<commit_message>
Aggiornamento dati nazionali al 15/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6257FC8-143D-4F90-89AA-8DCE390FBA2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493CAA15-C4B0-43AF-AA63-658F4EC6C3B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1011,6 +1011,9 @@
                 <c:pt idx="50">
                   <c:v>675</c:v>
                 </c:pt>
+                <c:pt idx="51">
+                  <c:v>1127</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3330,8 +3333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BC6" sqref="BC6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BD6" sqref="BD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3714,7 +3717,9 @@
       <c r="BC5" s="7">
         <v>675</v>
       </c>
-      <c r="BD5" s="7"/>
+      <c r="BD5" s="7">
+        <v>1127</v>
+      </c>
       <c r="BE5" s="7"/>
       <c r="BF5" s="7"/>
       <c r="BG5" s="7"/>
@@ -3732,7 +3737,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>104291</v>
+        <v>105418</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4191,7 +4196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AZ6" sqref="AZ6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
aggiornamento dati nazionali al 16/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493CAA15-C4B0-43AF-AA63-658F4EC6C3B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42106C8-0A64-4690-A3F6-0E8FB7346ACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1014,6 +1014,9 @@
                 <c:pt idx="51">
                   <c:v>1127</c:v>
                 </c:pt>
+                <c:pt idx="52">
+                  <c:v>1189</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1675,6 +1678,9 @@
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3333,8 +3339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BD6" sqref="BD6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BE6" sqref="BE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3720,7 +3726,9 @@
       <c r="BD5" s="7">
         <v>1127</v>
       </c>
-      <c r="BE5" s="7"/>
+      <c r="BE5" s="7">
+        <v>1189</v>
+      </c>
       <c r="BF5" s="7"/>
       <c r="BG5" s="7"/>
       <c r="BH5" s="7"/>
@@ -3737,7 +3745,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>105418</v>
+        <v>106607</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4196,8 +4204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AZ6" sqref="AZ6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BA6" sqref="BA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4561,7 +4569,9 @@
       <c r="AZ5" s="30">
         <v>38</v>
       </c>
-      <c r="BA5" s="30"/>
+      <c r="BA5" s="30">
+        <v>80</v>
+      </c>
       <c r="BB5" s="30"/>
       <c r="BC5" s="30"/>
       <c r="BD5" s="30"/>
@@ -4585,7 +4595,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="40">
         <f>SUM(E5:BG5)</f>
-        <v>3817</v>
+        <v>3897</v>
       </c>
       <c r="H7" s="40"/>
       <c r="I7" s="40"/>

</xml_diff>

<commit_message>
aggiornamento dati al 17/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42106C8-0A64-4690-A3F6-0E8FB7346ACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1909E4-93AB-442A-B2EE-3EA1DE08C30B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -1017,6 +1017,9 @@
                 <c:pt idx="52">
                   <c:v>1189</c:v>
                 </c:pt>
+                <c:pt idx="53">
+                  <c:v>355</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1681,6 +1684,9 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3340,7 +3346,7 @@
   <dimension ref="A2:BJ55"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BE6" sqref="BE6"/>
+      <selection activeCell="BF6" sqref="BF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3729,7 +3735,9 @@
       <c r="BE5" s="7">
         <v>1189</v>
       </c>
-      <c r="BF5" s="7"/>
+      <c r="BF5" s="7">
+        <v>355</v>
+      </c>
       <c r="BG5" s="7"/>
       <c r="BH5" s="7"/>
       <c r="BI5" s="7"/>
@@ -3745,7 +3753,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>106607</v>
+        <v>106962</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4205,7 +4213,7 @@
   <dimension ref="A2:BJ49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BA6" sqref="BA6"/>
+      <selection activeCell="BB6" sqref="BB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4572,7 +4580,9 @@
       <c r="BA5" s="30">
         <v>80</v>
       </c>
-      <c r="BB5" s="30"/>
+      <c r="BB5" s="30">
+        <v>64</v>
+      </c>
       <c r="BC5" s="30"/>
       <c r="BD5" s="30"/>
       <c r="BE5" s="30"/>
@@ -4595,7 +4605,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="40">
         <f>SUM(E5:BG5)</f>
-        <v>3897</v>
+        <v>3961</v>
       </c>
       <c r="H7" s="40"/>
       <c r="I7" s="40"/>

</xml_diff>

<commit_message>
aggiornamento dati al 19/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C045FB2-7BDE-4D48-9BE5-99146E43ED2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CF243A-29ED-495E-AA22-BCF6ED453C35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1023,6 +1023,9 @@
                 <c:pt idx="54">
                   <c:v>809</c:v>
                 </c:pt>
+                <c:pt idx="55">
+                  <c:v>486</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1693,6 +1696,12 @@
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3351,8 +3360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A2:BJ55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BG6" sqref="BG6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BH6" sqref="BH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3747,7 +3756,9 @@
       <c r="BG5" s="7">
         <v>809</v>
       </c>
-      <c r="BH5" s="7"/>
+      <c r="BH5" s="7">
+        <v>486</v>
+      </c>
       <c r="BI5" s="7"/>
       <c r="BJ5" s="7"/>
     </row>
@@ -3761,7 +3772,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>107771</v>
+        <v>108257</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4220,8 +4231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A2:BJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BC6" sqref="BC6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4594,8 +4605,12 @@
       <c r="BC5" s="30">
         <v>37</v>
       </c>
-      <c r="BD5" s="30"/>
-      <c r="BE5" s="30"/>
+      <c r="BD5" s="30">
+        <v>41</v>
+      </c>
+      <c r="BE5" s="30">
+        <v>45</v>
+      </c>
       <c r="BF5" s="30"/>
       <c r="BG5" s="30"/>
       <c r="BH5" s="30"/>
@@ -4615,7 +4630,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="40">
         <f>SUM(E5:BG5)</f>
-        <v>3998</v>
+        <v>4084</v>
       </c>
       <c r="H7" s="40"/>
       <c r="I7" s="40"/>

</xml_diff>

<commit_message>
aggiornamento dati al 21/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CF243A-29ED-495E-AA22-BCF6ED453C35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C117DC7-B274-45A1-A7BA-A928BEF3363E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -1026,6 +1026,9 @@
                 <c:pt idx="55">
                   <c:v>486</c:v>
                 </c:pt>
+                <c:pt idx="56">
+                  <c:v>-20</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1557,13 +1560,13 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>14</c:v>
@@ -1572,10 +1575,10 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>39</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>19</c:v>
@@ -1587,121 +1590,124 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>61</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>67</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>94</c:v>
-                </c:pt>
                 <c:pt idx="20">
-                  <c:v>87</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>92</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>99</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>108</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>77</c:v>
                 </c:pt>
-                <c:pt idx="26">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>193</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>122</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>164</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>221</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>151</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="40">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>75</c:v>
-                </c:pt>
                 <c:pt idx="44">
-                  <c:v>87</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>66</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>99</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>38</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>80</c:v>
+                  <c:v>-7</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>64</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>37</c:v>
+                  <c:v>-91</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>41</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>45</c:v>
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3361,7 +3367,7 @@
   <dimension ref="A2:BJ55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BH6" sqref="BH6"/>
+      <selection activeCell="BI6" sqref="BI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3759,7 +3765,9 @@
       <c r="BH5" s="7">
         <v>486</v>
       </c>
-      <c r="BI5" s="7"/>
+      <c r="BI5" s="7">
+        <v>-20</v>
+      </c>
       <c r="BJ5" s="7"/>
     </row>
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3772,7 +3780,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="37">
         <f>SUM(E5:BJ5)</f>
-        <v>108257</v>
+        <v>108237</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -4232,7 +4240,7 @@
   <dimension ref="A2:BJ49"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:I8"/>
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4465,13 +4473,13 @@
         <v>4</v>
       </c>
       <c r="I5" s="29">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J5" s="29">
         <v>13</v>
       </c>
       <c r="K5" s="29">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="L5" s="29">
         <v>14</v>
@@ -4480,10 +4488,10 @@
         <v>12</v>
       </c>
       <c r="N5" s="29">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="O5" s="29">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="P5" s="29">
         <v>19</v>
@@ -4495,123 +4503,125 @@
         <v>23</v>
       </c>
       <c r="S5" s="29">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="T5" s="29">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="U5" s="29">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="V5" s="29">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="W5" s="29">
+        <v>65</v>
+      </c>
+      <c r="X5" s="29">
         <v>60</v>
       </c>
-      <c r="X5" s="29">
-        <v>94</v>
-      </c>
       <c r="Y5" s="29">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="Z5" s="29">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="AA5" s="29">
         <v>97</v>
       </c>
       <c r="AB5" s="29">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="AC5" s="30">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="AD5" s="30">
+        <v>63</v>
+      </c>
+      <c r="AE5" s="30">
+        <v>63</v>
+      </c>
+      <c r="AF5" s="30">
+        <v>80</v>
+      </c>
+      <c r="AG5" s="30">
+        <v>97</v>
+      </c>
+      <c r="AH5" s="30">
+        <v>123</v>
+      </c>
+      <c r="AI5" s="30">
+        <v>115</v>
+      </c>
+      <c r="AJ5" s="30">
+        <v>149</v>
+      </c>
+      <c r="AK5" s="30">
+        <v>183</v>
+      </c>
+      <c r="AL5" s="30">
+        <v>132</v>
+      </c>
+      <c r="AM5" s="30">
+        <v>105</v>
+      </c>
+      <c r="AN5" s="30">
+        <v>164</v>
+      </c>
+      <c r="AO5" s="30">
+        <v>212</v>
+      </c>
+      <c r="AP5" s="30">
+        <v>144</v>
+      </c>
+      <c r="AQ5" s="30">
+        <v>125</v>
+      </c>
+      <c r="AR5" s="30">
         <v>77</v>
       </c>
-      <c r="AE5" s="30">
-        <v>91</v>
-      </c>
-      <c r="AF5" s="30">
-        <v>110</v>
-      </c>
-      <c r="AG5" s="30">
-        <v>145</v>
-      </c>
-      <c r="AH5" s="30">
-        <v>128</v>
-      </c>
-      <c r="AI5" s="30">
-        <v>170</v>
-      </c>
-      <c r="AJ5" s="30">
-        <v>193</v>
-      </c>
-      <c r="AK5" s="30">
-        <v>122</v>
-      </c>
-      <c r="AL5" s="30">
-        <v>164</v>
-      </c>
-      <c r="AM5" s="30">
-        <v>225</v>
-      </c>
-      <c r="AN5" s="30">
-        <v>221</v>
-      </c>
-      <c r="AO5" s="30">
-        <v>151</v>
-      </c>
-      <c r="AP5" s="30">
-        <v>132</v>
-      </c>
-      <c r="AQ5" s="30">
-        <v>108</v>
-      </c>
-      <c r="AR5" s="30">
+      <c r="AS5" s="30">
+        <v>67</v>
+      </c>
+      <c r="AT5" s="30">
+        <v>94</v>
+      </c>
+      <c r="AU5" s="30">
+        <v>14</v>
+      </c>
+      <c r="AV5" s="30">
         <v>90</v>
       </c>
-      <c r="AS5" s="30">
-        <v>120</v>
-      </c>
-      <c r="AT5" s="30">
-        <v>76</v>
-      </c>
-      <c r="AU5" s="30">
-        <v>98</v>
-      </c>
-      <c r="AV5" s="30">
-        <v>75</v>
-      </c>
       <c r="AW5" s="30">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="AX5" s="30">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="AY5" s="30">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="AZ5" s="30">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="BA5" s="30">
-        <v>80</v>
+        <v>-7</v>
       </c>
       <c r="BB5" s="30">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="BC5" s="30">
-        <v>37</v>
+        <v>-91</v>
       </c>
       <c r="BD5" s="30">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="BE5" s="30">
-        <v>45</v>
-      </c>
-      <c r="BF5" s="30"/>
+        <v>12</v>
+      </c>
+      <c r="BF5" s="30">
+        <v>-3</v>
+      </c>
       <c r="BG5" s="30"/>
       <c r="BH5" s="30"/>
       <c r="BI5" s="30"/>
@@ -4630,7 +4640,7 @@
       <c r="F7" s="38"/>
       <c r="G7" s="40">
         <f>SUM(E5:BG5)</f>
-        <v>4084</v>
+        <v>3019</v>
       </c>
       <c r="H7" s="40"/>
       <c r="I7" s="40"/>
@@ -4698,7 +4708,7 @@
       </c>
       <c r="Q48" s="15">
         <f>MAXA(G5:BL5)</f>
-        <v>225</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="16:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
aggiornamento dati al 22/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D5E18C-2742-416A-81E7-07A24AF8DCD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761EB0D3-35EE-4F39-B96A-322AFF54BE47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -69,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,29 +181,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="28"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -231,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,14 +242,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -319,6 +290,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -329,7 +337,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -357,18 +365,11 @@
     <xf numFmtId="164" fontId="12" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -376,28 +377,16 @@
     <xf numFmtId="164" fontId="12" fillId="5" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -405,10 +394,10 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -417,30 +406,40 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="20" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="17" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Colore 5" xfId="5" builtinId="46"/>
@@ -451,7 +450,185 @@
     <cellStyle name="Titolo 1" xfId="1" builtinId="16"/>
     <cellStyle name="Titolo 4" xfId="2" builtinId="19"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -552,6 +729,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.7777202552782357E-2"/>
+          <c:y val="0.13333333333333333"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -585,34 +770,34 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="3.0717562840302654E-2"/>
-          <c:y val="0.12437047189583907"/>
+          <c:x val="2.4618482555394887E-2"/>
+          <c:y val="9.1776285317276524E-2"/>
           <c:w val="0.93230409590243379"/>
           <c:h val="0.75948244448536006"/>
         </c:manualLayout>
       </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:solidFill>
+            <a:pattFill prst="ltUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
                 <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:round/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
-                <a:schemeClr val="accent1"/>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:solidFill>
@@ -642,7 +827,6 @@
                 <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -671,10 +855,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Italia!$E$4:$BJ$4</c:f>
+              <c:f>Italia!$E$3:$CU$3</c:f>
               <c:numCache>
                 <c:formatCode>d/m;@</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="95"/>
                 <c:pt idx="0">
                   <c:v>43885</c:v>
                 </c:pt>
@@ -848,16 +1032,127 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>43942</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>43943</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>43944</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>43946</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>43947</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>43948</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>43949</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>43950</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>43951</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>43953</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>43960</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>43961</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>43962</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>43963</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>43964</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>43965</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>43967</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>43968</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>43969</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>43970</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>43971</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>43972</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>43973</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>43974</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>43975</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>43976</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>43977</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>43978</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>43979</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Italia!$E$5:$BJ$5</c:f>
+              <c:f>Italia!$E$4:$CU$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="95"/>
                 <c:pt idx="0">
                   <c:v>221</c:v>
                 </c:pt>
@@ -1031,11 +1326,13 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>-528</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7D1F-4BC5-BB87-F508642597ED}"/>
@@ -1043,7 +1340,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -1051,32 +1347,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:dropLines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="lt1"/>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="lt1">
-                      <a:alpha val="0"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:dropLines>
-        <c:smooth val="0"/>
+        <c:gapWidth val="150"/>
         <c:axId val="1302010479"/>
         <c:axId val="1246378655"/>
-      </c:lineChart>
-      <c:dateAx>
+      </c:barChart>
+      <c:catAx>
         <c:axId val="1302010479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -1086,7 +1361,7 @@
         <c:numFmt formatCode="d/m;@" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="high"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -1113,10 +1388,11 @@
         </c:txPr>
         <c:crossAx val="1246378655"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="0"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="1246378655"/>
         <c:scaling>
@@ -1221,7 +1497,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1"/>
                 </a:solidFill>
@@ -1232,17 +1508,22 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT" sz="2400"/>
-              <a:t>Nuovi Infetti </a:t>
+              <a:t>Nuovi</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" sz="2400" baseline="0"/>
+              <a:t> infetti</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2400"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="it-IT" sz="2400"/>
-              <a:t>Campania</a:t>
+              <a:rPr lang="it-IT" sz="2400" baseline="0"/>
+              <a:t>Italia</a:t>
             </a:r>
+            <a:endParaRPr lang="it-IT" sz="2400"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1250,8 +1531,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.4328610975886919"/>
-          <c:y val="2.2855747999753935E-2"/>
+          <c:x val="3.7777202552782357E-2"/>
+          <c:y val="0.13333333333333333"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1267,7 +1548,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1"/>
               </a:solidFill>
@@ -1282,29 +1563,39 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.4618482555394887E-2"/>
+          <c:y val="9.1776285317276524E-2"/>
+          <c:w val="0.93230409590243379"/>
+          <c:h val="0.83438107503171466"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:solidFill>
+            <a:pattFill prst="ltUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
                 <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:round/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
-                <a:schemeClr val="accent1"/>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:solidFill>
@@ -1334,7 +1625,6 @@
                 <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1363,10 +1653,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Campania!$E$4:$BJ$4</c:f>
+              <c:f>Campania!$H$3:$CU$3</c:f>
               <c:numCache>
                 <c:formatCode>d/m;@</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="92"/>
                 <c:pt idx="0">
                   <c:v>43888</c:v>
                 </c:pt>
@@ -1540,16 +1830,118 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>43946</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>43947</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>43948</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>43949</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>43950</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>43951</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>43953</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>43960</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>43961</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>43962</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>43963</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>43964</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>43965</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>43967</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>43968</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>43969</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>43970</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>43971</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>43972</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>43973</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>43974</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>43975</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>43976</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>43977</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>43978</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>43979</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Campania!$E$5:$BJ$5</c:f>
+              <c:f>Campania!$H$4:$CU$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="92"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1714,19 +2106,20 @@
                 </c:pt>
                 <c:pt idx="54">
                   <c:v>-73</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4625-444B-8056-43FB1161545C}"/>
+              <c16:uniqueId val="{00000001-A77B-4C71-9642-7426BE3488FB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -1734,32 +2127,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:dropLines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="lt1"/>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="lt1">
-                      <a:alpha val="0"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:dropLines>
-        <c:smooth val="0"/>
+        <c:gapWidth val="150"/>
         <c:axId val="1302010479"/>
         <c:axId val="1246378655"/>
-      </c:lineChart>
-      <c:dateAx>
+      </c:barChart>
+      <c:catAx>
         <c:axId val="1302010479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -1769,7 +2141,7 @@
         <c:numFmt formatCode="d/m;@" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="high"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -1796,10 +2168,11 @@
         </c:txPr>
         <c:crossAx val="1246378655"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="0"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="1246378655"/>
         <c:scaling>
@@ -2993,16 +3366,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>64995</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>3361</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>20171</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>61</xdr:col>
-      <xdr:colOff>302558</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>134471</xdr:rowOff>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>268941</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3036,27 +3409,29 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>224118</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>20171</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>168089</xdr:rowOff>
+      <xdr:rowOff>22412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>62</xdr:col>
-      <xdr:colOff>235322</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>33618</xdr:rowOff>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>268941</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Grafico 1">
+        <xdr:cNvPr id="4" name="Grafico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E22DA4C8-8DB6-46F5-A433-74D72B8423DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D176794D-F6CF-45C9-A68E-0B848B7557DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3370,10 +3745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
-  <dimension ref="A2:BJ55"/>
+  <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BJ6" sqref="BJ6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AT4" sqref="AT4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3381,860 +3756,1022 @@
     <col min="2" max="4" width="5.7109375" style="1" customWidth="1"/>
     <col min="5" max="25" width="4.7109375" style="2" customWidth="1"/>
     <col min="26" max="28" width="4.7109375" style="3" customWidth="1"/>
-    <col min="29" max="62" width="4.7109375" customWidth="1"/>
+    <col min="29" max="99" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:62" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="32" t="s">
+    <row r="1" spans="1:99" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="32"/>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
     </row>
-    <row r="3" spans="1:62" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:62" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+    <row r="2" spans="1:99" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="4">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="4">
         <v>43885</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F3" s="4">
         <v>43886</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G3" s="4">
         <v>43887</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H3" s="4">
         <v>43888</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I3" s="4">
         <v>43889</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J3" s="4">
         <v>43890</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K3" s="4">
         <v>43891</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L3" s="4">
         <v>43892</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M3" s="4">
         <v>43893</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N3" s="4">
         <v>43894</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O3" s="4">
         <v>43895</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P3" s="4">
         <v>43896</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q3" s="4">
         <v>43897</v>
       </c>
-      <c r="R4" s="4">
+      <c r="R3" s="4">
         <v>43898</v>
       </c>
-      <c r="S4" s="4">
+      <c r="S3" s="4">
         <v>43899</v>
       </c>
-      <c r="T4" s="9">
+      <c r="T3" s="9">
         <v>43900</v>
       </c>
-      <c r="U4" s="10">
+      <c r="U3" s="10">
         <v>43901</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V3" s="4">
         <v>43902</v>
       </c>
-      <c r="W4" s="4">
+      <c r="W3" s="4">
         <v>43903</v>
       </c>
-      <c r="X4" s="4">
+      <c r="X3" s="4">
         <v>43904</v>
       </c>
-      <c r="Y4" s="4">
+      <c r="Y3" s="4">
         <v>43905</v>
       </c>
-      <c r="Z4" s="4">
+      <c r="Z3" s="4">
         <v>43906</v>
       </c>
-      <c r="AA4" s="4">
+      <c r="AA3" s="4">
         <v>43907</v>
       </c>
-      <c r="AB4" s="4">
+      <c r="AB3" s="4">
         <v>43908</v>
       </c>
-      <c r="AC4" s="4">
+      <c r="AC3" s="4">
         <v>43909</v>
       </c>
-      <c r="AD4" s="4">
+      <c r="AD3" s="4">
         <v>43910</v>
       </c>
-      <c r="AE4" s="4">
+      <c r="AE3" s="4">
         <v>43911</v>
       </c>
-      <c r="AF4" s="9">
+      <c r="AF3" s="9">
         <v>43912</v>
       </c>
-      <c r="AG4" s="17">
+      <c r="AG3" s="14">
         <v>43913</v>
       </c>
-      <c r="AH4" s="4">
+      <c r="AH3" s="4">
         <v>43914</v>
       </c>
-      <c r="AI4" s="4">
+      <c r="AI3" s="4">
         <v>43915</v>
       </c>
-      <c r="AJ4" s="4">
+      <c r="AJ3" s="4">
         <v>43916</v>
       </c>
-      <c r="AK4" s="4">
+      <c r="AK3" s="4">
         <v>43917</v>
       </c>
-      <c r="AL4" s="4">
+      <c r="AL3" s="4">
         <v>43918</v>
       </c>
-      <c r="AM4" s="4">
+      <c r="AM3" s="4">
         <v>43919</v>
       </c>
-      <c r="AN4" s="4">
+      <c r="AN3" s="4">
         <v>43920</v>
       </c>
-      <c r="AO4" s="4">
+      <c r="AO3" s="4">
         <v>43921</v>
       </c>
-      <c r="AP4" s="4">
+      <c r="AP3" s="4">
         <v>43922</v>
       </c>
-      <c r="AQ4" s="4">
+      <c r="AQ3" s="4">
         <v>43923</v>
       </c>
-      <c r="AR4" s="4">
+      <c r="AR3" s="4">
         <v>43924</v>
       </c>
-      <c r="AS4" s="4">
+      <c r="AS3" s="4">
         <v>43925</v>
       </c>
-      <c r="AT4" s="4">
+      <c r="AT3" s="4">
         <v>43926</v>
       </c>
-      <c r="AU4" s="4">
+      <c r="AU3" s="4">
         <v>43927</v>
       </c>
-      <c r="AV4" s="4">
+      <c r="AV3" s="4">
         <v>43928</v>
       </c>
-      <c r="AW4" s="4">
+      <c r="AW3" s="4">
         <v>43929</v>
       </c>
-      <c r="AX4" s="4">
+      <c r="AX3" s="4">
         <v>43930</v>
       </c>
-      <c r="AY4" s="4">
+      <c r="AY3" s="4">
         <v>43931</v>
       </c>
-      <c r="AZ4" s="4">
+      <c r="AZ3" s="4">
         <v>43932</v>
       </c>
-      <c r="BA4" s="4">
+      <c r="BA3" s="4">
         <v>43933</v>
       </c>
-      <c r="BB4" s="4">
+      <c r="BB3" s="4">
         <v>43934</v>
       </c>
-      <c r="BC4" s="4">
+      <c r="BC3" s="4">
         <v>43935</v>
       </c>
-      <c r="BD4" s="4">
+      <c r="BD3" s="4">
         <v>43936</v>
       </c>
-      <c r="BE4" s="4">
+      <c r="BE3" s="4">
         <v>43937</v>
       </c>
-      <c r="BF4" s="4">
+      <c r="BF3" s="4">
         <v>43938</v>
       </c>
-      <c r="BG4" s="4">
+      <c r="BG3" s="4">
         <v>43939</v>
       </c>
-      <c r="BH4" s="4">
+      <c r="BH3" s="4">
         <v>43940</v>
       </c>
-      <c r="BI4" s="4">
+      <c r="BI3" s="4">
         <v>43941</v>
       </c>
-      <c r="BJ4" s="4">
+      <c r="BJ3" s="4">
         <v>43942</v>
       </c>
+      <c r="BK3" s="4">
+        <v>43943</v>
+      </c>
+      <c r="BL3" s="4">
+        <v>43944</v>
+      </c>
+      <c r="BM3" s="4">
+        <v>43945</v>
+      </c>
+      <c r="BN3" s="4">
+        <v>43946</v>
+      </c>
+      <c r="BO3" s="4">
+        <v>43947</v>
+      </c>
+      <c r="BP3" s="4">
+        <v>43948</v>
+      </c>
+      <c r="BQ3" s="4">
+        <v>43949</v>
+      </c>
+      <c r="BR3" s="4">
+        <v>43950</v>
+      </c>
+      <c r="BS3" s="4">
+        <v>43951</v>
+      </c>
+      <c r="BT3" s="4">
+        <v>43952</v>
+      </c>
+      <c r="BU3" s="4">
+        <v>43953</v>
+      </c>
+      <c r="BV3" s="4">
+        <v>43954</v>
+      </c>
+      <c r="BW3" s="4">
+        <v>43955</v>
+      </c>
+      <c r="BX3" s="4">
+        <v>43956</v>
+      </c>
+      <c r="BY3" s="4">
+        <v>43957</v>
+      </c>
+      <c r="BZ3" s="4">
+        <v>43958</v>
+      </c>
+      <c r="CA3" s="4">
+        <v>43959</v>
+      </c>
+      <c r="CB3" s="4">
+        <v>43960</v>
+      </c>
+      <c r="CC3" s="4">
+        <v>43961</v>
+      </c>
+      <c r="CD3" s="4">
+        <v>43962</v>
+      </c>
+      <c r="CE3" s="4">
+        <v>43963</v>
+      </c>
+      <c r="CF3" s="4">
+        <v>43964</v>
+      </c>
+      <c r="CG3" s="4">
+        <v>43965</v>
+      </c>
+      <c r="CH3" s="4">
+        <v>43966</v>
+      </c>
+      <c r="CI3" s="4">
+        <v>43967</v>
+      </c>
+      <c r="CJ3" s="4">
+        <v>43968</v>
+      </c>
+      <c r="CK3" s="4">
+        <v>43969</v>
+      </c>
+      <c r="CL3" s="4">
+        <v>43970</v>
+      </c>
+      <c r="CM3" s="4">
+        <v>43971</v>
+      </c>
+      <c r="CN3" s="4">
+        <v>43972</v>
+      </c>
+      <c r="CO3" s="4">
+        <v>43973</v>
+      </c>
+      <c r="CP3" s="4">
+        <v>43974</v>
+      </c>
+      <c r="CQ3" s="4">
+        <v>43975</v>
+      </c>
+      <c r="CR3" s="4">
+        <v>43976</v>
+      </c>
+      <c r="CS3" s="4">
+        <v>43977</v>
+      </c>
+      <c r="CT3" s="4">
+        <v>43978</v>
+      </c>
+      <c r="CU3" s="4">
+        <v>43979</v>
+      </c>
     </row>
-    <row r="5" spans="1:62" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="35" t="s">
+    <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="6">
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="6">
         <v>221</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F4" s="6">
         <v>88</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G4" s="6">
         <v>76</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H4" s="6">
         <v>203</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I4" s="6">
         <v>233</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J4" s="6">
         <v>228</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K4" s="6">
         <v>288</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L4" s="6">
         <v>498</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M4" s="6">
         <v>428</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N4" s="6">
         <v>443</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O4" s="6">
         <v>570</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P4" s="6">
         <v>640</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q4" s="6">
         <v>1145</v>
       </c>
-      <c r="R5" s="6">
+      <c r="R4" s="6">
         <v>1326</v>
       </c>
-      <c r="S5" s="6">
+      <c r="S4" s="6">
         <v>1598</v>
       </c>
-      <c r="T5" s="6">
+      <c r="T4" s="6">
         <v>529</v>
       </c>
-      <c r="U5" s="6">
+      <c r="U4" s="6">
         <v>2076</v>
       </c>
-      <c r="V5" s="6">
+      <c r="V4" s="6">
         <v>2249</v>
       </c>
-      <c r="W5" s="6">
+      <c r="W4" s="6">
         <v>2116</v>
       </c>
-      <c r="X5" s="6">
+      <c r="X4" s="6">
         <v>2795</v>
       </c>
-      <c r="Y5" s="6">
+      <c r="Y4" s="6">
         <v>2853</v>
       </c>
-      <c r="Z5" s="6">
+      <c r="Z4" s="6">
         <v>2470</v>
       </c>
-      <c r="AA5" s="6">
+      <c r="AA4" s="6">
         <v>2989</v>
       </c>
-      <c r="AB5" s="6">
+      <c r="AB4" s="6">
         <v>2648</v>
       </c>
-      <c r="AC5" s="7">
+      <c r="AC4" s="7">
         <v>4480</v>
       </c>
-      <c r="AD5" s="7">
+      <c r="AD4" s="7">
         <v>4670</v>
       </c>
-      <c r="AE5" s="7">
+      <c r="AE4" s="7">
         <v>4821</v>
       </c>
-      <c r="AF5" s="7">
+      <c r="AF4" s="7">
         <v>3957</v>
       </c>
-      <c r="AG5" s="7">
+      <c r="AG4" s="7">
         <v>3780</v>
       </c>
-      <c r="AH5" s="7">
+      <c r="AH4" s="7">
         <v>3612</v>
       </c>
-      <c r="AI5" s="7">
+      <c r="AI4" s="7">
         <v>3491</v>
       </c>
-      <c r="AJ5" s="7">
+      <c r="AJ4" s="7">
         <v>4492</v>
       </c>
-      <c r="AK5" s="7">
+      <c r="AK4" s="7">
         <v>4401</v>
       </c>
-      <c r="AL5" s="7">
+      <c r="AL4" s="7">
         <v>3651</v>
       </c>
-      <c r="AM5" s="7">
+      <c r="AM4" s="7">
         <v>3815</v>
       </c>
-      <c r="AN5" s="7">
+      <c r="AN4" s="7">
         <v>1648</v>
       </c>
-      <c r="AO5" s="7">
+      <c r="AO4" s="7">
         <v>2107</v>
       </c>
-      <c r="AP5" s="7">
+      <c r="AP4" s="7">
         <v>2937</v>
       </c>
-      <c r="AQ5" s="7">
+      <c r="AQ4" s="7">
         <v>2477</v>
       </c>
-      <c r="AR5" s="7">
+      <c r="AR4" s="7">
         <v>2339</v>
       </c>
-      <c r="AS5" s="7">
+      <c r="AS4" s="7">
         <v>2886</v>
       </c>
-      <c r="AT5" s="7">
+      <c r="AT4" s="7">
         <v>2972</v>
       </c>
-      <c r="AU5" s="7">
+      <c r="AU4" s="7">
         <v>1941</v>
       </c>
-      <c r="AV5" s="7">
+      <c r="AV4" s="7">
         <v>880</v>
       </c>
-      <c r="AW5" s="7">
+      <c r="AW4" s="7">
         <v>1195</v>
       </c>
-      <c r="AX5" s="7">
+      <c r="AX4" s="7">
         <v>1615</v>
       </c>
-      <c r="AY5" s="7">
+      <c r="AY4" s="7">
         <v>1396</v>
       </c>
-      <c r="AZ5" s="7">
+      <c r="AZ4" s="7">
         <v>1996</v>
       </c>
-      <c r="BA5" s="7">
+      <c r="BA4" s="7">
         <v>1984</v>
       </c>
-      <c r="BB5" s="7">
+      <c r="BB4" s="7">
         <v>1363</v>
       </c>
-      <c r="BC5" s="7">
+      <c r="BC4" s="7">
         <v>675</v>
       </c>
-      <c r="BD5" s="7">
+      <c r="BD4" s="7">
         <v>1127</v>
       </c>
-      <c r="BE5" s="7">
+      <c r="BE4" s="7">
         <v>1189</v>
       </c>
-      <c r="BF5" s="7">
+      <c r="BF4" s="7">
         <v>355</v>
       </c>
-      <c r="BG5" s="7">
+      <c r="BG4" s="7">
         <v>809</v>
       </c>
-      <c r="BH5" s="7">
+      <c r="BH4" s="7">
         <v>486</v>
       </c>
-      <c r="BI5" s="7">
+      <c r="BI4" s="7">
         <v>-20</v>
       </c>
-      <c r="BJ5" s="7">
+      <c r="BJ4" s="7">
         <v>-528</v>
       </c>
+      <c r="BK4" s="7">
+        <v>-10</v>
+      </c>
+      <c r="BL4" s="7"/>
+      <c r="BM4" s="7"/>
+      <c r="BN4" s="7"/>
+      <c r="BO4" s="7"/>
+      <c r="BP4" s="7"/>
+      <c r="BQ4" s="7"/>
+      <c r="BR4" s="7"/>
+      <c r="BS4" s="7"/>
+      <c r="BT4" s="7"/>
+      <c r="BU4" s="7"/>
+      <c r="BV4" s="7"/>
+      <c r="BW4" s="7"/>
+      <c r="BX4" s="7"/>
+      <c r="BY4" s="7"/>
+      <c r="BZ4" s="7"/>
+      <c r="CA4" s="7"/>
+      <c r="CB4" s="7"/>
+      <c r="CC4" s="7"/>
+      <c r="CD4" s="7"/>
+      <c r="CE4" s="7"/>
+      <c r="CF4" s="7"/>
+      <c r="CG4" s="7"/>
+      <c r="CH4" s="7"/>
+      <c r="CI4" s="7"/>
+      <c r="CJ4" s="7"/>
+      <c r="CK4" s="7"/>
+      <c r="CL4" s="7"/>
+      <c r="CM4" s="7"/>
+      <c r="CN4" s="7"/>
+      <c r="CO4" s="7"/>
+      <c r="CP4" s="7"/>
+      <c r="CQ4" s="7"/>
+      <c r="CR4" s="7"/>
+      <c r="CS4" s="7"/>
+      <c r="CT4" s="7"/>
+      <c r="CU4" s="7"/>
     </row>
-    <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="38" t="s">
+    <row r="6" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:99" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K39" s="5"/>
+      <c r="L39" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="M39" s="30"/>
+      <c r="N39" s="30"/>
+      <c r="O39" s="30"/>
+      <c r="W39" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="37">
-        <f>SUM(E5:BJ5)</f>
-        <v>107709</v>
-      </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="28">
+        <f>SUM(E4:CU4)</f>
+        <v>107699</v>
+      </c>
+      <c r="AC39" s="28"/>
+      <c r="AD39" s="28"/>
+      <c r="AE39" s="28"/>
     </row>
-    <row r="8" spans="1:62" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
+    <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K40" s="13"/>
+      <c r="L40" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="M40" s="24"/>
+      <c r="N40" s="24"/>
+      <c r="O40" s="24"/>
+      <c r="P40" s="24"/>
+      <c r="Q40" s="24"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="28"/>
+      <c r="AC40" s="28"/>
+      <c r="AD40" s="28"/>
+      <c r="AE40" s="28"/>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
+    <row r="41" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="K41" s="11"/>
+      <c r="L41" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M41" s="24"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
+      <c r="Q41" s="24"/>
+      <c r="R41" s="24"/>
+      <c r="W41" s="29"/>
+      <c r="X41" s="29"/>
+      <c r="Y41" s="29"/>
+      <c r="Z41" s="29"/>
+      <c r="AA41" s="29"/>
+      <c r="AB41" s="28"/>
+      <c r="AC41" s="28"/>
+      <c r="AD41" s="28"/>
+      <c r="AE41" s="28"/>
     </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-    </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="B15" s="12"/>
-      <c r="C15" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
+    <row r="43" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+      <c r="S43" s="15"/>
+      <c r="T43" s="15"/>
+      <c r="U43" s="15"/>
+      <c r="V43" s="15"/>
+      <c r="W43" s="15"/>
+      <c r="X43" s="15"/>
+      <c r="Y43" s="15"/>
+      <c r="Z43" s="16"/>
+      <c r="AA43" s="16"/>
+      <c r="AB43" s="16"/>
+      <c r="AC43" s="17"/>
+      <c r="AD43" s="17"/>
+      <c r="AE43" s="17"/>
+      <c r="AF43" s="17"/>
+      <c r="AG43" s="17"/>
+      <c r="AH43" s="17"/>
+      <c r="AI43" s="17"/>
+      <c r="AJ43" s="17"/>
+      <c r="AK43" s="17"/>
     </row>
     <row r="44" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="18"/>
-      <c r="U44" s="18"/>
-      <c r="V44" s="18"/>
-      <c r="W44" s="18"/>
-      <c r="X44" s="18"/>
-      <c r="Y44" s="18"/>
-      <c r="Z44" s="19"/>
-      <c r="AA44" s="19"/>
-      <c r="AB44" s="19"/>
-      <c r="AC44" s="20"/>
-      <c r="AD44" s="20"/>
-      <c r="AE44" s="20"/>
-      <c r="AF44" s="20"/>
-      <c r="AG44" s="20"/>
-      <c r="AH44" s="20"/>
-      <c r="AI44" s="20"/>
-      <c r="AJ44" s="20"/>
-      <c r="AK44" s="20"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="15"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="15"/>
+      <c r="X44" s="15"/>
+      <c r="Y44" s="15"/>
+      <c r="Z44" s="16"/>
+      <c r="AA44" s="16"/>
+      <c r="AB44" s="16"/>
+      <c r="AC44" s="17"/>
+      <c r="AD44" s="17"/>
+      <c r="AE44" s="17"/>
+      <c r="AF44" s="17"/>
+      <c r="AG44" s="17"/>
+      <c r="AH44" s="17"/>
+      <c r="AI44" s="17"/>
+      <c r="AJ44" s="17"/>
+      <c r="AK44" s="17"/>
     </row>
     <row r="45" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="18"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
-      <c r="T45" s="18"/>
-      <c r="U45" s="18"/>
-      <c r="V45" s="18"/>
-      <c r="W45" s="18"/>
-      <c r="X45" s="18"/>
-      <c r="Y45" s="18"/>
-      <c r="Z45" s="19"/>
-      <c r="AA45" s="19"/>
-      <c r="AB45" s="19"/>
-      <c r="AC45" s="20"/>
-      <c r="AD45" s="20"/>
-      <c r="AE45" s="20"/>
-      <c r="AF45" s="20"/>
-      <c r="AG45" s="20"/>
-      <c r="AH45" s="20"/>
-      <c r="AI45" s="20"/>
-      <c r="AJ45" s="20"/>
-      <c r="AK45" s="20"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="15"/>
+      <c r="S45" s="15"/>
+      <c r="T45" s="15"/>
+      <c r="U45" s="15"/>
+      <c r="V45" s="15"/>
+      <c r="W45" s="15"/>
+      <c r="X45" s="15"/>
+      <c r="Y45" s="15"/>
+      <c r="Z45" s="16"/>
+      <c r="AA45" s="16"/>
+      <c r="AB45" s="16"/>
+      <c r="AC45" s="17"/>
+      <c r="AD45" s="17"/>
+      <c r="AE45" s="17"/>
+      <c r="AF45" s="17"/>
+      <c r="AG45" s="17"/>
+      <c r="AH45" s="17"/>
+      <c r="AI45" s="17"/>
+      <c r="AJ45" s="17"/>
+      <c r="AK45" s="17"/>
     </row>
     <row r="46" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
-      <c r="T46" s="18"/>
-      <c r="U46" s="18"/>
-      <c r="V46" s="18"/>
-      <c r="W46" s="18"/>
-      <c r="X46" s="18"/>
-      <c r="Y46" s="18"/>
-      <c r="Z46" s="19"/>
-      <c r="AA46" s="19"/>
-      <c r="AB46" s="19"/>
-      <c r="AC46" s="20"/>
-      <c r="AD46" s="20"/>
-      <c r="AE46" s="20"/>
-      <c r="AF46" s="20"/>
-      <c r="AG46" s="20"/>
-      <c r="AH46" s="20"/>
-      <c r="AI46" s="20"/>
-      <c r="AJ46" s="20"/>
-      <c r="AK46" s="20"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="15"/>
+      <c r="R46" s="15"/>
+      <c r="S46" s="15"/>
+      <c r="T46" s="15"/>
+      <c r="U46" s="15"/>
+      <c r="V46" s="15"/>
+      <c r="W46" s="15"/>
+      <c r="X46" s="15"/>
+      <c r="Y46" s="15"/>
+      <c r="Z46" s="16"/>
+      <c r="AA46" s="16"/>
+      <c r="AB46" s="16"/>
+      <c r="AC46" s="17"/>
+      <c r="AD46" s="17"/>
+      <c r="AE46" s="17"/>
+      <c r="AF46" s="17"/>
+      <c r="AG46" s="17"/>
+      <c r="AH46" s="17"/>
+      <c r="AI46" s="17"/>
+      <c r="AJ46" s="17"/>
+      <c r="AK46" s="17"/>
     </row>
     <row r="47" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
-      <c r="T47" s="18"/>
-      <c r="U47" s="18"/>
-      <c r="V47" s="18"/>
-      <c r="W47" s="18"/>
-      <c r="X47" s="18"/>
-      <c r="Y47" s="18"/>
-      <c r="Z47" s="19"/>
-      <c r="AA47" s="19"/>
-      <c r="AB47" s="19"/>
-      <c r="AC47" s="20"/>
-      <c r="AD47" s="20"/>
-      <c r="AE47" s="20"/>
-      <c r="AF47" s="20"/>
-      <c r="AG47" s="20"/>
-      <c r="AH47" s="20"/>
-      <c r="AI47" s="20"/>
-      <c r="AJ47" s="20"/>
-      <c r="AK47" s="20"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="O47" s="19">
+        <f>MAXA(E4:BJ4)</f>
+        <v>4821</v>
+      </c>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+      <c r="S47" s="15"/>
+      <c r="T47" s="15"/>
+      <c r="U47" s="15"/>
+      <c r="V47" s="15"/>
+      <c r="W47" s="15"/>
+      <c r="X47" s="15"/>
+      <c r="Y47" s="15"/>
+      <c r="Z47" s="16"/>
+      <c r="AA47" s="16"/>
+      <c r="AB47" s="16"/>
+      <c r="AC47" s="17"/>
+      <c r="AD47" s="17"/>
+      <c r="AE47" s="17"/>
+      <c r="AF47" s="17"/>
+      <c r="AG47" s="17"/>
+      <c r="AH47" s="17"/>
+      <c r="AI47" s="17"/>
+      <c r="AJ47" s="17"/>
+      <c r="AK47" s="17"/>
     </row>
     <row r="48" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="O48" s="22">
-        <f>MAXA(E5:BJ5)</f>
-        <v>4821</v>
-      </c>
-      <c r="P48" s="18"/>
-      <c r="Q48" s="18"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="18"/>
-      <c r="T48" s="18"/>
-      <c r="U48" s="18"/>
-      <c r="V48" s="18"/>
-      <c r="W48" s="18"/>
-      <c r="X48" s="18"/>
-      <c r="Y48" s="18"/>
-      <c r="Z48" s="19"/>
-      <c r="AA48" s="19"/>
-      <c r="AB48" s="19"/>
-      <c r="AC48" s="20"/>
-      <c r="AD48" s="20"/>
-      <c r="AE48" s="20"/>
-      <c r="AF48" s="20"/>
-      <c r="AG48" s="20"/>
-      <c r="AH48" s="20"/>
-      <c r="AI48" s="20"/>
-      <c r="AJ48" s="20"/>
-      <c r="AK48" s="20"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
+      <c r="S48" s="15"/>
+      <c r="T48" s="15"/>
+      <c r="U48" s="15"/>
+      <c r="V48" s="15"/>
+      <c r="W48" s="15"/>
+      <c r="X48" s="15"/>
+      <c r="Y48" s="15"/>
+      <c r="Z48" s="16"/>
+      <c r="AA48" s="16"/>
+      <c r="AB48" s="16"/>
+      <c r="AC48" s="17"/>
+      <c r="AD48" s="17"/>
+      <c r="AE48" s="17"/>
+      <c r="AF48" s="17"/>
+      <c r="AG48" s="17"/>
+      <c r="AH48" s="17"/>
+      <c r="AI48" s="17"/>
+      <c r="AJ48" s="17"/>
+      <c r="AK48" s="17"/>
     </row>
     <row r="49" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18"/>
-      <c r="L49" s="18"/>
-      <c r="M49" s="18"/>
-      <c r="N49" s="18"/>
-      <c r="O49" s="18"/>
-      <c r="P49" s="18"/>
-      <c r="Q49" s="18"/>
-      <c r="R49" s="18"/>
-      <c r="S49" s="18"/>
-      <c r="T49" s="18"/>
-      <c r="U49" s="18"/>
-      <c r="V49" s="18"/>
-      <c r="W49" s="18"/>
-      <c r="X49" s="18"/>
-      <c r="Y49" s="18"/>
-      <c r="Z49" s="19"/>
-      <c r="AA49" s="19"/>
-      <c r="AB49" s="19"/>
-      <c r="AC49" s="20"/>
-      <c r="AD49" s="20"/>
-      <c r="AE49" s="20"/>
-      <c r="AF49" s="20"/>
-      <c r="AG49" s="20"/>
-      <c r="AH49" s="20"/>
-      <c r="AI49" s="20"/>
-      <c r="AJ49" s="20"/>
-      <c r="AK49" s="20"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="15"/>
+      <c r="R49" s="15"/>
+      <c r="S49" s="15"/>
+      <c r="T49" s="15"/>
+      <c r="U49" s="15"/>
+      <c r="V49" s="15"/>
+      <c r="W49" s="15"/>
+      <c r="X49" s="15"/>
+      <c r="Y49" s="15"/>
+      <c r="Z49" s="16"/>
+      <c r="AA49" s="16"/>
+      <c r="AB49" s="16"/>
+      <c r="AC49" s="17"/>
+      <c r="AD49" s="17"/>
+      <c r="AE49" s="17"/>
+      <c r="AF49" s="17"/>
+      <c r="AG49" s="17"/>
+      <c r="AH49" s="17"/>
+      <c r="AI49" s="17"/>
+      <c r="AJ49" s="17"/>
+      <c r="AK49" s="17"/>
     </row>
     <row r="50" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="18"/>
-      <c r="N50" s="18"/>
-      <c r="O50" s="18"/>
-      <c r="P50" s="18"/>
-      <c r="Q50" s="18"/>
-      <c r="R50" s="18"/>
-      <c r="S50" s="18"/>
-      <c r="T50" s="18"/>
-      <c r="U50" s="18"/>
-      <c r="V50" s="18"/>
-      <c r="W50" s="18"/>
-      <c r="X50" s="18"/>
-      <c r="Y50" s="18"/>
-      <c r="Z50" s="19"/>
-      <c r="AA50" s="19"/>
-      <c r="AB50" s="19"/>
-      <c r="AC50" s="20"/>
-      <c r="AD50" s="20"/>
-      <c r="AE50" s="20"/>
-      <c r="AF50" s="20"/>
-      <c r="AG50" s="20"/>
-      <c r="AH50" s="20"/>
-      <c r="AI50" s="20"/>
-      <c r="AJ50" s="20"/>
-      <c r="AK50" s="20"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="15"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="15"/>
+      <c r="P50" s="15"/>
+      <c r="Q50" s="15"/>
+      <c r="R50" s="15"/>
+      <c r="S50" s="15"/>
+      <c r="T50" s="15"/>
+      <c r="U50" s="15"/>
+      <c r="V50" s="15"/>
+      <c r="W50" s="15"/>
+      <c r="X50" s="15"/>
+      <c r="Y50" s="15"/>
+      <c r="Z50" s="16"/>
+      <c r="AA50" s="16"/>
+      <c r="AB50" s="16"/>
+      <c r="AC50" s="17"/>
+      <c r="AD50" s="17"/>
+      <c r="AE50" s="17"/>
+      <c r="AF50" s="17"/>
+      <c r="AG50" s="17"/>
+      <c r="AH50" s="17"/>
+      <c r="AI50" s="17"/>
+      <c r="AJ50" s="17"/>
+      <c r="AK50" s="17"/>
     </row>
     <row r="51" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18"/>
-      <c r="L51" s="18"/>
-      <c r="M51" s="18"/>
-      <c r="N51" s="18"/>
-      <c r="O51" s="18"/>
-      <c r="P51" s="18"/>
-      <c r="Q51" s="18"/>
-      <c r="R51" s="18"/>
-      <c r="S51" s="18"/>
-      <c r="T51" s="18"/>
-      <c r="U51" s="18"/>
-      <c r="V51" s="18"/>
-      <c r="W51" s="18"/>
-      <c r="X51" s="18"/>
-      <c r="Y51" s="18"/>
-      <c r="Z51" s="19"/>
-      <c r="AA51" s="19"/>
-      <c r="AB51" s="19"/>
-      <c r="AC51" s="20"/>
-      <c r="AD51" s="20"/>
-      <c r="AE51" s="20"/>
-      <c r="AF51" s="20"/>
-      <c r="AG51" s="20"/>
-      <c r="AH51" s="20"/>
-      <c r="AI51" s="20"/>
-      <c r="AJ51" s="20"/>
-      <c r="AK51" s="20"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
+      <c r="Q51" s="15"/>
+      <c r="R51" s="15"/>
+      <c r="S51" s="15"/>
+      <c r="T51" s="15"/>
+      <c r="U51" s="15"/>
+      <c r="V51" s="15"/>
+      <c r="W51" s="15"/>
+      <c r="X51" s="15"/>
+      <c r="Y51" s="15"/>
+      <c r="Z51" s="16"/>
+      <c r="AA51" s="16"/>
+      <c r="AB51" s="16"/>
+      <c r="AC51" s="17"/>
+      <c r="AD51" s="17"/>
+      <c r="AE51" s="17"/>
+      <c r="AF51" s="17"/>
+      <c r="AG51" s="17"/>
+      <c r="AH51" s="17"/>
+      <c r="AI51" s="17"/>
+      <c r="AJ51" s="17"/>
+      <c r="AK51" s="17"/>
     </row>
     <row r="52" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I52" s="18"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="18"/>
-      <c r="L52" s="18"/>
-      <c r="M52" s="18"/>
-      <c r="N52" s="18"/>
-      <c r="O52" s="18"/>
-      <c r="P52" s="18"/>
-      <c r="Q52" s="18"/>
-      <c r="R52" s="18"/>
-      <c r="S52" s="18"/>
-      <c r="T52" s="18"/>
-      <c r="U52" s="18"/>
-      <c r="V52" s="18"/>
-      <c r="W52" s="18"/>
-      <c r="X52" s="18"/>
-      <c r="Y52" s="18"/>
-      <c r="Z52" s="19"/>
-      <c r="AA52" s="19"/>
-      <c r="AB52" s="19"/>
-      <c r="AC52" s="20"/>
-      <c r="AD52" s="20"/>
-      <c r="AE52" s="20"/>
-      <c r="AF52" s="20"/>
-      <c r="AG52" s="20"/>
-      <c r="AH52" s="20"/>
-      <c r="AI52" s="20"/>
-      <c r="AJ52" s="20"/>
-      <c r="AK52" s="20"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="15"/>
+      <c r="O52" s="15"/>
+      <c r="P52" s="15"/>
+      <c r="Q52" s="15"/>
+      <c r="R52" s="15"/>
+      <c r="S52" s="15"/>
+      <c r="T52" s="15"/>
+      <c r="U52" s="15"/>
+      <c r="V52" s="15"/>
+      <c r="W52" s="15"/>
+      <c r="X52" s="15"/>
+      <c r="Y52" s="15"/>
+      <c r="Z52" s="16"/>
+      <c r="AA52" s="16"/>
+      <c r="AB52" s="16"/>
+      <c r="AC52" s="17"/>
+      <c r="AD52" s="17"/>
+      <c r="AE52" s="17"/>
+      <c r="AF52" s="17"/>
+      <c r="AG52" s="17"/>
+      <c r="AH52" s="17"/>
+      <c r="AI52" s="17"/>
+      <c r="AJ52" s="17"/>
+      <c r="AK52" s="17"/>
     </row>
     <row r="53" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I53" s="18"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="18"/>
-      <c r="L53" s="18"/>
-      <c r="M53" s="18"/>
-      <c r="N53" s="18"/>
-      <c r="O53" s="18"/>
-      <c r="P53" s="18"/>
-      <c r="Q53" s="18"/>
-      <c r="R53" s="18"/>
-      <c r="S53" s="18"/>
-      <c r="T53" s="18"/>
-      <c r="U53" s="18"/>
-      <c r="V53" s="18"/>
-      <c r="W53" s="18"/>
-      <c r="X53" s="18"/>
-      <c r="Y53" s="18"/>
-      <c r="Z53" s="19"/>
-      <c r="AA53" s="19"/>
-      <c r="AB53" s="19"/>
-      <c r="AC53" s="20"/>
-      <c r="AD53" s="20"/>
-      <c r="AE53" s="20"/>
-      <c r="AF53" s="20"/>
-      <c r="AG53" s="20"/>
-      <c r="AH53" s="20"/>
-      <c r="AI53" s="20"/>
-      <c r="AJ53" s="20"/>
-      <c r="AK53" s="20"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="15"/>
+      <c r="S53" s="15"/>
+      <c r="T53" s="15"/>
+      <c r="U53" s="15"/>
+      <c r="V53" s="15"/>
+      <c r="W53" s="15"/>
+      <c r="X53" s="15"/>
+      <c r="Y53" s="15"/>
+      <c r="Z53" s="16"/>
+      <c r="AA53" s="16"/>
+      <c r="AB53" s="16"/>
+      <c r="AC53" s="17"/>
+      <c r="AD53" s="17"/>
+      <c r="AE53" s="17"/>
+      <c r="AF53" s="17"/>
+      <c r="AG53" s="17"/>
+      <c r="AH53" s="17"/>
+      <c r="AI53" s="17"/>
+      <c r="AJ53" s="17"/>
+      <c r="AK53" s="17"/>
     </row>
     <row r="54" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I54" s="18"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="18"/>
-      <c r="L54" s="18"/>
-      <c r="M54" s="18"/>
-      <c r="N54" s="18"/>
-      <c r="O54" s="18"/>
-      <c r="P54" s="18"/>
-      <c r="Q54" s="18"/>
-      <c r="R54" s="18"/>
-      <c r="S54" s="18"/>
-      <c r="T54" s="18"/>
-      <c r="U54" s="18"/>
-      <c r="V54" s="18"/>
-      <c r="W54" s="18"/>
-      <c r="X54" s="18"/>
-      <c r="Y54" s="18"/>
-      <c r="Z54" s="19"/>
-      <c r="AA54" s="19"/>
-      <c r="AB54" s="19"/>
-      <c r="AC54" s="20"/>
-      <c r="AD54" s="20"/>
-      <c r="AE54" s="20"/>
-      <c r="AF54" s="20"/>
-      <c r="AG54" s="20"/>
-      <c r="AH54" s="20"/>
-      <c r="AI54" s="20"/>
-      <c r="AJ54" s="20"/>
-      <c r="AK54" s="20"/>
-    </row>
-    <row r="55" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I55" s="18"/>
-      <c r="J55" s="18"/>
-      <c r="K55" s="18"/>
-      <c r="L55" s="18"/>
-      <c r="M55" s="18"/>
-      <c r="N55" s="18"/>
-      <c r="O55" s="18"/>
-      <c r="P55" s="18"/>
-      <c r="Q55" s="18"/>
-      <c r="R55" s="18"/>
-      <c r="S55" s="18"/>
-      <c r="T55" s="18"/>
-      <c r="U55" s="18"/>
-      <c r="V55" s="18"/>
-      <c r="W55" s="18"/>
-      <c r="X55" s="18"/>
-      <c r="Y55" s="18"/>
-      <c r="Z55" s="19"/>
-      <c r="AA55" s="19"/>
-      <c r="AB55" s="19"/>
-      <c r="AC55" s="20"/>
-      <c r="AD55" s="20"/>
-      <c r="AE55" s="20"/>
-      <c r="AF55" s="20"/>
-      <c r="AG55" s="20"/>
-      <c r="AH55" s="20"/>
-      <c r="AI55" s="20"/>
-      <c r="AJ55" s="20"/>
-      <c r="AK55" s="20"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
+      <c r="S54" s="15"/>
+      <c r="T54" s="15"/>
+      <c r="U54" s="15"/>
+      <c r="V54" s="15"/>
+      <c r="W54" s="15"/>
+      <c r="X54" s="15"/>
+      <c r="Y54" s="15"/>
+      <c r="Z54" s="16"/>
+      <c r="AA54" s="16"/>
+      <c r="AB54" s="16"/>
+      <c r="AC54" s="17"/>
+      <c r="AD54" s="17"/>
+      <c r="AE54" s="17"/>
+      <c r="AF54" s="17"/>
+      <c r="AG54" s="17"/>
+      <c r="AH54" s="17"/>
+      <c r="AI54" s="17"/>
+      <c r="AJ54" s="17"/>
+      <c r="AK54" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="Z2:AN2"/>
-    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="Z1:AN1"/>
+    <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="G7:J8"/>
-    <mergeCell ref="B7:F8"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="L40:Q40"/>
+    <mergeCell ref="L41:R41"/>
+    <mergeCell ref="W39:AA41"/>
+    <mergeCell ref="AB39:AE41"/>
   </mergeCells>
-  <conditionalFormatting sqref="E5:BJ5">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThanOrEqual">
-      <formula>$O$48</formula>
+  <conditionalFormatting sqref="E4:CU4">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThanOrEqual">
+      <formula>$O$47</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4245,10 +4782,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
-  <dimension ref="A2:BJ49"/>
+  <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BG6" sqref="BG6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL39" sqref="AL39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4256,492 +4793,1022 @@
     <col min="2" max="4" width="5.7109375" style="1" customWidth="1"/>
     <col min="5" max="25" width="4.7109375" style="2" customWidth="1"/>
     <col min="26" max="28" width="4.7109375" style="3" customWidth="1"/>
-    <col min="29" max="62" width="4.7109375" customWidth="1"/>
+    <col min="29" max="99" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:62" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z2" s="32" t="s">
+    <row r="1" spans="1:99" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="32"/>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
     </row>
-    <row r="3" spans="1:62" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:62" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A4" s="39" t="s">
+    <row r="2" spans="1:99" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:99" s="37" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="4">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="4">
+        <v>43885</v>
+      </c>
+      <c r="F3" s="4">
+        <v>43886</v>
+      </c>
+      <c r="G3" s="4">
+        <v>43887</v>
+      </c>
+      <c r="H3" s="4">
         <v>43888</v>
       </c>
-      <c r="F4" s="4">
+      <c r="I3" s="4">
         <v>43889</v>
       </c>
-      <c r="G4" s="4">
+      <c r="J3" s="4">
         <v>43890</v>
       </c>
-      <c r="H4" s="4">
+      <c r="K3" s="4">
         <v>43891</v>
       </c>
-      <c r="I4" s="4">
+      <c r="L3" s="4">
         <v>43892</v>
       </c>
-      <c r="J4" s="4">
+      <c r="M3" s="4">
         <v>43893</v>
       </c>
-      <c r="K4" s="4">
+      <c r="N3" s="4">
         <v>43894</v>
       </c>
-      <c r="L4" s="4">
+      <c r="O3" s="4">
         <v>43895</v>
       </c>
-      <c r="M4" s="4">
+      <c r="P3" s="4">
         <v>43896</v>
       </c>
-      <c r="N4" s="4">
+      <c r="Q3" s="4">
         <v>43897</v>
       </c>
-      <c r="O4" s="4">
+      <c r="R3" s="4">
         <v>43898</v>
       </c>
-      <c r="P4" s="4">
+      <c r="S3" s="4">
         <v>43899</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="T3" s="9">
         <v>43900</v>
       </c>
-      <c r="R4" s="10">
+      <c r="U3" s="10">
         <v>43901</v>
       </c>
-      <c r="S4" s="4">
+      <c r="V3" s="4">
         <v>43902</v>
       </c>
-      <c r="T4" s="4">
+      <c r="W3" s="4">
         <v>43903</v>
       </c>
-      <c r="U4" s="4">
+      <c r="X3" s="4">
         <v>43904</v>
       </c>
-      <c r="V4" s="4">
+      <c r="Y3" s="4">
         <v>43905</v>
       </c>
-      <c r="W4" s="4">
+      <c r="Z3" s="4">
         <v>43906</v>
       </c>
-      <c r="X4" s="4">
+      <c r="AA3" s="4">
         <v>43907</v>
       </c>
-      <c r="Y4" s="4">
+      <c r="AB3" s="4">
         <v>43908</v>
       </c>
-      <c r="Z4" s="4">
+      <c r="AC3" s="4">
         <v>43909</v>
       </c>
-      <c r="AA4" s="4">
+      <c r="AD3" s="4">
         <v>43910</v>
       </c>
-      <c r="AB4" s="4">
+      <c r="AE3" s="4">
         <v>43911</v>
       </c>
-      <c r="AC4" s="9">
+      <c r="AF3" s="9">
         <v>43912</v>
       </c>
-      <c r="AD4" s="17">
+      <c r="AG3" s="14">
         <v>43913</v>
       </c>
-      <c r="AE4" s="4">
+      <c r="AH3" s="4">
         <v>43914</v>
       </c>
-      <c r="AF4" s="4">
+      <c r="AI3" s="4">
         <v>43915</v>
       </c>
-      <c r="AG4" s="4">
+      <c r="AJ3" s="4">
         <v>43916</v>
       </c>
-      <c r="AH4" s="4">
+      <c r="AK3" s="4">
         <v>43917</v>
       </c>
-      <c r="AI4" s="4">
+      <c r="AL3" s="4">
         <v>43918</v>
       </c>
-      <c r="AJ4" s="4">
+      <c r="AM3" s="4">
         <v>43919</v>
       </c>
-      <c r="AK4" s="4">
+      <c r="AN3" s="4">
         <v>43920</v>
       </c>
-      <c r="AL4" s="4">
+      <c r="AO3" s="4">
         <v>43921</v>
       </c>
-      <c r="AM4" s="4">
+      <c r="AP3" s="4">
         <v>43922</v>
       </c>
-      <c r="AN4" s="4">
+      <c r="AQ3" s="4">
         <v>43923</v>
       </c>
-      <c r="AO4" s="4">
+      <c r="AR3" s="4">
         <v>43924</v>
       </c>
-      <c r="AP4" s="4">
+      <c r="AS3" s="4">
         <v>43925</v>
       </c>
-      <c r="AQ4" s="4">
+      <c r="AT3" s="4">
         <v>43926</v>
       </c>
-      <c r="AR4" s="4">
+      <c r="AU3" s="4">
         <v>43927</v>
       </c>
-      <c r="AS4" s="4">
+      <c r="AV3" s="4">
         <v>43928</v>
       </c>
-      <c r="AT4" s="4">
+      <c r="AW3" s="4">
         <v>43929</v>
       </c>
-      <c r="AU4" s="4">
+      <c r="AX3" s="4">
         <v>43930</v>
       </c>
-      <c r="AV4" s="4">
+      <c r="AY3" s="4">
         <v>43931</v>
       </c>
-      <c r="AW4" s="4">
+      <c r="AZ3" s="4">
         <v>43932</v>
       </c>
-      <c r="AX4" s="4">
+      <c r="BA3" s="4">
         <v>43933</v>
       </c>
-      <c r="AY4" s="4">
+      <c r="BB3" s="4">
         <v>43934</v>
       </c>
-      <c r="AZ4" s="4">
+      <c r="BC3" s="4">
         <v>43935</v>
       </c>
-      <c r="BA4" s="4">
+      <c r="BD3" s="4">
         <v>43936</v>
       </c>
-      <c r="BB4" s="4">
+      <c r="BE3" s="4">
         <v>43937</v>
       </c>
-      <c r="BC4" s="4">
+      <c r="BF3" s="4">
         <v>43938</v>
       </c>
-      <c r="BD4" s="4">
+      <c r="BG3" s="4">
         <v>43939</v>
       </c>
-      <c r="BE4" s="4">
+      <c r="BH3" s="4">
         <v>43940</v>
       </c>
-      <c r="BF4" s="4">
+      <c r="BI3" s="4">
         <v>43941</v>
       </c>
-      <c r="BG4" s="4">
+      <c r="BJ3" s="4">
         <v>43942</v>
       </c>
-      <c r="BH4" s="4">
+      <c r="BK3" s="4">
         <v>43943</v>
       </c>
-      <c r="BI4" s="4">
+      <c r="BL3" s="4">
         <v>43944</v>
       </c>
-      <c r="BJ4" s="4">
+      <c r="BM3" s="4">
         <v>43945</v>
       </c>
+      <c r="BN3" s="4">
+        <v>43946</v>
+      </c>
+      <c r="BO3" s="4">
+        <v>43947</v>
+      </c>
+      <c r="BP3" s="4">
+        <v>43948</v>
+      </c>
+      <c r="BQ3" s="4">
+        <v>43949</v>
+      </c>
+      <c r="BR3" s="4">
+        <v>43950</v>
+      </c>
+      <c r="BS3" s="4">
+        <v>43951</v>
+      </c>
+      <c r="BT3" s="4">
+        <v>43952</v>
+      </c>
+      <c r="BU3" s="4">
+        <v>43953</v>
+      </c>
+      <c r="BV3" s="4">
+        <v>43954</v>
+      </c>
+      <c r="BW3" s="4">
+        <v>43955</v>
+      </c>
+      <c r="BX3" s="4">
+        <v>43956</v>
+      </c>
+      <c r="BY3" s="4">
+        <v>43957</v>
+      </c>
+      <c r="BZ3" s="4">
+        <v>43958</v>
+      </c>
+      <c r="CA3" s="4">
+        <v>43959</v>
+      </c>
+      <c r="CB3" s="4">
+        <v>43960</v>
+      </c>
+      <c r="CC3" s="4">
+        <v>43961</v>
+      </c>
+      <c r="CD3" s="4">
+        <v>43962</v>
+      </c>
+      <c r="CE3" s="4">
+        <v>43963</v>
+      </c>
+      <c r="CF3" s="4">
+        <v>43964</v>
+      </c>
+      <c r="CG3" s="4">
+        <v>43965</v>
+      </c>
+      <c r="CH3" s="4">
+        <v>43966</v>
+      </c>
+      <c r="CI3" s="4">
+        <v>43967</v>
+      </c>
+      <c r="CJ3" s="4">
+        <v>43968</v>
+      </c>
+      <c r="CK3" s="4">
+        <v>43969</v>
+      </c>
+      <c r="CL3" s="4">
+        <v>43970</v>
+      </c>
+      <c r="CM3" s="4">
+        <v>43971</v>
+      </c>
+      <c r="CN3" s="4">
+        <v>43972</v>
+      </c>
+      <c r="CO3" s="4">
+        <v>43973</v>
+      </c>
+      <c r="CP3" s="4">
+        <v>43974</v>
+      </c>
+      <c r="CQ3" s="4">
+        <v>43975</v>
+      </c>
+      <c r="CR3" s="4">
+        <v>43976</v>
+      </c>
+      <c r="CS3" s="4">
+        <v>43977</v>
+      </c>
+      <c r="CT3" s="4">
+        <v>43978</v>
+      </c>
+      <c r="CU3" s="4">
+        <v>43979</v>
+      </c>
     </row>
-    <row r="5" spans="1:62" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A5" s="35" t="s">
+    <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="29">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="22">
+        <v>0</v>
+      </c>
+      <c r="F4" s="22">
+        <v>0</v>
+      </c>
+      <c r="G4" s="22">
+        <v>0</v>
+      </c>
+      <c r="H4" s="22">
         <v>3</v>
       </c>
-      <c r="F5" s="29">
+      <c r="I4" s="22">
         <v>1</v>
       </c>
-      <c r="G5" s="29">
+      <c r="J4" s="22">
         <v>9</v>
       </c>
-      <c r="H5" s="29">
+      <c r="K4" s="22">
         <v>4</v>
       </c>
-      <c r="I5" s="29">
+      <c r="L4" s="22">
         <v>0</v>
       </c>
-      <c r="J5" s="29">
+      <c r="M4" s="22">
         <v>13</v>
       </c>
-      <c r="K5" s="29">
+      <c r="N4" s="22">
         <v>1</v>
       </c>
-      <c r="L5" s="29">
+      <c r="O4" s="22">
         <v>14</v>
       </c>
-      <c r="M5" s="29">
+      <c r="P4" s="22">
         <v>12</v>
       </c>
-      <c r="N5" s="29">
+      <c r="Q4" s="22">
         <v>4</v>
       </c>
-      <c r="O5" s="29">
+      <c r="R4" s="22">
         <v>29</v>
       </c>
-      <c r="P5" s="29">
+      <c r="S4" s="22">
         <v>19</v>
       </c>
-      <c r="Q5" s="29">
+      <c r="T4" s="22">
         <v>7</v>
       </c>
-      <c r="R5" s="29">
+      <c r="U4" s="22">
         <v>23</v>
       </c>
-      <c r="S5" s="29">
+      <c r="V4" s="22">
         <v>25</v>
       </c>
-      <c r="T5" s="29">
+      <c r="W4" s="22">
         <v>29</v>
       </c>
-      <c r="U5" s="29">
+      <c r="X4" s="22">
         <v>30</v>
       </c>
-      <c r="V5" s="29">
+      <c r="Y4" s="22">
         <v>40</v>
       </c>
-      <c r="W5" s="29">
+      <c r="Z4" s="22">
         <v>65</v>
       </c>
-      <c r="X5" s="29">
+      <c r="AA4" s="22">
         <v>60</v>
       </c>
-      <c r="Y5" s="29">
+      <c r="AB4" s="22">
         <v>100</v>
       </c>
-      <c r="Z5" s="29">
+      <c r="AC4" s="22">
         <v>82</v>
       </c>
-      <c r="AA5" s="29">
+      <c r="AD4" s="22">
         <v>97</v>
       </c>
-      <c r="AB5" s="29">
+      <c r="AE4" s="22">
         <v>91</v>
       </c>
-      <c r="AC5" s="30">
+      <c r="AF4" s="23">
         <v>73</v>
       </c>
-      <c r="AD5" s="30">
+      <c r="AG4" s="23">
         <v>63</v>
       </c>
-      <c r="AE5" s="30">
+      <c r="AH4" s="23">
         <v>63</v>
       </c>
-      <c r="AF5" s="30">
+      <c r="AI4" s="23">
         <v>80</v>
       </c>
-      <c r="AG5" s="30">
+      <c r="AJ4" s="23">
         <v>97</v>
       </c>
-      <c r="AH5" s="30">
+      <c r="AK4" s="23">
         <v>123</v>
       </c>
-      <c r="AI5" s="30">
+      <c r="AL4" s="23">
         <v>115</v>
       </c>
-      <c r="AJ5" s="30">
+      <c r="AM4" s="23">
         <v>149</v>
       </c>
-      <c r="AK5" s="30">
+      <c r="AN4" s="23">
         <v>183</v>
       </c>
-      <c r="AL5" s="30">
+      <c r="AO4" s="23">
         <v>132</v>
       </c>
-      <c r="AM5" s="30">
+      <c r="AP4" s="23">
         <v>105</v>
       </c>
-      <c r="AN5" s="30">
+      <c r="AQ4" s="23">
         <v>164</v>
       </c>
-      <c r="AO5" s="30">
+      <c r="AR4" s="23">
         <v>212</v>
       </c>
-      <c r="AP5" s="30">
+      <c r="AS4" s="23">
         <v>144</v>
       </c>
-      <c r="AQ5" s="30">
+      <c r="AT4" s="23">
         <v>125</v>
       </c>
-      <c r="AR5" s="30">
+      <c r="AU4" s="23">
         <v>77</v>
       </c>
-      <c r="AS5" s="30">
+      <c r="AV4" s="23">
         <v>67</v>
       </c>
-      <c r="AT5" s="30">
+      <c r="AW4" s="23">
         <v>94</v>
       </c>
-      <c r="AU5" s="30">
+      <c r="AX4" s="23">
         <v>14</v>
       </c>
-      <c r="AV5" s="30">
+      <c r="AY4" s="23">
         <v>90</v>
       </c>
-      <c r="AW5" s="30">
+      <c r="AZ4" s="23">
         <v>39</v>
       </c>
-      <c r="AX5" s="30">
+      <c r="BA4" s="23">
         <v>55</v>
       </c>
-      <c r="AY5" s="30">
+      <c r="BB4" s="23">
         <v>5</v>
       </c>
-      <c r="AZ5" s="30">
+      <c r="BC4" s="23">
         <v>32</v>
       </c>
-      <c r="BA5" s="30">
+      <c r="BD4" s="23">
         <v>-7</v>
       </c>
-      <c r="BB5" s="30">
+      <c r="BE4" s="23">
         <v>31</v>
       </c>
-      <c r="BC5" s="30">
+      <c r="BF4" s="23">
         <v>-91</v>
       </c>
-      <c r="BD5" s="30">
+      <c r="BG4" s="23">
         <v>18</v>
       </c>
-      <c r="BE5" s="30">
+      <c r="BH4" s="23">
         <v>12</v>
       </c>
-      <c r="BF5" s="30">
+      <c r="BI4" s="23">
         <v>-3</v>
       </c>
-      <c r="BG5" s="30">
+      <c r="BJ4" s="23">
         <v>-73</v>
       </c>
-      <c r="BH5" s="30"/>
-      <c r="BI5" s="30"/>
-      <c r="BJ5" s="30"/>
+      <c r="BK4" s="23">
+        <v>52</v>
+      </c>
+      <c r="BL4" s="23"/>
+      <c r="BM4" s="23"/>
+      <c r="BN4" s="23"/>
+      <c r="BO4" s="23"/>
+      <c r="BP4" s="23"/>
+      <c r="BQ4" s="23"/>
+      <c r="BR4" s="23"/>
+      <c r="BS4" s="23"/>
+      <c r="BT4" s="23"/>
+      <c r="BU4" s="23"/>
+      <c r="BV4" s="23"/>
+      <c r="BW4" s="23"/>
+      <c r="BX4" s="23"/>
+      <c r="BY4" s="23"/>
+      <c r="BZ4" s="23"/>
+      <c r="CA4" s="23"/>
+      <c r="CB4" s="23"/>
+      <c r="CC4" s="23"/>
+      <c r="CD4" s="23"/>
+      <c r="CE4" s="23"/>
+      <c r="CF4" s="23"/>
+      <c r="CG4" s="23"/>
+      <c r="CH4" s="23"/>
+      <c r="CI4" s="23"/>
+      <c r="CJ4" s="23"/>
+      <c r="CK4" s="23"/>
+      <c r="CL4" s="23"/>
+      <c r="CM4" s="23"/>
+      <c r="CN4" s="23"/>
+      <c r="CO4" s="23"/>
+      <c r="CP4" s="23"/>
+      <c r="CQ4" s="23"/>
+      <c r="CR4" s="23"/>
+      <c r="CS4" s="23"/>
+      <c r="CT4" s="23"/>
+      <c r="CU4" s="23"/>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="AF6" s="11"/>
+    <row r="6" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:99" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="I14" s="12"/>
     </row>
-    <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="38" t="s">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K39" s="5"/>
+      <c r="L39" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="M39" s="30"/>
+      <c r="N39" s="30"/>
+      <c r="O39" s="30"/>
+      <c r="W39" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="40">
-        <f>SUM(E5:BG5)</f>
-        <v>2946</v>
-      </c>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="28">
+        <f>SUM(E4:CU4)</f>
+        <v>2998</v>
+      </c>
+      <c r="AC39" s="28"/>
+      <c r="AD39" s="28"/>
+      <c r="AE39" s="28"/>
     </row>
-    <row r="8" spans="1:62" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
+    <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K40" s="13"/>
+      <c r="L40" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="M40" s="24"/>
+      <c r="N40" s="24"/>
+      <c r="O40" s="24"/>
+      <c r="P40" s="24"/>
+      <c r="Q40" s="24"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="28"/>
+      <c r="AC40" s="28"/>
+      <c r="AD40" s="28"/>
+      <c r="AE40" s="28"/>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
+    <row r="41" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="K41" s="11"/>
+      <c r="L41" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M41" s="24"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
+      <c r="Q41" s="24"/>
+      <c r="R41" s="24"/>
+      <c r="W41" s="29"/>
+      <c r="X41" s="29"/>
+      <c r="Y41" s="29"/>
+      <c r="Z41" s="29"/>
+      <c r="AA41" s="29"/>
+      <c r="AB41" s="28"/>
+      <c r="AC41" s="28"/>
+      <c r="AD41" s="28"/>
+      <c r="AE41" s="28"/>
     </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
+    <row r="43" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+      <c r="S43" s="15"/>
+      <c r="T43" s="15"/>
+      <c r="U43" s="15"/>
+      <c r="V43" s="15"/>
+      <c r="W43" s="15"/>
+      <c r="X43" s="15"/>
+      <c r="Y43" s="15"/>
+      <c r="Z43" s="16"/>
+      <c r="AA43" s="16"/>
+      <c r="AB43" s="16"/>
+      <c r="AC43" s="17"/>
+      <c r="AD43" s="17"/>
+      <c r="AE43" s="17"/>
+      <c r="AF43" s="17"/>
+      <c r="AG43" s="17"/>
+      <c r="AH43" s="17"/>
+      <c r="AI43" s="17"/>
+      <c r="AJ43" s="17"/>
+      <c r="AK43" s="17"/>
     </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="B15" s="12"/>
-      <c r="C15" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+    <row r="44" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="15"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="15"/>
+      <c r="X44" s="15"/>
+      <c r="Y44" s="15"/>
+      <c r="Z44" s="16"/>
+      <c r="AA44" s="16"/>
+      <c r="AB44" s="16"/>
+      <c r="AC44" s="17"/>
+      <c r="AD44" s="17"/>
+      <c r="AE44" s="17"/>
+      <c r="AF44" s="17"/>
+      <c r="AG44" s="17"/>
+      <c r="AH44" s="17"/>
+      <c r="AI44" s="17"/>
+      <c r="AJ44" s="17"/>
+      <c r="AK44" s="17"/>
     </row>
-    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="B16" s="23"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
+    <row r="45" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="15"/>
+      <c r="S45" s="15"/>
+      <c r="T45" s="15"/>
+      <c r="U45" s="15"/>
+      <c r="V45" s="15"/>
+      <c r="W45" s="15"/>
+      <c r="X45" s="15"/>
+      <c r="Y45" s="15"/>
+      <c r="Z45" s="16"/>
+      <c r="AA45" s="16"/>
+      <c r="AB45" s="16"/>
+      <c r="AC45" s="17"/>
+      <c r="AD45" s="17"/>
+      <c r="AE45" s="17"/>
+      <c r="AF45" s="17"/>
+      <c r="AG45" s="17"/>
+      <c r="AH45" s="17"/>
+      <c r="AI45" s="17"/>
+      <c r="AJ45" s="17"/>
+      <c r="AK45" s="17"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
+    <row r="46" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="15"/>
+      <c r="R46" s="15"/>
+      <c r="S46" s="15"/>
+      <c r="T46" s="15"/>
+      <c r="U46" s="15"/>
+      <c r="V46" s="15"/>
+      <c r="W46" s="15"/>
+      <c r="X46" s="15"/>
+      <c r="Y46" s="15"/>
+      <c r="Z46" s="16"/>
+      <c r="AA46" s="16"/>
+      <c r="AB46" s="16"/>
+      <c r="AC46" s="17"/>
+      <c r="AD46" s="17"/>
+      <c r="AE46" s="17"/>
+      <c r="AF46" s="17"/>
+      <c r="AG46" s="17"/>
+      <c r="AH46" s="17"/>
+      <c r="AI46" s="17"/>
+      <c r="AJ46" s="17"/>
+      <c r="AK46" s="17"/>
     </row>
-    <row r="48" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P48" s="14" t="s">
+    <row r="47" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="Q48" s="15">
-        <f>MAXA(G5:BL5)</f>
+      <c r="O47" s="19">
+        <f>MAXA(E4:BJ4)</f>
         <v>212</v>
       </c>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+      <c r="S47" s="15"/>
+      <c r="T47" s="15"/>
+      <c r="U47" s="15"/>
+      <c r="V47" s="15"/>
+      <c r="W47" s="15"/>
+      <c r="X47" s="15"/>
+      <c r="Y47" s="15"/>
+      <c r="Z47" s="16"/>
+      <c r="AA47" s="16"/>
+      <c r="AB47" s="16"/>
+      <c r="AC47" s="17"/>
+      <c r="AD47" s="17"/>
+      <c r="AE47" s="17"/>
+      <c r="AF47" s="17"/>
+      <c r="AG47" s="17"/>
+      <c r="AH47" s="17"/>
+      <c r="AI47" s="17"/>
+      <c r="AJ47" s="17"/>
+      <c r="AK47" s="17"/>
     </row>
-    <row r="49" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P49" s="18"/>
-      <c r="Q49" s="18"/>
+    <row r="48" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
+      <c r="S48" s="15"/>
+      <c r="T48" s="15"/>
+      <c r="U48" s="15"/>
+      <c r="V48" s="15"/>
+      <c r="W48" s="15"/>
+      <c r="X48" s="15"/>
+      <c r="Y48" s="15"/>
+      <c r="Z48" s="16"/>
+      <c r="AA48" s="16"/>
+      <c r="AB48" s="16"/>
+      <c r="AC48" s="17"/>
+      <c r="AD48" s="17"/>
+      <c r="AE48" s="17"/>
+      <c r="AF48" s="17"/>
+      <c r="AG48" s="17"/>
+      <c r="AH48" s="17"/>
+      <c r="AI48" s="17"/>
+      <c r="AJ48" s="17"/>
+      <c r="AK48" s="17"/>
+    </row>
+    <row r="49" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="15"/>
+      <c r="R49" s="15"/>
+      <c r="S49" s="15"/>
+      <c r="T49" s="15"/>
+      <c r="U49" s="15"/>
+      <c r="V49" s="15"/>
+      <c r="W49" s="15"/>
+      <c r="X49" s="15"/>
+      <c r="Y49" s="15"/>
+      <c r="Z49" s="16"/>
+      <c r="AA49" s="16"/>
+      <c r="AB49" s="16"/>
+      <c r="AC49" s="17"/>
+      <c r="AD49" s="17"/>
+      <c r="AE49" s="17"/>
+      <c r="AF49" s="17"/>
+      <c r="AG49" s="17"/>
+      <c r="AH49" s="17"/>
+      <c r="AI49" s="17"/>
+      <c r="AJ49" s="17"/>
+      <c r="AK49" s="17"/>
+    </row>
+    <row r="50" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="15"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="15"/>
+      <c r="P50" s="15"/>
+      <c r="Q50" s="15"/>
+      <c r="R50" s="15"/>
+      <c r="S50" s="15"/>
+      <c r="T50" s="15"/>
+      <c r="U50" s="15"/>
+      <c r="V50" s="15"/>
+      <c r="W50" s="15"/>
+      <c r="X50" s="15"/>
+      <c r="Y50" s="15"/>
+      <c r="Z50" s="16"/>
+      <c r="AA50" s="16"/>
+      <c r="AB50" s="16"/>
+      <c r="AC50" s="17"/>
+      <c r="AD50" s="17"/>
+      <c r="AE50" s="17"/>
+      <c r="AF50" s="17"/>
+      <c r="AG50" s="17"/>
+      <c r="AH50" s="17"/>
+      <c r="AI50" s="17"/>
+      <c r="AJ50" s="17"/>
+      <c r="AK50" s="17"/>
+    </row>
+    <row r="51" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
+      <c r="Q51" s="15"/>
+      <c r="R51" s="15"/>
+      <c r="S51" s="15"/>
+      <c r="T51" s="15"/>
+      <c r="U51" s="15"/>
+      <c r="V51" s="15"/>
+      <c r="W51" s="15"/>
+      <c r="X51" s="15"/>
+      <c r="Y51" s="15"/>
+      <c r="Z51" s="16"/>
+      <c r="AA51" s="16"/>
+      <c r="AB51" s="16"/>
+      <c r="AC51" s="17"/>
+      <c r="AD51" s="17"/>
+      <c r="AE51" s="17"/>
+      <c r="AF51" s="17"/>
+      <c r="AG51" s="17"/>
+      <c r="AH51" s="17"/>
+      <c r="AI51" s="17"/>
+      <c r="AJ51" s="17"/>
+      <c r="AK51" s="17"/>
+    </row>
+    <row r="52" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="15"/>
+      <c r="O52" s="15"/>
+      <c r="P52" s="15"/>
+      <c r="Q52" s="15"/>
+      <c r="R52" s="15"/>
+      <c r="S52" s="15"/>
+      <c r="T52" s="15"/>
+      <c r="U52" s="15"/>
+      <c r="V52" s="15"/>
+      <c r="W52" s="15"/>
+      <c r="X52" s="15"/>
+      <c r="Y52" s="15"/>
+      <c r="Z52" s="16"/>
+      <c r="AA52" s="16"/>
+      <c r="AB52" s="16"/>
+      <c r="AC52" s="17"/>
+      <c r="AD52" s="17"/>
+      <c r="AE52" s="17"/>
+      <c r="AF52" s="17"/>
+      <c r="AG52" s="17"/>
+      <c r="AH52" s="17"/>
+      <c r="AI52" s="17"/>
+      <c r="AJ52" s="17"/>
+      <c r="AK52" s="17"/>
+    </row>
+    <row r="53" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="15"/>
+      <c r="S53" s="15"/>
+      <c r="T53" s="15"/>
+      <c r="U53" s="15"/>
+      <c r="V53" s="15"/>
+      <c r="W53" s="15"/>
+      <c r="X53" s="15"/>
+      <c r="Y53" s="15"/>
+      <c r="Z53" s="16"/>
+      <c r="AA53" s="16"/>
+      <c r="AB53" s="16"/>
+      <c r="AC53" s="17"/>
+      <c r="AD53" s="17"/>
+      <c r="AE53" s="17"/>
+      <c r="AF53" s="17"/>
+      <c r="AG53" s="17"/>
+      <c r="AH53" s="17"/>
+      <c r="AI53" s="17"/>
+      <c r="AJ53" s="17"/>
+      <c r="AK53" s="17"/>
+    </row>
+    <row r="54" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
+      <c r="S54" s="15"/>
+      <c r="T54" s="15"/>
+      <c r="U54" s="15"/>
+      <c r="V54" s="15"/>
+      <c r="W54" s="15"/>
+      <c r="X54" s="15"/>
+      <c r="Y54" s="15"/>
+      <c r="Z54" s="16"/>
+      <c r="AA54" s="16"/>
+      <c r="AB54" s="16"/>
+      <c r="AC54" s="17"/>
+      <c r="AD54" s="17"/>
+      <c r="AE54" s="17"/>
+      <c r="AF54" s="17"/>
+      <c r="AG54" s="17"/>
+      <c r="AH54" s="17"/>
+      <c r="AI54" s="17"/>
+      <c r="AJ54" s="17"/>
+      <c r="AK54" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="Z2:AN2"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="W39:AA41"/>
+    <mergeCell ref="AB39:AE41"/>
+    <mergeCell ref="L40:Q40"/>
+    <mergeCell ref="L41:R41"/>
+    <mergeCell ref="Z1:AN1"/>
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:I8"/>
+    <mergeCell ref="A3:D3"/>
   </mergeCells>
-  <conditionalFormatting sqref="E5:BJ5">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
-      <formula>$Q$48</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
-      <formula>$Q$48</formula>
+  <conditionalFormatting sqref="E4:BY4">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
+      <formula>$O$47</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
aggiornamento dati al 23/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761EB0D3-35EE-4F39-B96A-322AFF54BE47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973750A3-3209-49F1-89FD-8A655DEFB589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -400,9 +400,7 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -412,14 +410,17 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="17" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="3" fontId="17" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -439,7 +440,6 @@
     <xf numFmtId="164" fontId="9" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Colore 5" xfId="5" builtinId="46"/>
@@ -450,201 +450,9 @@
     <cellStyle name="Titolo 1" xfId="1" builtinId="16"/>
     <cellStyle name="Titolo 4" xfId="2" builtinId="19"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="2">
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -1329,6 +1137,9 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-851</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2109,6 +1920,9 @@
                 </c:pt>
                 <c:pt idx="55">
                   <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3748,7 +3562,7 @@
   <dimension ref="A1:CU54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT4" sqref="AT4"/>
+      <selection activeCell="BL5" sqref="BL5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4266,7 +4080,9 @@
       <c r="BK4" s="7">
         <v>-10</v>
       </c>
-      <c r="BL4" s="7"/>
+      <c r="BL4" s="7">
+        <v>-851</v>
+      </c>
       <c r="BM4" s="7"/>
       <c r="BN4" s="7"/>
       <c r="BO4" s="7"/>
@@ -4319,67 +4135,67 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K39" s="5"/>
-      <c r="L39" s="30" t="s">
+      <c r="L39" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="30"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="30"/>
-      <c r="W39" s="29" t="s">
+      <c r="M39" s="28"/>
+      <c r="N39" s="28"/>
+      <c r="O39" s="28"/>
+      <c r="W39" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="29"/>
-      <c r="Y39" s="29"/>
-      <c r="Z39" s="29"/>
-      <c r="AA39" s="29"/>
-      <c r="AB39" s="28">
+      <c r="X39" s="30"/>
+      <c r="Y39" s="30"/>
+      <c r="Z39" s="30"/>
+      <c r="AA39" s="30"/>
+      <c r="AB39" s="31">
         <f>SUM(E4:CU4)</f>
-        <v>107699</v>
-      </c>
-      <c r="AC39" s="28"/>
-      <c r="AD39" s="28"/>
-      <c r="AE39" s="28"/>
+        <v>106848</v>
+      </c>
+      <c r="AC39" s="31"/>
+      <c r="AD39" s="31"/>
+      <c r="AE39" s="31"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K40" s="13"/>
-      <c r="L40" s="24" t="s">
+      <c r="L40" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="24"/>
-      <c r="N40" s="24"/>
-      <c r="O40" s="24"/>
-      <c r="P40" s="24"/>
-      <c r="Q40" s="24"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="28"/>
-      <c r="AC40" s="28"/>
-      <c r="AD40" s="28"/>
-      <c r="AE40" s="28"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="29"/>
+      <c r="W40" s="30"/>
+      <c r="X40" s="30"/>
+      <c r="Y40" s="30"/>
+      <c r="Z40" s="30"/>
+      <c r="AA40" s="30"/>
+      <c r="AB40" s="31"/>
+      <c r="AC40" s="31"/>
+      <c r="AD40" s="31"/>
+      <c r="AE40" s="31"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.25">
       <c r="K41" s="11"/>
-      <c r="L41" s="24" t="s">
+      <c r="L41" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="24"/>
-      <c r="N41" s="24"/>
-      <c r="O41" s="24"/>
-      <c r="P41" s="24"/>
-      <c r="Q41" s="24"/>
-      <c r="R41" s="24"/>
-      <c r="W41" s="29"/>
-      <c r="X41" s="29"/>
-      <c r="Y41" s="29"/>
-      <c r="Z41" s="29"/>
-      <c r="AA41" s="29"/>
-      <c r="AB41" s="28"/>
-      <c r="AC41" s="28"/>
-      <c r="AD41" s="28"/>
-      <c r="AE41" s="28"/>
+      <c r="M41" s="29"/>
+      <c r="N41" s="29"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="29"/>
+      <c r="Q41" s="29"/>
+      <c r="R41" s="29"/>
+      <c r="W41" s="30"/>
+      <c r="X41" s="30"/>
+      <c r="Y41" s="30"/>
+      <c r="Z41" s="30"/>
+      <c r="AA41" s="30"/>
+      <c r="AB41" s="31"/>
+      <c r="AC41" s="31"/>
+      <c r="AD41" s="31"/>
+      <c r="AE41" s="31"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I43" s="15"/>
@@ -4517,6 +4333,1045 @@
       <c r="O47" s="19">
         <f>MAXA(E4:BJ4)</f>
         <v>4821</v>
+      </c>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+      <c r="S47" s="15"/>
+      <c r="T47" s="15"/>
+      <c r="U47" s="15"/>
+      <c r="V47" s="15"/>
+      <c r="W47" s="15"/>
+      <c r="X47" s="15"/>
+      <c r="Y47" s="15"/>
+      <c r="Z47" s="16"/>
+      <c r="AA47" s="16"/>
+      <c r="AB47" s="16"/>
+      <c r="AC47" s="17"/>
+      <c r="AD47" s="17"/>
+      <c r="AE47" s="17"/>
+      <c r="AF47" s="17"/>
+      <c r="AG47" s="17"/>
+      <c r="AH47" s="17"/>
+      <c r="AI47" s="17"/>
+      <c r="AJ47" s="17"/>
+      <c r="AK47" s="17"/>
+    </row>
+    <row r="48" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
+      <c r="S48" s="15"/>
+      <c r="T48" s="15"/>
+      <c r="U48" s="15"/>
+      <c r="V48" s="15"/>
+      <c r="W48" s="15"/>
+      <c r="X48" s="15"/>
+      <c r="Y48" s="15"/>
+      <c r="Z48" s="16"/>
+      <c r="AA48" s="16"/>
+      <c r="AB48" s="16"/>
+      <c r="AC48" s="17"/>
+      <c r="AD48" s="17"/>
+      <c r="AE48" s="17"/>
+      <c r="AF48" s="17"/>
+      <c r="AG48" s="17"/>
+      <c r="AH48" s="17"/>
+      <c r="AI48" s="17"/>
+      <c r="AJ48" s="17"/>
+      <c r="AK48" s="17"/>
+    </row>
+    <row r="49" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="15"/>
+      <c r="R49" s="15"/>
+      <c r="S49" s="15"/>
+      <c r="T49" s="15"/>
+      <c r="U49" s="15"/>
+      <c r="V49" s="15"/>
+      <c r="W49" s="15"/>
+      <c r="X49" s="15"/>
+      <c r="Y49" s="15"/>
+      <c r="Z49" s="16"/>
+      <c r="AA49" s="16"/>
+      <c r="AB49" s="16"/>
+      <c r="AC49" s="17"/>
+      <c r="AD49" s="17"/>
+      <c r="AE49" s="17"/>
+      <c r="AF49" s="17"/>
+      <c r="AG49" s="17"/>
+      <c r="AH49" s="17"/>
+      <c r="AI49" s="17"/>
+      <c r="AJ49" s="17"/>
+      <c r="AK49" s="17"/>
+    </row>
+    <row r="50" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="15"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="15"/>
+      <c r="P50" s="15"/>
+      <c r="Q50" s="15"/>
+      <c r="R50" s="15"/>
+      <c r="S50" s="15"/>
+      <c r="T50" s="15"/>
+      <c r="U50" s="15"/>
+      <c r="V50" s="15"/>
+      <c r="W50" s="15"/>
+      <c r="X50" s="15"/>
+      <c r="Y50" s="15"/>
+      <c r="Z50" s="16"/>
+      <c r="AA50" s="16"/>
+      <c r="AB50" s="16"/>
+      <c r="AC50" s="17"/>
+      <c r="AD50" s="17"/>
+      <c r="AE50" s="17"/>
+      <c r="AF50" s="17"/>
+      <c r="AG50" s="17"/>
+      <c r="AH50" s="17"/>
+      <c r="AI50" s="17"/>
+      <c r="AJ50" s="17"/>
+      <c r="AK50" s="17"/>
+    </row>
+    <row r="51" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
+      <c r="Q51" s="15"/>
+      <c r="R51" s="15"/>
+      <c r="S51" s="15"/>
+      <c r="T51" s="15"/>
+      <c r="U51" s="15"/>
+      <c r="V51" s="15"/>
+      <c r="W51" s="15"/>
+      <c r="X51" s="15"/>
+      <c r="Y51" s="15"/>
+      <c r="Z51" s="16"/>
+      <c r="AA51" s="16"/>
+      <c r="AB51" s="16"/>
+      <c r="AC51" s="17"/>
+      <c r="AD51" s="17"/>
+      <c r="AE51" s="17"/>
+      <c r="AF51" s="17"/>
+      <c r="AG51" s="17"/>
+      <c r="AH51" s="17"/>
+      <c r="AI51" s="17"/>
+      <c r="AJ51" s="17"/>
+      <c r="AK51" s="17"/>
+    </row>
+    <row r="52" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="15"/>
+      <c r="O52" s="15"/>
+      <c r="P52" s="15"/>
+      <c r="Q52" s="15"/>
+      <c r="R52" s="15"/>
+      <c r="S52" s="15"/>
+      <c r="T52" s="15"/>
+      <c r="U52" s="15"/>
+      <c r="V52" s="15"/>
+      <c r="W52" s="15"/>
+      <c r="X52" s="15"/>
+      <c r="Y52" s="15"/>
+      <c r="Z52" s="16"/>
+      <c r="AA52" s="16"/>
+      <c r="AB52" s="16"/>
+      <c r="AC52" s="17"/>
+      <c r="AD52" s="17"/>
+      <c r="AE52" s="17"/>
+      <c r="AF52" s="17"/>
+      <c r="AG52" s="17"/>
+      <c r="AH52" s="17"/>
+      <c r="AI52" s="17"/>
+      <c r="AJ52" s="17"/>
+      <c r="AK52" s="17"/>
+    </row>
+    <row r="53" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="15"/>
+      <c r="S53" s="15"/>
+      <c r="T53" s="15"/>
+      <c r="U53" s="15"/>
+      <c r="V53" s="15"/>
+      <c r="W53" s="15"/>
+      <c r="X53" s="15"/>
+      <c r="Y53" s="15"/>
+      <c r="Z53" s="16"/>
+      <c r="AA53" s="16"/>
+      <c r="AB53" s="16"/>
+      <c r="AC53" s="17"/>
+      <c r="AD53" s="17"/>
+      <c r="AE53" s="17"/>
+      <c r="AF53" s="17"/>
+      <c r="AG53" s="17"/>
+      <c r="AH53" s="17"/>
+      <c r="AI53" s="17"/>
+      <c r="AJ53" s="17"/>
+      <c r="AK53" s="17"/>
+    </row>
+    <row r="54" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
+      <c r="S54" s="15"/>
+      <c r="T54" s="15"/>
+      <c r="U54" s="15"/>
+      <c r="V54" s="15"/>
+      <c r="W54" s="15"/>
+      <c r="X54" s="15"/>
+      <c r="Y54" s="15"/>
+      <c r="Z54" s="16"/>
+      <c r="AA54" s="16"/>
+      <c r="AB54" s="16"/>
+      <c r="AC54" s="17"/>
+      <c r="AD54" s="17"/>
+      <c r="AE54" s="17"/>
+      <c r="AF54" s="17"/>
+      <c r="AG54" s="17"/>
+      <c r="AH54" s="17"/>
+      <c r="AI54" s="17"/>
+      <c r="AJ54" s="17"/>
+      <c r="AK54" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="L41:R41"/>
+    <mergeCell ref="W39:AA41"/>
+    <mergeCell ref="AB39:AE41"/>
+    <mergeCell ref="Z1:AN1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="L40:Q40"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E4:CU4">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
+      <formula>$O$47</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
+  <dimension ref="A1:CU54"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BL5" sqref="BL5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="5.7109375" style="1" customWidth="1"/>
+    <col min="5" max="25" width="4.7109375" style="2" customWidth="1"/>
+    <col min="26" max="28" width="4.7109375" style="3" customWidth="1"/>
+    <col min="29" max="99" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:99" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+    </row>
+    <row r="2" spans="1:99" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:99" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="4">
+        <v>43885</v>
+      </c>
+      <c r="F3" s="4">
+        <v>43886</v>
+      </c>
+      <c r="G3" s="4">
+        <v>43887</v>
+      </c>
+      <c r="H3" s="4">
+        <v>43888</v>
+      </c>
+      <c r="I3" s="4">
+        <v>43889</v>
+      </c>
+      <c r="J3" s="4">
+        <v>43890</v>
+      </c>
+      <c r="K3" s="4">
+        <v>43891</v>
+      </c>
+      <c r="L3" s="4">
+        <v>43892</v>
+      </c>
+      <c r="M3" s="4">
+        <v>43893</v>
+      </c>
+      <c r="N3" s="4">
+        <v>43894</v>
+      </c>
+      <c r="O3" s="4">
+        <v>43895</v>
+      </c>
+      <c r="P3" s="4">
+        <v>43896</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>43897</v>
+      </c>
+      <c r="R3" s="4">
+        <v>43898</v>
+      </c>
+      <c r="S3" s="4">
+        <v>43899</v>
+      </c>
+      <c r="T3" s="9">
+        <v>43900</v>
+      </c>
+      <c r="U3" s="10">
+        <v>43901</v>
+      </c>
+      <c r="V3" s="4">
+        <v>43902</v>
+      </c>
+      <c r="W3" s="4">
+        <v>43903</v>
+      </c>
+      <c r="X3" s="4">
+        <v>43904</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>43905</v>
+      </c>
+      <c r="Z3" s="4">
+        <v>43906</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>43907</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>43908</v>
+      </c>
+      <c r="AC3" s="4">
+        <v>43909</v>
+      </c>
+      <c r="AD3" s="4">
+        <v>43910</v>
+      </c>
+      <c r="AE3" s="4">
+        <v>43911</v>
+      </c>
+      <c r="AF3" s="9">
+        <v>43912</v>
+      </c>
+      <c r="AG3" s="14">
+        <v>43913</v>
+      </c>
+      <c r="AH3" s="4">
+        <v>43914</v>
+      </c>
+      <c r="AI3" s="4">
+        <v>43915</v>
+      </c>
+      <c r="AJ3" s="4">
+        <v>43916</v>
+      </c>
+      <c r="AK3" s="4">
+        <v>43917</v>
+      </c>
+      <c r="AL3" s="4">
+        <v>43918</v>
+      </c>
+      <c r="AM3" s="4">
+        <v>43919</v>
+      </c>
+      <c r="AN3" s="4">
+        <v>43920</v>
+      </c>
+      <c r="AO3" s="4">
+        <v>43921</v>
+      </c>
+      <c r="AP3" s="4">
+        <v>43922</v>
+      </c>
+      <c r="AQ3" s="4">
+        <v>43923</v>
+      </c>
+      <c r="AR3" s="4">
+        <v>43924</v>
+      </c>
+      <c r="AS3" s="4">
+        <v>43925</v>
+      </c>
+      <c r="AT3" s="4">
+        <v>43926</v>
+      </c>
+      <c r="AU3" s="4">
+        <v>43927</v>
+      </c>
+      <c r="AV3" s="4">
+        <v>43928</v>
+      </c>
+      <c r="AW3" s="4">
+        <v>43929</v>
+      </c>
+      <c r="AX3" s="4">
+        <v>43930</v>
+      </c>
+      <c r="AY3" s="4">
+        <v>43931</v>
+      </c>
+      <c r="AZ3" s="4">
+        <v>43932</v>
+      </c>
+      <c r="BA3" s="4">
+        <v>43933</v>
+      </c>
+      <c r="BB3" s="4">
+        <v>43934</v>
+      </c>
+      <c r="BC3" s="4">
+        <v>43935</v>
+      </c>
+      <c r="BD3" s="4">
+        <v>43936</v>
+      </c>
+      <c r="BE3" s="4">
+        <v>43937</v>
+      </c>
+      <c r="BF3" s="4">
+        <v>43938</v>
+      </c>
+      <c r="BG3" s="4">
+        <v>43939</v>
+      </c>
+      <c r="BH3" s="4">
+        <v>43940</v>
+      </c>
+      <c r="BI3" s="4">
+        <v>43941</v>
+      </c>
+      <c r="BJ3" s="4">
+        <v>43942</v>
+      </c>
+      <c r="BK3" s="4">
+        <v>43943</v>
+      </c>
+      <c r="BL3" s="4">
+        <v>43944</v>
+      </c>
+      <c r="BM3" s="4">
+        <v>43945</v>
+      </c>
+      <c r="BN3" s="4">
+        <v>43946</v>
+      </c>
+      <c r="BO3" s="4">
+        <v>43947</v>
+      </c>
+      <c r="BP3" s="4">
+        <v>43948</v>
+      </c>
+      <c r="BQ3" s="4">
+        <v>43949</v>
+      </c>
+      <c r="BR3" s="4">
+        <v>43950</v>
+      </c>
+      <c r="BS3" s="4">
+        <v>43951</v>
+      </c>
+      <c r="BT3" s="4">
+        <v>43952</v>
+      </c>
+      <c r="BU3" s="4">
+        <v>43953</v>
+      </c>
+      <c r="BV3" s="4">
+        <v>43954</v>
+      </c>
+      <c r="BW3" s="4">
+        <v>43955</v>
+      </c>
+      <c r="BX3" s="4">
+        <v>43956</v>
+      </c>
+      <c r="BY3" s="4">
+        <v>43957</v>
+      </c>
+      <c r="BZ3" s="4">
+        <v>43958</v>
+      </c>
+      <c r="CA3" s="4">
+        <v>43959</v>
+      </c>
+      <c r="CB3" s="4">
+        <v>43960</v>
+      </c>
+      <c r="CC3" s="4">
+        <v>43961</v>
+      </c>
+      <c r="CD3" s="4">
+        <v>43962</v>
+      </c>
+      <c r="CE3" s="4">
+        <v>43963</v>
+      </c>
+      <c r="CF3" s="4">
+        <v>43964</v>
+      </c>
+      <c r="CG3" s="4">
+        <v>43965</v>
+      </c>
+      <c r="CH3" s="4">
+        <v>43966</v>
+      </c>
+      <c r="CI3" s="4">
+        <v>43967</v>
+      </c>
+      <c r="CJ3" s="4">
+        <v>43968</v>
+      </c>
+      <c r="CK3" s="4">
+        <v>43969</v>
+      </c>
+      <c r="CL3" s="4">
+        <v>43970</v>
+      </c>
+      <c r="CM3" s="4">
+        <v>43971</v>
+      </c>
+      <c r="CN3" s="4">
+        <v>43972</v>
+      </c>
+      <c r="CO3" s="4">
+        <v>43973</v>
+      </c>
+      <c r="CP3" s="4">
+        <v>43974</v>
+      </c>
+      <c r="CQ3" s="4">
+        <v>43975</v>
+      </c>
+      <c r="CR3" s="4">
+        <v>43976</v>
+      </c>
+      <c r="CS3" s="4">
+        <v>43977</v>
+      </c>
+      <c r="CT3" s="4">
+        <v>43978</v>
+      </c>
+      <c r="CU3" s="4">
+        <v>43979</v>
+      </c>
+    </row>
+    <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="22">
+        <v>0</v>
+      </c>
+      <c r="F4" s="22">
+        <v>0</v>
+      </c>
+      <c r="G4" s="22">
+        <v>0</v>
+      </c>
+      <c r="H4" s="22">
+        <v>3</v>
+      </c>
+      <c r="I4" s="22">
+        <v>1</v>
+      </c>
+      <c r="J4" s="22">
+        <v>9</v>
+      </c>
+      <c r="K4" s="22">
+        <v>4</v>
+      </c>
+      <c r="L4" s="22">
+        <v>0</v>
+      </c>
+      <c r="M4" s="22">
+        <v>13</v>
+      </c>
+      <c r="N4" s="22">
+        <v>1</v>
+      </c>
+      <c r="O4" s="22">
+        <v>14</v>
+      </c>
+      <c r="P4" s="22">
+        <v>12</v>
+      </c>
+      <c r="Q4" s="22">
+        <v>4</v>
+      </c>
+      <c r="R4" s="22">
+        <v>29</v>
+      </c>
+      <c r="S4" s="22">
+        <v>19</v>
+      </c>
+      <c r="T4" s="22">
+        <v>7</v>
+      </c>
+      <c r="U4" s="22">
+        <v>23</v>
+      </c>
+      <c r="V4" s="22">
+        <v>25</v>
+      </c>
+      <c r="W4" s="22">
+        <v>29</v>
+      </c>
+      <c r="X4" s="22">
+        <v>30</v>
+      </c>
+      <c r="Y4" s="22">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="22">
+        <v>65</v>
+      </c>
+      <c r="AA4" s="22">
+        <v>60</v>
+      </c>
+      <c r="AB4" s="22">
+        <v>100</v>
+      </c>
+      <c r="AC4" s="22">
+        <v>82</v>
+      </c>
+      <c r="AD4" s="22">
+        <v>97</v>
+      </c>
+      <c r="AE4" s="22">
+        <v>91</v>
+      </c>
+      <c r="AF4" s="23">
+        <v>73</v>
+      </c>
+      <c r="AG4" s="23">
+        <v>63</v>
+      </c>
+      <c r="AH4" s="23">
+        <v>63</v>
+      </c>
+      <c r="AI4" s="23">
+        <v>80</v>
+      </c>
+      <c r="AJ4" s="23">
+        <v>97</v>
+      </c>
+      <c r="AK4" s="23">
+        <v>123</v>
+      </c>
+      <c r="AL4" s="23">
+        <v>115</v>
+      </c>
+      <c r="AM4" s="23">
+        <v>149</v>
+      </c>
+      <c r="AN4" s="23">
+        <v>183</v>
+      </c>
+      <c r="AO4" s="23">
+        <v>132</v>
+      </c>
+      <c r="AP4" s="23">
+        <v>105</v>
+      </c>
+      <c r="AQ4" s="23">
+        <v>164</v>
+      </c>
+      <c r="AR4" s="23">
+        <v>212</v>
+      </c>
+      <c r="AS4" s="23">
+        <v>144</v>
+      </c>
+      <c r="AT4" s="23">
+        <v>125</v>
+      </c>
+      <c r="AU4" s="23">
+        <v>77</v>
+      </c>
+      <c r="AV4" s="23">
+        <v>67</v>
+      </c>
+      <c r="AW4" s="23">
+        <v>94</v>
+      </c>
+      <c r="AX4" s="23">
+        <v>14</v>
+      </c>
+      <c r="AY4" s="23">
+        <v>90</v>
+      </c>
+      <c r="AZ4" s="23">
+        <v>39</v>
+      </c>
+      <c r="BA4" s="23">
+        <v>55</v>
+      </c>
+      <c r="BB4" s="23">
+        <v>5</v>
+      </c>
+      <c r="BC4" s="23">
+        <v>32</v>
+      </c>
+      <c r="BD4" s="23">
+        <v>-7</v>
+      </c>
+      <c r="BE4" s="23">
+        <v>31</v>
+      </c>
+      <c r="BF4" s="23">
+        <v>-91</v>
+      </c>
+      <c r="BG4" s="23">
+        <v>18</v>
+      </c>
+      <c r="BH4" s="23">
+        <v>12</v>
+      </c>
+      <c r="BI4" s="23">
+        <v>-3</v>
+      </c>
+      <c r="BJ4" s="23">
+        <v>-73</v>
+      </c>
+      <c r="BK4" s="23">
+        <v>52</v>
+      </c>
+      <c r="BL4" s="23">
+        <v>-20</v>
+      </c>
+      <c r="BM4" s="23"/>
+      <c r="BN4" s="23"/>
+      <c r="BO4" s="23"/>
+      <c r="BP4" s="23"/>
+      <c r="BQ4" s="23"/>
+      <c r="BR4" s="23"/>
+      <c r="BS4" s="23"/>
+      <c r="BT4" s="23"/>
+      <c r="BU4" s="23"/>
+      <c r="BV4" s="23"/>
+      <c r="BW4" s="23"/>
+      <c r="BX4" s="23"/>
+      <c r="BY4" s="23"/>
+      <c r="BZ4" s="23"/>
+      <c r="CA4" s="23"/>
+      <c r="CB4" s="23"/>
+      <c r="CC4" s="23"/>
+      <c r="CD4" s="23"/>
+      <c r="CE4" s="23"/>
+      <c r="CF4" s="23"/>
+      <c r="CG4" s="23"/>
+      <c r="CH4" s="23"/>
+      <c r="CI4" s="23"/>
+      <c r="CJ4" s="23"/>
+      <c r="CK4" s="23"/>
+      <c r="CL4" s="23"/>
+      <c r="CM4" s="23"/>
+      <c r="CN4" s="23"/>
+      <c r="CO4" s="23"/>
+      <c r="CP4" s="23"/>
+      <c r="CQ4" s="23"/>
+      <c r="CR4" s="23"/>
+      <c r="CS4" s="23"/>
+      <c r="CT4" s="23"/>
+      <c r="CU4" s="23"/>
+    </row>
+    <row r="6" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:99" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K39" s="5"/>
+      <c r="L39" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="M39" s="28"/>
+      <c r="N39" s="28"/>
+      <c r="O39" s="28"/>
+      <c r="W39" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="X39" s="30"/>
+      <c r="Y39" s="30"/>
+      <c r="Z39" s="30"/>
+      <c r="AA39" s="30"/>
+      <c r="AB39" s="31">
+        <f>SUM(E4:CU4)</f>
+        <v>2978</v>
+      </c>
+      <c r="AC39" s="31"/>
+      <c r="AD39" s="31"/>
+      <c r="AE39" s="31"/>
+    </row>
+    <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K40" s="13"/>
+      <c r="L40" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="29"/>
+      <c r="W40" s="30"/>
+      <c r="X40" s="30"/>
+      <c r="Y40" s="30"/>
+      <c r="Z40" s="30"/>
+      <c r="AA40" s="30"/>
+      <c r="AB40" s="31"/>
+      <c r="AC40" s="31"/>
+      <c r="AD40" s="31"/>
+      <c r="AE40" s="31"/>
+    </row>
+    <row r="41" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="K41" s="11"/>
+      <c r="L41" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="M41" s="29"/>
+      <c r="N41" s="29"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="29"/>
+      <c r="Q41" s="29"/>
+      <c r="R41" s="29"/>
+      <c r="W41" s="30"/>
+      <c r="X41" s="30"/>
+      <c r="Y41" s="30"/>
+      <c r="Z41" s="30"/>
+      <c r="AA41" s="30"/>
+      <c r="AB41" s="31"/>
+      <c r="AC41" s="31"/>
+      <c r="AD41" s="31"/>
+      <c r="AE41" s="31"/>
+    </row>
+    <row r="43" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+      <c r="S43" s="15"/>
+      <c r="T43" s="15"/>
+      <c r="U43" s="15"/>
+      <c r="V43" s="15"/>
+      <c r="W43" s="15"/>
+      <c r="X43" s="15"/>
+      <c r="Y43" s="15"/>
+      <c r="Z43" s="16"/>
+      <c r="AA43" s="16"/>
+      <c r="AB43" s="16"/>
+      <c r="AC43" s="17"/>
+      <c r="AD43" s="17"/>
+      <c r="AE43" s="17"/>
+      <c r="AF43" s="17"/>
+      <c r="AG43" s="17"/>
+      <c r="AH43" s="17"/>
+      <c r="AI43" s="17"/>
+      <c r="AJ43" s="17"/>
+      <c r="AK43" s="17"/>
+    </row>
+    <row r="44" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="15"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="15"/>
+      <c r="X44" s="15"/>
+      <c r="Y44" s="15"/>
+      <c r="Z44" s="16"/>
+      <c r="AA44" s="16"/>
+      <c r="AB44" s="16"/>
+      <c r="AC44" s="17"/>
+      <c r="AD44" s="17"/>
+      <c r="AE44" s="17"/>
+      <c r="AF44" s="17"/>
+      <c r="AG44" s="17"/>
+      <c r="AH44" s="17"/>
+      <c r="AI44" s="17"/>
+      <c r="AJ44" s="17"/>
+      <c r="AK44" s="17"/>
+    </row>
+    <row r="45" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="15"/>
+      <c r="S45" s="15"/>
+      <c r="T45" s="15"/>
+      <c r="U45" s="15"/>
+      <c r="V45" s="15"/>
+      <c r="W45" s="15"/>
+      <c r="X45" s="15"/>
+      <c r="Y45" s="15"/>
+      <c r="Z45" s="16"/>
+      <c r="AA45" s="16"/>
+      <c r="AB45" s="16"/>
+      <c r="AC45" s="17"/>
+      <c r="AD45" s="17"/>
+      <c r="AE45" s="17"/>
+      <c r="AF45" s="17"/>
+      <c r="AG45" s="17"/>
+      <c r="AH45" s="17"/>
+      <c r="AI45" s="17"/>
+      <c r="AJ45" s="17"/>
+      <c r="AK45" s="17"/>
+    </row>
+    <row r="46" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="15"/>
+      <c r="R46" s="15"/>
+      <c r="S46" s="15"/>
+      <c r="T46" s="15"/>
+      <c r="U46" s="15"/>
+      <c r="V46" s="15"/>
+      <c r="W46" s="15"/>
+      <c r="X46" s="15"/>
+      <c r="Y46" s="15"/>
+      <c r="Z46" s="16"/>
+      <c r="AA46" s="16"/>
+      <c r="AB46" s="16"/>
+      <c r="AC46" s="17"/>
+      <c r="AD46" s="17"/>
+      <c r="AE46" s="17"/>
+      <c r="AF46" s="17"/>
+      <c r="AG46" s="17"/>
+      <c r="AH46" s="17"/>
+      <c r="AI46" s="17"/>
+      <c r="AJ46" s="17"/>
+      <c r="AK46" s="17"/>
+    </row>
+    <row r="47" spans="9:37" x14ac:dyDescent="0.25">
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="O47" s="19">
+        <f>MAXA(E4:BJ4)</f>
+        <v>212</v>
       </c>
       <c r="P47" s="15"/>
       <c r="Q47" s="15"/>
@@ -4761,1050 +5616,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="Z1:AN1"/>
+    <mergeCell ref="A4:D4"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L39:O39"/>
-    <mergeCell ref="L40:Q40"/>
-    <mergeCell ref="L41:R41"/>
-    <mergeCell ref="W39:AA41"/>
-    <mergeCell ref="AB39:AE41"/>
-  </mergeCells>
-  <conditionalFormatting sqref="E4:CU4">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThanOrEqual">
-      <formula>$O$47</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
-  <dimension ref="A1:CU54"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL39" sqref="AL39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="4" width="5.7109375" style="1" customWidth="1"/>
-    <col min="5" max="25" width="4.7109375" style="2" customWidth="1"/>
-    <col min="26" max="28" width="4.7109375" style="3" customWidth="1"/>
-    <col min="29" max="99" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:99" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="25"/>
-      <c r="AN1" s="25"/>
-    </row>
-    <row r="2" spans="1:99" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:99" s="37" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="4">
-        <v>43885</v>
-      </c>
-      <c r="F3" s="4">
-        <v>43886</v>
-      </c>
-      <c r="G3" s="4">
-        <v>43887</v>
-      </c>
-      <c r="H3" s="4">
-        <v>43888</v>
-      </c>
-      <c r="I3" s="4">
-        <v>43889</v>
-      </c>
-      <c r="J3" s="4">
-        <v>43890</v>
-      </c>
-      <c r="K3" s="4">
-        <v>43891</v>
-      </c>
-      <c r="L3" s="4">
-        <v>43892</v>
-      </c>
-      <c r="M3" s="4">
-        <v>43893</v>
-      </c>
-      <c r="N3" s="4">
-        <v>43894</v>
-      </c>
-      <c r="O3" s="4">
-        <v>43895</v>
-      </c>
-      <c r="P3" s="4">
-        <v>43896</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>43897</v>
-      </c>
-      <c r="R3" s="4">
-        <v>43898</v>
-      </c>
-      <c r="S3" s="4">
-        <v>43899</v>
-      </c>
-      <c r="T3" s="9">
-        <v>43900</v>
-      </c>
-      <c r="U3" s="10">
-        <v>43901</v>
-      </c>
-      <c r="V3" s="4">
-        <v>43902</v>
-      </c>
-      <c r="W3" s="4">
-        <v>43903</v>
-      </c>
-      <c r="X3" s="4">
-        <v>43904</v>
-      </c>
-      <c r="Y3" s="4">
-        <v>43905</v>
-      </c>
-      <c r="Z3" s="4">
-        <v>43906</v>
-      </c>
-      <c r="AA3" s="4">
-        <v>43907</v>
-      </c>
-      <c r="AB3" s="4">
-        <v>43908</v>
-      </c>
-      <c r="AC3" s="4">
-        <v>43909</v>
-      </c>
-      <c r="AD3" s="4">
-        <v>43910</v>
-      </c>
-      <c r="AE3" s="4">
-        <v>43911</v>
-      </c>
-      <c r="AF3" s="9">
-        <v>43912</v>
-      </c>
-      <c r="AG3" s="14">
-        <v>43913</v>
-      </c>
-      <c r="AH3" s="4">
-        <v>43914</v>
-      </c>
-      <c r="AI3" s="4">
-        <v>43915</v>
-      </c>
-      <c r="AJ3" s="4">
-        <v>43916</v>
-      </c>
-      <c r="AK3" s="4">
-        <v>43917</v>
-      </c>
-      <c r="AL3" s="4">
-        <v>43918</v>
-      </c>
-      <c r="AM3" s="4">
-        <v>43919</v>
-      </c>
-      <c r="AN3" s="4">
-        <v>43920</v>
-      </c>
-      <c r="AO3" s="4">
-        <v>43921</v>
-      </c>
-      <c r="AP3" s="4">
-        <v>43922</v>
-      </c>
-      <c r="AQ3" s="4">
-        <v>43923</v>
-      </c>
-      <c r="AR3" s="4">
-        <v>43924</v>
-      </c>
-      <c r="AS3" s="4">
-        <v>43925</v>
-      </c>
-      <c r="AT3" s="4">
-        <v>43926</v>
-      </c>
-      <c r="AU3" s="4">
-        <v>43927</v>
-      </c>
-      <c r="AV3" s="4">
-        <v>43928</v>
-      </c>
-      <c r="AW3" s="4">
-        <v>43929</v>
-      </c>
-      <c r="AX3" s="4">
-        <v>43930</v>
-      </c>
-      <c r="AY3" s="4">
-        <v>43931</v>
-      </c>
-      <c r="AZ3" s="4">
-        <v>43932</v>
-      </c>
-      <c r="BA3" s="4">
-        <v>43933</v>
-      </c>
-      <c r="BB3" s="4">
-        <v>43934</v>
-      </c>
-      <c r="BC3" s="4">
-        <v>43935</v>
-      </c>
-      <c r="BD3" s="4">
-        <v>43936</v>
-      </c>
-      <c r="BE3" s="4">
-        <v>43937</v>
-      </c>
-      <c r="BF3" s="4">
-        <v>43938</v>
-      </c>
-      <c r="BG3" s="4">
-        <v>43939</v>
-      </c>
-      <c r="BH3" s="4">
-        <v>43940</v>
-      </c>
-      <c r="BI3" s="4">
-        <v>43941</v>
-      </c>
-      <c r="BJ3" s="4">
-        <v>43942</v>
-      </c>
-      <c r="BK3" s="4">
-        <v>43943</v>
-      </c>
-      <c r="BL3" s="4">
-        <v>43944</v>
-      </c>
-      <c r="BM3" s="4">
-        <v>43945</v>
-      </c>
-      <c r="BN3" s="4">
-        <v>43946</v>
-      </c>
-      <c r="BO3" s="4">
-        <v>43947</v>
-      </c>
-      <c r="BP3" s="4">
-        <v>43948</v>
-      </c>
-      <c r="BQ3" s="4">
-        <v>43949</v>
-      </c>
-      <c r="BR3" s="4">
-        <v>43950</v>
-      </c>
-      <c r="BS3" s="4">
-        <v>43951</v>
-      </c>
-      <c r="BT3" s="4">
-        <v>43952</v>
-      </c>
-      <c r="BU3" s="4">
-        <v>43953</v>
-      </c>
-      <c r="BV3" s="4">
-        <v>43954</v>
-      </c>
-      <c r="BW3" s="4">
-        <v>43955</v>
-      </c>
-      <c r="BX3" s="4">
-        <v>43956</v>
-      </c>
-      <c r="BY3" s="4">
-        <v>43957</v>
-      </c>
-      <c r="BZ3" s="4">
-        <v>43958</v>
-      </c>
-      <c r="CA3" s="4">
-        <v>43959</v>
-      </c>
-      <c r="CB3" s="4">
-        <v>43960</v>
-      </c>
-      <c r="CC3" s="4">
-        <v>43961</v>
-      </c>
-      <c r="CD3" s="4">
-        <v>43962</v>
-      </c>
-      <c r="CE3" s="4">
-        <v>43963</v>
-      </c>
-      <c r="CF3" s="4">
-        <v>43964</v>
-      </c>
-      <c r="CG3" s="4">
-        <v>43965</v>
-      </c>
-      <c r="CH3" s="4">
-        <v>43966</v>
-      </c>
-      <c r="CI3" s="4">
-        <v>43967</v>
-      </c>
-      <c r="CJ3" s="4">
-        <v>43968</v>
-      </c>
-      <c r="CK3" s="4">
-        <v>43969</v>
-      </c>
-      <c r="CL3" s="4">
-        <v>43970</v>
-      </c>
-      <c r="CM3" s="4">
-        <v>43971</v>
-      </c>
-      <c r="CN3" s="4">
-        <v>43972</v>
-      </c>
-      <c r="CO3" s="4">
-        <v>43973</v>
-      </c>
-      <c r="CP3" s="4">
-        <v>43974</v>
-      </c>
-      <c r="CQ3" s="4">
-        <v>43975</v>
-      </c>
-      <c r="CR3" s="4">
-        <v>43976</v>
-      </c>
-      <c r="CS3" s="4">
-        <v>43977</v>
-      </c>
-      <c r="CT3" s="4">
-        <v>43978</v>
-      </c>
-      <c r="CU3" s="4">
-        <v>43979</v>
-      </c>
-    </row>
-    <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="22">
-        <v>0</v>
-      </c>
-      <c r="F4" s="22">
-        <v>0</v>
-      </c>
-      <c r="G4" s="22">
-        <v>0</v>
-      </c>
-      <c r="H4" s="22">
-        <v>3</v>
-      </c>
-      <c r="I4" s="22">
-        <v>1</v>
-      </c>
-      <c r="J4" s="22">
-        <v>9</v>
-      </c>
-      <c r="K4" s="22">
-        <v>4</v>
-      </c>
-      <c r="L4" s="22">
-        <v>0</v>
-      </c>
-      <c r="M4" s="22">
-        <v>13</v>
-      </c>
-      <c r="N4" s="22">
-        <v>1</v>
-      </c>
-      <c r="O4" s="22">
-        <v>14</v>
-      </c>
-      <c r="P4" s="22">
-        <v>12</v>
-      </c>
-      <c r="Q4" s="22">
-        <v>4</v>
-      </c>
-      <c r="R4" s="22">
-        <v>29</v>
-      </c>
-      <c r="S4" s="22">
-        <v>19</v>
-      </c>
-      <c r="T4" s="22">
-        <v>7</v>
-      </c>
-      <c r="U4" s="22">
-        <v>23</v>
-      </c>
-      <c r="V4" s="22">
-        <v>25</v>
-      </c>
-      <c r="W4" s="22">
-        <v>29</v>
-      </c>
-      <c r="X4" s="22">
-        <v>30</v>
-      </c>
-      <c r="Y4" s="22">
-        <v>40</v>
-      </c>
-      <c r="Z4" s="22">
-        <v>65</v>
-      </c>
-      <c r="AA4" s="22">
-        <v>60</v>
-      </c>
-      <c r="AB4" s="22">
-        <v>100</v>
-      </c>
-      <c r="AC4" s="22">
-        <v>82</v>
-      </c>
-      <c r="AD4" s="22">
-        <v>97</v>
-      </c>
-      <c r="AE4" s="22">
-        <v>91</v>
-      </c>
-      <c r="AF4" s="23">
-        <v>73</v>
-      </c>
-      <c r="AG4" s="23">
-        <v>63</v>
-      </c>
-      <c r="AH4" s="23">
-        <v>63</v>
-      </c>
-      <c r="AI4" s="23">
-        <v>80</v>
-      </c>
-      <c r="AJ4" s="23">
-        <v>97</v>
-      </c>
-      <c r="AK4" s="23">
-        <v>123</v>
-      </c>
-      <c r="AL4" s="23">
-        <v>115</v>
-      </c>
-      <c r="AM4" s="23">
-        <v>149</v>
-      </c>
-      <c r="AN4" s="23">
-        <v>183</v>
-      </c>
-      <c r="AO4" s="23">
-        <v>132</v>
-      </c>
-      <c r="AP4" s="23">
-        <v>105</v>
-      </c>
-      <c r="AQ4" s="23">
-        <v>164</v>
-      </c>
-      <c r="AR4" s="23">
-        <v>212</v>
-      </c>
-      <c r="AS4" s="23">
-        <v>144</v>
-      </c>
-      <c r="AT4" s="23">
-        <v>125</v>
-      </c>
-      <c r="AU4" s="23">
-        <v>77</v>
-      </c>
-      <c r="AV4" s="23">
-        <v>67</v>
-      </c>
-      <c r="AW4" s="23">
-        <v>94</v>
-      </c>
-      <c r="AX4" s="23">
-        <v>14</v>
-      </c>
-      <c r="AY4" s="23">
-        <v>90</v>
-      </c>
-      <c r="AZ4" s="23">
-        <v>39</v>
-      </c>
-      <c r="BA4" s="23">
-        <v>55</v>
-      </c>
-      <c r="BB4" s="23">
-        <v>5</v>
-      </c>
-      <c r="BC4" s="23">
-        <v>32</v>
-      </c>
-      <c r="BD4" s="23">
-        <v>-7</v>
-      </c>
-      <c r="BE4" s="23">
-        <v>31</v>
-      </c>
-      <c r="BF4" s="23">
-        <v>-91</v>
-      </c>
-      <c r="BG4" s="23">
-        <v>18</v>
-      </c>
-      <c r="BH4" s="23">
-        <v>12</v>
-      </c>
-      <c r="BI4" s="23">
-        <v>-3</v>
-      </c>
-      <c r="BJ4" s="23">
-        <v>-73</v>
-      </c>
-      <c r="BK4" s="23">
-        <v>52</v>
-      </c>
-      <c r="BL4" s="23"/>
-      <c r="BM4" s="23"/>
-      <c r="BN4" s="23"/>
-      <c r="BO4" s="23"/>
-      <c r="BP4" s="23"/>
-      <c r="BQ4" s="23"/>
-      <c r="BR4" s="23"/>
-      <c r="BS4" s="23"/>
-      <c r="BT4" s="23"/>
-      <c r="BU4" s="23"/>
-      <c r="BV4" s="23"/>
-      <c r="BW4" s="23"/>
-      <c r="BX4" s="23"/>
-      <c r="BY4" s="23"/>
-      <c r="BZ4" s="23"/>
-      <c r="CA4" s="23"/>
-      <c r="CB4" s="23"/>
-      <c r="CC4" s="23"/>
-      <c r="CD4" s="23"/>
-      <c r="CE4" s="23"/>
-      <c r="CF4" s="23"/>
-      <c r="CG4" s="23"/>
-      <c r="CH4" s="23"/>
-      <c r="CI4" s="23"/>
-      <c r="CJ4" s="23"/>
-      <c r="CK4" s="23"/>
-      <c r="CL4" s="23"/>
-      <c r="CM4" s="23"/>
-      <c r="CN4" s="23"/>
-      <c r="CO4" s="23"/>
-      <c r="CP4" s="23"/>
-      <c r="CQ4" s="23"/>
-      <c r="CR4" s="23"/>
-      <c r="CS4" s="23"/>
-      <c r="CT4" s="23"/>
-      <c r="CU4" s="23"/>
-    </row>
-    <row r="6" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:99" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-    </row>
-    <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K39" s="5"/>
-      <c r="L39" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="M39" s="30"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="30"/>
-      <c r="W39" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="X39" s="29"/>
-      <c r="Y39" s="29"/>
-      <c r="Z39" s="29"/>
-      <c r="AA39" s="29"/>
-      <c r="AB39" s="28">
-        <f>SUM(E4:CU4)</f>
-        <v>2998</v>
-      </c>
-      <c r="AC39" s="28"/>
-      <c r="AD39" s="28"/>
-      <c r="AE39" s="28"/>
-    </row>
-    <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K40" s="13"/>
-      <c r="L40" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="M40" s="24"/>
-      <c r="N40" s="24"/>
-      <c r="O40" s="24"/>
-      <c r="P40" s="24"/>
-      <c r="Q40" s="24"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="28"/>
-      <c r="AC40" s="28"/>
-      <c r="AD40" s="28"/>
-      <c r="AE40" s="28"/>
-    </row>
-    <row r="41" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="K41" s="11"/>
-      <c r="L41" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="M41" s="24"/>
-      <c r="N41" s="24"/>
-      <c r="O41" s="24"/>
-      <c r="P41" s="24"/>
-      <c r="Q41" s="24"/>
-      <c r="R41" s="24"/>
-      <c r="W41" s="29"/>
-      <c r="X41" s="29"/>
-      <c r="Y41" s="29"/>
-      <c r="Z41" s="29"/>
-      <c r="AA41" s="29"/>
-      <c r="AB41" s="28"/>
-      <c r="AC41" s="28"/>
-      <c r="AD41" s="28"/>
-      <c r="AE41" s="28"/>
-    </row>
-    <row r="43" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="15"/>
-      <c r="U43" s="15"/>
-      <c r="V43" s="15"/>
-      <c r="W43" s="15"/>
-      <c r="X43" s="15"/>
-      <c r="Y43" s="15"/>
-      <c r="Z43" s="16"/>
-      <c r="AA43" s="16"/>
-      <c r="AB43" s="16"/>
-      <c r="AC43" s="17"/>
-      <c r="AD43" s="17"/>
-      <c r="AE43" s="17"/>
-      <c r="AF43" s="17"/>
-      <c r="AG43" s="17"/>
-      <c r="AH43" s="17"/>
-      <c r="AI43" s="17"/>
-      <c r="AJ43" s="17"/>
-      <c r="AK43" s="17"/>
-    </row>
-    <row r="44" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
-      <c r="T44" s="15"/>
-      <c r="U44" s="15"/>
-      <c r="V44" s="15"/>
-      <c r="W44" s="15"/>
-      <c r="X44" s="15"/>
-      <c r="Y44" s="15"/>
-      <c r="Z44" s="16"/>
-      <c r="AA44" s="16"/>
-      <c r="AB44" s="16"/>
-      <c r="AC44" s="17"/>
-      <c r="AD44" s="17"/>
-      <c r="AE44" s="17"/>
-      <c r="AF44" s="17"/>
-      <c r="AG44" s="17"/>
-      <c r="AH44" s="17"/>
-      <c r="AI44" s="17"/>
-      <c r="AJ44" s="17"/>
-      <c r="AK44" s="17"/>
-    </row>
-    <row r="45" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
-      <c r="P45" s="15"/>
-      <c r="Q45" s="15"/>
-      <c r="R45" s="15"/>
-      <c r="S45" s="15"/>
-      <c r="T45" s="15"/>
-      <c r="U45" s="15"/>
-      <c r="V45" s="15"/>
-      <c r="W45" s="15"/>
-      <c r="X45" s="15"/>
-      <c r="Y45" s="15"/>
-      <c r="Z45" s="16"/>
-      <c r="AA45" s="16"/>
-      <c r="AB45" s="16"/>
-      <c r="AC45" s="17"/>
-      <c r="AD45" s="17"/>
-      <c r="AE45" s="17"/>
-      <c r="AF45" s="17"/>
-      <c r="AG45" s="17"/>
-      <c r="AH45" s="17"/>
-      <c r="AI45" s="17"/>
-      <c r="AJ45" s="17"/>
-      <c r="AK45" s="17"/>
-    </row>
-    <row r="46" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
-      <c r="P46" s="15"/>
-      <c r="Q46" s="15"/>
-      <c r="R46" s="15"/>
-      <c r="S46" s="15"/>
-      <c r="T46" s="15"/>
-      <c r="U46" s="15"/>
-      <c r="V46" s="15"/>
-      <c r="W46" s="15"/>
-      <c r="X46" s="15"/>
-      <c r="Y46" s="15"/>
-      <c r="Z46" s="16"/>
-      <c r="AA46" s="16"/>
-      <c r="AB46" s="16"/>
-      <c r="AC46" s="17"/>
-      <c r="AD46" s="17"/>
-      <c r="AE46" s="17"/>
-      <c r="AF46" s="17"/>
-      <c r="AG46" s="17"/>
-      <c r="AH46" s="17"/>
-      <c r="AI46" s="17"/>
-      <c r="AJ46" s="17"/>
-      <c r="AK46" s="17"/>
-    </row>
-    <row r="47" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="O47" s="19">
-        <f>MAXA(E4:BJ4)</f>
-        <v>212</v>
-      </c>
-      <c r="P47" s="15"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="15"/>
-      <c r="S47" s="15"/>
-      <c r="T47" s="15"/>
-      <c r="U47" s="15"/>
-      <c r="V47" s="15"/>
-      <c r="W47" s="15"/>
-      <c r="X47" s="15"/>
-      <c r="Y47" s="15"/>
-      <c r="Z47" s="16"/>
-      <c r="AA47" s="16"/>
-      <c r="AB47" s="16"/>
-      <c r="AC47" s="17"/>
-      <c r="AD47" s="17"/>
-      <c r="AE47" s="17"/>
-      <c r="AF47" s="17"/>
-      <c r="AG47" s="17"/>
-      <c r="AH47" s="17"/>
-      <c r="AI47" s="17"/>
-      <c r="AJ47" s="17"/>
-      <c r="AK47" s="17"/>
-    </row>
-    <row r="48" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I48" s="15"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="15"/>
-      <c r="R48" s="15"/>
-      <c r="S48" s="15"/>
-      <c r="T48" s="15"/>
-      <c r="U48" s="15"/>
-      <c r="V48" s="15"/>
-      <c r="W48" s="15"/>
-      <c r="X48" s="15"/>
-      <c r="Y48" s="15"/>
-      <c r="Z48" s="16"/>
-      <c r="AA48" s="16"/>
-      <c r="AB48" s="16"/>
-      <c r="AC48" s="17"/>
-      <c r="AD48" s="17"/>
-      <c r="AE48" s="17"/>
-      <c r="AF48" s="17"/>
-      <c r="AG48" s="17"/>
-      <c r="AH48" s="17"/>
-      <c r="AI48" s="17"/>
-      <c r="AJ48" s="17"/>
-      <c r="AK48" s="17"/>
-    </row>
-    <row r="49" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I49" s="15"/>
-      <c r="J49" s="15"/>
-      <c r="K49" s="15"/>
-      <c r="L49" s="15"/>
-      <c r="M49" s="15"/>
-      <c r="N49" s="15"/>
-      <c r="O49" s="15"/>
-      <c r="P49" s="15"/>
-      <c r="Q49" s="15"/>
-      <c r="R49" s="15"/>
-      <c r="S49" s="15"/>
-      <c r="T49" s="15"/>
-      <c r="U49" s="15"/>
-      <c r="V49" s="15"/>
-      <c r="W49" s="15"/>
-      <c r="X49" s="15"/>
-      <c r="Y49" s="15"/>
-      <c r="Z49" s="16"/>
-      <c r="AA49" s="16"/>
-      <c r="AB49" s="16"/>
-      <c r="AC49" s="17"/>
-      <c r="AD49" s="17"/>
-      <c r="AE49" s="17"/>
-      <c r="AF49" s="17"/>
-      <c r="AG49" s="17"/>
-      <c r="AH49" s="17"/>
-      <c r="AI49" s="17"/>
-      <c r="AJ49" s="17"/>
-      <c r="AK49" s="17"/>
-    </row>
-    <row r="50" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I50" s="15"/>
-      <c r="J50" s="15"/>
-      <c r="K50" s="15"/>
-      <c r="L50" s="15"/>
-      <c r="M50" s="15"/>
-      <c r="N50" s="15"/>
-      <c r="O50" s="15"/>
-      <c r="P50" s="15"/>
-      <c r="Q50" s="15"/>
-      <c r="R50" s="15"/>
-      <c r="S50" s="15"/>
-      <c r="T50" s="15"/>
-      <c r="U50" s="15"/>
-      <c r="V50" s="15"/>
-      <c r="W50" s="15"/>
-      <c r="X50" s="15"/>
-      <c r="Y50" s="15"/>
-      <c r="Z50" s="16"/>
-      <c r="AA50" s="16"/>
-      <c r="AB50" s="16"/>
-      <c r="AC50" s="17"/>
-      <c r="AD50" s="17"/>
-      <c r="AE50" s="17"/>
-      <c r="AF50" s="17"/>
-      <c r="AG50" s="17"/>
-      <c r="AH50" s="17"/>
-      <c r="AI50" s="17"/>
-      <c r="AJ50" s="17"/>
-      <c r="AK50" s="17"/>
-    </row>
-    <row r="51" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I51" s="15"/>
-      <c r="J51" s="15"/>
-      <c r="K51" s="15"/>
-      <c r="L51" s="15"/>
-      <c r="M51" s="15"/>
-      <c r="N51" s="15"/>
-      <c r="O51" s="15"/>
-      <c r="P51" s="15"/>
-      <c r="Q51" s="15"/>
-      <c r="R51" s="15"/>
-      <c r="S51" s="15"/>
-      <c r="T51" s="15"/>
-      <c r="U51" s="15"/>
-      <c r="V51" s="15"/>
-      <c r="W51" s="15"/>
-      <c r="X51" s="15"/>
-      <c r="Y51" s="15"/>
-      <c r="Z51" s="16"/>
-      <c r="AA51" s="16"/>
-      <c r="AB51" s="16"/>
-      <c r="AC51" s="17"/>
-      <c r="AD51" s="17"/>
-      <c r="AE51" s="17"/>
-      <c r="AF51" s="17"/>
-      <c r="AG51" s="17"/>
-      <c r="AH51" s="17"/>
-      <c r="AI51" s="17"/>
-      <c r="AJ51" s="17"/>
-      <c r="AK51" s="17"/>
-    </row>
-    <row r="52" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
-      <c r="K52" s="15"/>
-      <c r="L52" s="15"/>
-      <c r="M52" s="15"/>
-      <c r="N52" s="15"/>
-      <c r="O52" s="15"/>
-      <c r="P52" s="15"/>
-      <c r="Q52" s="15"/>
-      <c r="R52" s="15"/>
-      <c r="S52" s="15"/>
-      <c r="T52" s="15"/>
-      <c r="U52" s="15"/>
-      <c r="V52" s="15"/>
-      <c r="W52" s="15"/>
-      <c r="X52" s="15"/>
-      <c r="Y52" s="15"/>
-      <c r="Z52" s="16"/>
-      <c r="AA52" s="16"/>
-      <c r="AB52" s="16"/>
-      <c r="AC52" s="17"/>
-      <c r="AD52" s="17"/>
-      <c r="AE52" s="17"/>
-      <c r="AF52" s="17"/>
-      <c r="AG52" s="17"/>
-      <c r="AH52" s="17"/>
-      <c r="AI52" s="17"/>
-      <c r="AJ52" s="17"/>
-      <c r="AK52" s="17"/>
-    </row>
-    <row r="53" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="15"/>
-      <c r="P53" s="15"/>
-      <c r="Q53" s="15"/>
-      <c r="R53" s="15"/>
-      <c r="S53" s="15"/>
-      <c r="T53" s="15"/>
-      <c r="U53" s="15"/>
-      <c r="V53" s="15"/>
-      <c r="W53" s="15"/>
-      <c r="X53" s="15"/>
-      <c r="Y53" s="15"/>
-      <c r="Z53" s="16"/>
-      <c r="AA53" s="16"/>
-      <c r="AB53" s="16"/>
-      <c r="AC53" s="17"/>
-      <c r="AD53" s="17"/>
-      <c r="AE53" s="17"/>
-      <c r="AF53" s="17"/>
-      <c r="AG53" s="17"/>
-      <c r="AH53" s="17"/>
-      <c r="AI53" s="17"/>
-      <c r="AJ53" s="17"/>
-      <c r="AK53" s="17"/>
-    </row>
-    <row r="54" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="15"/>
-      <c r="M54" s="15"/>
-      <c r="N54" s="15"/>
-      <c r="O54" s="15"/>
-      <c r="P54" s="15"/>
-      <c r="Q54" s="15"/>
-      <c r="R54" s="15"/>
-      <c r="S54" s="15"/>
-      <c r="T54" s="15"/>
-      <c r="U54" s="15"/>
-      <c r="V54" s="15"/>
-      <c r="W54" s="15"/>
-      <c r="X54" s="15"/>
-      <c r="Y54" s="15"/>
-      <c r="Z54" s="16"/>
-      <c r="AA54" s="16"/>
-      <c r="AB54" s="16"/>
-      <c r="AC54" s="17"/>
-      <c r="AD54" s="17"/>
-      <c r="AE54" s="17"/>
-      <c r="AF54" s="17"/>
-      <c r="AG54" s="17"/>
-      <c r="AH54" s="17"/>
-      <c r="AI54" s="17"/>
-      <c r="AJ54" s="17"/>
-      <c r="AK54" s="17"/>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
     <mergeCell ref="L39:O39"/>
     <mergeCell ref="W39:AA41"/>
     <mergeCell ref="AB39:AE41"/>
     <mergeCell ref="L40:Q40"/>
     <mergeCell ref="L41:R41"/>
-    <mergeCell ref="Z1:AN1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:BY4">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">

</xml_diff>

<commit_message>
aggiornamento dati al 24/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973750A3-3209-49F1-89FD-8A655DEFB589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0156C8E0-140E-424A-BA07-0000FBBD4757}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -401,6 +401,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -412,15 +421,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="17" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1140,6 +1140,9 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>-851</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-321</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1923,6 +1926,9 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3562,7 +3568,7 @@
   <dimension ref="A1:CU54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BL5" sqref="BL5"/>
+      <selection activeCell="BM5" sqref="BM5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3584,32 +3590,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="25" t="s">
+      <c r="Z1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="25"/>
-      <c r="AN1" s="25"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="28"/>
     </row>
     <row r="2" spans="1:99" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -3897,12 +3903,12 @@
       </c>
     </row>
     <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -4083,7 +4089,9 @@
       <c r="BL4" s="7">
         <v>-851</v>
       </c>
-      <c r="BM4" s="7"/>
+      <c r="BM4" s="7">
+        <v>-321</v>
+      </c>
       <c r="BN4" s="7"/>
       <c r="BO4" s="7"/>
       <c r="BP4" s="7"/>
@@ -4135,67 +4143,67 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K39" s="5"/>
-      <c r="L39" s="28" t="s">
+      <c r="L39" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="28"/>
-      <c r="N39" s="28"/>
-      <c r="O39" s="28"/>
-      <c r="W39" s="30" t="s">
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="W39" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="30"/>
-      <c r="Z39" s="30"/>
-      <c r="AA39" s="30"/>
-      <c r="AB39" s="31">
+      <c r="X39" s="26"/>
+      <c r="Y39" s="26"/>
+      <c r="Z39" s="26"/>
+      <c r="AA39" s="26"/>
+      <c r="AB39" s="27">
         <f>SUM(E4:CU4)</f>
-        <v>106848</v>
-      </c>
-      <c r="AC39" s="31"/>
-      <c r="AD39" s="31"/>
-      <c r="AE39" s="31"/>
+        <v>106527</v>
+      </c>
+      <c r="AC39" s="27"/>
+      <c r="AD39" s="27"/>
+      <c r="AE39" s="27"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K40" s="13"/>
-      <c r="L40" s="29" t="s">
+      <c r="L40" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="29"/>
-      <c r="W40" s="30"/>
-      <c r="X40" s="30"/>
-      <c r="Y40" s="30"/>
-      <c r="Z40" s="30"/>
-      <c r="AA40" s="30"/>
-      <c r="AB40" s="31"/>
-      <c r="AC40" s="31"/>
-      <c r="AD40" s="31"/>
-      <c r="AE40" s="31"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="25"/>
+      <c r="O40" s="25"/>
+      <c r="P40" s="25"/>
+      <c r="Q40" s="25"/>
+      <c r="W40" s="26"/>
+      <c r="X40" s="26"/>
+      <c r="Y40" s="26"/>
+      <c r="Z40" s="26"/>
+      <c r="AA40" s="26"/>
+      <c r="AB40" s="27"/>
+      <c r="AC40" s="27"/>
+      <c r="AD40" s="27"/>
+      <c r="AE40" s="27"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.25">
       <c r="K41" s="11"/>
-      <c r="L41" s="29" t="s">
+      <c r="L41" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="29"/>
-      <c r="N41" s="29"/>
-      <c r="O41" s="29"/>
-      <c r="P41" s="29"/>
-      <c r="Q41" s="29"/>
-      <c r="R41" s="29"/>
-      <c r="W41" s="30"/>
-      <c r="X41" s="30"/>
-      <c r="Y41" s="30"/>
-      <c r="Z41" s="30"/>
-      <c r="AA41" s="30"/>
-      <c r="AB41" s="31"/>
-      <c r="AC41" s="31"/>
-      <c r="AD41" s="31"/>
-      <c r="AE41" s="31"/>
+      <c r="M41" s="25"/>
+      <c r="N41" s="25"/>
+      <c r="O41" s="25"/>
+      <c r="P41" s="25"/>
+      <c r="Q41" s="25"/>
+      <c r="R41" s="25"/>
+      <c r="W41" s="26"/>
+      <c r="X41" s="26"/>
+      <c r="Y41" s="26"/>
+      <c r="Z41" s="26"/>
+      <c r="AA41" s="26"/>
+      <c r="AB41" s="27"/>
+      <c r="AC41" s="27"/>
+      <c r="AD41" s="27"/>
+      <c r="AE41" s="27"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I43" s="15"/>
@@ -4601,7 +4609,7 @@
   <dimension ref="A1:CU54"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BL5" sqref="BL5"/>
+      <selection activeCell="BM5" sqref="BM5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4623,23 +4631,23 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="25" t="s">
+      <c r="Z1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="25"/>
-      <c r="AN1" s="25"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="28"/>
     </row>
     <row r="2" spans="1:99" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:99" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5122,7 +5130,9 @@
       <c r="BL4" s="23">
         <v>-20</v>
       </c>
-      <c r="BM4" s="23"/>
+      <c r="BM4" s="23">
+        <v>-35</v>
+      </c>
       <c r="BN4" s="23"/>
       <c r="BO4" s="23"/>
       <c r="BP4" s="23"/>
@@ -5174,67 +5184,67 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K39" s="5"/>
-      <c r="L39" s="28" t="s">
+      <c r="L39" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="28"/>
-      <c r="N39" s="28"/>
-      <c r="O39" s="28"/>
-      <c r="W39" s="30" t="s">
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="W39" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="30"/>
-      <c r="Z39" s="30"/>
-      <c r="AA39" s="30"/>
-      <c r="AB39" s="31">
+      <c r="X39" s="26"/>
+      <c r="Y39" s="26"/>
+      <c r="Z39" s="26"/>
+      <c r="AA39" s="26"/>
+      <c r="AB39" s="27">
         <f>SUM(E4:CU4)</f>
-        <v>2978</v>
-      </c>
-      <c r="AC39" s="31"/>
-      <c r="AD39" s="31"/>
-      <c r="AE39" s="31"/>
+        <v>2943</v>
+      </c>
+      <c r="AC39" s="27"/>
+      <c r="AD39" s="27"/>
+      <c r="AE39" s="27"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K40" s="13"/>
-      <c r="L40" s="29" t="s">
+      <c r="L40" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="29"/>
-      <c r="W40" s="30"/>
-      <c r="X40" s="30"/>
-      <c r="Y40" s="30"/>
-      <c r="Z40" s="30"/>
-      <c r="AA40" s="30"/>
-      <c r="AB40" s="31"/>
-      <c r="AC40" s="31"/>
-      <c r="AD40" s="31"/>
-      <c r="AE40" s="31"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="25"/>
+      <c r="O40" s="25"/>
+      <c r="P40" s="25"/>
+      <c r="Q40" s="25"/>
+      <c r="W40" s="26"/>
+      <c r="X40" s="26"/>
+      <c r="Y40" s="26"/>
+      <c r="Z40" s="26"/>
+      <c r="AA40" s="26"/>
+      <c r="AB40" s="27"/>
+      <c r="AC40" s="27"/>
+      <c r="AD40" s="27"/>
+      <c r="AE40" s="27"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.25">
       <c r="K41" s="11"/>
-      <c r="L41" s="29" t="s">
+      <c r="L41" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="29"/>
-      <c r="N41" s="29"/>
-      <c r="O41" s="29"/>
-      <c r="P41" s="29"/>
-      <c r="Q41" s="29"/>
-      <c r="R41" s="29"/>
-      <c r="W41" s="30"/>
-      <c r="X41" s="30"/>
-      <c r="Y41" s="30"/>
-      <c r="Z41" s="30"/>
-      <c r="AA41" s="30"/>
-      <c r="AB41" s="31"/>
-      <c r="AC41" s="31"/>
-      <c r="AD41" s="31"/>
-      <c r="AE41" s="31"/>
+      <c r="M41" s="25"/>
+      <c r="N41" s="25"/>
+      <c r="O41" s="25"/>
+      <c r="P41" s="25"/>
+      <c r="Q41" s="25"/>
+      <c r="R41" s="25"/>
+      <c r="W41" s="26"/>
+      <c r="X41" s="26"/>
+      <c r="Y41" s="26"/>
+      <c r="Z41" s="26"/>
+      <c r="AA41" s="26"/>
+      <c r="AB41" s="27"/>
+      <c r="AC41" s="27"/>
+      <c r="AD41" s="27"/>
+      <c r="AE41" s="27"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 26/04/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0156C8E0-140E-424A-BA07-0000FBBD4757}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A255661-9173-4562-870B-D84743DD79EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -1144,6 +1144,12 @@
                 <c:pt idx="60">
                   <c:v>-321</c:v>
                 </c:pt>
+                <c:pt idx="61">
+                  <c:v>-680</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>256</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1929,6 +1935,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>-35</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3567,8 +3579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BM5" sqref="BM5"/>
+    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BO5" sqref="BO5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4092,8 +4104,12 @@
       <c r="BM4" s="7">
         <v>-321</v>
       </c>
-      <c r="BN4" s="7"/>
-      <c r="BO4" s="7"/>
+      <c r="BN4" s="7">
+        <v>-680</v>
+      </c>
+      <c r="BO4" s="7">
+        <v>256</v>
+      </c>
       <c r="BP4" s="7"/>
       <c r="BQ4" s="7"/>
       <c r="BR4" s="7"/>
@@ -4158,7 +4174,7 @@
       <c r="AA39" s="26"/>
       <c r="AB39" s="27">
         <f>SUM(E4:CU4)</f>
-        <v>106527</v>
+        <v>106103</v>
       </c>
       <c r="AC39" s="27"/>
       <c r="AD39" s="27"/>
@@ -4608,8 +4624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BM5" sqref="BM5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BN5" sqref="BN5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5133,8 +5149,12 @@
       <c r="BM4" s="23">
         <v>-35</v>
       </c>
-      <c r="BN4" s="23"/>
-      <c r="BO4" s="23"/>
+      <c r="BN4" s="23">
+        <v>-8</v>
+      </c>
+      <c r="BO4" s="23">
+        <v>-11</v>
+      </c>
       <c r="BP4" s="23"/>
       <c r="BQ4" s="23"/>
       <c r="BR4" s="23"/>
@@ -5199,7 +5219,7 @@
       <c r="AA39" s="26"/>
       <c r="AB39" s="27">
         <f>SUM(E4:CU4)</f>
-        <v>2943</v>
+        <v>2924</v>
       </c>
       <c r="AC39" s="27"/>
       <c r="AD39" s="27"/>

</xml_diff>

<commit_message>
aggiornamento dati al 01/05/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -1,32 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpicc\Desktop\covid_19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A255661-9173-4562-870B-D84743DD79EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABB4447-802F-0744-9372-56326AED43BC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
     <sheet name="Campania" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -69,7 +63,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m;@"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,12 +181,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -203,6 +191,13 @@
       <b/>
       <sz val="26"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -337,7 +332,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -382,32 +377,35 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="17" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="16" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1149,6 +1147,21 @@
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-290</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-608</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-548</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-3106</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1941,6 +1954,21 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-47</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-75</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3579,19 +3607,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BO5" sqref="BO5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BT5" sqref="BT5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="4" width="5.7109375" style="1" customWidth="1"/>
-    <col min="5" max="25" width="4.7109375" style="2" customWidth="1"/>
-    <col min="26" max="28" width="4.7109375" style="3" customWidth="1"/>
-    <col min="29" max="99" width="4.7109375" customWidth="1"/>
+    <col min="2" max="4" width="5.6640625" style="1" customWidth="1"/>
+    <col min="5" max="25" width="4.6640625" style="2" customWidth="1"/>
+    <col min="26" max="28" width="4.6640625" style="3" customWidth="1"/>
+    <col min="29" max="99" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:99" ht="34.5" customHeight="1" thickBot="1">
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
@@ -3602,32 +3630,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="28" t="s">
+      <c r="Z1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
     </row>
-    <row r="2" spans="1:99" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+    <row r="2" spans="1:99" ht="16" thickTop="1"/>
+    <row r="3" spans="1:99" ht="24.75" customHeight="1">
+      <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -3914,13 +3942,13 @@
         <v>43979</v>
       </c>
     </row>
-    <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:99" ht="29.25" customHeight="1">
+      <c r="A4" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -4110,11 +4138,21 @@
       <c r="BO4" s="7">
         <v>256</v>
       </c>
-      <c r="BP4" s="7"/>
-      <c r="BQ4" s="7"/>
-      <c r="BR4" s="7"/>
-      <c r="BS4" s="7"/>
-      <c r="BT4" s="7"/>
+      <c r="BP4" s="7">
+        <v>-290</v>
+      </c>
+      <c r="BQ4" s="7">
+        <v>-608</v>
+      </c>
+      <c r="BR4" s="7">
+        <v>-548</v>
+      </c>
+      <c r="BS4" s="7">
+        <v>-3106</v>
+      </c>
+      <c r="BT4" s="7">
+        <v>-608</v>
+      </c>
       <c r="BU4" s="7"/>
       <c r="BV4" s="7"/>
       <c r="BW4" s="7"/>
@@ -4143,85 +4181,85 @@
       <c r="CT4" s="7"/>
       <c r="CU4" s="7"/>
     </row>
-    <row r="6" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:99" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:99" ht="15" customHeight="1"/>
+    <row r="7" spans="1:99" ht="35.25" customHeight="1"/>
+    <row r="14" spans="1:99">
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
+    <row r="15" spans="1:99">
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
     </row>
-    <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="31" t="s">
+      <c r="L39" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="31"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="31"/>
-      <c r="W39" s="26" t="s">
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
+      <c r="W39" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="26"/>
-      <c r="Y39" s="26"/>
-      <c r="Z39" s="26"/>
-      <c r="AA39" s="26"/>
-      <c r="AB39" s="27">
+      <c r="X39" s="27"/>
+      <c r="Y39" s="27"/>
+      <c r="Z39" s="27"/>
+      <c r="AA39" s="27"/>
+      <c r="AB39" s="28">
         <f>SUM(E4:CU4)</f>
-        <v>106103</v>
-      </c>
-      <c r="AC39" s="27"/>
-      <c r="AD39" s="27"/>
-      <c r="AE39" s="27"/>
+        <v>100943</v>
+      </c>
+      <c r="AC39" s="28"/>
+      <c r="AD39" s="28"/>
+      <c r="AE39" s="28"/>
     </row>
-    <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="25" t="s">
+      <c r="L40" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
-      <c r="O40" s="25"/>
-      <c r="P40" s="25"/>
-      <c r="Q40" s="25"/>
-      <c r="W40" s="26"/>
-      <c r="X40" s="26"/>
-      <c r="Y40" s="26"/>
-      <c r="Z40" s="26"/>
-      <c r="AA40" s="26"/>
-      <c r="AB40" s="27"/>
-      <c r="AC40" s="27"/>
-      <c r="AD40" s="27"/>
-      <c r="AE40" s="27"/>
+      <c r="M40" s="26"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="26"/>
+      <c r="W40" s="27"/>
+      <c r="X40" s="27"/>
+      <c r="Y40" s="27"/>
+      <c r="Z40" s="27"/>
+      <c r="AA40" s="27"/>
+      <c r="AB40" s="28"/>
+      <c r="AC40" s="28"/>
+      <c r="AD40" s="28"/>
+      <c r="AE40" s="28"/>
     </row>
-    <row r="41" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="25" t="s">
+      <c r="L41" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="25"/>
-      <c r="N41" s="25"/>
-      <c r="O41" s="25"/>
-      <c r="P41" s="25"/>
-      <c r="Q41" s="25"/>
-      <c r="R41" s="25"/>
-      <c r="W41" s="26"/>
-      <c r="X41" s="26"/>
-      <c r="Y41" s="26"/>
-      <c r="Z41" s="26"/>
-      <c r="AA41" s="26"/>
-      <c r="AB41" s="27"/>
-      <c r="AC41" s="27"/>
-      <c r="AD41" s="27"/>
-      <c r="AE41" s="27"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26"/>
+      <c r="W41" s="27"/>
+      <c r="X41" s="27"/>
+      <c r="Y41" s="27"/>
+      <c r="Z41" s="27"/>
+      <c r="AA41" s="27"/>
+      <c r="AB41" s="28"/>
+      <c r="AC41" s="28"/>
+      <c r="AD41" s="28"/>
+      <c r="AE41" s="28"/>
     </row>
-    <row r="43" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:37">
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
       <c r="K43" s="15"/>
@@ -4252,7 +4290,7 @@
       <c r="AJ43" s="17"/>
       <c r="AK43" s="17"/>
     </row>
-    <row r="44" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="44" spans="9:37">
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
@@ -4283,7 +4321,7 @@
       <c r="AJ44" s="17"/>
       <c r="AK44" s="17"/>
     </row>
-    <row r="45" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="45" spans="9:37">
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
@@ -4314,15 +4352,15 @@
       <c r="AJ45" s="17"/>
       <c r="AK45" s="17"/>
     </row>
-    <row r="46" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="46" spans="9:37">
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
-      <c r="P46" s="15"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="23"/>
+      <c r="O46" s="23"/>
+      <c r="P46" s="23"/>
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
       <c r="S46" s="15"/>
@@ -4345,20 +4383,20 @@
       <c r="AJ46" s="17"/>
       <c r="AK46" s="17"/>
     </row>
-    <row r="47" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="47" spans="9:37">
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="18" t="s">
+      <c r="M47" s="23"/>
+      <c r="N47" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="O47" s="19">
+      <c r="O47" s="25">
         <f>MAXA(E4:BJ4)</f>
         <v>4821</v>
       </c>
-      <c r="P47" s="15"/>
+      <c r="P47" s="23"/>
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
       <c r="S47" s="15"/>
@@ -4381,15 +4419,15 @@
       <c r="AJ47" s="17"/>
       <c r="AK47" s="17"/>
     </row>
-    <row r="48" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="48" spans="9:37">
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
       <c r="K48" s="15"/>
       <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
+      <c r="M48" s="23"/>
+      <c r="N48" s="23"/>
+      <c r="O48" s="23"/>
+      <c r="P48" s="23"/>
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
       <c r="S48" s="15"/>
@@ -4412,7 +4450,7 @@
       <c r="AJ48" s="17"/>
       <c r="AK48" s="17"/>
     </row>
-    <row r="49" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="49" spans="9:37">
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
       <c r="K49" s="15"/>
@@ -4443,7 +4481,7 @@
       <c r="AJ49" s="17"/>
       <c r="AK49" s="17"/>
     </row>
-    <row r="50" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="50" spans="9:37">
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
       <c r="K50" s="15"/>
@@ -4474,7 +4512,7 @@
       <c r="AJ50" s="17"/>
       <c r="AK50" s="17"/>
     </row>
-    <row r="51" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="51" spans="9:37">
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15"/>
@@ -4505,7 +4543,7 @@
       <c r="AJ51" s="17"/>
       <c r="AK51" s="17"/>
     </row>
-    <row r="52" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="52" spans="9:37">
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="K52" s="15"/>
@@ -4536,7 +4574,7 @@
       <c r="AJ52" s="17"/>
       <c r="AK52" s="17"/>
     </row>
-    <row r="53" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="53" spans="9:37">
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
       <c r="K53" s="15"/>
@@ -4567,7 +4605,7 @@
       <c r="AJ53" s="17"/>
       <c r="AK53" s="17"/>
     </row>
-    <row r="54" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="54" spans="9:37">
       <c r="I54" s="15"/>
       <c r="J54" s="15"/>
       <c r="K54" s="15"/>
@@ -4625,18 +4663,18 @@
   <dimension ref="A1:CU54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BN5" sqref="BN5"/>
+      <selection activeCell="BU4" sqref="BU4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="4" width="5.7109375" style="1" customWidth="1"/>
-    <col min="5" max="25" width="4.7109375" style="2" customWidth="1"/>
-    <col min="26" max="28" width="4.7109375" style="3" customWidth="1"/>
-    <col min="29" max="99" width="4.7109375" customWidth="1"/>
+    <col min="2" max="4" width="5.6640625" style="1" customWidth="1"/>
+    <col min="5" max="25" width="4.6640625" style="2" customWidth="1"/>
+    <col min="26" max="28" width="4.6640625" style="3" customWidth="1"/>
+    <col min="29" max="99" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:99" ht="34.5" customHeight="1" thickBot="1">
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
@@ -4647,32 +4685,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="28" t="s">
+      <c r="Z1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
     </row>
-    <row r="2" spans="1:99" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:99" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+    <row r="2" spans="1:99" ht="16" thickTop="1"/>
+    <row r="3" spans="1:99" s="22" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -4959,314 +4997,324 @@
         <v>43979</v>
       </c>
     </row>
-    <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:99" ht="29.25" customHeight="1">
+      <c r="A4" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="22">
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="20">
         <v>0</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="20">
         <v>0</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="20">
         <v>0</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="20">
         <v>3</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="20">
         <v>1</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="20">
         <v>9</v>
       </c>
-      <c r="K4" s="22">
+      <c r="K4" s="20">
         <v>4</v>
       </c>
-      <c r="L4" s="22">
+      <c r="L4" s="20">
         <v>0</v>
       </c>
-      <c r="M4" s="22">
+      <c r="M4" s="20">
         <v>13</v>
       </c>
-      <c r="N4" s="22">
+      <c r="N4" s="20">
         <v>1</v>
       </c>
-      <c r="O4" s="22">
+      <c r="O4" s="20">
         <v>14</v>
       </c>
-      <c r="P4" s="22">
+      <c r="P4" s="20">
         <v>12</v>
       </c>
-      <c r="Q4" s="22">
+      <c r="Q4" s="20">
         <v>4</v>
       </c>
-      <c r="R4" s="22">
+      <c r="R4" s="20">
         <v>29</v>
       </c>
-      <c r="S4" s="22">
+      <c r="S4" s="20">
         <v>19</v>
       </c>
-      <c r="T4" s="22">
+      <c r="T4" s="20">
         <v>7</v>
       </c>
-      <c r="U4" s="22">
+      <c r="U4" s="20">
         <v>23</v>
       </c>
-      <c r="V4" s="22">
+      <c r="V4" s="20">
         <v>25</v>
       </c>
-      <c r="W4" s="22">
+      <c r="W4" s="20">
         <v>29</v>
       </c>
-      <c r="X4" s="22">
+      <c r="X4" s="20">
         <v>30</v>
       </c>
-      <c r="Y4" s="22">
+      <c r="Y4" s="20">
         <v>40</v>
       </c>
-      <c r="Z4" s="22">
+      <c r="Z4" s="20">
         <v>65</v>
       </c>
-      <c r="AA4" s="22">
+      <c r="AA4" s="20">
         <v>60</v>
       </c>
-      <c r="AB4" s="22">
+      <c r="AB4" s="20">
         <v>100</v>
       </c>
-      <c r="AC4" s="22">
+      <c r="AC4" s="20">
         <v>82</v>
       </c>
-      <c r="AD4" s="22">
+      <c r="AD4" s="20">
         <v>97</v>
       </c>
-      <c r="AE4" s="22">
+      <c r="AE4" s="20">
         <v>91</v>
       </c>
-      <c r="AF4" s="23">
+      <c r="AF4" s="21">
         <v>73</v>
       </c>
-      <c r="AG4" s="23">
+      <c r="AG4" s="21">
         <v>63</v>
       </c>
-      <c r="AH4" s="23">
+      <c r="AH4" s="21">
         <v>63</v>
       </c>
-      <c r="AI4" s="23">
+      <c r="AI4" s="21">
         <v>80</v>
       </c>
-      <c r="AJ4" s="23">
+      <c r="AJ4" s="21">
         <v>97</v>
       </c>
-      <c r="AK4" s="23">
+      <c r="AK4" s="21">
         <v>123</v>
       </c>
-      <c r="AL4" s="23">
+      <c r="AL4" s="21">
         <v>115</v>
       </c>
-      <c r="AM4" s="23">
+      <c r="AM4" s="21">
         <v>149</v>
       </c>
-      <c r="AN4" s="23">
+      <c r="AN4" s="21">
         <v>183</v>
       </c>
-      <c r="AO4" s="23">
+      <c r="AO4" s="21">
         <v>132</v>
       </c>
-      <c r="AP4" s="23">
+      <c r="AP4" s="21">
         <v>105</v>
       </c>
-      <c r="AQ4" s="23">
+      <c r="AQ4" s="21">
         <v>164</v>
       </c>
-      <c r="AR4" s="23">
+      <c r="AR4" s="21">
         <v>212</v>
       </c>
-      <c r="AS4" s="23">
+      <c r="AS4" s="21">
         <v>144</v>
       </c>
-      <c r="AT4" s="23">
+      <c r="AT4" s="21">
         <v>125</v>
       </c>
-      <c r="AU4" s="23">
+      <c r="AU4" s="21">
         <v>77</v>
       </c>
-      <c r="AV4" s="23">
+      <c r="AV4" s="21">
         <v>67</v>
       </c>
-      <c r="AW4" s="23">
+      <c r="AW4" s="21">
         <v>94</v>
       </c>
-      <c r="AX4" s="23">
+      <c r="AX4" s="21">
         <v>14</v>
       </c>
-      <c r="AY4" s="23">
+      <c r="AY4" s="21">
         <v>90</v>
       </c>
-      <c r="AZ4" s="23">
+      <c r="AZ4" s="21">
         <v>39</v>
       </c>
-      <c r="BA4" s="23">
+      <c r="BA4" s="21">
         <v>55</v>
       </c>
-      <c r="BB4" s="23">
+      <c r="BB4" s="21">
         <v>5</v>
       </c>
-      <c r="BC4" s="23">
+      <c r="BC4" s="21">
         <v>32</v>
       </c>
-      <c r="BD4" s="23">
+      <c r="BD4" s="21">
         <v>-7</v>
       </c>
-      <c r="BE4" s="23">
+      <c r="BE4" s="21">
         <v>31</v>
       </c>
-      <c r="BF4" s="23">
+      <c r="BF4" s="21">
         <v>-91</v>
       </c>
-      <c r="BG4" s="23">
+      <c r="BG4" s="21">
         <v>18</v>
       </c>
-      <c r="BH4" s="23">
+      <c r="BH4" s="21">
         <v>12</v>
       </c>
-      <c r="BI4" s="23">
+      <c r="BI4" s="21">
         <v>-3</v>
       </c>
-      <c r="BJ4" s="23">
+      <c r="BJ4" s="21">
         <v>-73</v>
       </c>
-      <c r="BK4" s="23">
+      <c r="BK4" s="21">
         <v>52</v>
       </c>
-      <c r="BL4" s="23">
+      <c r="BL4" s="21">
         <v>-20</v>
       </c>
-      <c r="BM4" s="23">
+      <c r="BM4" s="21">
         <v>-35</v>
       </c>
-      <c r="BN4" s="23">
+      <c r="BN4" s="21">
         <v>-8</v>
       </c>
-      <c r="BO4" s="23">
+      <c r="BO4" s="21">
         <v>-11</v>
       </c>
-      <c r="BP4" s="23"/>
-      <c r="BQ4" s="23"/>
-      <c r="BR4" s="23"/>
-      <c r="BS4" s="23"/>
-      <c r="BT4" s="23"/>
-      <c r="BU4" s="23"/>
-      <c r="BV4" s="23"/>
-      <c r="BW4" s="23"/>
-      <c r="BX4" s="23"/>
-      <c r="BY4" s="23"/>
-      <c r="BZ4" s="23"/>
-      <c r="CA4" s="23"/>
-      <c r="CB4" s="23"/>
-      <c r="CC4" s="23"/>
-      <c r="CD4" s="23"/>
-      <c r="CE4" s="23"/>
-      <c r="CF4" s="23"/>
-      <c r="CG4" s="23"/>
-      <c r="CH4" s="23"/>
-      <c r="CI4" s="23"/>
-      <c r="CJ4" s="23"/>
-      <c r="CK4" s="23"/>
-      <c r="CL4" s="23"/>
-      <c r="CM4" s="23"/>
-      <c r="CN4" s="23"/>
-      <c r="CO4" s="23"/>
-      <c r="CP4" s="23"/>
-      <c r="CQ4" s="23"/>
-      <c r="CR4" s="23"/>
-      <c r="CS4" s="23"/>
-      <c r="CT4" s="23"/>
-      <c r="CU4" s="23"/>
+      <c r="BP4" s="21">
+        <v>-47</v>
+      </c>
+      <c r="BQ4" s="21">
+        <v>-75</v>
+      </c>
+      <c r="BR4" s="21">
+        <v>-20</v>
+      </c>
+      <c r="BS4" s="21">
+        <v>-9</v>
+      </c>
+      <c r="BT4" s="21">
+        <v>-20</v>
+      </c>
+      <c r="BU4" s="21"/>
+      <c r="BV4" s="21"/>
+      <c r="BW4" s="21"/>
+      <c r="BX4" s="21"/>
+      <c r="BY4" s="21"/>
+      <c r="BZ4" s="21"/>
+      <c r="CA4" s="21"/>
+      <c r="CB4" s="21"/>
+      <c r="CC4" s="21"/>
+      <c r="CD4" s="21"/>
+      <c r="CE4" s="21"/>
+      <c r="CF4" s="21"/>
+      <c r="CG4" s="21"/>
+      <c r="CH4" s="21"/>
+      <c r="CI4" s="21"/>
+      <c r="CJ4" s="21"/>
+      <c r="CK4" s="21"/>
+      <c r="CL4" s="21"/>
+      <c r="CM4" s="21"/>
+      <c r="CN4" s="21"/>
+      <c r="CO4" s="21"/>
+      <c r="CP4" s="21"/>
+      <c r="CQ4" s="21"/>
+      <c r="CR4" s="21"/>
+      <c r="CS4" s="21"/>
+      <c r="CT4" s="21"/>
+      <c r="CU4" s="21"/>
     </row>
-    <row r="6" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:99" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:99" ht="15" customHeight="1"/>
+    <row r="7" spans="1:99" ht="35.25" customHeight="1"/>
+    <row r="14" spans="1:99">
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
+    <row r="15" spans="1:99">
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
     </row>
-    <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="31" t="s">
+      <c r="L39" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="31"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="31"/>
-      <c r="W39" s="26" t="s">
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
+      <c r="W39" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="26"/>
-      <c r="Y39" s="26"/>
-      <c r="Z39" s="26"/>
-      <c r="AA39" s="26"/>
-      <c r="AB39" s="27">
+      <c r="X39" s="27"/>
+      <c r="Y39" s="27"/>
+      <c r="Z39" s="27"/>
+      <c r="AA39" s="27"/>
+      <c r="AB39" s="28">
         <f>SUM(E4:CU4)</f>
-        <v>2924</v>
-      </c>
-      <c r="AC39" s="27"/>
-      <c r="AD39" s="27"/>
-      <c r="AE39" s="27"/>
+        <v>2753</v>
+      </c>
+      <c r="AC39" s="28"/>
+      <c r="AD39" s="28"/>
+      <c r="AE39" s="28"/>
     </row>
-    <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="25" t="s">
+      <c r="L40" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
-      <c r="O40" s="25"/>
-      <c r="P40" s="25"/>
-      <c r="Q40" s="25"/>
-      <c r="W40" s="26"/>
-      <c r="X40" s="26"/>
-      <c r="Y40" s="26"/>
-      <c r="Z40" s="26"/>
-      <c r="AA40" s="26"/>
-      <c r="AB40" s="27"/>
-      <c r="AC40" s="27"/>
-      <c r="AD40" s="27"/>
-      <c r="AE40" s="27"/>
+      <c r="M40" s="26"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="26"/>
+      <c r="W40" s="27"/>
+      <c r="X40" s="27"/>
+      <c r="Y40" s="27"/>
+      <c r="Z40" s="27"/>
+      <c r="AA40" s="27"/>
+      <c r="AB40" s="28"/>
+      <c r="AC40" s="28"/>
+      <c r="AD40" s="28"/>
+      <c r="AE40" s="28"/>
     </row>
-    <row r="41" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="25" t="s">
+      <c r="L41" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="25"/>
-      <c r="N41" s="25"/>
-      <c r="O41" s="25"/>
-      <c r="P41" s="25"/>
-      <c r="Q41" s="25"/>
-      <c r="R41" s="25"/>
-      <c r="W41" s="26"/>
-      <c r="X41" s="26"/>
-      <c r="Y41" s="26"/>
-      <c r="Z41" s="26"/>
-      <c r="AA41" s="26"/>
-      <c r="AB41" s="27"/>
-      <c r="AC41" s="27"/>
-      <c r="AD41" s="27"/>
-      <c r="AE41" s="27"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26"/>
+      <c r="W41" s="27"/>
+      <c r="X41" s="27"/>
+      <c r="Y41" s="27"/>
+      <c r="Z41" s="27"/>
+      <c r="AA41" s="27"/>
+      <c r="AB41" s="28"/>
+      <c r="AC41" s="28"/>
+      <c r="AD41" s="28"/>
+      <c r="AE41" s="28"/>
     </row>
-    <row r="43" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:37">
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
       <c r="K43" s="15"/>
@@ -5297,7 +5345,7 @@
       <c r="AJ43" s="17"/>
       <c r="AK43" s="17"/>
     </row>
-    <row r="44" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="44" spans="9:37">
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
@@ -5328,7 +5376,7 @@
       <c r="AJ44" s="17"/>
       <c r="AK44" s="17"/>
     </row>
-    <row r="45" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="45" spans="9:37">
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
@@ -5359,7 +5407,7 @@
       <c r="AJ45" s="17"/>
       <c r="AK45" s="17"/>
     </row>
-    <row r="46" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="46" spans="9:37">
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
@@ -5390,16 +5438,16 @@
       <c r="AJ46" s="17"/>
       <c r="AK46" s="17"/>
     </row>
-    <row r="47" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="47" spans="9:37">
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
-      <c r="N47" s="18" t="s">
+      <c r="N47" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="O47" s="19">
+      <c r="O47" s="25">
         <f>MAXA(E4:BJ4)</f>
         <v>212</v>
       </c>
@@ -5426,7 +5474,7 @@
       <c r="AJ47" s="17"/>
       <c r="AK47" s="17"/>
     </row>
-    <row r="48" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="48" spans="9:37">
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
       <c r="K48" s="15"/>
@@ -5457,7 +5505,7 @@
       <c r="AJ48" s="17"/>
       <c r="AK48" s="17"/>
     </row>
-    <row r="49" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="49" spans="9:37">
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
       <c r="K49" s="15"/>
@@ -5488,7 +5536,7 @@
       <c r="AJ49" s="17"/>
       <c r="AK49" s="17"/>
     </row>
-    <row r="50" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="50" spans="9:37">
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
       <c r="K50" s="15"/>
@@ -5519,7 +5567,7 @@
       <c r="AJ50" s="17"/>
       <c r="AK50" s="17"/>
     </row>
-    <row r="51" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="51" spans="9:37">
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15"/>
@@ -5550,7 +5598,7 @@
       <c r="AJ51" s="17"/>
       <c r="AK51" s="17"/>
     </row>
-    <row r="52" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="52" spans="9:37">
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="K52" s="15"/>
@@ -5581,7 +5629,7 @@
       <c r="AJ52" s="17"/>
       <c r="AK52" s="17"/>
     </row>
-    <row r="53" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="53" spans="9:37">
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
       <c r="K53" s="15"/>
@@ -5612,7 +5660,7 @@
       <c r="AJ53" s="17"/>
       <c r="AK53" s="17"/>
     </row>
-    <row r="54" spans="9:37" x14ac:dyDescent="0.25">
+    <row r="54" spans="9:37">
       <c r="I54" s="15"/>
       <c r="J54" s="15"/>
       <c r="K54" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 02/05/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABB4447-802F-0744-9372-56326AED43BC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954DC992-5B67-8E49-82CC-12F35E54CD9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
     <sheet name="Campania" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -63,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m;@"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1163,6 +1169,9 @@
                 <c:pt idx="67">
                   <c:v>-608</c:v>
                 </c:pt>
+                <c:pt idx="68">
+                  <c:v>-239</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1969,6 +1978,9 @@
                 </c:pt>
                 <c:pt idx="64">
                   <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3607,11 +3619,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BT5" sqref="BT5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BV4" sqref="BV4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="4" width="5.6640625" style="1" customWidth="1"/>
     <col min="5" max="25" width="4.6640625" style="2" customWidth="1"/>
@@ -3619,7 +3631,7 @@
     <col min="29" max="99" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="34.5" customHeight="1" thickBot="1">
+    <row r="1" spans="1:99" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
@@ -3648,8 +3660,8 @@
       <c r="AM1" s="29"/>
       <c r="AN1" s="29"/>
     </row>
-    <row r="2" spans="1:99" ht="16" thickTop="1"/>
-    <row r="3" spans="1:99" ht="24.75" customHeight="1">
+    <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
@@ -3942,7 +3954,7 @@
         <v>43979</v>
       </c>
     </row>
-    <row r="4" spans="1:99" ht="29.25" customHeight="1">
+    <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>0</v>
       </c>
@@ -4153,7 +4165,9 @@
       <c r="BT4" s="7">
         <v>-608</v>
       </c>
-      <c r="BU4" s="7"/>
+      <c r="BU4" s="7">
+        <v>-239</v>
+      </c>
       <c r="BV4" s="7"/>
       <c r="BW4" s="7"/>
       <c r="BX4" s="7"/>
@@ -4181,12 +4195,12 @@
       <c r="CT4" s="7"/>
       <c r="CU4" s="7"/>
     </row>
-    <row r="6" spans="1:99" ht="15" customHeight="1"/>
-    <row r="7" spans="1:99" ht="35.25" customHeight="1"/>
-    <row r="14" spans="1:99">
+    <row r="6" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:99" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:99" x14ac:dyDescent="0.2">
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:99">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.2">
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -4195,7 +4209,7 @@
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="39" spans="9:37" ht="15" customHeight="1">
+    <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
       <c r="L39" s="32" t="s">
         <v>3</v>
@@ -4212,13 +4226,13 @@
       <c r="AA39" s="27"/>
       <c r="AB39" s="28">
         <f>SUM(E4:CU4)</f>
-        <v>100943</v>
+        <v>100704</v>
       </c>
       <c r="AC39" s="28"/>
       <c r="AD39" s="28"/>
       <c r="AE39" s="28"/>
     </row>
-    <row r="40" spans="9:37" ht="15" customHeight="1">
+    <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
       <c r="L40" s="26" t="s">
         <v>6</v>
@@ -4238,7 +4252,7 @@
       <c r="AD40" s="28"/>
       <c r="AE40" s="28"/>
     </row>
-    <row r="41" spans="9:37">
+    <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
       <c r="L41" s="26" t="s">
         <v>8</v>
@@ -4259,7 +4273,7 @@
       <c r="AD41" s="28"/>
       <c r="AE41" s="28"/>
     </row>
-    <row r="43" spans="9:37">
+    <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
       <c r="K43" s="15"/>
@@ -4290,7 +4304,7 @@
       <c r="AJ43" s="17"/>
       <c r="AK43" s="17"/>
     </row>
-    <row r="44" spans="9:37">
+    <row r="44" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
@@ -4321,7 +4335,7 @@
       <c r="AJ44" s="17"/>
       <c r="AK44" s="17"/>
     </row>
-    <row r="45" spans="9:37">
+    <row r="45" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
@@ -4352,7 +4366,7 @@
       <c r="AJ45" s="17"/>
       <c r="AK45" s="17"/>
     </row>
-    <row r="46" spans="9:37">
+    <row r="46" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
@@ -4383,7 +4397,7 @@
       <c r="AJ46" s="17"/>
       <c r="AK46" s="17"/>
     </row>
-    <row r="47" spans="9:37">
+    <row r="47" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
       <c r="K47" s="15"/>
@@ -4419,7 +4433,7 @@
       <c r="AJ47" s="17"/>
       <c r="AK47" s="17"/>
     </row>
-    <row r="48" spans="9:37">
+    <row r="48" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
       <c r="K48" s="15"/>
@@ -4450,7 +4464,7 @@
       <c r="AJ48" s="17"/>
       <c r="AK48" s="17"/>
     </row>
-    <row r="49" spans="9:37">
+    <row r="49" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
       <c r="K49" s="15"/>
@@ -4481,7 +4495,7 @@
       <c r="AJ49" s="17"/>
       <c r="AK49" s="17"/>
     </row>
-    <row r="50" spans="9:37">
+    <row r="50" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
       <c r="K50" s="15"/>
@@ -4512,7 +4526,7 @@
       <c r="AJ50" s="17"/>
       <c r="AK50" s="17"/>
     </row>
-    <row r="51" spans="9:37">
+    <row r="51" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15"/>
@@ -4543,7 +4557,7 @@
       <c r="AJ51" s="17"/>
       <c r="AK51" s="17"/>
     </row>
-    <row r="52" spans="9:37">
+    <row r="52" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="K52" s="15"/>
@@ -4574,7 +4588,7 @@
       <c r="AJ52" s="17"/>
       <c r="AK52" s="17"/>
     </row>
-    <row r="53" spans="9:37">
+    <row r="53" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
       <c r="K53" s="15"/>
@@ -4605,7 +4619,7 @@
       <c r="AJ53" s="17"/>
       <c r="AK53" s="17"/>
     </row>
-    <row r="54" spans="9:37">
+    <row r="54" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I54" s="15"/>
       <c r="J54" s="15"/>
       <c r="K54" s="15"/>
@@ -4662,11 +4676,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BU4" sqref="BU4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BV4" sqref="BV4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="4" width="5.6640625" style="1" customWidth="1"/>
     <col min="5" max="25" width="4.6640625" style="2" customWidth="1"/>
@@ -4674,7 +4688,7 @@
     <col min="29" max="99" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="34.5" customHeight="1" thickBot="1">
+    <row r="1" spans="1:99" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
@@ -4703,8 +4717,8 @@
       <c r="AM1" s="29"/>
       <c r="AN1" s="29"/>
     </row>
-    <row r="2" spans="1:99" ht="16" thickTop="1"/>
-    <row r="3" spans="1:99" s="22" customFormat="1" ht="24.75" customHeight="1">
+    <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:99" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>2</v>
       </c>
@@ -4997,7 +5011,7 @@
         <v>43979</v>
       </c>
     </row>
-    <row r="4" spans="1:99" ht="29.25" customHeight="1">
+    <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>0</v>
       </c>
@@ -5208,7 +5222,9 @@
       <c r="BT4" s="21">
         <v>-20</v>
       </c>
-      <c r="BU4" s="21"/>
+      <c r="BU4" s="21">
+        <v>-32</v>
+      </c>
       <c r="BV4" s="21"/>
       <c r="BW4" s="21"/>
       <c r="BX4" s="21"/>
@@ -5236,12 +5252,12 @@
       <c r="CT4" s="21"/>
       <c r="CU4" s="21"/>
     </row>
-    <row r="6" spans="1:99" ht="15" customHeight="1"/>
-    <row r="7" spans="1:99" ht="35.25" customHeight="1"/>
-    <row r="14" spans="1:99">
+    <row r="6" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:99" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:99" x14ac:dyDescent="0.2">
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:99">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.2">
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -5250,7 +5266,7 @@
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="39" spans="9:37" ht="15" customHeight="1">
+    <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
       <c r="L39" s="32" t="s">
         <v>3</v>
@@ -5267,13 +5283,13 @@
       <c r="AA39" s="27"/>
       <c r="AB39" s="28">
         <f>SUM(E4:CU4)</f>
-        <v>2753</v>
+        <v>2721</v>
       </c>
       <c r="AC39" s="28"/>
       <c r="AD39" s="28"/>
       <c r="AE39" s="28"/>
     </row>
-    <row r="40" spans="9:37" ht="15" customHeight="1">
+    <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
       <c r="L40" s="26" t="s">
         <v>6</v>
@@ -5293,7 +5309,7 @@
       <c r="AD40" s="28"/>
       <c r="AE40" s="28"/>
     </row>
-    <row r="41" spans="9:37">
+    <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
       <c r="L41" s="26" t="s">
         <v>8</v>
@@ -5314,7 +5330,7 @@
       <c r="AD41" s="28"/>
       <c r="AE41" s="28"/>
     </row>
-    <row r="43" spans="9:37">
+    <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
       <c r="K43" s="15"/>
@@ -5345,7 +5361,7 @@
       <c r="AJ43" s="17"/>
       <c r="AK43" s="17"/>
     </row>
-    <row r="44" spans="9:37">
+    <row r="44" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
@@ -5376,7 +5392,7 @@
       <c r="AJ44" s="17"/>
       <c r="AK44" s="17"/>
     </row>
-    <row r="45" spans="9:37">
+    <row r="45" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
@@ -5407,7 +5423,7 @@
       <c r="AJ45" s="17"/>
       <c r="AK45" s="17"/>
     </row>
-    <row r="46" spans="9:37">
+    <row r="46" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
@@ -5438,7 +5454,7 @@
       <c r="AJ46" s="17"/>
       <c r="AK46" s="17"/>
     </row>
-    <row r="47" spans="9:37">
+    <row r="47" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
       <c r="K47" s="15"/>
@@ -5474,7 +5490,7 @@
       <c r="AJ47" s="17"/>
       <c r="AK47" s="17"/>
     </row>
-    <row r="48" spans="9:37">
+    <row r="48" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
       <c r="K48" s="15"/>
@@ -5505,7 +5521,7 @@
       <c r="AJ48" s="17"/>
       <c r="AK48" s="17"/>
     </row>
-    <row r="49" spans="9:37">
+    <row r="49" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
       <c r="K49" s="15"/>
@@ -5536,7 +5552,7 @@
       <c r="AJ49" s="17"/>
       <c r="AK49" s="17"/>
     </row>
-    <row r="50" spans="9:37">
+    <row r="50" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
       <c r="K50" s="15"/>
@@ -5567,7 +5583,7 @@
       <c r="AJ50" s="17"/>
       <c r="AK50" s="17"/>
     </row>
-    <row r="51" spans="9:37">
+    <row r="51" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15"/>
@@ -5598,7 +5614,7 @@
       <c r="AJ51" s="17"/>
       <c r="AK51" s="17"/>
     </row>
-    <row r="52" spans="9:37">
+    <row r="52" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="K52" s="15"/>
@@ -5629,7 +5645,7 @@
       <c r="AJ52" s="17"/>
       <c r="AK52" s="17"/>
     </row>
-    <row r="53" spans="9:37">
+    <row r="53" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
       <c r="K53" s="15"/>
@@ -5660,7 +5676,7 @@
       <c r="AJ53" s="17"/>
       <c r="AK53" s="17"/>
     </row>
-    <row r="54" spans="9:37">
+    <row r="54" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I54" s="15"/>
       <c r="J54" s="15"/>
       <c r="K54" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 03/05/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52051675-D373-7640-92ED-E4869C777BCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E6E5B6-1024-7B48-903F-2E8249595241}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -405,6 +405,7 @@
     <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -444,7 +445,6 @@
     <xf numFmtId="164" fontId="9" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Colore 5" xfId="5" builtinId="46"/>
@@ -1172,6 +1172,9 @@
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>-239</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-525</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1982,6 +1985,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>-32</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3620,8 +3626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BT7" sqref="BT7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BV5" sqref="BV5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3643,32 +3649,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="29" t="s">
+      <c r="Z1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="29"/>
-      <c r="AG1" s="29"/>
-      <c r="AH1" s="29"/>
-      <c r="AI1" s="29"/>
-      <c r="AJ1" s="29"/>
-      <c r="AK1" s="29"/>
-      <c r="AL1" s="29"/>
-      <c r="AM1" s="29"/>
-      <c r="AN1" s="29"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
     </row>
     <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -3956,12 +3962,12 @@
       </c>
     </row>
     <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -4169,7 +4175,9 @@
       <c r="BU4" s="7">
         <v>-239</v>
       </c>
-      <c r="BV4" s="7"/>
+      <c r="BV4" s="7">
+        <v>-525</v>
+      </c>
       <c r="BW4" s="7"/>
       <c r="BX4" s="7"/>
       <c r="BY4" s="7"/>
@@ -4198,7 +4206,7 @@
     </row>
     <row r="6" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:99" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="BT7" s="39"/>
+      <c r="BT7" s="26"/>
     </row>
     <row r="14" spans="1:99" x14ac:dyDescent="0.2">
       <c r="I14" s="12"/>
@@ -4214,67 +4222,67 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="32" t="s">
+      <c r="L39" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
-      <c r="W39" s="27" t="s">
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="33"/>
+      <c r="W39" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="27"/>
-      <c r="Y39" s="27"/>
-      <c r="Z39" s="27"/>
-      <c r="AA39" s="27"/>
-      <c r="AB39" s="28">
+      <c r="X39" s="28"/>
+      <c r="Y39" s="28"/>
+      <c r="Z39" s="28"/>
+      <c r="AA39" s="28"/>
+      <c r="AB39" s="29">
         <f>SUM(E4:CU4)</f>
-        <v>100704</v>
-      </c>
-      <c r="AC39" s="28"/>
-      <c r="AD39" s="28"/>
-      <c r="AE39" s="28"/>
+        <v>100179</v>
+      </c>
+      <c r="AC39" s="29"/>
+      <c r="AD39" s="29"/>
+      <c r="AE39" s="29"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="26" t="s">
+      <c r="L40" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="26"/>
-      <c r="N40" s="26"/>
-      <c r="O40" s="26"/>
-      <c r="P40" s="26"/>
-      <c r="Q40" s="26"/>
-      <c r="W40" s="27"/>
-      <c r="X40" s="27"/>
-      <c r="Y40" s="27"/>
-      <c r="Z40" s="27"/>
-      <c r="AA40" s="27"/>
-      <c r="AB40" s="28"/>
-      <c r="AC40" s="28"/>
-      <c r="AD40" s="28"/>
-      <c r="AE40" s="28"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="27"/>
+      <c r="Q40" s="27"/>
+      <c r="W40" s="28"/>
+      <c r="X40" s="28"/>
+      <c r="Y40" s="28"/>
+      <c r="Z40" s="28"/>
+      <c r="AA40" s="28"/>
+      <c r="AB40" s="29"/>
+      <c r="AC40" s="29"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="29"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="26" t="s">
+      <c r="L41" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="26"/>
-      <c r="N41" s="26"/>
-      <c r="O41" s="26"/>
-      <c r="P41" s="26"/>
-      <c r="Q41" s="26"/>
-      <c r="R41" s="26"/>
-      <c r="W41" s="27"/>
-      <c r="X41" s="27"/>
-      <c r="Y41" s="27"/>
-      <c r="Z41" s="27"/>
-      <c r="AA41" s="27"/>
-      <c r="AB41" s="28"/>
-      <c r="AC41" s="28"/>
-      <c r="AD41" s="28"/>
-      <c r="AE41" s="28"/>
+      <c r="M41" s="27"/>
+      <c r="N41" s="27"/>
+      <c r="O41" s="27"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="27"/>
+      <c r="R41" s="27"/>
+      <c r="W41" s="28"/>
+      <c r="X41" s="28"/>
+      <c r="Y41" s="28"/>
+      <c r="Z41" s="28"/>
+      <c r="AA41" s="28"/>
+      <c r="AB41" s="29"/>
+      <c r="AC41" s="29"/>
+      <c r="AD41" s="29"/>
+      <c r="AE41" s="29"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
@@ -4679,8 +4687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BV4" sqref="BV4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BW4" sqref="BW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4702,32 +4710,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="29" t="s">
+      <c r="Z1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="29"/>
-      <c r="AG1" s="29"/>
-      <c r="AH1" s="29"/>
-      <c r="AI1" s="29"/>
-      <c r="AJ1" s="29"/>
-      <c r="AK1" s="29"/>
-      <c r="AL1" s="29"/>
-      <c r="AM1" s="29"/>
-      <c r="AN1" s="29"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
     </row>
     <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:99" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -5015,12 +5023,12 @@
       </c>
     </row>
     <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="20">
         <v>0</v>
       </c>
@@ -5228,7 +5236,9 @@
       <c r="BU4" s="21">
         <v>-32</v>
       </c>
-      <c r="BV4" s="21"/>
+      <c r="BV4" s="21">
+        <v>5</v>
+      </c>
       <c r="BW4" s="21"/>
       <c r="BX4" s="21"/>
       <c r="BY4" s="21"/>
@@ -5271,67 +5281,67 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="32" t="s">
+      <c r="L39" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
-      <c r="W39" s="27" t="s">
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="33"/>
+      <c r="W39" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="27"/>
-      <c r="Y39" s="27"/>
-      <c r="Z39" s="27"/>
-      <c r="AA39" s="27"/>
-      <c r="AB39" s="28">
+      <c r="X39" s="28"/>
+      <c r="Y39" s="28"/>
+      <c r="Z39" s="28"/>
+      <c r="AA39" s="28"/>
+      <c r="AB39" s="29">
         <f>SUM(E4:CU4)</f>
-        <v>2721</v>
-      </c>
-      <c r="AC39" s="28"/>
-      <c r="AD39" s="28"/>
-      <c r="AE39" s="28"/>
+        <v>2726</v>
+      </c>
+      <c r="AC39" s="29"/>
+      <c r="AD39" s="29"/>
+      <c r="AE39" s="29"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="26" t="s">
+      <c r="L40" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="26"/>
-      <c r="N40" s="26"/>
-      <c r="O40" s="26"/>
-      <c r="P40" s="26"/>
-      <c r="Q40" s="26"/>
-      <c r="W40" s="27"/>
-      <c r="X40" s="27"/>
-      <c r="Y40" s="27"/>
-      <c r="Z40" s="27"/>
-      <c r="AA40" s="27"/>
-      <c r="AB40" s="28"/>
-      <c r="AC40" s="28"/>
-      <c r="AD40" s="28"/>
-      <c r="AE40" s="28"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="27"/>
+      <c r="Q40" s="27"/>
+      <c r="W40" s="28"/>
+      <c r="X40" s="28"/>
+      <c r="Y40" s="28"/>
+      <c r="Z40" s="28"/>
+      <c r="AA40" s="28"/>
+      <c r="AB40" s="29"/>
+      <c r="AC40" s="29"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="29"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="26" t="s">
+      <c r="L41" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="26"/>
-      <c r="N41" s="26"/>
-      <c r="O41" s="26"/>
-      <c r="P41" s="26"/>
-      <c r="Q41" s="26"/>
-      <c r="R41" s="26"/>
-      <c r="W41" s="27"/>
-      <c r="X41" s="27"/>
-      <c r="Y41" s="27"/>
-      <c r="Z41" s="27"/>
-      <c r="AA41" s="27"/>
-      <c r="AB41" s="28"/>
-      <c r="AC41" s="28"/>
-      <c r="AD41" s="28"/>
-      <c r="AE41" s="28"/>
+      <c r="M41" s="27"/>
+      <c r="N41" s="27"/>
+      <c r="O41" s="27"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="27"/>
+      <c r="R41" s="27"/>
+      <c r="W41" s="28"/>
+      <c r="X41" s="28"/>
+      <c r="Y41" s="28"/>
+      <c r="Z41" s="28"/>
+      <c r="AA41" s="28"/>
+      <c r="AB41" s="29"/>
+      <c r="AC41" s="29"/>
+      <c r="AD41" s="29"/>
+      <c r="AE41" s="29"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
Aggiornamento dati al 05/05/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E6E5B6-1024-7B48-903F-2E8249595241}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB8D580-0389-C74B-A81E-439882A6D61E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t xml:space="preserve"> NUOVI INFETTI</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Massimo contaggiati in un giorno</t>
+  </si>
+  <si>
+    <t>Inizio fase 2</t>
   </si>
 </sst>
 </file>
@@ -209,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +243,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA80ED"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,7 +347,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -445,6 +454,15 @@
     <xf numFmtId="164" fontId="9" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Colore 5" xfId="5" builtinId="46"/>
@@ -480,6 +498,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFA80ED"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1175,6 +1198,12 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>-525</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-199</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-1513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1988,6 +2017,12 @@
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3627,7 +3662,7 @@
   <dimension ref="A1:CU54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BV5" sqref="BV5"/>
+      <selection activeCell="L42" sqref="L42:N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3885,7 +3920,7 @@
       <c r="BV3" s="4">
         <v>43954</v>
       </c>
-      <c r="BW3" s="4">
+      <c r="BW3" s="40">
         <v>43955</v>
       </c>
       <c r="BX3" s="4">
@@ -4178,8 +4213,12 @@
       <c r="BV4" s="7">
         <v>-525</v>
       </c>
-      <c r="BW4" s="7"/>
-      <c r="BX4" s="7"/>
+      <c r="BW4" s="7">
+        <v>-199</v>
+      </c>
+      <c r="BX4" s="7">
+        <v>-1513</v>
+      </c>
       <c r="BY4" s="7"/>
       <c r="BZ4" s="7"/>
       <c r="CA4" s="7"/>
@@ -4208,6 +4247,9 @@
     <row r="7" spans="1:99" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="BT7" s="26"/>
     </row>
+    <row r="10" spans="1:99" x14ac:dyDescent="0.2">
+      <c r="BQ10" s="26"/>
+    </row>
     <row r="14" spans="1:99" x14ac:dyDescent="0.2">
       <c r="I14" s="12"/>
     </row>
@@ -4237,7 +4279,7 @@
       <c r="AA39" s="28"/>
       <c r="AB39" s="29">
         <f>SUM(E4:CU4)</f>
-        <v>100179</v>
+        <v>98467</v>
       </c>
       <c r="AC39" s="29"/>
       <c r="AD39" s="29"/>
@@ -4283,6 +4325,14 @@
       <c r="AC41" s="29"/>
       <c r="AD41" s="29"/>
       <c r="AE41" s="29"/>
+    </row>
+    <row r="42" spans="9:37" x14ac:dyDescent="0.2">
+      <c r="K42" s="41"/>
+      <c r="L42" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="M42" s="42"/>
+      <c r="N42" s="42"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
@@ -4662,7 +4712,8 @@
       <c r="AK54" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="L42:N42"/>
     <mergeCell ref="L41:R41"/>
     <mergeCell ref="W39:AA41"/>
     <mergeCell ref="AB39:AE41"/>
@@ -4687,8 +4738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BW4" sqref="BW4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42:N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4946,7 +4997,7 @@
       <c r="BV3" s="4">
         <v>43954</v>
       </c>
-      <c r="BW3" s="4">
+      <c r="BW3" s="40">
         <v>43955</v>
       </c>
       <c r="BX3" s="4">
@@ -5239,8 +5290,12 @@
       <c r="BV4" s="21">
         <v>5</v>
       </c>
-      <c r="BW4" s="21"/>
-      <c r="BX4" s="21"/>
+      <c r="BW4" s="21">
+        <v>-15</v>
+      </c>
+      <c r="BX4" s="21">
+        <v>-181</v>
+      </c>
       <c r="BY4" s="21"/>
       <c r="BZ4" s="21"/>
       <c r="CA4" s="21"/>
@@ -5296,7 +5351,7 @@
       <c r="AA39" s="28"/>
       <c r="AB39" s="29">
         <f>SUM(E4:CU4)</f>
-        <v>2726</v>
+        <v>2530</v>
       </c>
       <c r="AC39" s="29"/>
       <c r="AD39" s="29"/>
@@ -5342,6 +5397,14 @@
       <c r="AC41" s="29"/>
       <c r="AD41" s="29"/>
       <c r="AE41" s="29"/>
+    </row>
+    <row r="42" spans="9:37" x14ac:dyDescent="0.2">
+      <c r="K42" s="41"/>
+      <c r="L42" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="M42" s="42"/>
+      <c r="N42" s="42"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
@@ -5721,7 +5784,8 @@
       <c r="AK54" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="L42:N42"/>
     <mergeCell ref="Z1:AN1"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A3:D3"/>

</xml_diff>

<commit_message>
aggiornamento dati al 08/05/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB8D580-0389-C74B-A81E-439882A6D61E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7D856A-65C8-B949-8716-58F7B233F9AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -415,6 +415,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="12" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -453,15 +462,6 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1204,6 +1204,15 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>-1513</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-6939</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-1904</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-1663</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2023,6 +2032,15 @@
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>-181</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-190</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-201</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3662,7 +3680,7 @@
   <dimension ref="A1:CU54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42:N42"/>
+      <selection activeCell="CB4" sqref="CB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3684,32 +3702,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="30" t="s">
+      <c r="Z1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
-      <c r="AN1" s="30"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
     </row>
     <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -3920,7 +3938,7 @@
       <c r="BV3" s="4">
         <v>43954</v>
       </c>
-      <c r="BW3" s="40">
+      <c r="BW3" s="27">
         <v>43955</v>
       </c>
       <c r="BX3" s="4">
@@ -3997,12 +4015,12 @@
       </c>
     </row>
     <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -4219,9 +4237,15 @@
       <c r="BX4" s="7">
         <v>-1513</v>
       </c>
-      <c r="BY4" s="7"/>
-      <c r="BZ4" s="7"/>
-      <c r="CA4" s="7"/>
+      <c r="BY4" s="7">
+        <v>-6939</v>
+      </c>
+      <c r="BZ4" s="7">
+        <v>-1904</v>
+      </c>
+      <c r="CA4" s="7">
+        <v>-1663</v>
+      </c>
       <c r="CB4" s="7"/>
       <c r="CC4" s="7"/>
       <c r="CD4" s="7"/>
@@ -4264,75 +4288,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="33" t="s">
+      <c r="L39" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="33"/>
-      <c r="N39" s="33"/>
-      <c r="O39" s="33"/>
-      <c r="W39" s="28" t="s">
+      <c r="M39" s="36"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="36"/>
+      <c r="W39" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="28"/>
-      <c r="Y39" s="28"/>
-      <c r="Z39" s="28"/>
-      <c r="AA39" s="28"/>
-      <c r="AB39" s="29">
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="32">
         <f>SUM(E4:CU4)</f>
-        <v>98467</v>
-      </c>
-      <c r="AC39" s="29"/>
-      <c r="AD39" s="29"/>
-      <c r="AE39" s="29"/>
+        <v>87961</v>
+      </c>
+      <c r="AC39" s="32"/>
+      <c r="AD39" s="32"/>
+      <c r="AE39" s="32"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="27" t="s">
+      <c r="L40" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="27"/>
-      <c r="P40" s="27"/>
-      <c r="Q40" s="27"/>
-      <c r="W40" s="28"/>
-      <c r="X40" s="28"/>
-      <c r="Y40" s="28"/>
-      <c r="Z40" s="28"/>
-      <c r="AA40" s="28"/>
-      <c r="AB40" s="29"/>
-      <c r="AC40" s="29"/>
-      <c r="AD40" s="29"/>
-      <c r="AE40" s="29"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="31"/>
+      <c r="Y40" s="31"/>
+      <c r="Z40" s="31"/>
+      <c r="AA40" s="31"/>
+      <c r="AB40" s="32"/>
+      <c r="AC40" s="32"/>
+      <c r="AD40" s="32"/>
+      <c r="AE40" s="32"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="27" t="s">
+      <c r="L41" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-      <c r="R41" s="27"/>
-      <c r="W41" s="28"/>
-      <c r="X41" s="28"/>
-      <c r="Y41" s="28"/>
-      <c r="Z41" s="28"/>
-      <c r="AA41" s="28"/>
-      <c r="AB41" s="29"/>
-      <c r="AC41" s="29"/>
-      <c r="AD41" s="29"/>
-      <c r="AE41" s="29"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="32"/>
+      <c r="AC41" s="32"/>
+      <c r="AD41" s="32"/>
+      <c r="AE41" s="32"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
-      <c r="K42" s="41"/>
-      <c r="L42" s="42" t="s">
+      <c r="K42" s="28"/>
+      <c r="L42" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="42"/>
-      <c r="N42" s="42"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
@@ -4713,15 +4737,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="L40:Q40"/>
     <mergeCell ref="L42:N42"/>
     <mergeCell ref="L41:R41"/>
     <mergeCell ref="W39:AA41"/>
     <mergeCell ref="AB39:AE41"/>
     <mergeCell ref="Z1:AN1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L39:O39"/>
-    <mergeCell ref="L40:Q40"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:CU4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -4739,7 +4763,7 @@
   <dimension ref="A1:CU54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42:N42"/>
+      <selection activeCell="CB4" sqref="CB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4761,32 +4785,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="30" t="s">
+      <c r="Z1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
-      <c r="AN1" s="30"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
     </row>
     <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:99" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -4997,7 +5021,7 @@
       <c r="BV3" s="4">
         <v>43954</v>
       </c>
-      <c r="BW3" s="40">
+      <c r="BW3" s="27">
         <v>43955</v>
       </c>
       <c r="BX3" s="4">
@@ -5074,12 +5098,12 @@
       </c>
     </row>
     <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="20">
         <v>0</v>
       </c>
@@ -5296,9 +5320,15 @@
       <c r="BX4" s="21">
         <v>-181</v>
       </c>
-      <c r="BY4" s="21"/>
-      <c r="BZ4" s="21"/>
-      <c r="CA4" s="21"/>
+      <c r="BY4" s="21">
+        <v>-190</v>
+      </c>
+      <c r="BZ4" s="21">
+        <v>-201</v>
+      </c>
+      <c r="CA4" s="21">
+        <v>-127</v>
+      </c>
       <c r="CB4" s="21"/>
       <c r="CC4" s="21"/>
       <c r="CD4" s="21"/>
@@ -5336,75 +5366,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="33" t="s">
+      <c r="L39" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="33"/>
-      <c r="N39" s="33"/>
-      <c r="O39" s="33"/>
-      <c r="W39" s="28" t="s">
+      <c r="M39" s="36"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="36"/>
+      <c r="W39" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="28"/>
-      <c r="Y39" s="28"/>
-      <c r="Z39" s="28"/>
-      <c r="AA39" s="28"/>
-      <c r="AB39" s="29">
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="32">
         <f>SUM(E4:CU4)</f>
-        <v>2530</v>
-      </c>
-      <c r="AC39" s="29"/>
-      <c r="AD39" s="29"/>
-      <c r="AE39" s="29"/>
+        <v>2012</v>
+      </c>
+      <c r="AC39" s="32"/>
+      <c r="AD39" s="32"/>
+      <c r="AE39" s="32"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="27" t="s">
+      <c r="L40" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="27"/>
-      <c r="P40" s="27"/>
-      <c r="Q40" s="27"/>
-      <c r="W40" s="28"/>
-      <c r="X40" s="28"/>
-      <c r="Y40" s="28"/>
-      <c r="Z40" s="28"/>
-      <c r="AA40" s="28"/>
-      <c r="AB40" s="29"/>
-      <c r="AC40" s="29"/>
-      <c r="AD40" s="29"/>
-      <c r="AE40" s="29"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="31"/>
+      <c r="Y40" s="31"/>
+      <c r="Z40" s="31"/>
+      <c r="AA40" s="31"/>
+      <c r="AB40" s="32"/>
+      <c r="AC40" s="32"/>
+      <c r="AD40" s="32"/>
+      <c r="AE40" s="32"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="27" t="s">
+      <c r="L41" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-      <c r="R41" s="27"/>
-      <c r="W41" s="28"/>
-      <c r="X41" s="28"/>
-      <c r="Y41" s="28"/>
-      <c r="Z41" s="28"/>
-      <c r="AA41" s="28"/>
-      <c r="AB41" s="29"/>
-      <c r="AC41" s="29"/>
-      <c r="AD41" s="29"/>
-      <c r="AE41" s="29"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="32"/>
+      <c r="AC41" s="32"/>
+      <c r="AD41" s="32"/>
+      <c r="AE41" s="32"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
-      <c r="K42" s="41"/>
-      <c r="L42" s="42" t="s">
+      <c r="K42" s="28"/>
+      <c r="L42" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="42"/>
-      <c r="N42" s="42"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 09/05/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7D856A-65C8-B949-8716-58F7B233F9AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B369ECA-86F6-6146-A12C-7BEFA29542AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -421,10 +421,19 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -435,15 +444,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1213,6 +1213,9 @@
                 </c:pt>
                 <c:pt idx="74">
                   <c:v>-1663</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-3119</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2041,6 +2044,9 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>-127</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3680,7 +3686,7 @@
   <dimension ref="A1:CU54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CB4" sqref="CB4"/>
+      <selection activeCell="CC4" sqref="CC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3702,32 +3708,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="33" t="s">
+      <c r="Z1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36"/>
     </row>
     <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -4015,12 +4021,12 @@
       </c>
     </row>
     <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -4246,7 +4252,9 @@
       <c r="CA4" s="7">
         <v>-1663</v>
       </c>
-      <c r="CB4" s="7"/>
+      <c r="CB4" s="7">
+        <v>-3119</v>
+      </c>
       <c r="CC4" s="7"/>
       <c r="CD4" s="7"/>
       <c r="CE4" s="7"/>
@@ -4288,75 +4296,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="36" t="s">
+      <c r="L39" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="W39" s="31" t="s">
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="W39" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="31"/>
-      <c r="Y39" s="31"/>
-      <c r="Z39" s="31"/>
-      <c r="AA39" s="31"/>
-      <c r="AB39" s="32">
+      <c r="X39" s="34"/>
+      <c r="Y39" s="34"/>
+      <c r="Z39" s="34"/>
+      <c r="AA39" s="34"/>
+      <c r="AB39" s="35">
         <f>SUM(E4:CU4)</f>
-        <v>87961</v>
-      </c>
-      <c r="AC39" s="32"/>
-      <c r="AD39" s="32"/>
-      <c r="AE39" s="32"/>
+        <v>84842</v>
+      </c>
+      <c r="AC39" s="35"/>
+      <c r="AD39" s="35"/>
+      <c r="AE39" s="35"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="30" t="s">
+      <c r="L40" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="W40" s="31"/>
-      <c r="X40" s="31"/>
-      <c r="Y40" s="31"/>
-      <c r="Z40" s="31"/>
-      <c r="AA40" s="31"/>
-      <c r="AB40" s="32"/>
-      <c r="AC40" s="32"/>
-      <c r="AD40" s="32"/>
-      <c r="AE40" s="32"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="32"/>
+      <c r="P40" s="32"/>
+      <c r="Q40" s="32"/>
+      <c r="W40" s="34"/>
+      <c r="X40" s="34"/>
+      <c r="Y40" s="34"/>
+      <c r="Z40" s="34"/>
+      <c r="AA40" s="34"/>
+      <c r="AB40" s="35"/>
+      <c r="AC40" s="35"/>
+      <c r="AD40" s="35"/>
+      <c r="AE40" s="35"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="30" t="s">
+      <c r="L41" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="30"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-      <c r="W41" s="31"/>
-      <c r="X41" s="31"/>
-      <c r="Y41" s="31"/>
-      <c r="Z41" s="31"/>
-      <c r="AA41" s="31"/>
-      <c r="AB41" s="32"/>
-      <c r="AC41" s="32"/>
-      <c r="AD41" s="32"/>
-      <c r="AE41" s="32"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="W41" s="34"/>
+      <c r="X41" s="34"/>
+      <c r="Y41" s="34"/>
+      <c r="Z41" s="34"/>
+      <c r="AA41" s="34"/>
+      <c r="AB41" s="35"/>
+      <c r="AC41" s="35"/>
+      <c r="AD41" s="35"/>
+      <c r="AE41" s="35"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="29" t="s">
+      <c r="L42" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
@@ -4737,15 +4745,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="W39:AA41"/>
+    <mergeCell ref="AB39:AE41"/>
+    <mergeCell ref="Z1:AN1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L39:O39"/>
     <mergeCell ref="L40:Q40"/>
     <mergeCell ref="L42:N42"/>
     <mergeCell ref="L41:R41"/>
-    <mergeCell ref="W39:AA41"/>
-    <mergeCell ref="AB39:AE41"/>
-    <mergeCell ref="Z1:AN1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:CU4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -4763,7 +4771,7 @@
   <dimension ref="A1:CU54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CB4" sqref="CB4"/>
+      <selection activeCell="CC4" sqref="CC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4785,23 +4793,23 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="33" t="s">
+      <c r="Z1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36"/>
     </row>
     <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:99" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5329,7 +5337,9 @@
       <c r="CA4" s="21">
         <v>-127</v>
       </c>
-      <c r="CB4" s="21"/>
+      <c r="CB4" s="21">
+        <v>-47</v>
+      </c>
       <c r="CC4" s="21"/>
       <c r="CD4" s="21"/>
       <c r="CE4" s="21"/>
@@ -5366,75 +5376,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="36" t="s">
+      <c r="L39" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="W39" s="31" t="s">
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="W39" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="31"/>
-      <c r="Y39" s="31"/>
-      <c r="Z39" s="31"/>
-      <c r="AA39" s="31"/>
-      <c r="AB39" s="32">
+      <c r="X39" s="34"/>
+      <c r="Y39" s="34"/>
+      <c r="Z39" s="34"/>
+      <c r="AA39" s="34"/>
+      <c r="AB39" s="35">
         <f>SUM(E4:CU4)</f>
-        <v>2012</v>
-      </c>
-      <c r="AC39" s="32"/>
-      <c r="AD39" s="32"/>
-      <c r="AE39" s="32"/>
+        <v>1965</v>
+      </c>
+      <c r="AC39" s="35"/>
+      <c r="AD39" s="35"/>
+      <c r="AE39" s="35"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="30" t="s">
+      <c r="L40" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="W40" s="31"/>
-      <c r="X40" s="31"/>
-      <c r="Y40" s="31"/>
-      <c r="Z40" s="31"/>
-      <c r="AA40" s="31"/>
-      <c r="AB40" s="32"/>
-      <c r="AC40" s="32"/>
-      <c r="AD40" s="32"/>
-      <c r="AE40" s="32"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="32"/>
+      <c r="P40" s="32"/>
+      <c r="Q40" s="32"/>
+      <c r="W40" s="34"/>
+      <c r="X40" s="34"/>
+      <c r="Y40" s="34"/>
+      <c r="Z40" s="34"/>
+      <c r="AA40" s="34"/>
+      <c r="AB40" s="35"/>
+      <c r="AC40" s="35"/>
+      <c r="AD40" s="35"/>
+      <c r="AE40" s="35"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="30" t="s">
+      <c r="L41" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="30"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-      <c r="W41" s="31"/>
-      <c r="X41" s="31"/>
-      <c r="Y41" s="31"/>
-      <c r="Z41" s="31"/>
-      <c r="AA41" s="31"/>
-      <c r="AB41" s="32"/>
-      <c r="AC41" s="32"/>
-      <c r="AD41" s="32"/>
-      <c r="AE41" s="32"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="W41" s="34"/>
+      <c r="X41" s="34"/>
+      <c r="Y41" s="34"/>
+      <c r="Z41" s="34"/>
+      <c r="AA41" s="34"/>
+      <c r="AB41" s="35"/>
+      <c r="AC41" s="35"/>
+      <c r="AD41" s="35"/>
+      <c r="AE41" s="35"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="29" t="s">
+      <c r="L42" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 13/05/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B369ECA-86F6-6146-A12C-7BEFA29542AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90AF9FE-B685-2A4E-8428-286FAD87E107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -421,6 +421,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -435,15 +444,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1216,6 +1216,18 @@
                 </c:pt>
                 <c:pt idx="75">
                   <c:v>-3119</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-1518</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-836</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-1222</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-2809</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2047,6 +2059,18 @@
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>-47</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-32</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3685,8 +3709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CC4" sqref="CC4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CG4" sqref="CG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3708,32 +3732,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="36" t="s">
+      <c r="Z1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="36"/>
-      <c r="AL1" s="36"/>
-      <c r="AM1" s="36"/>
-      <c r="AN1" s="36"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
     </row>
     <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -4021,12 +4045,12 @@
       </c>
     </row>
     <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -4255,10 +4279,18 @@
       <c r="CB4" s="7">
         <v>-3119</v>
       </c>
-      <c r="CC4" s="7"/>
-      <c r="CD4" s="7"/>
-      <c r="CE4" s="7"/>
-      <c r="CF4" s="7"/>
+      <c r="CC4" s="7">
+        <v>-1518</v>
+      </c>
+      <c r="CD4" s="7">
+        <v>-836</v>
+      </c>
+      <c r="CE4" s="7">
+        <v>-1222</v>
+      </c>
+      <c r="CF4" s="7">
+        <v>-2809</v>
+      </c>
       <c r="CG4" s="7"/>
       <c r="CH4" s="7"/>
       <c r="CI4" s="7"/>
@@ -4296,75 +4328,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="31" t="s">
+      <c r="L39" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="31"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="31"/>
-      <c r="W39" s="34" t="s">
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="34"/>
+      <c r="W39" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="34"/>
-      <c r="Y39" s="34"/>
-      <c r="Z39" s="34"/>
-      <c r="AA39" s="34"/>
-      <c r="AB39" s="35">
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="30">
         <f>SUM(E4:CU4)</f>
-        <v>84842</v>
-      </c>
-      <c r="AC39" s="35"/>
-      <c r="AD39" s="35"/>
-      <c r="AE39" s="35"/>
+        <v>78457</v>
+      </c>
+      <c r="AC39" s="30"/>
+      <c r="AD39" s="30"/>
+      <c r="AE39" s="30"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="32" t="s">
+      <c r="L40" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
-      <c r="Q40" s="32"/>
-      <c r="W40" s="34"/>
-      <c r="X40" s="34"/>
-      <c r="Y40" s="34"/>
-      <c r="Z40" s="34"/>
-      <c r="AA40" s="34"/>
-      <c r="AB40" s="35"/>
-      <c r="AC40" s="35"/>
-      <c r="AD40" s="35"/>
-      <c r="AE40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="30"/>
+      <c r="AC40" s="30"/>
+      <c r="AD40" s="30"/>
+      <c r="AE40" s="30"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="32" t="s">
+      <c r="L41" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="32"/>
-      <c r="R41" s="32"/>
-      <c r="W41" s="34"/>
-      <c r="X41" s="34"/>
-      <c r="Y41" s="34"/>
-      <c r="Z41" s="34"/>
-      <c r="AA41" s="34"/>
-      <c r="AB41" s="35"/>
-      <c r="AC41" s="35"/>
-      <c r="AD41" s="35"/>
-      <c r="AE41" s="35"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35"/>
+      <c r="R41" s="35"/>
+      <c r="W41" s="29"/>
+      <c r="X41" s="29"/>
+      <c r="Y41" s="29"/>
+      <c r="Z41" s="29"/>
+      <c r="AA41" s="29"/>
+      <c r="AB41" s="30"/>
+      <c r="AC41" s="30"/>
+      <c r="AD41" s="30"/>
+      <c r="AE41" s="30"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="33" t="s">
+      <c r="L42" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="33"/>
-      <c r="N42" s="33"/>
+      <c r="M42" s="36"/>
+      <c r="N42" s="36"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
@@ -4745,6 +4777,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="L41:R41"/>
     <mergeCell ref="W39:AA41"/>
     <mergeCell ref="AB39:AE41"/>
     <mergeCell ref="Z1:AN1"/>
@@ -4752,8 +4786,6 @@
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L39:O39"/>
     <mergeCell ref="L40:Q40"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="L41:R41"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:CU4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -4770,8 +4802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CC4" sqref="CC4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CG4" sqref="CG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4793,23 +4825,23 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="36" t="s">
+      <c r="Z1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="36"/>
-      <c r="AL1" s="36"/>
-      <c r="AM1" s="36"/>
-      <c r="AN1" s="36"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
     </row>
     <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:99" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5340,10 +5372,18 @@
       <c r="CB4" s="21">
         <v>-47</v>
       </c>
-      <c r="CC4" s="21"/>
-      <c r="CD4" s="21"/>
-      <c r="CE4" s="21"/>
-      <c r="CF4" s="21"/>
+      <c r="CC4" s="21">
+        <v>-50</v>
+      </c>
+      <c r="CD4" s="21">
+        <v>-6</v>
+      </c>
+      <c r="CE4" s="21">
+        <v>-32</v>
+      </c>
+      <c r="CF4" s="21">
+        <v>-62</v>
+      </c>
       <c r="CG4" s="21"/>
       <c r="CH4" s="21"/>
       <c r="CI4" s="21"/>
@@ -5376,75 +5416,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="31" t="s">
+      <c r="L39" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="31"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="31"/>
-      <c r="W39" s="34" t="s">
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="34"/>
+      <c r="W39" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="34"/>
-      <c r="Y39" s="34"/>
-      <c r="Z39" s="34"/>
-      <c r="AA39" s="34"/>
-      <c r="AB39" s="35">
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="30">
         <f>SUM(E4:CU4)</f>
-        <v>1965</v>
-      </c>
-      <c r="AC39" s="35"/>
-      <c r="AD39" s="35"/>
-      <c r="AE39" s="35"/>
+        <v>1815</v>
+      </c>
+      <c r="AC39" s="30"/>
+      <c r="AD39" s="30"/>
+      <c r="AE39" s="30"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="32" t="s">
+      <c r="L40" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
-      <c r="Q40" s="32"/>
-      <c r="W40" s="34"/>
-      <c r="X40" s="34"/>
-      <c r="Y40" s="34"/>
-      <c r="Z40" s="34"/>
-      <c r="AA40" s="34"/>
-      <c r="AB40" s="35"/>
-      <c r="AC40" s="35"/>
-      <c r="AD40" s="35"/>
-      <c r="AE40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="30"/>
+      <c r="AC40" s="30"/>
+      <c r="AD40" s="30"/>
+      <c r="AE40" s="30"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="32" t="s">
+      <c r="L41" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="32"/>
-      <c r="R41" s="32"/>
-      <c r="W41" s="34"/>
-      <c r="X41" s="34"/>
-      <c r="Y41" s="34"/>
-      <c r="Z41" s="34"/>
-      <c r="AA41" s="34"/>
-      <c r="AB41" s="35"/>
-      <c r="AC41" s="35"/>
-      <c r="AD41" s="35"/>
-      <c r="AE41" s="35"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35"/>
+      <c r="R41" s="35"/>
+      <c r="W41" s="29"/>
+      <c r="X41" s="29"/>
+      <c r="Y41" s="29"/>
+      <c r="Z41" s="29"/>
+      <c r="AA41" s="29"/>
+      <c r="AB41" s="30"/>
+      <c r="AC41" s="30"/>
+      <c r="AD41" s="30"/>
+      <c r="AE41" s="30"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="33" t="s">
+      <c r="L42" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="33"/>
-      <c r="N42" s="33"/>
+      <c r="M42" s="36"/>
+      <c r="N42" s="36"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggirnamento dati al 14/05/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90AF9FE-B685-2A4E-8428-286FAD87E107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECCFC38-7395-654E-B0EF-D03030D79A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -421,6 +421,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -437,12 +443,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1228,6 +1228,9 @@
                 </c:pt>
                 <c:pt idx="79">
                   <c:v>-2809</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-2017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2071,6 +2074,9 @@
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>-62</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3710,7 +3716,7 @@
   <dimension ref="A1:CU54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CG4" sqref="CG4"/>
+      <selection activeCell="CG5" sqref="CG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3732,32 +3738,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="31" t="s">
+      <c r="Z1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
     </row>
     <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -4045,12 +4051,12 @@
       </c>
     </row>
     <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -4291,7 +4297,9 @@
       <c r="CF4" s="7">
         <v>-2809</v>
       </c>
-      <c r="CG4" s="7"/>
+      <c r="CG4" s="7">
+        <v>-2017</v>
+      </c>
       <c r="CH4" s="7"/>
       <c r="CI4" s="7"/>
       <c r="CJ4" s="7"/>
@@ -4328,75 +4336,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="34" t="s">
+      <c r="L39" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34"/>
-      <c r="W39" s="29" t="s">
+      <c r="M39" s="36"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="36"/>
+      <c r="W39" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="29"/>
-      <c r="Y39" s="29"/>
-      <c r="Z39" s="29"/>
-      <c r="AA39" s="29"/>
-      <c r="AB39" s="30">
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="32">
         <f>SUM(E4:CU4)</f>
-        <v>78457</v>
-      </c>
-      <c r="AC39" s="30"/>
-      <c r="AD39" s="30"/>
-      <c r="AE39" s="30"/>
+        <v>76440</v>
+      </c>
+      <c r="AC39" s="32"/>
+      <c r="AD39" s="32"/>
+      <c r="AE39" s="32"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="35" t="s">
+      <c r="L40" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
-      <c r="O40" s="35"/>
-      <c r="P40" s="35"/>
-      <c r="Q40" s="35"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="30"/>
-      <c r="AC40" s="30"/>
-      <c r="AD40" s="30"/>
-      <c r="AE40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="31"/>
+      <c r="Y40" s="31"/>
+      <c r="Z40" s="31"/>
+      <c r="AA40" s="31"/>
+      <c r="AB40" s="32"/>
+      <c r="AC40" s="32"/>
+      <c r="AD40" s="32"/>
+      <c r="AE40" s="32"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="35" t="s">
+      <c r="L41" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="35"/>
-      <c r="P41" s="35"/>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="35"/>
-      <c r="W41" s="29"/>
-      <c r="X41" s="29"/>
-      <c r="Y41" s="29"/>
-      <c r="Z41" s="29"/>
-      <c r="AA41" s="29"/>
-      <c r="AB41" s="30"/>
-      <c r="AC41" s="30"/>
-      <c r="AD41" s="30"/>
-      <c r="AE41" s="30"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="32"/>
+      <c r="AC41" s="32"/>
+      <c r="AD41" s="32"/>
+      <c r="AE41" s="32"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="36" t="s">
+      <c r="L42" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="36"/>
-      <c r="N42" s="36"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
@@ -4777,15 +4785,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="L40:Q40"/>
     <mergeCell ref="L42:N42"/>
     <mergeCell ref="L41:R41"/>
     <mergeCell ref="W39:AA41"/>
     <mergeCell ref="AB39:AE41"/>
     <mergeCell ref="Z1:AN1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L39:O39"/>
-    <mergeCell ref="L40:Q40"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:CU4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -4803,7 +4811,7 @@
   <dimension ref="A1:CU54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CG4" sqref="CG4"/>
+      <selection activeCell="CH4" sqref="CH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4825,23 +4833,23 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="31" t="s">
+      <c r="Z1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
     </row>
     <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:99" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5384,7 +5392,9 @@
       <c r="CF4" s="21">
         <v>-62</v>
       </c>
-      <c r="CG4" s="21"/>
+      <c r="CG4" s="21">
+        <v>-50</v>
+      </c>
       <c r="CH4" s="21"/>
       <c r="CI4" s="21"/>
       <c r="CJ4" s="21"/>
@@ -5416,75 +5426,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="34" t="s">
+      <c r="L39" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34"/>
-      <c r="W39" s="29" t="s">
+      <c r="M39" s="36"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="36"/>
+      <c r="W39" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="29"/>
-      <c r="Y39" s="29"/>
-      <c r="Z39" s="29"/>
-      <c r="AA39" s="29"/>
-      <c r="AB39" s="30">
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="32">
         <f>SUM(E4:CU4)</f>
-        <v>1815</v>
-      </c>
-      <c r="AC39" s="30"/>
-      <c r="AD39" s="30"/>
-      <c r="AE39" s="30"/>
+        <v>1765</v>
+      </c>
+      <c r="AC39" s="32"/>
+      <c r="AD39" s="32"/>
+      <c r="AE39" s="32"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="35" t="s">
+      <c r="L40" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
-      <c r="O40" s="35"/>
-      <c r="P40" s="35"/>
-      <c r="Q40" s="35"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="30"/>
-      <c r="AC40" s="30"/>
-      <c r="AD40" s="30"/>
-      <c r="AE40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="31"/>
+      <c r="Y40" s="31"/>
+      <c r="Z40" s="31"/>
+      <c r="AA40" s="31"/>
+      <c r="AB40" s="32"/>
+      <c r="AC40" s="32"/>
+      <c r="AD40" s="32"/>
+      <c r="AE40" s="32"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="35" t="s">
+      <c r="L41" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="35"/>
-      <c r="P41" s="35"/>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="35"/>
-      <c r="W41" s="29"/>
-      <c r="X41" s="29"/>
-      <c r="Y41" s="29"/>
-      <c r="Z41" s="29"/>
-      <c r="AA41" s="29"/>
-      <c r="AB41" s="30"/>
-      <c r="AC41" s="30"/>
-      <c r="AD41" s="30"/>
-      <c r="AE41" s="30"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="32"/>
+      <c r="AC41" s="32"/>
+      <c r="AD41" s="32"/>
+      <c r="AE41" s="32"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="36" t="s">
+      <c r="L42" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="36"/>
-      <c r="N42" s="36"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 15/05/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECCFC38-7395-654E-B0EF-D03030D79A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB20093-4ABF-4D42-8962-2221C00FAD51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -421,10 +421,19 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -435,15 +444,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1231,6 +1231,9 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>-2017</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-4370</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2077,6 +2080,9 @@
                 </c:pt>
                 <c:pt idx="77">
                   <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3715,8 +3721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CG5" sqref="CG5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CI4" sqref="CI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3738,32 +3744,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="33" t="s">
+      <c r="Z1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36"/>
     </row>
     <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -4051,12 +4057,12 @@
       </c>
     </row>
     <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -4300,7 +4306,9 @@
       <c r="CG4" s="7">
         <v>-2017</v>
       </c>
-      <c r="CH4" s="7"/>
+      <c r="CH4" s="7">
+        <v>-4370</v>
+      </c>
       <c r="CI4" s="7"/>
       <c r="CJ4" s="7"/>
       <c r="CK4" s="7"/>
@@ -4336,75 +4344,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="36" t="s">
+      <c r="L39" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="W39" s="31" t="s">
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="W39" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="31"/>
-      <c r="Y39" s="31"/>
-      <c r="Z39" s="31"/>
-      <c r="AA39" s="31"/>
-      <c r="AB39" s="32">
+      <c r="X39" s="34"/>
+      <c r="Y39" s="34"/>
+      <c r="Z39" s="34"/>
+      <c r="AA39" s="34"/>
+      <c r="AB39" s="35">
         <f>SUM(E4:CU4)</f>
-        <v>76440</v>
-      </c>
-      <c r="AC39" s="32"/>
-      <c r="AD39" s="32"/>
-      <c r="AE39" s="32"/>
+        <v>72070</v>
+      </c>
+      <c r="AC39" s="35"/>
+      <c r="AD39" s="35"/>
+      <c r="AE39" s="35"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="30" t="s">
+      <c r="L40" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="W40" s="31"/>
-      <c r="X40" s="31"/>
-      <c r="Y40" s="31"/>
-      <c r="Z40" s="31"/>
-      <c r="AA40" s="31"/>
-      <c r="AB40" s="32"/>
-      <c r="AC40" s="32"/>
-      <c r="AD40" s="32"/>
-      <c r="AE40" s="32"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="32"/>
+      <c r="P40" s="32"/>
+      <c r="Q40" s="32"/>
+      <c r="W40" s="34"/>
+      <c r="X40" s="34"/>
+      <c r="Y40" s="34"/>
+      <c r="Z40" s="34"/>
+      <c r="AA40" s="34"/>
+      <c r="AB40" s="35"/>
+      <c r="AC40" s="35"/>
+      <c r="AD40" s="35"/>
+      <c r="AE40" s="35"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="30" t="s">
+      <c r="L41" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="30"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-      <c r="W41" s="31"/>
-      <c r="X41" s="31"/>
-      <c r="Y41" s="31"/>
-      <c r="Z41" s="31"/>
-      <c r="AA41" s="31"/>
-      <c r="AB41" s="32"/>
-      <c r="AC41" s="32"/>
-      <c r="AD41" s="32"/>
-      <c r="AE41" s="32"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="W41" s="34"/>
+      <c r="X41" s="34"/>
+      <c r="Y41" s="34"/>
+      <c r="Z41" s="34"/>
+      <c r="AA41" s="34"/>
+      <c r="AB41" s="35"/>
+      <c r="AC41" s="35"/>
+      <c r="AD41" s="35"/>
+      <c r="AE41" s="35"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="29" t="s">
+      <c r="L42" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
@@ -4785,15 +4793,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="W39:AA41"/>
+    <mergeCell ref="AB39:AE41"/>
+    <mergeCell ref="Z1:AN1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L39:O39"/>
     <mergeCell ref="L40:Q40"/>
     <mergeCell ref="L42:N42"/>
     <mergeCell ref="L41:R41"/>
-    <mergeCell ref="W39:AA41"/>
-    <mergeCell ref="AB39:AE41"/>
-    <mergeCell ref="Z1:AN1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:CU4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -4810,8 +4818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CH4" sqref="CH4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CI4" sqref="CI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4833,23 +4841,23 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="33" t="s">
+      <c r="Z1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36"/>
     </row>
     <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:99" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5395,7 +5403,9 @@
       <c r="CG4" s="21">
         <v>-50</v>
       </c>
-      <c r="CH4" s="21"/>
+      <c r="CH4" s="21">
+        <v>-29</v>
+      </c>
       <c r="CI4" s="21"/>
       <c r="CJ4" s="21"/>
       <c r="CK4" s="21"/>
@@ -5426,75 +5436,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="36" t="s">
+      <c r="L39" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="W39" s="31" t="s">
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="W39" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="31"/>
-      <c r="Y39" s="31"/>
-      <c r="Z39" s="31"/>
-      <c r="AA39" s="31"/>
-      <c r="AB39" s="32">
+      <c r="X39" s="34"/>
+      <c r="Y39" s="34"/>
+      <c r="Z39" s="34"/>
+      <c r="AA39" s="34"/>
+      <c r="AB39" s="35">
         <f>SUM(E4:CU4)</f>
-        <v>1765</v>
-      </c>
-      <c r="AC39" s="32"/>
-      <c r="AD39" s="32"/>
-      <c r="AE39" s="32"/>
+        <v>1736</v>
+      </c>
+      <c r="AC39" s="35"/>
+      <c r="AD39" s="35"/>
+      <c r="AE39" s="35"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="30" t="s">
+      <c r="L40" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="W40" s="31"/>
-      <c r="X40" s="31"/>
-      <c r="Y40" s="31"/>
-      <c r="Z40" s="31"/>
-      <c r="AA40" s="31"/>
-      <c r="AB40" s="32"/>
-      <c r="AC40" s="32"/>
-      <c r="AD40" s="32"/>
-      <c r="AE40" s="32"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="32"/>
+      <c r="P40" s="32"/>
+      <c r="Q40" s="32"/>
+      <c r="W40" s="34"/>
+      <c r="X40" s="34"/>
+      <c r="Y40" s="34"/>
+      <c r="Z40" s="34"/>
+      <c r="AA40" s="34"/>
+      <c r="AB40" s="35"/>
+      <c r="AC40" s="35"/>
+      <c r="AD40" s="35"/>
+      <c r="AE40" s="35"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="30" t="s">
+      <c r="L41" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="30"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-      <c r="W41" s="31"/>
-      <c r="X41" s="31"/>
-      <c r="Y41" s="31"/>
-      <c r="Z41" s="31"/>
-      <c r="AA41" s="31"/>
-      <c r="AB41" s="32"/>
-      <c r="AC41" s="32"/>
-      <c r="AD41" s="32"/>
-      <c r="AE41" s="32"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="W41" s="34"/>
+      <c r="X41" s="34"/>
+      <c r="Y41" s="34"/>
+      <c r="Z41" s="34"/>
+      <c r="AA41" s="34"/>
+      <c r="AB41" s="35"/>
+      <c r="AC41" s="35"/>
+      <c r="AD41" s="35"/>
+      <c r="AE41" s="35"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="29" t="s">
+      <c r="L42" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 18/05/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB20093-4ABF-4D42-8962-2221C00FAD51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B86F361-1836-8144-9491-4B417BC52572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -421,6 +421,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -435,15 +444,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1234,6 +1234,15 @@
                 </c:pt>
                 <c:pt idx="81">
                   <c:v>-4370</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-1883</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-1836</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-1798</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2083,6 +2092,15 @@
                 </c:pt>
                 <c:pt idx="78">
                   <c:v>-29</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3721,8 +3739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CI4" sqref="CI4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CL4" sqref="CL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3744,32 +3762,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="36" t="s">
+      <c r="Z1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="36"/>
-      <c r="AL1" s="36"/>
-      <c r="AM1" s="36"/>
-      <c r="AN1" s="36"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
     </row>
     <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -4057,12 +4075,12 @@
       </c>
     </row>
     <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -4309,9 +4327,15 @@
       <c r="CH4" s="7">
         <v>-4370</v>
       </c>
-      <c r="CI4" s="7"/>
-      <c r="CJ4" s="7"/>
-      <c r="CK4" s="7"/>
+      <c r="CI4" s="7">
+        <v>-1883</v>
+      </c>
+      <c r="CJ4" s="7">
+        <v>-1836</v>
+      </c>
+      <c r="CK4" s="7">
+        <v>-1798</v>
+      </c>
       <c r="CL4" s="7"/>
       <c r="CM4" s="7"/>
       <c r="CN4" s="7"/>
@@ -4344,75 +4368,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="31" t="s">
+      <c r="L39" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="31"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="31"/>
-      <c r="W39" s="34" t="s">
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="34"/>
+      <c r="W39" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="34"/>
-      <c r="Y39" s="34"/>
-      <c r="Z39" s="34"/>
-      <c r="AA39" s="34"/>
-      <c r="AB39" s="35">
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="30">
         <f>SUM(E4:CU4)</f>
-        <v>72070</v>
-      </c>
-      <c r="AC39" s="35"/>
-      <c r="AD39" s="35"/>
-      <c r="AE39" s="35"/>
+        <v>66553</v>
+      </c>
+      <c r="AC39" s="30"/>
+      <c r="AD39" s="30"/>
+      <c r="AE39" s="30"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="32" t="s">
+      <c r="L40" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
-      <c r="Q40" s="32"/>
-      <c r="W40" s="34"/>
-      <c r="X40" s="34"/>
-      <c r="Y40" s="34"/>
-      <c r="Z40" s="34"/>
-      <c r="AA40" s="34"/>
-      <c r="AB40" s="35"/>
-      <c r="AC40" s="35"/>
-      <c r="AD40" s="35"/>
-      <c r="AE40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="30"/>
+      <c r="AC40" s="30"/>
+      <c r="AD40" s="30"/>
+      <c r="AE40" s="30"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="32" t="s">
+      <c r="L41" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="32"/>
-      <c r="R41" s="32"/>
-      <c r="W41" s="34"/>
-      <c r="X41" s="34"/>
-      <c r="Y41" s="34"/>
-      <c r="Z41" s="34"/>
-      <c r="AA41" s="34"/>
-      <c r="AB41" s="35"/>
-      <c r="AC41" s="35"/>
-      <c r="AD41" s="35"/>
-      <c r="AE41" s="35"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35"/>
+      <c r="R41" s="35"/>
+      <c r="W41" s="29"/>
+      <c r="X41" s="29"/>
+      <c r="Y41" s="29"/>
+      <c r="Z41" s="29"/>
+      <c r="AA41" s="29"/>
+      <c r="AB41" s="30"/>
+      <c r="AC41" s="30"/>
+      <c r="AD41" s="30"/>
+      <c r="AE41" s="30"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="33" t="s">
+      <c r="L42" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="33"/>
-      <c r="N42" s="33"/>
+      <c r="M42" s="36"/>
+      <c r="N42" s="36"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
@@ -4793,6 +4817,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="L41:R41"/>
     <mergeCell ref="W39:AA41"/>
     <mergeCell ref="AB39:AE41"/>
     <mergeCell ref="Z1:AN1"/>
@@ -4800,8 +4826,6 @@
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L39:O39"/>
     <mergeCell ref="L40:Q40"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="L41:R41"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:CU4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -4818,8 +4842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A1:CU54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CI4" sqref="CI4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CL4" sqref="CL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4841,23 +4865,23 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="36" t="s">
+      <c r="Z1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="36"/>
-      <c r="AL1" s="36"/>
-      <c r="AM1" s="36"/>
-      <c r="AN1" s="36"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
     </row>
     <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:99" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5406,9 +5430,15 @@
       <c r="CH4" s="21">
         <v>-29</v>
       </c>
-      <c r="CI4" s="21"/>
-      <c r="CJ4" s="21"/>
-      <c r="CK4" s="21"/>
+      <c r="CI4" s="21">
+        <v>-26</v>
+      </c>
+      <c r="CJ4" s="21">
+        <v>-14</v>
+      </c>
+      <c r="CK4" s="21">
+        <v>-23</v>
+      </c>
       <c r="CL4" s="21"/>
       <c r="CM4" s="21"/>
       <c r="CN4" s="21"/>
@@ -5436,75 +5466,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="31" t="s">
+      <c r="L39" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="31"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="31"/>
-      <c r="W39" s="34" t="s">
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="34"/>
+      <c r="W39" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="34"/>
-      <c r="Y39" s="34"/>
-      <c r="Z39" s="34"/>
-      <c r="AA39" s="34"/>
-      <c r="AB39" s="35">
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="30">
         <f>SUM(E4:CU4)</f>
-        <v>1736</v>
-      </c>
-      <c r="AC39" s="35"/>
-      <c r="AD39" s="35"/>
-      <c r="AE39" s="35"/>
+        <v>1673</v>
+      </c>
+      <c r="AC39" s="30"/>
+      <c r="AD39" s="30"/>
+      <c r="AE39" s="30"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="32" t="s">
+      <c r="L40" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
-      <c r="Q40" s="32"/>
-      <c r="W40" s="34"/>
-      <c r="X40" s="34"/>
-      <c r="Y40" s="34"/>
-      <c r="Z40" s="34"/>
-      <c r="AA40" s="34"/>
-      <c r="AB40" s="35"/>
-      <c r="AC40" s="35"/>
-      <c r="AD40" s="35"/>
-      <c r="AE40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="30"/>
+      <c r="AC40" s="30"/>
+      <c r="AD40" s="30"/>
+      <c r="AE40" s="30"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="32" t="s">
+      <c r="L41" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="32"/>
-      <c r="R41" s="32"/>
-      <c r="W41" s="34"/>
-      <c r="X41" s="34"/>
-      <c r="Y41" s="34"/>
-      <c r="Z41" s="34"/>
-      <c r="AA41" s="34"/>
-      <c r="AB41" s="35"/>
-      <c r="AC41" s="35"/>
-      <c r="AD41" s="35"/>
-      <c r="AE41" s="35"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35"/>
+      <c r="R41" s="35"/>
+      <c r="W41" s="29"/>
+      <c r="X41" s="29"/>
+      <c r="Y41" s="29"/>
+      <c r="Z41" s="29"/>
+      <c r="AA41" s="29"/>
+      <c r="AB41" s="30"/>
+      <c r="AC41" s="30"/>
+      <c r="AD41" s="30"/>
+      <c r="AE41" s="30"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="33" t="s">
+      <c r="L42" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="33"/>
-      <c r="N42" s="33"/>
+      <c r="M42" s="36"/>
+      <c r="N42" s="36"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 03/06/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B86F361-1836-8144-9491-4B417BC52572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C52787-DB55-1A4A-8348-92063CAA7487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -421,6 +421,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -437,12 +443,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -691,10 +691,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Italia!$E$3:$CU$3</c:f>
+              <c:f>Italia!$E$3:$DL$3</c:f>
               <c:numCache>
                 <c:formatCode>d/m;@</c:formatCode>
-                <c:ptCount val="95"/>
+                <c:ptCount val="112"/>
                 <c:pt idx="0">
                   <c:v>43885</c:v>
                 </c:pt>
@@ -979,16 +979,67 @@
                 </c:pt>
                 <c:pt idx="94">
                   <c:v>43979</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>43980</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>43981</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>43982</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>43984</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>43985</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>43986</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>43987</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>43988</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>43989</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>43990</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>43991</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>43992</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>43993</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>43994</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>43995</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>43996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Italia!$E$4:$CU$4</c:f>
+              <c:f>Italia!$E$4:$DL$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="95"/>
+                <c:ptCount val="112"/>
                 <c:pt idx="0">
                   <c:v>221</c:v>
                 </c:pt>
@@ -1243,6 +1294,54 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>-1798</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-1424</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-2377</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-1792</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-1638</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-1570</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-1158</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-1294</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-2358</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-1976</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-2980</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-1811</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-2484</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-1594</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-730</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-1474</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-596</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1270,36 +1369,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d/m;@" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="high"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="30" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="1246378655"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
@@ -1567,10 +1642,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Campania!$H$3:$CU$3</c:f>
+              <c:f>Campania!$H$3:$DL$3</c:f>
               <c:numCache>
                 <c:formatCode>d/m;@</c:formatCode>
-                <c:ptCount val="92"/>
+                <c:ptCount val="109"/>
                 <c:pt idx="0">
                   <c:v>43888</c:v>
                 </c:pt>
@@ -1846,16 +1921,67 @@
                 </c:pt>
                 <c:pt idx="91">
                   <c:v>43979</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>43980</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>43981</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>43982</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>43984</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>43985</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>43986</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>43987</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>43988</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>43989</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>43990</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>43991</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>43992</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>43993</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>43994</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>43995</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>43996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Campania!$H$4:$CU$4</c:f>
+              <c:f>Campania!$H$4:$DL$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="92"/>
+                <c:ptCount val="109"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -2101,6 +2227,54 @@
                 </c:pt>
                 <c:pt idx="81">
                   <c:v>-23</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-155</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-76</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-69</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-81</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-19</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-55</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-29</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-38</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-134</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-41</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-49</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2128,36 +2302,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="d/m;@" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="high"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="30" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="1246378655"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
@@ -3402,15 +3552,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>20171</xdr:colOff>
+      <xdr:colOff>20170</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>22412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>64</xdr:col>
-      <xdr:colOff>268941</xdr:colOff>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>215899</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>112059</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3737,10 +3887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
-  <dimension ref="A1:CU54"/>
+  <dimension ref="A1:DL54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CL4" sqref="CL4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="DA5" sqref="DA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3748,10 +3898,10 @@
     <col min="2" max="4" width="5.6640625" style="1" customWidth="1"/>
     <col min="5" max="25" width="4.6640625" style="2" customWidth="1"/>
     <col min="26" max="28" width="4.6640625" style="3" customWidth="1"/>
-    <col min="29" max="99" width="4.6640625" customWidth="1"/>
+    <col min="29" max="116" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:116" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
@@ -3762,32 +3912,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="31" t="s">
+      <c r="Z1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
     </row>
-    <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+    <row r="2" spans="1:116" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:116" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -4073,14 +4223,65 @@
       <c r="CU3" s="4">
         <v>43979</v>
       </c>
+      <c r="CV3" s="4">
+        <v>43980</v>
+      </c>
+      <c r="CW3" s="4">
+        <v>43981</v>
+      </c>
+      <c r="CX3" s="4">
+        <v>43982</v>
+      </c>
+      <c r="CY3" s="4">
+        <v>43983</v>
+      </c>
+      <c r="CZ3" s="4">
+        <v>43984</v>
+      </c>
+      <c r="DA3" s="4">
+        <v>43985</v>
+      </c>
+      <c r="DB3" s="4">
+        <v>43986</v>
+      </c>
+      <c r="DC3" s="4">
+        <v>43987</v>
+      </c>
+      <c r="DD3" s="4">
+        <v>43988</v>
+      </c>
+      <c r="DE3" s="4">
+        <v>43989</v>
+      </c>
+      <c r="DF3" s="4">
+        <v>43990</v>
+      </c>
+      <c r="DG3" s="4">
+        <v>43991</v>
+      </c>
+      <c r="DH3" s="4">
+        <v>43992</v>
+      </c>
+      <c r="DI3" s="4">
+        <v>43993</v>
+      </c>
+      <c r="DJ3" s="4">
+        <v>43994</v>
+      </c>
+      <c r="DK3" s="4">
+        <v>43995</v>
+      </c>
+      <c r="DL3" s="4">
+        <v>43996</v>
+      </c>
     </row>
-    <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:116" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -4336,28 +4537,77 @@
       <c r="CK4" s="7">
         <v>-1798</v>
       </c>
-      <c r="CL4" s="7"/>
-      <c r="CM4" s="7"/>
-      <c r="CN4" s="7"/>
-      <c r="CO4" s="7"/>
-      <c r="CP4" s="7"/>
-      <c r="CQ4" s="7"/>
-      <c r="CR4" s="7"/>
-      <c r="CS4" s="7"/>
-      <c r="CT4" s="7"/>
-      <c r="CU4" s="7"/>
+      <c r="CL4" s="7">
+        <v>-1424</v>
+      </c>
+      <c r="CM4" s="7">
+        <v>-2377</v>
+      </c>
+      <c r="CN4" s="7">
+        <v>-1792</v>
+      </c>
+      <c r="CO4" s="7">
+        <v>-1638</v>
+      </c>
+      <c r="CP4" s="7">
+        <v>-1570</v>
+      </c>
+      <c r="CQ4" s="7">
+        <v>-1158</v>
+      </c>
+      <c r="CR4" s="7">
+        <v>-1294</v>
+      </c>
+      <c r="CS4" s="7">
+        <v>-2358</v>
+      </c>
+      <c r="CT4" s="7">
+        <v>-1976</v>
+      </c>
+      <c r="CU4" s="7">
+        <v>-2980</v>
+      </c>
+      <c r="CV4" s="7">
+        <v>-1811</v>
+      </c>
+      <c r="CW4" s="7">
+        <v>-2484</v>
+      </c>
+      <c r="CX4" s="7">
+        <v>-1594</v>
+      </c>
+      <c r="CY4" s="7">
+        <v>-730</v>
+      </c>
+      <c r="CZ4" s="7">
+        <v>-1474</v>
+      </c>
+      <c r="DA4" s="7">
+        <v>-596</v>
+      </c>
+      <c r="DB4" s="7"/>
+      <c r="DC4" s="7"/>
+      <c r="DD4" s="7"/>
+      <c r="DE4" s="7"/>
+      <c r="DF4" s="7"/>
+      <c r="DG4" s="7"/>
+      <c r="DH4" s="7"/>
+      <c r="DI4" s="7"/>
+      <c r="DJ4" s="7"/>
+      <c r="DK4" s="7"/>
+      <c r="DL4" s="7"/>
     </row>
-    <row r="6" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:99" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:116" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:116" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="BT7" s="26"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:116" x14ac:dyDescent="0.2">
       <c r="BQ10" s="26"/>
     </row>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:116" x14ac:dyDescent="0.2">
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:116" x14ac:dyDescent="0.2">
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -4368,75 +4618,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="34" t="s">
+      <c r="L39" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34"/>
-      <c r="W39" s="29" t="s">
+      <c r="M39" s="36"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="36"/>
+      <c r="W39" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="29"/>
-      <c r="Y39" s="29"/>
-      <c r="Z39" s="29"/>
-      <c r="AA39" s="29"/>
-      <c r="AB39" s="30">
-        <f>SUM(E4:CU4)</f>
-        <v>66553</v>
-      </c>
-      <c r="AC39" s="30"/>
-      <c r="AD39" s="30"/>
-      <c r="AE39" s="30"/>
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="32">
+        <f>SUM(E4:DL4)</f>
+        <v>39297</v>
+      </c>
+      <c r="AC39" s="32"/>
+      <c r="AD39" s="32"/>
+      <c r="AE39" s="32"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="35" t="s">
+      <c r="L40" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
-      <c r="O40" s="35"/>
-      <c r="P40" s="35"/>
-      <c r="Q40" s="35"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="30"/>
-      <c r="AC40" s="30"/>
-      <c r="AD40" s="30"/>
-      <c r="AE40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="31"/>
+      <c r="Y40" s="31"/>
+      <c r="Z40" s="31"/>
+      <c r="AA40" s="31"/>
+      <c r="AB40" s="32"/>
+      <c r="AC40" s="32"/>
+      <c r="AD40" s="32"/>
+      <c r="AE40" s="32"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="35" t="s">
+      <c r="L41" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="35"/>
-      <c r="P41" s="35"/>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="35"/>
-      <c r="W41" s="29"/>
-      <c r="X41" s="29"/>
-      <c r="Y41" s="29"/>
-      <c r="Z41" s="29"/>
-      <c r="AA41" s="29"/>
-      <c r="AB41" s="30"/>
-      <c r="AC41" s="30"/>
-      <c r="AD41" s="30"/>
-      <c r="AE41" s="30"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="32"/>
+      <c r="AC41" s="32"/>
+      <c r="AD41" s="32"/>
+      <c r="AE41" s="32"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="36" t="s">
+      <c r="L42" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="36"/>
-      <c r="N42" s="36"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
@@ -4817,17 +5067,17 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="L40:Q40"/>
     <mergeCell ref="L42:N42"/>
     <mergeCell ref="L41:R41"/>
     <mergeCell ref="W39:AA41"/>
     <mergeCell ref="AB39:AE41"/>
     <mergeCell ref="Z1:AN1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L39:O39"/>
-    <mergeCell ref="L40:Q40"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4:CU4">
+  <conditionalFormatting sqref="E4:DL4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
       <formula>$O$47</formula>
     </cfRule>
@@ -4840,10 +5090,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
-  <dimension ref="A1:CU54"/>
+  <dimension ref="A1:DL54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CL4" sqref="CL4"/>
+    <sheetView zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="DB4" sqref="DB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4851,10 +5101,10 @@
     <col min="2" max="4" width="5.6640625" style="1" customWidth="1"/>
     <col min="5" max="25" width="4.6640625" style="2" customWidth="1"/>
     <col min="26" max="28" width="4.6640625" style="3" customWidth="1"/>
-    <col min="29" max="99" width="4.6640625" customWidth="1"/>
+    <col min="29" max="116" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:116" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
@@ -4865,26 +5115,26 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="31" t="s">
+      <c r="Z1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
     </row>
-    <row r="2" spans="1:99" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:99" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:116" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:116" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
@@ -5176,8 +5426,59 @@
       <c r="CU3" s="4">
         <v>43979</v>
       </c>
+      <c r="CV3" s="4">
+        <v>43980</v>
+      </c>
+      <c r="CW3" s="4">
+        <v>43981</v>
+      </c>
+      <c r="CX3" s="4">
+        <v>43982</v>
+      </c>
+      <c r="CY3" s="4">
+        <v>43983</v>
+      </c>
+      <c r="CZ3" s="4">
+        <v>43984</v>
+      </c>
+      <c r="DA3" s="4">
+        <v>43985</v>
+      </c>
+      <c r="DB3" s="4">
+        <v>43986</v>
+      </c>
+      <c r="DC3" s="4">
+        <v>43987</v>
+      </c>
+      <c r="DD3" s="4">
+        <v>43988</v>
+      </c>
+      <c r="DE3" s="4">
+        <v>43989</v>
+      </c>
+      <c r="DF3" s="4">
+        <v>43990</v>
+      </c>
+      <c r="DG3" s="4">
+        <v>43991</v>
+      </c>
+      <c r="DH3" s="4">
+        <v>43992</v>
+      </c>
+      <c r="DI3" s="4">
+        <v>43993</v>
+      </c>
+      <c r="DJ3" s="4">
+        <v>43994</v>
+      </c>
+      <c r="DK3" s="4">
+        <v>43995</v>
+      </c>
+      <c r="DL3" s="4">
+        <v>43996</v>
+      </c>
     </row>
-    <row r="4" spans="1:99" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:116" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
@@ -5439,23 +5740,72 @@
       <c r="CK4" s="21">
         <v>-23</v>
       </c>
-      <c r="CL4" s="21"/>
-      <c r="CM4" s="21"/>
-      <c r="CN4" s="21"/>
-      <c r="CO4" s="21"/>
-      <c r="CP4" s="21"/>
-      <c r="CQ4" s="21"/>
-      <c r="CR4" s="21"/>
-      <c r="CS4" s="21"/>
-      <c r="CT4" s="21"/>
-      <c r="CU4" s="21"/>
+      <c r="CL4" s="21">
+        <v>-155</v>
+      </c>
+      <c r="CM4" s="21">
+        <v>-76</v>
+      </c>
+      <c r="CN4" s="21">
+        <v>-69</v>
+      </c>
+      <c r="CO4" s="21">
+        <v>-81</v>
+      </c>
+      <c r="CP4" s="21">
+        <v>-19</v>
+      </c>
+      <c r="CQ4" s="21">
+        <v>-5</v>
+      </c>
+      <c r="CR4" s="21">
+        <v>-55</v>
+      </c>
+      <c r="CS4" s="21">
+        <v>-29</v>
+      </c>
+      <c r="CT4" s="21">
+        <v>-38</v>
+      </c>
+      <c r="CU4" s="21">
+        <v>-134</v>
+      </c>
+      <c r="CV4" s="21">
+        <v>-26</v>
+      </c>
+      <c r="CW4" s="21">
+        <v>-5</v>
+      </c>
+      <c r="CX4" s="21">
+        <v>-1</v>
+      </c>
+      <c r="CY4" s="21">
+        <v>-41</v>
+      </c>
+      <c r="CZ4" s="21">
+        <v>-49</v>
+      </c>
+      <c r="DA4" s="21">
+        <v>-21</v>
+      </c>
+      <c r="DB4" s="21"/>
+      <c r="DC4" s="21"/>
+      <c r="DD4" s="21"/>
+      <c r="DE4" s="21"/>
+      <c r="DF4" s="21"/>
+      <c r="DG4" s="21"/>
+      <c r="DH4" s="21"/>
+      <c r="DI4" s="21"/>
+      <c r="DJ4" s="21"/>
+      <c r="DK4" s="21"/>
+      <c r="DL4" s="21"/>
     </row>
-    <row r="6" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:99" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:116" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:116" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:116" x14ac:dyDescent="0.2">
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:116" x14ac:dyDescent="0.2">
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -5466,75 +5816,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="34" t="s">
+      <c r="L39" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34"/>
-      <c r="W39" s="29" t="s">
+      <c r="M39" s="36"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="36"/>
+      <c r="W39" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="29"/>
-      <c r="Y39" s="29"/>
-      <c r="Z39" s="29"/>
-      <c r="AA39" s="29"/>
-      <c r="AB39" s="30">
-        <f>SUM(E4:CU4)</f>
-        <v>1673</v>
-      </c>
-      <c r="AC39" s="30"/>
-      <c r="AD39" s="30"/>
-      <c r="AE39" s="30"/>
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="32">
+        <f>SUM(E4:DL4)</f>
+        <v>869</v>
+      </c>
+      <c r="AC39" s="32"/>
+      <c r="AD39" s="32"/>
+      <c r="AE39" s="32"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="35" t="s">
+      <c r="L40" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
-      <c r="O40" s="35"/>
-      <c r="P40" s="35"/>
-      <c r="Q40" s="35"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="30"/>
-      <c r="AC40" s="30"/>
-      <c r="AD40" s="30"/>
-      <c r="AE40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="31"/>
+      <c r="Y40" s="31"/>
+      <c r="Z40" s="31"/>
+      <c r="AA40" s="31"/>
+      <c r="AB40" s="32"/>
+      <c r="AC40" s="32"/>
+      <c r="AD40" s="32"/>
+      <c r="AE40" s="32"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="35" t="s">
+      <c r="L41" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="35"/>
-      <c r="P41" s="35"/>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="35"/>
-      <c r="W41" s="29"/>
-      <c r="X41" s="29"/>
-      <c r="Y41" s="29"/>
-      <c r="Z41" s="29"/>
-      <c r="AA41" s="29"/>
-      <c r="AB41" s="30"/>
-      <c r="AC41" s="30"/>
-      <c r="AD41" s="30"/>
-      <c r="AE41" s="30"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="32"/>
+      <c r="AC41" s="32"/>
+      <c r="AD41" s="32"/>
+      <c r="AE41" s="32"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="36" t="s">
+      <c r="L42" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="36"/>
-      <c r="N42" s="36"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 09/06/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C52787-DB55-1A4A-8348-92063CAA7487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C24CE3-8B49-354C-9967-969C928ED0AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -421,10 +421,19 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -435,15 +444,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1342,6 +1342,24 @@
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>-596</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-868</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-1453</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-1099</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-615</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>-532</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-1858</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2275,6 +2293,24 @@
                 </c:pt>
                 <c:pt idx="97">
                   <c:v>-21</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-39</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-56</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-36</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3889,8 +3925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A1:DL54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="DA5" sqref="DA5"/>
+    <sheetView zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="DH4" sqref="DH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3912,32 +3948,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="33" t="s">
+      <c r="Z1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36"/>
     </row>
     <row r="2" spans="1:116" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:116" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -4276,12 +4312,12 @@
       </c>
     </row>
     <row r="4" spans="1:116" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -4585,12 +4621,24 @@
       <c r="DA4" s="7">
         <v>-596</v>
       </c>
-      <c r="DB4" s="7"/>
-      <c r="DC4" s="7"/>
-      <c r="DD4" s="7"/>
-      <c r="DE4" s="7"/>
-      <c r="DF4" s="7"/>
-      <c r="DG4" s="7"/>
+      <c r="DB4" s="7">
+        <v>-868</v>
+      </c>
+      <c r="DC4" s="7">
+        <v>-1453</v>
+      </c>
+      <c r="DD4" s="7">
+        <v>-1099</v>
+      </c>
+      <c r="DE4" s="7">
+        <v>-615</v>
+      </c>
+      <c r="DF4" s="7">
+        <v>-532</v>
+      </c>
+      <c r="DG4" s="7">
+        <v>-1858</v>
+      </c>
       <c r="DH4" s="7"/>
       <c r="DI4" s="7"/>
       <c r="DJ4" s="7"/>
@@ -4618,75 +4666,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="36" t="s">
+      <c r="L39" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="W39" s="31" t="s">
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="W39" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="31"/>
-      <c r="Y39" s="31"/>
-      <c r="Z39" s="31"/>
-      <c r="AA39" s="31"/>
-      <c r="AB39" s="32">
+      <c r="X39" s="34"/>
+      <c r="Y39" s="34"/>
+      <c r="Z39" s="34"/>
+      <c r="AA39" s="34"/>
+      <c r="AB39" s="35">
         <f>SUM(E4:DL4)</f>
-        <v>39297</v>
-      </c>
-      <c r="AC39" s="32"/>
-      <c r="AD39" s="32"/>
-      <c r="AE39" s="32"/>
+        <v>32872</v>
+      </c>
+      <c r="AC39" s="35"/>
+      <c r="AD39" s="35"/>
+      <c r="AE39" s="35"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="30" t="s">
+      <c r="L40" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="W40" s="31"/>
-      <c r="X40" s="31"/>
-      <c r="Y40" s="31"/>
-      <c r="Z40" s="31"/>
-      <c r="AA40" s="31"/>
-      <c r="AB40" s="32"/>
-      <c r="AC40" s="32"/>
-      <c r="AD40" s="32"/>
-      <c r="AE40" s="32"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="32"/>
+      <c r="P40" s="32"/>
+      <c r="Q40" s="32"/>
+      <c r="W40" s="34"/>
+      <c r="X40" s="34"/>
+      <c r="Y40" s="34"/>
+      <c r="Z40" s="34"/>
+      <c r="AA40" s="34"/>
+      <c r="AB40" s="35"/>
+      <c r="AC40" s="35"/>
+      <c r="AD40" s="35"/>
+      <c r="AE40" s="35"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="30" t="s">
+      <c r="L41" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="30"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-      <c r="W41" s="31"/>
-      <c r="X41" s="31"/>
-      <c r="Y41" s="31"/>
-      <c r="Z41" s="31"/>
-      <c r="AA41" s="31"/>
-      <c r="AB41" s="32"/>
-      <c r="AC41" s="32"/>
-      <c r="AD41" s="32"/>
-      <c r="AE41" s="32"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="W41" s="34"/>
+      <c r="X41" s="34"/>
+      <c r="Y41" s="34"/>
+      <c r="Z41" s="34"/>
+      <c r="AA41" s="34"/>
+      <c r="AB41" s="35"/>
+      <c r="AC41" s="35"/>
+      <c r="AD41" s="35"/>
+      <c r="AE41" s="35"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="29" t="s">
+      <c r="L42" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
@@ -5067,15 +5115,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="W39:AA41"/>
+    <mergeCell ref="AB39:AE41"/>
+    <mergeCell ref="Z1:AN1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L39:O39"/>
     <mergeCell ref="L40:Q40"/>
     <mergeCell ref="L42:N42"/>
     <mergeCell ref="L41:R41"/>
-    <mergeCell ref="W39:AA41"/>
-    <mergeCell ref="AB39:AE41"/>
-    <mergeCell ref="Z1:AN1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:DL4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -5092,8 +5140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A1:DL54"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="DB4" sqref="DB4"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="DH4" sqref="DH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5115,23 +5163,23 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="33" t="s">
+      <c r="Z1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36"/>
     </row>
     <row r="2" spans="1:116" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:116" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5788,12 +5836,24 @@
       <c r="DA4" s="21">
         <v>-21</v>
       </c>
-      <c r="DB4" s="21"/>
-      <c r="DC4" s="21"/>
-      <c r="DD4" s="21"/>
-      <c r="DE4" s="21"/>
-      <c r="DF4" s="21"/>
-      <c r="DG4" s="21"/>
+      <c r="DB4" s="21">
+        <v>-39</v>
+      </c>
+      <c r="DC4" s="21">
+        <v>-56</v>
+      </c>
+      <c r="DD4" s="21">
+        <v>-36</v>
+      </c>
+      <c r="DE4" s="21">
+        <v>-13</v>
+      </c>
+      <c r="DF4" s="21">
+        <v>-8</v>
+      </c>
+      <c r="DG4" s="21">
+        <v>-42</v>
+      </c>
       <c r="DH4" s="21"/>
       <c r="DI4" s="21"/>
       <c r="DJ4" s="21"/>
@@ -5816,75 +5876,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="36" t="s">
+      <c r="L39" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="W39" s="31" t="s">
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="W39" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="31"/>
-      <c r="Y39" s="31"/>
-      <c r="Z39" s="31"/>
-      <c r="AA39" s="31"/>
-      <c r="AB39" s="32">
+      <c r="X39" s="34"/>
+      <c r="Y39" s="34"/>
+      <c r="Z39" s="34"/>
+      <c r="AA39" s="34"/>
+      <c r="AB39" s="35">
         <f>SUM(E4:DL4)</f>
-        <v>869</v>
-      </c>
-      <c r="AC39" s="32"/>
-      <c r="AD39" s="32"/>
-      <c r="AE39" s="32"/>
+        <v>675</v>
+      </c>
+      <c r="AC39" s="35"/>
+      <c r="AD39" s="35"/>
+      <c r="AE39" s="35"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="30" t="s">
+      <c r="L40" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="W40" s="31"/>
-      <c r="X40" s="31"/>
-      <c r="Y40" s="31"/>
-      <c r="Z40" s="31"/>
-      <c r="AA40" s="31"/>
-      <c r="AB40" s="32"/>
-      <c r="AC40" s="32"/>
-      <c r="AD40" s="32"/>
-      <c r="AE40" s="32"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="32"/>
+      <c r="P40" s="32"/>
+      <c r="Q40" s="32"/>
+      <c r="W40" s="34"/>
+      <c r="X40" s="34"/>
+      <c r="Y40" s="34"/>
+      <c r="Z40" s="34"/>
+      <c r="AA40" s="34"/>
+      <c r="AB40" s="35"/>
+      <c r="AC40" s="35"/>
+      <c r="AD40" s="35"/>
+      <c r="AE40" s="35"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="30" t="s">
+      <c r="L41" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="30"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-      <c r="W41" s="31"/>
-      <c r="X41" s="31"/>
-      <c r="Y41" s="31"/>
-      <c r="Z41" s="31"/>
-      <c r="AA41" s="31"/>
-      <c r="AB41" s="32"/>
-      <c r="AC41" s="32"/>
-      <c r="AD41" s="32"/>
-      <c r="AE41" s="32"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="W41" s="34"/>
+      <c r="X41" s="34"/>
+      <c r="Y41" s="34"/>
+      <c r="Z41" s="34"/>
+      <c r="AA41" s="34"/>
+      <c r="AB41" s="35"/>
+      <c r="AC41" s="35"/>
+      <c r="AD41" s="35"/>
+      <c r="AE41" s="35"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="29" t="s">
+      <c r="L42" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 18/06/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C24CE3-8B49-354C-9967-969C928ED0AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E09947-A807-A04B-922A-5265427802D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -21,12 +21,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -421,6 +415,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -435,15 +438,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1360,6 +1354,21 @@
                 </c:pt>
                 <c:pt idx="106">
                   <c:v>-1858</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>-1162</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>-1073</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>-1640</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>-1512</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>-1211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2311,6 +2320,21 @@
                 </c:pt>
                 <c:pt idx="103">
                   <c:v>-42</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-33</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>-32</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-264</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>-18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3923,10 +3947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
-  <dimension ref="A1:DL54"/>
+  <dimension ref="A1:EA54"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="DH4" sqref="DH4"/>
+      <selection activeCell="AB42" sqref="AB42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3934,10 +3958,10 @@
     <col min="2" max="4" width="5.6640625" style="1" customWidth="1"/>
     <col min="5" max="25" width="4.6640625" style="2" customWidth="1"/>
     <col min="26" max="28" width="4.6640625" style="3" customWidth="1"/>
-    <col min="29" max="116" width="4.6640625" customWidth="1"/>
+    <col min="29" max="131" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:116" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:131" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
@@ -3948,32 +3972,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="36" t="s">
+      <c r="Z1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="36"/>
-      <c r="AL1" s="36"/>
-      <c r="AM1" s="36"/>
-      <c r="AN1" s="36"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
     </row>
-    <row r="2" spans="1:116" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:116" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+    <row r="2" spans="1:131" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:131" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -4310,14 +4334,59 @@
       <c r="DL3" s="4">
         <v>43996</v>
       </c>
+      <c r="DM3" s="4">
+        <v>43997</v>
+      </c>
+      <c r="DN3" s="4">
+        <v>43998</v>
+      </c>
+      <c r="DO3" s="4">
+        <v>43999</v>
+      </c>
+      <c r="DP3" s="4">
+        <v>44000</v>
+      </c>
+      <c r="DQ3" s="4">
+        <v>44001</v>
+      </c>
+      <c r="DR3" s="4">
+        <v>44002</v>
+      </c>
+      <c r="DS3" s="4">
+        <v>44003</v>
+      </c>
+      <c r="DT3" s="4">
+        <v>44004</v>
+      </c>
+      <c r="DU3" s="4">
+        <v>44005</v>
+      </c>
+      <c r="DV3" s="4">
+        <v>44006</v>
+      </c>
+      <c r="DW3" s="4">
+        <v>44007</v>
+      </c>
+      <c r="DX3" s="4">
+        <v>44008</v>
+      </c>
+      <c r="DY3" s="4">
+        <v>44009</v>
+      </c>
+      <c r="DZ3" s="4">
+        <v>44010</v>
+      </c>
+      <c r="EA3" s="4">
+        <v>44011</v>
+      </c>
     </row>
-    <row r="4" spans="1:116" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:131" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -4639,23 +4708,56 @@
       <c r="DG4" s="7">
         <v>-1858</v>
       </c>
-      <c r="DH4" s="7"/>
-      <c r="DI4" s="7"/>
-      <c r="DJ4" s="7"/>
-      <c r="DK4" s="7"/>
-      <c r="DL4" s="7"/>
+      <c r="DH4" s="7">
+        <v>-1162</v>
+      </c>
+      <c r="DI4" s="7">
+        <v>-1073</v>
+      </c>
+      <c r="DJ4" s="7">
+        <v>-1640</v>
+      </c>
+      <c r="DK4" s="7">
+        <v>-1512</v>
+      </c>
+      <c r="DL4" s="7">
+        <v>-1211</v>
+      </c>
+      <c r="DM4" s="7">
+        <v>-365</v>
+      </c>
+      <c r="DN4" s="7">
+        <v>-1340</v>
+      </c>
+      <c r="DO4" s="7">
+        <v>-644</v>
+      </c>
+      <c r="DP4" s="7">
+        <v>-824</v>
+      </c>
+      <c r="DQ4" s="7"/>
+      <c r="DR4" s="7"/>
+      <c r="DS4" s="7"/>
+      <c r="DT4" s="7"/>
+      <c r="DU4" s="7"/>
+      <c r="DV4" s="7"/>
+      <c r="DW4" s="7"/>
+      <c r="DX4" s="7"/>
+      <c r="DY4" s="7"/>
+      <c r="DZ4" s="7"/>
+      <c r="EA4" s="7"/>
     </row>
-    <row r="6" spans="1:116" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:116" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:131" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:131" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="BT7" s="26"/>
     </row>
-    <row r="10" spans="1:116" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:131" x14ac:dyDescent="0.2">
       <c r="BQ10" s="26"/>
     </row>
-    <row r="14" spans="1:116" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:131" x14ac:dyDescent="0.2">
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:116" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:131" x14ac:dyDescent="0.2">
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -4666,75 +4768,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="31" t="s">
+      <c r="L39" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="31"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="31"/>
-      <c r="W39" s="34" t="s">
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="34"/>
+      <c r="W39" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="34"/>
-      <c r="Y39" s="34"/>
-      <c r="Z39" s="34"/>
-      <c r="AA39" s="34"/>
-      <c r="AB39" s="35">
-        <f>SUM(E4:DL4)</f>
-        <v>32872</v>
-      </c>
-      <c r="AC39" s="35"/>
-      <c r="AD39" s="35"/>
-      <c r="AE39" s="35"/>
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="30">
+        <f>SUM(E4:EA4)</f>
+        <v>23101</v>
+      </c>
+      <c r="AC39" s="30"/>
+      <c r="AD39" s="30"/>
+      <c r="AE39" s="30"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="32" t="s">
+      <c r="L40" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
-      <c r="Q40" s="32"/>
-      <c r="W40" s="34"/>
-      <c r="X40" s="34"/>
-      <c r="Y40" s="34"/>
-      <c r="Z40" s="34"/>
-      <c r="AA40" s="34"/>
-      <c r="AB40" s="35"/>
-      <c r="AC40" s="35"/>
-      <c r="AD40" s="35"/>
-      <c r="AE40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="30"/>
+      <c r="AC40" s="30"/>
+      <c r="AD40" s="30"/>
+      <c r="AE40" s="30"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="32" t="s">
+      <c r="L41" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="32"/>
-      <c r="R41" s="32"/>
-      <c r="W41" s="34"/>
-      <c r="X41" s="34"/>
-      <c r="Y41" s="34"/>
-      <c r="Z41" s="34"/>
-      <c r="AA41" s="34"/>
-      <c r="AB41" s="35"/>
-      <c r="AC41" s="35"/>
-      <c r="AD41" s="35"/>
-      <c r="AE41" s="35"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35"/>
+      <c r="R41" s="35"/>
+      <c r="W41" s="29"/>
+      <c r="X41" s="29"/>
+      <c r="Y41" s="29"/>
+      <c r="Z41" s="29"/>
+      <c r="AA41" s="29"/>
+      <c r="AB41" s="30"/>
+      <c r="AC41" s="30"/>
+      <c r="AD41" s="30"/>
+      <c r="AE41" s="30"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="33" t="s">
+      <c r="L42" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="33"/>
-      <c r="N42" s="33"/>
+      <c r="M42" s="36"/>
+      <c r="N42" s="36"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
@@ -5115,6 +5217,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="L41:R41"/>
     <mergeCell ref="W39:AA41"/>
     <mergeCell ref="AB39:AE41"/>
     <mergeCell ref="Z1:AN1"/>
@@ -5122,10 +5226,8 @@
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L39:O39"/>
     <mergeCell ref="L40:Q40"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="L41:R41"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4:DL4">
+  <conditionalFormatting sqref="E4:EA4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
       <formula>$O$47</formula>
     </cfRule>
@@ -5138,10 +5240,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
-  <dimension ref="A1:DL54"/>
+  <dimension ref="A1:DZ54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="DH4" sqref="DH4"/>
+      <selection activeCell="AB42" sqref="AB42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5149,10 +5251,10 @@
     <col min="2" max="4" width="5.6640625" style="1" customWidth="1"/>
     <col min="5" max="25" width="4.6640625" style="2" customWidth="1"/>
     <col min="26" max="28" width="4.6640625" style="3" customWidth="1"/>
-    <col min="29" max="116" width="4.6640625" customWidth="1"/>
+    <col min="29" max="130" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:116" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:130" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
@@ -5163,26 +5265,26 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="36" t="s">
+      <c r="Z1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="36"/>
-      <c r="AL1" s="36"/>
-      <c r="AM1" s="36"/>
-      <c r="AN1" s="36"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
     </row>
-    <row r="2" spans="1:116" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:116" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:130" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:130" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
@@ -5525,8 +5627,50 @@
       <c r="DL3" s="4">
         <v>43996</v>
       </c>
+      <c r="DM3" s="4">
+        <v>43997</v>
+      </c>
+      <c r="DN3" s="4">
+        <v>43998</v>
+      </c>
+      <c r="DO3" s="4">
+        <v>43999</v>
+      </c>
+      <c r="DP3" s="4">
+        <v>44000</v>
+      </c>
+      <c r="DQ3" s="4">
+        <v>44001</v>
+      </c>
+      <c r="DR3" s="4">
+        <v>44002</v>
+      </c>
+      <c r="DS3" s="4">
+        <v>44003</v>
+      </c>
+      <c r="DT3" s="4">
+        <v>44004</v>
+      </c>
+      <c r="DU3" s="4">
+        <v>44005</v>
+      </c>
+      <c r="DV3" s="4">
+        <v>44006</v>
+      </c>
+      <c r="DW3" s="4">
+        <v>44007</v>
+      </c>
+      <c r="DX3" s="4">
+        <v>44008</v>
+      </c>
+      <c r="DY3" s="4">
+        <v>44009</v>
+      </c>
+      <c r="DZ3" s="4">
+        <v>44010</v>
+      </c>
     </row>
-    <row r="4" spans="1:116" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:130" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
@@ -5854,18 +5998,50 @@
       <c r="DG4" s="21">
         <v>-42</v>
       </c>
-      <c r="DH4" s="21"/>
-      <c r="DI4" s="21"/>
-      <c r="DJ4" s="21"/>
-      <c r="DK4" s="21"/>
-      <c r="DL4" s="21"/>
+      <c r="DH4" s="21">
+        <v>-33</v>
+      </c>
+      <c r="DI4" s="21">
+        <v>-32</v>
+      </c>
+      <c r="DJ4" s="21">
+        <v>-264</v>
+      </c>
+      <c r="DK4" s="21">
+        <v>-9</v>
+      </c>
+      <c r="DL4" s="21">
+        <v>-18</v>
+      </c>
+      <c r="DM4" s="21">
+        <v>-30</v>
+      </c>
+      <c r="DN4" s="21">
+        <v>-16</v>
+      </c>
+      <c r="DO4" s="21">
+        <v>-15</v>
+      </c>
+      <c r="DP4" s="21">
+        <v>-16</v>
+      </c>
+      <c r="DQ4" s="21"/>
+      <c r="DR4" s="21"/>
+      <c r="DS4" s="21"/>
+      <c r="DT4" s="21"/>
+      <c r="DU4" s="21"/>
+      <c r="DV4" s="21"/>
+      <c r="DW4" s="21"/>
+      <c r="DX4" s="21"/>
+      <c r="DY4" s="21"/>
+      <c r="DZ4" s="21"/>
     </row>
-    <row r="6" spans="1:116" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:116" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:116" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:130" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:130" x14ac:dyDescent="0.2">
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:116" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:130" x14ac:dyDescent="0.2">
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -5876,75 +6052,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="31" t="s">
+      <c r="L39" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="31"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="31"/>
-      <c r="W39" s="34" t="s">
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="34"/>
+      <c r="W39" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="34"/>
-      <c r="Y39" s="34"/>
-      <c r="Z39" s="34"/>
-      <c r="AA39" s="34"/>
-      <c r="AB39" s="35">
-        <f>SUM(E4:DL4)</f>
-        <v>675</v>
-      </c>
-      <c r="AC39" s="35"/>
-      <c r="AD39" s="35"/>
-      <c r="AE39" s="35"/>
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="30">
+        <f>SUM(E4:DZ4)</f>
+        <v>242</v>
+      </c>
+      <c r="AC39" s="30"/>
+      <c r="AD39" s="30"/>
+      <c r="AE39" s="30"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="32" t="s">
+      <c r="L40" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
-      <c r="Q40" s="32"/>
-      <c r="W40" s="34"/>
-      <c r="X40" s="34"/>
-      <c r="Y40" s="34"/>
-      <c r="Z40" s="34"/>
-      <c r="AA40" s="34"/>
-      <c r="AB40" s="35"/>
-      <c r="AC40" s="35"/>
-      <c r="AD40" s="35"/>
-      <c r="AE40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="30"/>
+      <c r="AC40" s="30"/>
+      <c r="AD40" s="30"/>
+      <c r="AE40" s="30"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="32" t="s">
+      <c r="L41" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="32"/>
-      <c r="R41" s="32"/>
-      <c r="W41" s="34"/>
-      <c r="X41" s="34"/>
-      <c r="Y41" s="34"/>
-      <c r="Z41" s="34"/>
-      <c r="AA41" s="34"/>
-      <c r="AB41" s="35"/>
-      <c r="AC41" s="35"/>
-      <c r="AD41" s="35"/>
-      <c r="AE41" s="35"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35"/>
+      <c r="R41" s="35"/>
+      <c r="W41" s="29"/>
+      <c r="X41" s="29"/>
+      <c r="Y41" s="29"/>
+      <c r="Z41" s="29"/>
+      <c r="AA41" s="29"/>
+      <c r="AB41" s="30"/>
+      <c r="AC41" s="30"/>
+      <c r="AD41" s="30"/>
+      <c r="AE41" s="30"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="33" t="s">
+      <c r="L42" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="33"/>
-      <c r="N42" s="33"/>
+      <c r="M42" s="36"/>
+      <c r="N42" s="36"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 07/07/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E09947-A807-A04B-922A-5265427802D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F43C8B-6E0E-5940-B8D8-81A20F2588E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -66,9 +66,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m;@"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -334,14 +341,14 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -350,23 +357,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -375,86 +382,89 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="16" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="17" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -522,78 +532,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="it-IT" sz="2400"/>
-              <a:t>Nuovi</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="it-IT" sz="2400" baseline="0"/>
-              <a:t> infetti</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="2400"/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="it-IT" sz="2400" baseline="0"/>
-              <a:t>Italia</a:t>
-            </a:r>
-            <a:endParaRPr lang="it-IT" sz="2400"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="3.7777202552782357E-2"/>
-          <c:y val="0.13333333333333333"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -601,9 +540,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="2.4618482555394887E-2"/>
-          <c:y val="9.1776285317276524E-2"/>
-          <c:w val="0.93230409590243379"/>
-          <c:h val="0.75948244448536006"/>
+          <c:y val="2.6994227674904454E-2"/>
+          <c:w val="0.96974463218555373"/>
+          <c:h val="0.94430182621513248"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -629,66 +568,14 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4472C4"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent1">
-                          <a:lumMod val="60000"/>
-                          <a:lumOff val="40000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Italia!$E$3:$DL$3</c:f>
+              <c:f>Italia!$E$3:$GW$3</c:f>
               <c:numCache>
                 <c:formatCode>d/m;@</c:formatCode>
-                <c:ptCount val="112"/>
+                <c:ptCount val="201"/>
                 <c:pt idx="0">
                   <c:v>43885</c:v>
                 </c:pt>
@@ -1024,16 +911,283 @@
                 </c:pt>
                 <c:pt idx="111">
                   <c:v>43996</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>43997</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>43998</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>43999</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>44000</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>44001</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>44002</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>44003</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>44004</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>44005</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>44006</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>44007</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>44008</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>44009</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>44010</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>44011</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>44012</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>44014</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>44015</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>44016</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>44017</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>44018</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>44019</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>44020</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>44021</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>44022</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>44023</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>44024</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>44025</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>44026</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>44027</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>44028</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>44029</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>44030</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>44031</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>44032</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>44033</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>44034</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>44035</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>44036</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>44037</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>44038</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>44039</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>44040</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>44041</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>44042</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>44045</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>44046</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>44047</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>44048</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>44049</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>44050</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>44051</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>44052</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>44053</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>44054</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>44055</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>44056</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>44057</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>44058</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>44059</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>44060</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>44061</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>44062</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>44063</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>44064</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>44065</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>44066</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>44067</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>44068</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>44069</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>44070</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>44071</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>44072</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>44073</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>44074</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>44076</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>44077</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>44078</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>44079</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>44080</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>44081</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>44082</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>44083</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>44084</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>44085</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Italia!$E$4:$DL$4</c:f>
+              <c:f>Italia!$E$4:$GW$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="112"/>
+                <c:ptCount val="201"/>
                 <c:pt idx="0">
                   <c:v>221</c:v>
                 </c:pt>
@@ -1230,7 +1384,7 @@
                   <c:v>-608</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>-548</c:v>
+                  <c:v>-557</c:v>
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>-3106</c:v>
@@ -1369,6 +1523,75 @@
                 </c:pt>
                 <c:pt idx="111">
                   <c:v>-1211</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>-365</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>-1340</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>-644</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>-824</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>-1558</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>-331</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>-240</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>-335</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>-1064</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>-918</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>-352</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>-656</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>-802</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>-155</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>-185</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>-933</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>-308</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-195</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-176</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>-263</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>-467</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1506,78 +1729,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="it-IT" sz="2400"/>
-              <a:t>Nuovi</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="it-IT" sz="2400" baseline="0"/>
-              <a:t> infetti</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="2400"/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="it-IT" sz="2400" baseline="0"/>
-              <a:t>Italia</a:t>
-            </a:r>
-            <a:endParaRPr lang="it-IT" sz="2400"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="3.7777202552782357E-2"/>
-          <c:y val="0.13333333333333333"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -1585,9 +1737,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="2.4618482555394887E-2"/>
-          <c:y val="9.1776285317276524E-2"/>
-          <c:w val="0.93230409590243379"/>
-          <c:h val="0.83438107503171466"/>
+          <c:y val="3.3150891921543524E-2"/>
+          <c:w val="0.97166792881369968"/>
+          <c:h val="0.93599845512079738"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1613,66 +1765,14 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4472C4"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent1">
-                          <a:lumMod val="60000"/>
-                          <a:lumOff val="40000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Campania!$H$3:$DL$3</c:f>
+              <c:f>Campania!$H$3:$GZ$3</c:f>
               <c:numCache>
                 <c:formatCode>d/m;@</c:formatCode>
-                <c:ptCount val="109"/>
+                <c:ptCount val="201"/>
                 <c:pt idx="0">
                   <c:v>43888</c:v>
                 </c:pt>
@@ -1999,16 +2099,292 @@
                 </c:pt>
                 <c:pt idx="108">
                   <c:v>43996</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>43997</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>43998</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>43999</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>44000</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>44001</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>44002</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>44003</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>44004</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>44005</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>44006</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>44007</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>44008</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>44009</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>44010</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>44011</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>44012</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>44014</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>44015</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>44016</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>44017</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>44018</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>44019</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>44020</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>44021</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>44022</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>44023</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>44024</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>44025</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>44026</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>44027</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>44028</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>44029</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>44030</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>44031</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>44032</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>44033</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>44034</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>44035</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>44036</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>44037</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>44038</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>44039</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>44040</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>44041</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>44042</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>44045</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>44046</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>44047</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>44048</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>44049</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>44050</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>44051</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>44052</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>44053</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>44054</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>44055</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>44056</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>44057</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>44058</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>44059</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>44060</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>44061</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>44062</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>44063</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>44064</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>44065</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>44066</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>44067</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>44068</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>44069</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>44070</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>44071</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>44072</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>44073</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>44074</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>44076</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>44077</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>44078</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>44079</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>44080</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>44081</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>44082</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>44083</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>44084</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>44085</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>44086</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>44087</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>44088</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Campania!$H$4:$DL$4</c:f>
+              <c:f>Campania!$H$4:$GZ$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="109"/>
+                <c:ptCount val="201"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -2335,6 +2711,75 @@
                 </c:pt>
                 <c:pt idx="108">
                   <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>-117</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>-1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3947,10 +4392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
-  <dimension ref="A1:EA54"/>
+  <dimension ref="A1:GW54"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB42" sqref="AB42"/>
+      <selection activeCell="BR5" sqref="BR5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3958,10 +4403,10 @@
     <col min="2" max="4" width="5.6640625" style="1" customWidth="1"/>
     <col min="5" max="25" width="4.6640625" style="2" customWidth="1"/>
     <col min="26" max="28" width="4.6640625" style="3" customWidth="1"/>
-    <col min="29" max="131" width="4.6640625" customWidth="1"/>
+    <col min="29" max="205" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:131" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:205" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
@@ -3972,32 +4417,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="31" t="s">
+      <c r="Z1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
     </row>
-    <row r="2" spans="1:131" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:131" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+    <row r="2" spans="1:205" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:205" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -4379,14 +4824,236 @@
       <c r="EA3" s="4">
         <v>44011</v>
       </c>
+      <c r="EB3" s="4">
+        <v>44012</v>
+      </c>
+      <c r="EC3" s="4">
+        <v>44013</v>
+      </c>
+      <c r="ED3" s="4">
+        <v>44014</v>
+      </c>
+      <c r="EE3" s="4">
+        <v>44015</v>
+      </c>
+      <c r="EF3" s="4">
+        <v>44016</v>
+      </c>
+      <c r="EG3" s="4">
+        <v>44017</v>
+      </c>
+      <c r="EH3" s="4">
+        <v>44018</v>
+      </c>
+      <c r="EI3" s="4">
+        <v>44019</v>
+      </c>
+      <c r="EJ3" s="4">
+        <v>44020</v>
+      </c>
+      <c r="EK3" s="4">
+        <v>44021</v>
+      </c>
+      <c r="EL3" s="4">
+        <v>44022</v>
+      </c>
+      <c r="EM3" s="4">
+        <v>44023</v>
+      </c>
+      <c r="EN3" s="4">
+        <v>44024</v>
+      </c>
+      <c r="EO3" s="4">
+        <v>44025</v>
+      </c>
+      <c r="EP3" s="4">
+        <v>44026</v>
+      </c>
+      <c r="EQ3" s="4">
+        <v>44027</v>
+      </c>
+      <c r="ER3" s="4">
+        <v>44028</v>
+      </c>
+      <c r="ES3" s="4">
+        <v>44029</v>
+      </c>
+      <c r="ET3" s="4">
+        <v>44030</v>
+      </c>
+      <c r="EU3" s="4">
+        <v>44031</v>
+      </c>
+      <c r="EV3" s="4">
+        <v>44032</v>
+      </c>
+      <c r="EW3" s="4">
+        <v>44033</v>
+      </c>
+      <c r="EX3" s="4">
+        <v>44034</v>
+      </c>
+      <c r="EY3" s="4">
+        <v>44035</v>
+      </c>
+      <c r="EZ3" s="4">
+        <v>44036</v>
+      </c>
+      <c r="FA3" s="4">
+        <v>44037</v>
+      </c>
+      <c r="FB3" s="4">
+        <v>44038</v>
+      </c>
+      <c r="FC3" s="4">
+        <v>44039</v>
+      </c>
+      <c r="FD3" s="4">
+        <v>44040</v>
+      </c>
+      <c r="FE3" s="4">
+        <v>44041</v>
+      </c>
+      <c r="FF3" s="4">
+        <v>44042</v>
+      </c>
+      <c r="FG3" s="4">
+        <v>44043</v>
+      </c>
+      <c r="FH3" s="4">
+        <v>44044</v>
+      </c>
+      <c r="FI3" s="4">
+        <v>44045</v>
+      </c>
+      <c r="FJ3" s="4">
+        <v>44046</v>
+      </c>
+      <c r="FK3" s="4">
+        <v>44047</v>
+      </c>
+      <c r="FL3" s="4">
+        <v>44048</v>
+      </c>
+      <c r="FM3" s="4">
+        <v>44049</v>
+      </c>
+      <c r="FN3" s="4">
+        <v>44050</v>
+      </c>
+      <c r="FO3" s="4">
+        <v>44051</v>
+      </c>
+      <c r="FP3" s="4">
+        <v>44052</v>
+      </c>
+      <c r="FQ3" s="4">
+        <v>44053</v>
+      </c>
+      <c r="FR3" s="4">
+        <v>44054</v>
+      </c>
+      <c r="FS3" s="4">
+        <v>44055</v>
+      </c>
+      <c r="FT3" s="4">
+        <v>44056</v>
+      </c>
+      <c r="FU3" s="4">
+        <v>44057</v>
+      </c>
+      <c r="FV3" s="4">
+        <v>44058</v>
+      </c>
+      <c r="FW3" s="4">
+        <v>44059</v>
+      </c>
+      <c r="FX3" s="4">
+        <v>44060</v>
+      </c>
+      <c r="FY3" s="4">
+        <v>44061</v>
+      </c>
+      <c r="FZ3" s="4">
+        <v>44062</v>
+      </c>
+      <c r="GA3" s="4">
+        <v>44063</v>
+      </c>
+      <c r="GB3" s="4">
+        <v>44064</v>
+      </c>
+      <c r="GC3" s="4">
+        <v>44065</v>
+      </c>
+      <c r="GD3" s="4">
+        <v>44066</v>
+      </c>
+      <c r="GE3" s="4">
+        <v>44067</v>
+      </c>
+      <c r="GF3" s="4">
+        <v>44068</v>
+      </c>
+      <c r="GG3" s="4">
+        <v>44069</v>
+      </c>
+      <c r="GH3" s="4">
+        <v>44070</v>
+      </c>
+      <c r="GI3" s="4">
+        <v>44071</v>
+      </c>
+      <c r="GJ3" s="4">
+        <v>44072</v>
+      </c>
+      <c r="GK3" s="4">
+        <v>44073</v>
+      </c>
+      <c r="GL3" s="4">
+        <v>44074</v>
+      </c>
+      <c r="GM3" s="4">
+        <v>44075</v>
+      </c>
+      <c r="GN3" s="4">
+        <v>44076</v>
+      </c>
+      <c r="GO3" s="4">
+        <v>44077</v>
+      </c>
+      <c r="GP3" s="4">
+        <v>44078</v>
+      </c>
+      <c r="GQ3" s="4">
+        <v>44079</v>
+      </c>
+      <c r="GR3" s="4">
+        <v>44080</v>
+      </c>
+      <c r="GS3" s="4">
+        <v>44081</v>
+      </c>
+      <c r="GT3" s="4">
+        <v>44082</v>
+      </c>
+      <c r="GU3" s="4">
+        <v>44083</v>
+      </c>
+      <c r="GV3" s="4">
+        <v>44084</v>
+      </c>
+      <c r="GW3" s="4">
+        <v>44085</v>
+      </c>
     </row>
-    <row r="4" spans="1:131" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:205" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -4583,7 +5250,7 @@
         <v>-608</v>
       </c>
       <c r="BR4" s="7">
-        <v>-548</v>
+        <v>-557</v>
       </c>
       <c r="BS4" s="7">
         <v>-3106</v>
@@ -4735,29 +5402,141 @@
       <c r="DP4" s="7">
         <v>-824</v>
       </c>
-      <c r="DQ4" s="7"/>
-      <c r="DR4" s="7"/>
-      <c r="DS4" s="7"/>
-      <c r="DT4" s="7"/>
-      <c r="DU4" s="7"/>
-      <c r="DV4" s="7"/>
-      <c r="DW4" s="7"/>
-      <c r="DX4" s="7"/>
-      <c r="DY4" s="7"/>
-      <c r="DZ4" s="7"/>
-      <c r="EA4" s="7"/>
+      <c r="DQ4" s="7">
+        <v>-1558</v>
+      </c>
+      <c r="DR4" s="7">
+        <v>-331</v>
+      </c>
+      <c r="DS4" s="7">
+        <v>-240</v>
+      </c>
+      <c r="DT4" s="7">
+        <v>-335</v>
+      </c>
+      <c r="DU4" s="7">
+        <v>-1064</v>
+      </c>
+      <c r="DV4" s="7">
+        <v>-918</v>
+      </c>
+      <c r="DW4" s="7">
+        <v>-352</v>
+      </c>
+      <c r="DX4" s="7">
+        <v>-656</v>
+      </c>
+      <c r="DY4" s="7">
+        <v>-802</v>
+      </c>
+      <c r="DZ4" s="7">
+        <v>-155</v>
+      </c>
+      <c r="EA4" s="7">
+        <v>-185</v>
+      </c>
+      <c r="EB4" s="7">
+        <v>-933</v>
+      </c>
+      <c r="EC4" s="7">
+        <v>-308</v>
+      </c>
+      <c r="ED4" s="7">
+        <v>-195</v>
+      </c>
+      <c r="EE4" s="7">
+        <v>-176</v>
+      </c>
+      <c r="EF4" s="7">
+        <v>-263</v>
+      </c>
+      <c r="EG4" s="7">
+        <v>21</v>
+      </c>
+      <c r="EH4" s="7">
+        <v>67</v>
+      </c>
+      <c r="EI4" s="7">
+        <v>-467</v>
+      </c>
+      <c r="EJ4" s="7"/>
+      <c r="EK4" s="7"/>
+      <c r="EL4" s="7"/>
+      <c r="EM4" s="7"/>
+      <c r="EN4" s="7"/>
+      <c r="EO4" s="7"/>
+      <c r="EP4" s="7"/>
+      <c r="EQ4" s="7"/>
+      <c r="ER4" s="7"/>
+      <c r="ES4" s="7"/>
+      <c r="ET4" s="7"/>
+      <c r="EU4" s="7"/>
+      <c r="EV4" s="7"/>
+      <c r="EW4" s="7"/>
+      <c r="EX4" s="7"/>
+      <c r="EY4" s="7"/>
+      <c r="EZ4" s="7"/>
+      <c r="FA4" s="7"/>
+      <c r="FB4" s="7"/>
+      <c r="FC4" s="7"/>
+      <c r="FD4" s="7"/>
+      <c r="FE4" s="7"/>
+      <c r="FF4" s="7"/>
+      <c r="FG4" s="7"/>
+      <c r="FH4" s="7"/>
+      <c r="FI4" s="7"/>
+      <c r="FJ4" s="7"/>
+      <c r="FK4" s="7"/>
+      <c r="FL4" s="7"/>
+      <c r="FM4" s="7"/>
+      <c r="FN4" s="7"/>
+      <c r="FO4" s="7"/>
+      <c r="FP4" s="7"/>
+      <c r="FQ4" s="7"/>
+      <c r="FR4" s="7"/>
+      <c r="FS4" s="7"/>
+      <c r="FT4" s="7"/>
+      <c r="FU4" s="7"/>
+      <c r="FV4" s="7"/>
+      <c r="FW4" s="7"/>
+      <c r="FX4" s="7"/>
+      <c r="FY4" s="7"/>
+      <c r="FZ4" s="7"/>
+      <c r="GA4" s="7"/>
+      <c r="GB4" s="7"/>
+      <c r="GC4" s="7"/>
+      <c r="GD4" s="7"/>
+      <c r="GE4" s="7"/>
+      <c r="GF4" s="7"/>
+      <c r="GG4" s="7"/>
+      <c r="GH4" s="7"/>
+      <c r="GI4" s="7"/>
+      <c r="GJ4" s="7"/>
+      <c r="GK4" s="7"/>
+      <c r="GL4" s="7"/>
+      <c r="GM4" s="7"/>
+      <c r="GN4" s="7"/>
+      <c r="GO4" s="7"/>
+      <c r="GP4" s="7"/>
+      <c r="GQ4" s="7"/>
+      <c r="GR4" s="7"/>
+      <c r="GS4" s="7"/>
+      <c r="GT4" s="7"/>
+      <c r="GU4" s="7"/>
+      <c r="GV4" s="7"/>
+      <c r="GW4" s="7"/>
     </row>
-    <row r="6" spans="1:131" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:131" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:205" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:205" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="BT7" s="26"/>
     </row>
-    <row r="10" spans="1:131" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:205" x14ac:dyDescent="0.2">
       <c r="BQ10" s="26"/>
     </row>
-    <row r="14" spans="1:131" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:205" x14ac:dyDescent="0.2">
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:131" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:205" x14ac:dyDescent="0.2">
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -4768,75 +5547,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="34" t="s">
+      <c r="L39" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34"/>
-      <c r="W39" s="29" t="s">
+      <c r="M39" s="36"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="36"/>
+      <c r="W39" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="29"/>
-      <c r="Y39" s="29"/>
-      <c r="Z39" s="29"/>
-      <c r="AA39" s="29"/>
-      <c r="AB39" s="30">
-        <f>SUM(E4:EA4)</f>
-        <v>23101</v>
-      </c>
-      <c r="AC39" s="30"/>
-      <c r="AD39" s="30"/>
-      <c r="AE39" s="30"/>
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="32">
+        <f>SUM(E4:GW4)</f>
+        <v>14242</v>
+      </c>
+      <c r="AC39" s="32"/>
+      <c r="AD39" s="32"/>
+      <c r="AE39" s="32"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="35" t="s">
+      <c r="L40" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
-      <c r="O40" s="35"/>
-      <c r="P40" s="35"/>
-      <c r="Q40" s="35"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="30"/>
-      <c r="AC40" s="30"/>
-      <c r="AD40" s="30"/>
-      <c r="AE40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="31"/>
+      <c r="Y40" s="31"/>
+      <c r="Z40" s="31"/>
+      <c r="AA40" s="31"/>
+      <c r="AB40" s="32"/>
+      <c r="AC40" s="32"/>
+      <c r="AD40" s="32"/>
+      <c r="AE40" s="32"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="35" t="s">
+      <c r="L41" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="35"/>
-      <c r="P41" s="35"/>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="35"/>
-      <c r="W41" s="29"/>
-      <c r="X41" s="29"/>
-      <c r="Y41" s="29"/>
-      <c r="Z41" s="29"/>
-      <c r="AA41" s="29"/>
-      <c r="AB41" s="30"/>
-      <c r="AC41" s="30"/>
-      <c r="AD41" s="30"/>
-      <c r="AE41" s="30"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="32"/>
+      <c r="AC41" s="32"/>
+      <c r="AD41" s="32"/>
+      <c r="AE41" s="32"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="36" t="s">
+      <c r="L42" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="36"/>
-      <c r="N42" s="36"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
@@ -5217,17 +5996,17 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="L40:Q40"/>
     <mergeCell ref="L42:N42"/>
     <mergeCell ref="L41:R41"/>
     <mergeCell ref="W39:AA41"/>
     <mergeCell ref="AB39:AE41"/>
     <mergeCell ref="Z1:AN1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L39:O39"/>
-    <mergeCell ref="L40:Q40"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4:EA4">
+  <conditionalFormatting sqref="E4:GW4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
       <formula>$O$47</formula>
     </cfRule>
@@ -5240,7 +6019,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
-  <dimension ref="A1:DZ54"/>
+  <dimension ref="A1:GZ54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB42" sqref="AB42"/>
@@ -5251,10 +6030,10 @@
     <col min="2" max="4" width="5.6640625" style="1" customWidth="1"/>
     <col min="5" max="25" width="4.6640625" style="2" customWidth="1"/>
     <col min="26" max="28" width="4.6640625" style="3" customWidth="1"/>
-    <col min="29" max="130" width="4.6640625" customWidth="1"/>
+    <col min="29" max="208" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:130" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:208" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
@@ -5265,26 +6044,26 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="31" t="s">
+      <c r="Z1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
     </row>
-    <row r="2" spans="1:130" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:130" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:208" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:208" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
@@ -5669,8 +6448,242 @@
       <c r="DZ3" s="4">
         <v>44010</v>
       </c>
+      <c r="EA3" s="4">
+        <v>44011</v>
+      </c>
+      <c r="EB3" s="4">
+        <v>44012</v>
+      </c>
+      <c r="EC3" s="4">
+        <v>44013</v>
+      </c>
+      <c r="ED3" s="4">
+        <v>44014</v>
+      </c>
+      <c r="EE3" s="4">
+        <v>44015</v>
+      </c>
+      <c r="EF3" s="4">
+        <v>44016</v>
+      </c>
+      <c r="EG3" s="4">
+        <v>44017</v>
+      </c>
+      <c r="EH3" s="4">
+        <v>44018</v>
+      </c>
+      <c r="EI3" s="4">
+        <v>44019</v>
+      </c>
+      <c r="EJ3" s="4">
+        <v>44020</v>
+      </c>
+      <c r="EK3" s="4">
+        <v>44021</v>
+      </c>
+      <c r="EL3" s="4">
+        <v>44022</v>
+      </c>
+      <c r="EM3" s="4">
+        <v>44023</v>
+      </c>
+      <c r="EN3" s="4">
+        <v>44024</v>
+      </c>
+      <c r="EO3" s="4">
+        <v>44025</v>
+      </c>
+      <c r="EP3" s="4">
+        <v>44026</v>
+      </c>
+      <c r="EQ3" s="4">
+        <v>44027</v>
+      </c>
+      <c r="ER3" s="4">
+        <v>44028</v>
+      </c>
+      <c r="ES3" s="4">
+        <v>44029</v>
+      </c>
+      <c r="ET3" s="4">
+        <v>44030</v>
+      </c>
+      <c r="EU3" s="4">
+        <v>44031</v>
+      </c>
+      <c r="EV3" s="4">
+        <v>44032</v>
+      </c>
+      <c r="EW3" s="4">
+        <v>44033</v>
+      </c>
+      <c r="EX3" s="4">
+        <v>44034</v>
+      </c>
+      <c r="EY3" s="4">
+        <v>44035</v>
+      </c>
+      <c r="EZ3" s="4">
+        <v>44036</v>
+      </c>
+      <c r="FA3" s="4">
+        <v>44037</v>
+      </c>
+      <c r="FB3" s="4">
+        <v>44038</v>
+      </c>
+      <c r="FC3" s="4">
+        <v>44039</v>
+      </c>
+      <c r="FD3" s="4">
+        <v>44040</v>
+      </c>
+      <c r="FE3" s="4">
+        <v>44041</v>
+      </c>
+      <c r="FF3" s="4">
+        <v>44042</v>
+      </c>
+      <c r="FG3" s="4">
+        <v>44043</v>
+      </c>
+      <c r="FH3" s="4">
+        <v>44044</v>
+      </c>
+      <c r="FI3" s="4">
+        <v>44045</v>
+      </c>
+      <c r="FJ3" s="4">
+        <v>44046</v>
+      </c>
+      <c r="FK3" s="4">
+        <v>44047</v>
+      </c>
+      <c r="FL3" s="4">
+        <v>44048</v>
+      </c>
+      <c r="FM3" s="4">
+        <v>44049</v>
+      </c>
+      <c r="FN3" s="4">
+        <v>44050</v>
+      </c>
+      <c r="FO3" s="4">
+        <v>44051</v>
+      </c>
+      <c r="FP3" s="4">
+        <v>44052</v>
+      </c>
+      <c r="FQ3" s="4">
+        <v>44053</v>
+      </c>
+      <c r="FR3" s="4">
+        <v>44054</v>
+      </c>
+      <c r="FS3" s="4">
+        <v>44055</v>
+      </c>
+      <c r="FT3" s="4">
+        <v>44056</v>
+      </c>
+      <c r="FU3" s="4">
+        <v>44057</v>
+      </c>
+      <c r="FV3" s="4">
+        <v>44058</v>
+      </c>
+      <c r="FW3" s="4">
+        <v>44059</v>
+      </c>
+      <c r="FX3" s="4">
+        <v>44060</v>
+      </c>
+      <c r="FY3" s="4">
+        <v>44061</v>
+      </c>
+      <c r="FZ3" s="4">
+        <v>44062</v>
+      </c>
+      <c r="GA3" s="4">
+        <v>44063</v>
+      </c>
+      <c r="GB3" s="4">
+        <v>44064</v>
+      </c>
+      <c r="GC3" s="4">
+        <v>44065</v>
+      </c>
+      <c r="GD3" s="4">
+        <v>44066</v>
+      </c>
+      <c r="GE3" s="4">
+        <v>44067</v>
+      </c>
+      <c r="GF3" s="4">
+        <v>44068</v>
+      </c>
+      <c r="GG3" s="4">
+        <v>44069</v>
+      </c>
+      <c r="GH3" s="4">
+        <v>44070</v>
+      </c>
+      <c r="GI3" s="4">
+        <v>44071</v>
+      </c>
+      <c r="GJ3" s="4">
+        <v>44072</v>
+      </c>
+      <c r="GK3" s="4">
+        <v>44073</v>
+      </c>
+      <c r="GL3" s="4">
+        <v>44074</v>
+      </c>
+      <c r="GM3" s="4">
+        <v>44075</v>
+      </c>
+      <c r="GN3" s="4">
+        <v>44076</v>
+      </c>
+      <c r="GO3" s="4">
+        <v>44077</v>
+      </c>
+      <c r="GP3" s="4">
+        <v>44078</v>
+      </c>
+      <c r="GQ3" s="4">
+        <v>44079</v>
+      </c>
+      <c r="GR3" s="4">
+        <v>44080</v>
+      </c>
+      <c r="GS3" s="4">
+        <v>44081</v>
+      </c>
+      <c r="GT3" s="4">
+        <v>44082</v>
+      </c>
+      <c r="GU3" s="4">
+        <v>44083</v>
+      </c>
+      <c r="GV3" s="4">
+        <v>44084</v>
+      </c>
+      <c r="GW3" s="4">
+        <v>44085</v>
+      </c>
+      <c r="GX3" s="4">
+        <v>44086</v>
+      </c>
+      <c r="GY3" s="4">
+        <v>44087</v>
+      </c>
+      <c r="GZ3" s="4">
+        <v>44088</v>
+      </c>
     </row>
-    <row r="4" spans="1:130" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:208" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
@@ -6025,23 +7038,139 @@
       <c r="DP4" s="21">
         <v>-16</v>
       </c>
-      <c r="DQ4" s="21"/>
-      <c r="DR4" s="21"/>
-      <c r="DS4" s="21"/>
-      <c r="DT4" s="21"/>
-      <c r="DU4" s="21"/>
-      <c r="DV4" s="21"/>
-      <c r="DW4" s="21"/>
-      <c r="DX4" s="21"/>
-      <c r="DY4" s="21"/>
-      <c r="DZ4" s="21"/>
+      <c r="DQ4" s="21">
+        <v>-117</v>
+      </c>
+      <c r="DR4" s="21">
+        <v>0</v>
+      </c>
+      <c r="DS4" s="21">
+        <v>1</v>
+      </c>
+      <c r="DT4" s="21">
+        <v>7</v>
+      </c>
+      <c r="DU4" s="21">
+        <v>8</v>
+      </c>
+      <c r="DV4" s="21">
+        <v>7</v>
+      </c>
+      <c r="DW4" s="21">
+        <v>16</v>
+      </c>
+      <c r="DX4" s="21">
+        <v>0</v>
+      </c>
+      <c r="DY4" s="43">
+        <v>-1</v>
+      </c>
+      <c r="DZ4" s="21">
+        <v>0</v>
+      </c>
+      <c r="EA4" s="21">
+        <v>-1</v>
+      </c>
+      <c r="EB4" s="21">
+        <v>19</v>
+      </c>
+      <c r="EC4" s="21">
+        <v>8</v>
+      </c>
+      <c r="ED4" s="21">
+        <v>1</v>
+      </c>
+      <c r="EE4" s="21">
+        <v>7</v>
+      </c>
+      <c r="EF4" s="21">
+        <v>1</v>
+      </c>
+      <c r="EG4" s="21">
+        <v>3</v>
+      </c>
+      <c r="EH4" s="21">
+        <v>26</v>
+      </c>
+      <c r="EI4" s="21">
+        <v>-1</v>
+      </c>
+      <c r="EJ4" s="21"/>
+      <c r="EK4" s="21"/>
+      <c r="EL4" s="21"/>
+      <c r="EM4" s="21"/>
+      <c r="EN4" s="21"/>
+      <c r="EO4" s="21"/>
+      <c r="EP4" s="21"/>
+      <c r="EQ4" s="21"/>
+      <c r="ER4" s="21"/>
+      <c r="ES4" s="21"/>
+      <c r="ET4" s="21"/>
+      <c r="EU4" s="21"/>
+      <c r="EV4" s="21"/>
+      <c r="EW4" s="21"/>
+      <c r="EX4" s="21"/>
+      <c r="EY4" s="21"/>
+      <c r="EZ4" s="21"/>
+      <c r="FA4" s="21"/>
+      <c r="FB4" s="21"/>
+      <c r="FC4" s="21"/>
+      <c r="FD4" s="21"/>
+      <c r="FE4" s="21"/>
+      <c r="FF4" s="21"/>
+      <c r="FG4" s="21"/>
+      <c r="FH4" s="21"/>
+      <c r="FI4" s="21"/>
+      <c r="FJ4" s="21"/>
+      <c r="FK4" s="21"/>
+      <c r="FL4" s="21"/>
+      <c r="FM4" s="21"/>
+      <c r="FN4" s="21"/>
+      <c r="FO4" s="21"/>
+      <c r="FP4" s="21"/>
+      <c r="FQ4" s="21"/>
+      <c r="FR4" s="21"/>
+      <c r="FS4" s="21"/>
+      <c r="FT4" s="21"/>
+      <c r="FU4" s="21"/>
+      <c r="FV4" s="21"/>
+      <c r="FW4" s="21"/>
+      <c r="FX4" s="21"/>
+      <c r="FY4" s="21"/>
+      <c r="FZ4" s="21"/>
+      <c r="GA4" s="21"/>
+      <c r="GB4" s="21"/>
+      <c r="GC4" s="21"/>
+      <c r="GD4" s="21"/>
+      <c r="GE4" s="21"/>
+      <c r="GF4" s="21"/>
+      <c r="GG4" s="21"/>
+      <c r="GH4" s="21"/>
+      <c r="GI4" s="21"/>
+      <c r="GJ4" s="21"/>
+      <c r="GK4" s="21"/>
+      <c r="GL4" s="21"/>
+      <c r="GM4" s="21"/>
+      <c r="GN4" s="21"/>
+      <c r="GO4" s="21"/>
+      <c r="GP4" s="21"/>
+      <c r="GQ4" s="21"/>
+      <c r="GR4" s="21"/>
+      <c r="GS4" s="21"/>
+      <c r="GT4" s="21"/>
+      <c r="GU4" s="21"/>
+      <c r="GV4" s="21"/>
+      <c r="GW4" s="21"/>
+      <c r="GX4" s="21"/>
+      <c r="GY4" s="21"/>
+      <c r="GZ4" s="21"/>
     </row>
-    <row r="6" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:130" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:208" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:208" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:208" x14ac:dyDescent="0.2">
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:208" x14ac:dyDescent="0.2">
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -6052,75 +7181,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="5"/>
-      <c r="L39" s="34" t="s">
+      <c r="L39" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34"/>
-      <c r="W39" s="29" t="s">
+      <c r="M39" s="36"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="36"/>
+      <c r="W39" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="29"/>
-      <c r="Y39" s="29"/>
-      <c r="Z39" s="29"/>
-      <c r="AA39" s="29"/>
-      <c r="AB39" s="30">
-        <f>SUM(E4:DZ4)</f>
-        <v>242</v>
-      </c>
-      <c r="AC39" s="30"/>
-      <c r="AD39" s="30"/>
-      <c r="AE39" s="30"/>
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="32">
+        <f>SUM(E4:GZ4)</f>
+        <v>226</v>
+      </c>
+      <c r="AC39" s="32"/>
+      <c r="AD39" s="32"/>
+      <c r="AE39" s="32"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="13"/>
-      <c r="L40" s="35" t="s">
+      <c r="L40" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
-      <c r="O40" s="35"/>
-      <c r="P40" s="35"/>
-      <c r="Q40" s="35"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="30"/>
-      <c r="AC40" s="30"/>
-      <c r="AD40" s="30"/>
-      <c r="AE40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="31"/>
+      <c r="Y40" s="31"/>
+      <c r="Z40" s="31"/>
+      <c r="AA40" s="31"/>
+      <c r="AB40" s="32"/>
+      <c r="AC40" s="32"/>
+      <c r="AD40" s="32"/>
+      <c r="AE40" s="32"/>
     </row>
     <row r="41" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K41" s="11"/>
-      <c r="L41" s="35" t="s">
+      <c r="L41" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="35"/>
-      <c r="P41" s="35"/>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="35"/>
-      <c r="W41" s="29"/>
-      <c r="X41" s="29"/>
-      <c r="Y41" s="29"/>
-      <c r="Z41" s="29"/>
-      <c r="AA41" s="29"/>
-      <c r="AB41" s="30"/>
-      <c r="AC41" s="30"/>
-      <c r="AD41" s="30"/>
-      <c r="AE41" s="30"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="32"/>
+      <c r="AC41" s="32"/>
+      <c r="AD41" s="32"/>
+      <c r="AE41" s="32"/>
     </row>
     <row r="42" spans="9:37" x14ac:dyDescent="0.2">
       <c r="K42" s="28"/>
-      <c r="L42" s="36" t="s">
+      <c r="L42" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="36"/>
-      <c r="N42" s="36"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
     </row>
     <row r="43" spans="9:37" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 08/07/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F43C8B-6E0E-5940-B8D8-81A20F2588E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EAC96E-474D-0C41-9039-967A153F804A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -66,7 +66,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m;@"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,10 +422,22 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -436,15 +448,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -462,9 +465,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1592,6 +1592,9 @@
                 </c:pt>
                 <c:pt idx="134">
                   <c:v>-467</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>-647</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2780,6 +2783,9 @@
                 </c:pt>
                 <c:pt idx="131">
                   <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4395,10 +4401,10 @@
   <dimension ref="A1:GW54"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BR5" sqref="BR5"/>
+      <selection activeCell="EK4" sqref="EK4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="4" width="5.6640625" style="1" customWidth="1"/>
     <col min="5" max="25" width="4.6640625" style="2" customWidth="1"/>
@@ -4406,7 +4412,7 @@
     <col min="29" max="205" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:205" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:205" ht="34.5" customHeight="1" thickBot="1">
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
@@ -4417,32 +4423,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="33" t="s">
+      <c r="Z1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
     </row>
-    <row r="2" spans="1:205" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:205" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+    <row r="2" spans="1:205" ht="16" thickTop="1"/>
+    <row r="3" spans="1:205" ht="24.75" customHeight="1">
+      <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -5047,13 +5053,13 @@
         <v>44085</v>
       </c>
     </row>
-    <row r="4" spans="1:205" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
+    <row r="4" spans="1:205" ht="29.25" customHeight="1">
+      <c r="A4" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -5459,7 +5465,9 @@
       <c r="EI4" s="7">
         <v>-467</v>
       </c>
-      <c r="EJ4" s="7"/>
+      <c r="EJ4" s="7">
+        <v>-647</v>
+      </c>
       <c r="EK4" s="7"/>
       <c r="EL4" s="7"/>
       <c r="EM4" s="7"/>
@@ -5526,17 +5534,17 @@
       <c r="GV4" s="7"/>
       <c r="GW4" s="7"/>
     </row>
-    <row r="6" spans="1:205" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:205" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:205" ht="15" customHeight="1"/>
+    <row r="7" spans="1:205" ht="35.25" customHeight="1">
       <c r="BT7" s="26"/>
     </row>
-    <row r="10" spans="1:205" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:205">
       <c r="BQ10" s="26"/>
     </row>
-    <row r="14" spans="1:205" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:205">
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:205" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:205">
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -5545,79 +5553,79 @@
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="36" t="s">
+      <c r="L39" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="W39" s="31" t="s">
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
+      <c r="W39" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="31"/>
-      <c r="Y39" s="31"/>
-      <c r="Z39" s="31"/>
-      <c r="AA39" s="31"/>
-      <c r="AB39" s="32">
+      <c r="X39" s="35"/>
+      <c r="Y39" s="35"/>
+      <c r="Z39" s="35"/>
+      <c r="AA39" s="35"/>
+      <c r="AB39" s="36">
         <f>SUM(E4:GW4)</f>
-        <v>14242</v>
-      </c>
-      <c r="AC39" s="32"/>
-      <c r="AD39" s="32"/>
-      <c r="AE39" s="32"/>
+        <v>13595</v>
+      </c>
+      <c r="AC39" s="36"/>
+      <c r="AD39" s="36"/>
+      <c r="AE39" s="36"/>
     </row>
-    <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="30" t="s">
+      <c r="L40" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="W40" s="31"/>
-      <c r="X40" s="31"/>
-      <c r="Y40" s="31"/>
-      <c r="Z40" s="31"/>
-      <c r="AA40" s="31"/>
-      <c r="AB40" s="32"/>
-      <c r="AC40" s="32"/>
-      <c r="AD40" s="32"/>
-      <c r="AE40" s="32"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+      <c r="W40" s="35"/>
+      <c r="X40" s="35"/>
+      <c r="Y40" s="35"/>
+      <c r="Z40" s="35"/>
+      <c r="AA40" s="35"/>
+      <c r="AB40" s="36"/>
+      <c r="AC40" s="36"/>
+      <c r="AD40" s="36"/>
+      <c r="AE40" s="36"/>
     </row>
-    <row r="41" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="30" t="s">
+      <c r="L41" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="30"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-      <c r="W41" s="31"/>
-      <c r="X41" s="31"/>
-      <c r="Y41" s="31"/>
-      <c r="Z41" s="31"/>
-      <c r="AA41" s="31"/>
-      <c r="AB41" s="32"/>
-      <c r="AC41" s="32"/>
-      <c r="AD41" s="32"/>
-      <c r="AE41" s="32"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="33"/>
+      <c r="W41" s="35"/>
+      <c r="X41" s="35"/>
+      <c r="Y41" s="35"/>
+      <c r="Z41" s="35"/>
+      <c r="AA41" s="35"/>
+      <c r="AB41" s="36"/>
+      <c r="AC41" s="36"/>
+      <c r="AD41" s="36"/>
+      <c r="AE41" s="36"/>
     </row>
-    <row r="42" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="42" spans="9:37">
       <c r="K42" s="28"/>
-      <c r="L42" s="29" t="s">
+      <c r="L42" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
     </row>
-    <row r="43" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="43" spans="9:37">
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
       <c r="K43" s="15"/>
@@ -5648,7 +5656,7 @@
       <c r="AJ43" s="17"/>
       <c r="AK43" s="17"/>
     </row>
-    <row r="44" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="44" spans="9:37">
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
@@ -5679,7 +5687,7 @@
       <c r="AJ44" s="17"/>
       <c r="AK44" s="17"/>
     </row>
-    <row r="45" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="45" spans="9:37">
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
@@ -5710,7 +5718,7 @@
       <c r="AJ45" s="17"/>
       <c r="AK45" s="17"/>
     </row>
-    <row r="46" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="46" spans="9:37">
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
@@ -5741,7 +5749,7 @@
       <c r="AJ46" s="17"/>
       <c r="AK46" s="17"/>
     </row>
-    <row r="47" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="47" spans="9:37">
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
       <c r="K47" s="15"/>
@@ -5777,7 +5785,7 @@
       <c r="AJ47" s="17"/>
       <c r="AK47" s="17"/>
     </row>
-    <row r="48" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="48" spans="9:37">
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
       <c r="K48" s="15"/>
@@ -5808,7 +5816,7 @@
       <c r="AJ48" s="17"/>
       <c r="AK48" s="17"/>
     </row>
-    <row r="49" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="49" spans="9:37">
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
       <c r="K49" s="15"/>
@@ -5839,7 +5847,7 @@
       <c r="AJ49" s="17"/>
       <c r="AK49" s="17"/>
     </row>
-    <row r="50" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="50" spans="9:37">
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
       <c r="K50" s="15"/>
@@ -5870,7 +5878,7 @@
       <c r="AJ50" s="17"/>
       <c r="AK50" s="17"/>
     </row>
-    <row r="51" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="51" spans="9:37">
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15"/>
@@ -5901,7 +5909,7 @@
       <c r="AJ51" s="17"/>
       <c r="AK51" s="17"/>
     </row>
-    <row r="52" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="52" spans="9:37">
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="K52" s="15"/>
@@ -5932,7 +5940,7 @@
       <c r="AJ52" s="17"/>
       <c r="AK52" s="17"/>
     </row>
-    <row r="53" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="53" spans="9:37">
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
       <c r="K53" s="15"/>
@@ -5963,7 +5971,7 @@
       <c r="AJ53" s="17"/>
       <c r="AK53" s="17"/>
     </row>
-    <row r="54" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="54" spans="9:37">
       <c r="I54" s="15"/>
       <c r="J54" s="15"/>
       <c r="K54" s="15"/>
@@ -5996,15 +6004,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="W39:AA41"/>
+    <mergeCell ref="AB39:AE41"/>
+    <mergeCell ref="Z1:AN1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L39:O39"/>
     <mergeCell ref="L40:Q40"/>
     <mergeCell ref="L42:N42"/>
     <mergeCell ref="L41:R41"/>
-    <mergeCell ref="W39:AA41"/>
-    <mergeCell ref="AB39:AE41"/>
-    <mergeCell ref="Z1:AN1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:GW4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -6022,10 +6030,10 @@
   <dimension ref="A1:GZ54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB42" sqref="AB42"/>
+      <selection activeCell="EK4" sqref="EK4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="4" width="5.6640625" style="1" customWidth="1"/>
     <col min="5" max="25" width="4.6640625" style="2" customWidth="1"/>
@@ -6033,7 +6041,7 @@
     <col min="29" max="208" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:208" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:208" ht="34.5" customHeight="1" thickBot="1">
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
@@ -6044,32 +6052,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="33" t="s">
+      <c r="Z1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
     </row>
-    <row r="2" spans="1:208" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:208" s="22" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+    <row r="2" spans="1:208" ht="16" thickTop="1"/>
+    <row r="3" spans="1:208" s="22" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="43"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -6683,13 +6691,13 @@
         <v>44088</v>
       </c>
     </row>
-    <row r="4" spans="1:208" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:208" ht="29.25" customHeight="1">
+      <c r="A4" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="20">
         <v>0</v>
       </c>
@@ -7062,7 +7070,7 @@
       <c r="DX4" s="21">
         <v>0</v>
       </c>
-      <c r="DY4" s="43">
+      <c r="DY4" s="29">
         <v>-1</v>
       </c>
       <c r="DZ4" s="21">
@@ -7095,7 +7103,9 @@
       <c r="EI4" s="21">
         <v>-1</v>
       </c>
-      <c r="EJ4" s="21"/>
+      <c r="EJ4" s="21">
+        <v>2</v>
+      </c>
       <c r="EK4" s="21"/>
       <c r="EL4" s="21"/>
       <c r="EM4" s="21"/>
@@ -7165,12 +7175,12 @@
       <c r="GY4" s="21"/>
       <c r="GZ4" s="21"/>
     </row>
-    <row r="6" spans="1:208" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:208" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:208" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:208" ht="15" customHeight="1"/>
+    <row r="7" spans="1:208" ht="35.25" customHeight="1"/>
+    <row r="14" spans="1:208">
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:208" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:208">
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -7179,79 +7189,79 @@
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="39" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="36" t="s">
+      <c r="L39" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="W39" s="31" t="s">
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
+      <c r="W39" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="31"/>
-      <c r="Y39" s="31"/>
-      <c r="Z39" s="31"/>
-      <c r="AA39" s="31"/>
-      <c r="AB39" s="32">
+      <c r="X39" s="35"/>
+      <c r="Y39" s="35"/>
+      <c r="Z39" s="35"/>
+      <c r="AA39" s="35"/>
+      <c r="AB39" s="36">
         <f>SUM(E4:GZ4)</f>
-        <v>226</v>
-      </c>
-      <c r="AC39" s="32"/>
-      <c r="AD39" s="32"/>
-      <c r="AE39" s="32"/>
+        <v>228</v>
+      </c>
+      <c r="AC39" s="36"/>
+      <c r="AD39" s="36"/>
+      <c r="AE39" s="36"/>
     </row>
-    <row r="40" spans="9:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="30" t="s">
+      <c r="L40" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="W40" s="31"/>
-      <c r="X40" s="31"/>
-      <c r="Y40" s="31"/>
-      <c r="Z40" s="31"/>
-      <c r="AA40" s="31"/>
-      <c r="AB40" s="32"/>
-      <c r="AC40" s="32"/>
-      <c r="AD40" s="32"/>
-      <c r="AE40" s="32"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+      <c r="W40" s="35"/>
+      <c r="X40" s="35"/>
+      <c r="Y40" s="35"/>
+      <c r="Z40" s="35"/>
+      <c r="AA40" s="35"/>
+      <c r="AB40" s="36"/>
+      <c r="AC40" s="36"/>
+      <c r="AD40" s="36"/>
+      <c r="AE40" s="36"/>
     </row>
-    <row r="41" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="30" t="s">
+      <c r="L41" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="30"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-      <c r="W41" s="31"/>
-      <c r="X41" s="31"/>
-      <c r="Y41" s="31"/>
-      <c r="Z41" s="31"/>
-      <c r="AA41" s="31"/>
-      <c r="AB41" s="32"/>
-      <c r="AC41" s="32"/>
-      <c r="AD41" s="32"/>
-      <c r="AE41" s="32"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="33"/>
+      <c r="W41" s="35"/>
+      <c r="X41" s="35"/>
+      <c r="Y41" s="35"/>
+      <c r="Z41" s="35"/>
+      <c r="AA41" s="35"/>
+      <c r="AB41" s="36"/>
+      <c r="AC41" s="36"/>
+      <c r="AD41" s="36"/>
+      <c r="AE41" s="36"/>
     </row>
-    <row r="42" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="42" spans="9:37">
       <c r="K42" s="28"/>
-      <c r="L42" s="29" t="s">
+      <c r="L42" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
     </row>
-    <row r="43" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="43" spans="9:37">
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
       <c r="K43" s="15"/>
@@ -7282,7 +7292,7 @@
       <c r="AJ43" s="17"/>
       <c r="AK43" s="17"/>
     </row>
-    <row r="44" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="44" spans="9:37">
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
@@ -7313,7 +7323,7 @@
       <c r="AJ44" s="17"/>
       <c r="AK44" s="17"/>
     </row>
-    <row r="45" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="45" spans="9:37">
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
@@ -7344,7 +7354,7 @@
       <c r="AJ45" s="17"/>
       <c r="AK45" s="17"/>
     </row>
-    <row r="46" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="46" spans="9:37">
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
@@ -7375,7 +7385,7 @@
       <c r="AJ46" s="17"/>
       <c r="AK46" s="17"/>
     </row>
-    <row r="47" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="47" spans="9:37">
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
       <c r="K47" s="15"/>
@@ -7411,7 +7421,7 @@
       <c r="AJ47" s="17"/>
       <c r="AK47" s="17"/>
     </row>
-    <row r="48" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="48" spans="9:37">
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
       <c r="K48" s="15"/>
@@ -7442,7 +7452,7 @@
       <c r="AJ48" s="17"/>
       <c r="AK48" s="17"/>
     </row>
-    <row r="49" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="49" spans="9:37">
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
       <c r="K49" s="15"/>
@@ -7473,7 +7483,7 @@
       <c r="AJ49" s="17"/>
       <c r="AK49" s="17"/>
     </row>
-    <row r="50" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="50" spans="9:37">
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
       <c r="K50" s="15"/>
@@ -7504,7 +7514,7 @@
       <c r="AJ50" s="17"/>
       <c r="AK50" s="17"/>
     </row>
-    <row r="51" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="51" spans="9:37">
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15"/>
@@ -7535,7 +7545,7 @@
       <c r="AJ51" s="17"/>
       <c r="AK51" s="17"/>
     </row>
-    <row r="52" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="52" spans="9:37">
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="K52" s="15"/>
@@ -7566,7 +7576,7 @@
       <c r="AJ52" s="17"/>
       <c r="AK52" s="17"/>
     </row>
-    <row r="53" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="53" spans="9:37">
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
       <c r="K53" s="15"/>
@@ -7597,7 +7607,7 @@
       <c r="AJ53" s="17"/>
       <c r="AK53" s="17"/>
     </row>
-    <row r="54" spans="9:37" x14ac:dyDescent="0.2">
+    <row r="54" spans="9:37">
       <c r="I54" s="15"/>
       <c r="J54" s="15"/>
       <c r="K54" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 15/07/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EAC96E-474D-0C41-9039-967A153F804A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B2B393-AB07-C54F-BE6D-568148CF19E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -425,6 +425,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -439,15 +448,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="17" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1595,6 +1595,27 @@
                 </c:pt>
                 <c:pt idx="135">
                   <c:v>-647</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>-136</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>-31</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>-125</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>-124</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>-22</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>-238</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>-426</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2786,6 +2807,27 @@
                 </c:pt>
                 <c:pt idx="132">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4401,7 +4443,7 @@
   <dimension ref="A1:GW54"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="EK4" sqref="EK4"/>
+      <selection activeCell="ER4" sqref="ER4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4423,32 +4465,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="37" t="s">
+      <c r="Z1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="37"/>
-      <c r="AN1" s="37"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
     </row>
     <row r="2" spans="1:205" ht="16" thickTop="1"/>
     <row r="3" spans="1:205" ht="24.75" customHeight="1">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -5054,12 +5096,12 @@
       </c>
     </row>
     <row r="4" spans="1:205" ht="29.25" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -5468,13 +5510,27 @@
       <c r="EJ4" s="7">
         <v>-647</v>
       </c>
-      <c r="EK4" s="7"/>
-      <c r="EL4" s="7"/>
-      <c r="EM4" s="7"/>
-      <c r="EN4" s="7"/>
-      <c r="EO4" s="7"/>
-      <c r="EP4" s="7"/>
-      <c r="EQ4" s="7"/>
+      <c r="EK4" s="7">
+        <v>-136</v>
+      </c>
+      <c r="EL4" s="7">
+        <v>-31</v>
+      </c>
+      <c r="EM4" s="7">
+        <v>-125</v>
+      </c>
+      <c r="EN4" s="7">
+        <v>-124</v>
+      </c>
+      <c r="EO4" s="7">
+        <v>-22</v>
+      </c>
+      <c r="EP4" s="7">
+        <v>-238</v>
+      </c>
+      <c r="EQ4" s="7">
+        <v>-426</v>
+      </c>
       <c r="ER4" s="7"/>
       <c r="ES4" s="7"/>
       <c r="ET4" s="7"/>
@@ -5555,75 +5611,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="32" t="s">
+      <c r="L39" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
-      <c r="W39" s="35" t="s">
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="35"/>
+      <c r="W39" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="35"/>
-      <c r="Y39" s="35"/>
-      <c r="Z39" s="35"/>
-      <c r="AA39" s="35"/>
-      <c r="AB39" s="36">
+      <c r="X39" s="30"/>
+      <c r="Y39" s="30"/>
+      <c r="Z39" s="30"/>
+      <c r="AA39" s="30"/>
+      <c r="AB39" s="31">
         <f>SUM(E4:GW4)</f>
-        <v>13595</v>
-      </c>
-      <c r="AC39" s="36"/>
-      <c r="AD39" s="36"/>
-      <c r="AE39" s="36"/>
+        <v>12493</v>
+      </c>
+      <c r="AC39" s="31"/>
+      <c r="AD39" s="31"/>
+      <c r="AE39" s="31"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="33" t="s">
+      <c r="L40" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33"/>
-      <c r="Q40" s="33"/>
-      <c r="W40" s="35"/>
-      <c r="X40" s="35"/>
-      <c r="Y40" s="35"/>
-      <c r="Z40" s="35"/>
-      <c r="AA40" s="35"/>
-      <c r="AB40" s="36"/>
-      <c r="AC40" s="36"/>
-      <c r="AD40" s="36"/>
-      <c r="AE40" s="36"/>
+      <c r="M40" s="36"/>
+      <c r="N40" s="36"/>
+      <c r="O40" s="36"/>
+      <c r="P40" s="36"/>
+      <c r="Q40" s="36"/>
+      <c r="W40" s="30"/>
+      <c r="X40" s="30"/>
+      <c r="Y40" s="30"/>
+      <c r="Z40" s="30"/>
+      <c r="AA40" s="30"/>
+      <c r="AB40" s="31"/>
+      <c r="AC40" s="31"/>
+      <c r="AD40" s="31"/>
+      <c r="AE40" s="31"/>
     </row>
     <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="33" t="s">
+      <c r="L41" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="33"/>
-      <c r="N41" s="33"/>
-      <c r="O41" s="33"/>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="33"/>
-      <c r="R41" s="33"/>
-      <c r="W41" s="35"/>
-      <c r="X41" s="35"/>
-      <c r="Y41" s="35"/>
-      <c r="Z41" s="35"/>
-      <c r="AA41" s="35"/>
-      <c r="AB41" s="36"/>
-      <c r="AC41" s="36"/>
-      <c r="AD41" s="36"/>
-      <c r="AE41" s="36"/>
+      <c r="M41" s="36"/>
+      <c r="N41" s="36"/>
+      <c r="O41" s="36"/>
+      <c r="P41" s="36"/>
+      <c r="Q41" s="36"/>
+      <c r="R41" s="36"/>
+      <c r="W41" s="30"/>
+      <c r="X41" s="30"/>
+      <c r="Y41" s="30"/>
+      <c r="Z41" s="30"/>
+      <c r="AA41" s="30"/>
+      <c r="AB41" s="31"/>
+      <c r="AC41" s="31"/>
+      <c r="AD41" s="31"/>
+      <c r="AE41" s="31"/>
     </row>
     <row r="42" spans="9:37">
       <c r="K42" s="28"/>
-      <c r="L42" s="34" t="s">
+      <c r="L42" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="34"/>
-      <c r="N42" s="34"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37"/>
     </row>
     <row r="43" spans="9:37">
       <c r="I43" s="15"/>
@@ -6004,6 +6060,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="L41:R41"/>
     <mergeCell ref="W39:AA41"/>
     <mergeCell ref="AB39:AE41"/>
     <mergeCell ref="Z1:AN1"/>
@@ -6011,8 +6069,6 @@
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L39:O39"/>
     <mergeCell ref="L40:Q40"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="L41:R41"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:GW4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -6030,7 +6086,7 @@
   <dimension ref="A1:GZ54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="EK4" sqref="EK4"/>
+      <selection activeCell="ER4" sqref="ER4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6052,23 +6108,23 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="37" t="s">
+      <c r="Z1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="37"/>
-      <c r="AN1" s="37"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
     </row>
     <row r="2" spans="1:208" ht="16" thickTop="1"/>
     <row r="3" spans="1:208" s="22" customFormat="1" ht="24.75" customHeight="1">
@@ -7106,13 +7162,27 @@
       <c r="EJ4" s="21">
         <v>2</v>
       </c>
-      <c r="EK4" s="21"/>
-      <c r="EL4" s="21"/>
-      <c r="EM4" s="21"/>
-      <c r="EN4" s="21"/>
-      <c r="EO4" s="21"/>
-      <c r="EP4" s="21"/>
-      <c r="EQ4" s="21"/>
+      <c r="EK4" s="21">
+        <v>4</v>
+      </c>
+      <c r="EL4" s="21">
+        <v>5</v>
+      </c>
+      <c r="EM4" s="21">
+        <v>5</v>
+      </c>
+      <c r="EN4" s="21">
+        <v>4</v>
+      </c>
+      <c r="EO4" s="21">
+        <v>7</v>
+      </c>
+      <c r="EP4" s="21">
+        <v>-1</v>
+      </c>
+      <c r="EQ4" s="21">
+        <v>7</v>
+      </c>
       <c r="ER4" s="21"/>
       <c r="ES4" s="21"/>
       <c r="ET4" s="21"/>
@@ -7191,75 +7261,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="32" t="s">
+      <c r="L39" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
-      <c r="W39" s="35" t="s">
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="35"/>
+      <c r="W39" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="35"/>
-      <c r="Y39" s="35"/>
-      <c r="Z39" s="35"/>
-      <c r="AA39" s="35"/>
-      <c r="AB39" s="36">
+      <c r="X39" s="30"/>
+      <c r="Y39" s="30"/>
+      <c r="Z39" s="30"/>
+      <c r="AA39" s="30"/>
+      <c r="AB39" s="31">
         <f>SUM(E4:GZ4)</f>
-        <v>228</v>
-      </c>
-      <c r="AC39" s="36"/>
-      <c r="AD39" s="36"/>
-      <c r="AE39" s="36"/>
+        <v>259</v>
+      </c>
+      <c r="AC39" s="31"/>
+      <c r="AD39" s="31"/>
+      <c r="AE39" s="31"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="33" t="s">
+      <c r="L40" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33"/>
-      <c r="Q40" s="33"/>
-      <c r="W40" s="35"/>
-      <c r="X40" s="35"/>
-      <c r="Y40" s="35"/>
-      <c r="Z40" s="35"/>
-      <c r="AA40" s="35"/>
-      <c r="AB40" s="36"/>
-      <c r="AC40" s="36"/>
-      <c r="AD40" s="36"/>
-      <c r="AE40" s="36"/>
+      <c r="M40" s="36"/>
+      <c r="N40" s="36"/>
+      <c r="O40" s="36"/>
+      <c r="P40" s="36"/>
+      <c r="Q40" s="36"/>
+      <c r="W40" s="30"/>
+      <c r="X40" s="30"/>
+      <c r="Y40" s="30"/>
+      <c r="Z40" s="30"/>
+      <c r="AA40" s="30"/>
+      <c r="AB40" s="31"/>
+      <c r="AC40" s="31"/>
+      <c r="AD40" s="31"/>
+      <c r="AE40" s="31"/>
     </row>
     <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="33" t="s">
+      <c r="L41" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="33"/>
-      <c r="N41" s="33"/>
-      <c r="O41" s="33"/>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="33"/>
-      <c r="R41" s="33"/>
-      <c r="W41" s="35"/>
-      <c r="X41" s="35"/>
-      <c r="Y41" s="35"/>
-      <c r="Z41" s="35"/>
-      <c r="AA41" s="35"/>
-      <c r="AB41" s="36"/>
-      <c r="AC41" s="36"/>
-      <c r="AD41" s="36"/>
-      <c r="AE41" s="36"/>
+      <c r="M41" s="36"/>
+      <c r="N41" s="36"/>
+      <c r="O41" s="36"/>
+      <c r="P41" s="36"/>
+      <c r="Q41" s="36"/>
+      <c r="R41" s="36"/>
+      <c r="W41" s="30"/>
+      <c r="X41" s="30"/>
+      <c r="Y41" s="30"/>
+      <c r="Z41" s="30"/>
+      <c r="AA41" s="30"/>
+      <c r="AB41" s="31"/>
+      <c r="AC41" s="31"/>
+      <c r="AD41" s="31"/>
+      <c r="AE41" s="31"/>
     </row>
     <row r="42" spans="9:37">
       <c r="K42" s="28"/>
-      <c r="L42" s="34" t="s">
+      <c r="L42" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="34"/>
-      <c r="N42" s="34"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37"/>
     </row>
     <row r="43" spans="9:37">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 16/07/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B2B393-AB07-C54F-BE6D-568148CF19E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE4D91E-7DEB-EE40-A2FB-F9866F11B269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Italia" sheetId="2" r:id="rId1"/>
@@ -425,6 +425,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -441,12 +447,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1616,6 +1616,9 @@
                 </c:pt>
                 <c:pt idx="142">
                   <c:v>-426</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>-20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2828,6 +2831,9 @@
                 </c:pt>
                 <c:pt idx="139">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4442,8 +4448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD285B58-BF01-498B-A55F-CDC02C6CE357}">
   <dimension ref="A1:GW54"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="ER4" sqref="ER4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="ES4" sqref="ES4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4465,32 +4471,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="32" t="s">
+      <c r="Z1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
+      <c r="AK1" s="34"/>
+      <c r="AL1" s="34"/>
+      <c r="AM1" s="34"/>
+      <c r="AN1" s="34"/>
     </row>
     <row r="2" spans="1:205" ht="16" thickTop="1"/>
     <row r="3" spans="1:205" ht="24.75" customHeight="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -5096,12 +5102,12 @@
       </c>
     </row>
     <row r="4" spans="1:205" ht="29.25" customHeight="1">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -5531,7 +5537,9 @@
       <c r="EQ4" s="7">
         <v>-426</v>
       </c>
-      <c r="ER4" s="7"/>
+      <c r="ER4" s="7">
+        <v>-20</v>
+      </c>
       <c r="ES4" s="7"/>
       <c r="ET4" s="7"/>
       <c r="EU4" s="7"/>
@@ -5611,75 +5619,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="35" t="s">
+      <c r="L39" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="35"/>
-      <c r="N39" s="35"/>
-      <c r="O39" s="35"/>
-      <c r="W39" s="30" t="s">
+      <c r="M39" s="37"/>
+      <c r="N39" s="37"/>
+      <c r="O39" s="37"/>
+      <c r="W39" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="30"/>
-      <c r="Z39" s="30"/>
-      <c r="AA39" s="30"/>
-      <c r="AB39" s="31">
+      <c r="X39" s="32"/>
+      <c r="Y39" s="32"/>
+      <c r="Z39" s="32"/>
+      <c r="AA39" s="32"/>
+      <c r="AB39" s="33">
         <f>SUM(E4:GW4)</f>
-        <v>12493</v>
-      </c>
-      <c r="AC39" s="31"/>
-      <c r="AD39" s="31"/>
-      <c r="AE39" s="31"/>
+        <v>12473</v>
+      </c>
+      <c r="AC39" s="33"/>
+      <c r="AD39" s="33"/>
+      <c r="AE39" s="33"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="36" t="s">
+      <c r="L40" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="36"/>
-      <c r="N40" s="36"/>
-      <c r="O40" s="36"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="36"/>
-      <c r="W40" s="30"/>
-      <c r="X40" s="30"/>
-      <c r="Y40" s="30"/>
-      <c r="Z40" s="30"/>
-      <c r="AA40" s="30"/>
-      <c r="AB40" s="31"/>
-      <c r="AC40" s="31"/>
-      <c r="AD40" s="31"/>
-      <c r="AE40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="31"/>
+      <c r="W40" s="32"/>
+      <c r="X40" s="32"/>
+      <c r="Y40" s="32"/>
+      <c r="Z40" s="32"/>
+      <c r="AA40" s="32"/>
+      <c r="AB40" s="33"/>
+      <c r="AC40" s="33"/>
+      <c r="AD40" s="33"/>
+      <c r="AE40" s="33"/>
     </row>
     <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="36" t="s">
+      <c r="L41" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="36"/>
-      <c r="N41" s="36"/>
-      <c r="O41" s="36"/>
-      <c r="P41" s="36"/>
-      <c r="Q41" s="36"/>
-      <c r="R41" s="36"/>
-      <c r="W41" s="30"/>
-      <c r="X41" s="30"/>
-      <c r="Y41" s="30"/>
-      <c r="Z41" s="30"/>
-      <c r="AA41" s="30"/>
-      <c r="AB41" s="31"/>
-      <c r="AC41" s="31"/>
-      <c r="AD41" s="31"/>
-      <c r="AE41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="W41" s="32"/>
+      <c r="X41" s="32"/>
+      <c r="Y41" s="32"/>
+      <c r="Z41" s="32"/>
+      <c r="AA41" s="32"/>
+      <c r="AB41" s="33"/>
+      <c r="AC41" s="33"/>
+      <c r="AD41" s="33"/>
+      <c r="AE41" s="33"/>
     </row>
     <row r="42" spans="9:37">
       <c r="K42" s="28"/>
-      <c r="L42" s="37" t="s">
+      <c r="L42" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="37"/>
-      <c r="N42" s="37"/>
+      <c r="M42" s="30"/>
+      <c r="N42" s="30"/>
     </row>
     <row r="43" spans="9:37">
       <c r="I43" s="15"/>
@@ -6060,15 +6068,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="L40:Q40"/>
     <mergeCell ref="L42:N42"/>
     <mergeCell ref="L41:R41"/>
     <mergeCell ref="W39:AA41"/>
     <mergeCell ref="AB39:AE41"/>
     <mergeCell ref="Z1:AN1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L39:O39"/>
-    <mergeCell ref="L40:Q40"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:GW4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -6085,8 +6093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A1:GZ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="ER4" sqref="ER4"/>
+    <sheetView topLeftCell="A2" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="ES4" sqref="ES4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6108,23 +6116,23 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="32" t="s">
+      <c r="Z1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
+      <c r="AK1" s="34"/>
+      <c r="AL1" s="34"/>
+      <c r="AM1" s="34"/>
+      <c r="AN1" s="34"/>
     </row>
     <row r="2" spans="1:208" ht="16" thickTop="1"/>
     <row r="3" spans="1:208" s="22" customFormat="1" ht="24.75" customHeight="1">
@@ -7183,7 +7191,9 @@
       <c r="EQ4" s="21">
         <v>7</v>
       </c>
-      <c r="ER4" s="21"/>
+      <c r="ER4" s="21">
+        <v>3</v>
+      </c>
       <c r="ES4" s="21"/>
       <c r="ET4" s="21"/>
       <c r="EU4" s="21"/>
@@ -7261,75 +7271,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="35" t="s">
+      <c r="L39" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="35"/>
-      <c r="N39" s="35"/>
-      <c r="O39" s="35"/>
-      <c r="W39" s="30" t="s">
+      <c r="M39" s="37"/>
+      <c r="N39" s="37"/>
+      <c r="O39" s="37"/>
+      <c r="W39" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="30"/>
-      <c r="Z39" s="30"/>
-      <c r="AA39" s="30"/>
-      <c r="AB39" s="31">
+      <c r="X39" s="32"/>
+      <c r="Y39" s="32"/>
+      <c r="Z39" s="32"/>
+      <c r="AA39" s="32"/>
+      <c r="AB39" s="33">
         <f>SUM(E4:GZ4)</f>
-        <v>259</v>
-      </c>
-      <c r="AC39" s="31"/>
-      <c r="AD39" s="31"/>
-      <c r="AE39" s="31"/>
+        <v>262</v>
+      </c>
+      <c r="AC39" s="33"/>
+      <c r="AD39" s="33"/>
+      <c r="AE39" s="33"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="36" t="s">
+      <c r="L40" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="36"/>
-      <c r="N40" s="36"/>
-      <c r="O40" s="36"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="36"/>
-      <c r="W40" s="30"/>
-      <c r="X40" s="30"/>
-      <c r="Y40" s="30"/>
-      <c r="Z40" s="30"/>
-      <c r="AA40" s="30"/>
-      <c r="AB40" s="31"/>
-      <c r="AC40" s="31"/>
-      <c r="AD40" s="31"/>
-      <c r="AE40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="31"/>
+      <c r="W40" s="32"/>
+      <c r="X40" s="32"/>
+      <c r="Y40" s="32"/>
+      <c r="Z40" s="32"/>
+      <c r="AA40" s="32"/>
+      <c r="AB40" s="33"/>
+      <c r="AC40" s="33"/>
+      <c r="AD40" s="33"/>
+      <c r="AE40" s="33"/>
     </row>
     <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="36" t="s">
+      <c r="L41" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="36"/>
-      <c r="N41" s="36"/>
-      <c r="O41" s="36"/>
-      <c r="P41" s="36"/>
-      <c r="Q41" s="36"/>
-      <c r="R41" s="36"/>
-      <c r="W41" s="30"/>
-      <c r="X41" s="30"/>
-      <c r="Y41" s="30"/>
-      <c r="Z41" s="30"/>
-      <c r="AA41" s="30"/>
-      <c r="AB41" s="31"/>
-      <c r="AC41" s="31"/>
-      <c r="AD41" s="31"/>
-      <c r="AE41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="W41" s="32"/>
+      <c r="X41" s="32"/>
+      <c r="Y41" s="32"/>
+      <c r="Z41" s="32"/>
+      <c r="AA41" s="32"/>
+      <c r="AB41" s="33"/>
+      <c r="AC41" s="33"/>
+      <c r="AD41" s="33"/>
+      <c r="AE41" s="33"/>
     </row>
     <row r="42" spans="9:37">
       <c r="K42" s="28"/>
-      <c r="L42" s="37" t="s">
+      <c r="L42" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="37"/>
-      <c r="N42" s="37"/>
+      <c r="M42" s="30"/>
+      <c r="N42" s="30"/>
     </row>
     <row r="43" spans="9:37">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 20/07/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE4D91E-7DEB-EE40-A2FB-F9866F11B269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95931A9F-79CB-8540-BCDE-8D4D32998354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -425,10 +425,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -439,15 +448,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1619,6 +1619,18 @@
                 </c:pt>
                 <c:pt idx="143">
                   <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>-17</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>-88</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>-36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2834,6 +2846,18 @@
                 </c:pt>
                 <c:pt idx="140">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4449,7 +4473,7 @@
   <dimension ref="A1:GW54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="ES4" sqref="ES4"/>
+      <selection activeCell="EW4" sqref="EW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4471,32 +4495,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="34" t="s">
+      <c r="Z1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
     </row>
     <row r="2" spans="1:205" ht="16" thickTop="1"/>
     <row r="3" spans="1:205" ht="24.75" customHeight="1">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -5102,12 +5126,12 @@
       </c>
     </row>
     <row r="4" spans="1:205" ht="29.25" customHeight="1">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -5540,10 +5564,18 @@
       <c r="ER4" s="7">
         <v>-20</v>
       </c>
-      <c r="ES4" s="7"/>
-      <c r="ET4" s="7"/>
-      <c r="EU4" s="7"/>
-      <c r="EV4" s="7"/>
+      <c r="ES4" s="7">
+        <v>-17</v>
+      </c>
+      <c r="ET4" s="7">
+        <v>-88</v>
+      </c>
+      <c r="EU4" s="7">
+        <v>72</v>
+      </c>
+      <c r="EV4" s="7">
+        <v>-36</v>
+      </c>
       <c r="EW4" s="7"/>
       <c r="EX4" s="7"/>
       <c r="EY4" s="7"/>
@@ -5619,75 +5651,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="37" t="s">
+      <c r="L39" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="37"/>
-      <c r="N39" s="37"/>
-      <c r="O39" s="37"/>
-      <c r="W39" s="32" t="s">
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
+      <c r="W39" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="32"/>
-      <c r="Y39" s="32"/>
-      <c r="Z39" s="32"/>
-      <c r="AA39" s="32"/>
-      <c r="AB39" s="33">
+      <c r="X39" s="35"/>
+      <c r="Y39" s="35"/>
+      <c r="Z39" s="35"/>
+      <c r="AA39" s="35"/>
+      <c r="AB39" s="36">
         <f>SUM(E4:GW4)</f>
-        <v>12473</v>
-      </c>
-      <c r="AC39" s="33"/>
-      <c r="AD39" s="33"/>
-      <c r="AE39" s="33"/>
+        <v>12404</v>
+      </c>
+      <c r="AC39" s="36"/>
+      <c r="AD39" s="36"/>
+      <c r="AE39" s="36"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="31" t="s">
+      <c r="L40" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="31"/>
-      <c r="N40" s="31"/>
-      <c r="O40" s="31"/>
-      <c r="P40" s="31"/>
-      <c r="Q40" s="31"/>
-      <c r="W40" s="32"/>
-      <c r="X40" s="32"/>
-      <c r="Y40" s="32"/>
-      <c r="Z40" s="32"/>
-      <c r="AA40" s="32"/>
-      <c r="AB40" s="33"/>
-      <c r="AC40" s="33"/>
-      <c r="AD40" s="33"/>
-      <c r="AE40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+      <c r="W40" s="35"/>
+      <c r="X40" s="35"/>
+      <c r="Y40" s="35"/>
+      <c r="Z40" s="35"/>
+      <c r="AA40" s="35"/>
+      <c r="AB40" s="36"/>
+      <c r="AC40" s="36"/>
+      <c r="AD40" s="36"/>
+      <c r="AE40" s="36"/>
     </row>
     <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="31" t="s">
+      <c r="L41" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="31"/>
-      <c r="P41" s="31"/>
-      <c r="Q41" s="31"/>
-      <c r="R41" s="31"/>
-      <c r="W41" s="32"/>
-      <c r="X41" s="32"/>
-      <c r="Y41" s="32"/>
-      <c r="Z41" s="32"/>
-      <c r="AA41" s="32"/>
-      <c r="AB41" s="33"/>
-      <c r="AC41" s="33"/>
-      <c r="AD41" s="33"/>
-      <c r="AE41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="33"/>
+      <c r="W41" s="35"/>
+      <c r="X41" s="35"/>
+      <c r="Y41" s="35"/>
+      <c r="Z41" s="35"/>
+      <c r="AA41" s="35"/>
+      <c r="AB41" s="36"/>
+      <c r="AC41" s="36"/>
+      <c r="AD41" s="36"/>
+      <c r="AE41" s="36"/>
     </row>
     <row r="42" spans="9:37">
       <c r="K42" s="28"/>
-      <c r="L42" s="30" t="s">
+      <c r="L42" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="30"/>
-      <c r="N42" s="30"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
     </row>
     <row r="43" spans="9:37">
       <c r="I43" s="15"/>
@@ -6068,15 +6100,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="W39:AA41"/>
+    <mergeCell ref="AB39:AE41"/>
+    <mergeCell ref="Z1:AN1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L39:O39"/>
     <mergeCell ref="L40:Q40"/>
     <mergeCell ref="L42:N42"/>
     <mergeCell ref="L41:R41"/>
-    <mergeCell ref="W39:AA41"/>
-    <mergeCell ref="AB39:AE41"/>
-    <mergeCell ref="Z1:AN1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:GW4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -6093,8 +6125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C490A9C4-9020-41A5-8FC8-A6CC518B8439}">
   <dimension ref="A1:GZ54"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="ES4" sqref="ES4"/>
+    <sheetView zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="EW4" sqref="EW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6116,23 +6148,23 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="34" t="s">
+      <c r="Z1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
     </row>
     <row r="2" spans="1:208" ht="16" thickTop="1"/>
     <row r="3" spans="1:208" s="22" customFormat="1" ht="24.75" customHeight="1">
@@ -7194,10 +7226,18 @@
       <c r="ER4" s="21">
         <v>3</v>
       </c>
-      <c r="ES4" s="21"/>
-      <c r="ET4" s="21"/>
-      <c r="EU4" s="21"/>
-      <c r="EV4" s="21"/>
+      <c r="ES4" s="21">
+        <v>10</v>
+      </c>
+      <c r="ET4" s="21">
+        <v>15</v>
+      </c>
+      <c r="EU4" s="21">
+        <v>7</v>
+      </c>
+      <c r="EV4" s="21">
+        <v>2</v>
+      </c>
       <c r="EW4" s="21"/>
       <c r="EX4" s="21"/>
       <c r="EY4" s="21"/>
@@ -7271,75 +7311,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="37" t="s">
+      <c r="L39" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="37"/>
-      <c r="N39" s="37"/>
-      <c r="O39" s="37"/>
-      <c r="W39" s="32" t="s">
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
+      <c r="W39" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="32"/>
-      <c r="Y39" s="32"/>
-      <c r="Z39" s="32"/>
-      <c r="AA39" s="32"/>
-      <c r="AB39" s="33">
+      <c r="X39" s="35"/>
+      <c r="Y39" s="35"/>
+      <c r="Z39" s="35"/>
+      <c r="AA39" s="35"/>
+      <c r="AB39" s="36">
         <f>SUM(E4:GZ4)</f>
-        <v>262</v>
-      </c>
-      <c r="AC39" s="33"/>
-      <c r="AD39" s="33"/>
-      <c r="AE39" s="33"/>
+        <v>296</v>
+      </c>
+      <c r="AC39" s="36"/>
+      <c r="AD39" s="36"/>
+      <c r="AE39" s="36"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="31" t="s">
+      <c r="L40" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="31"/>
-      <c r="N40" s="31"/>
-      <c r="O40" s="31"/>
-      <c r="P40" s="31"/>
-      <c r="Q40" s="31"/>
-      <c r="W40" s="32"/>
-      <c r="X40" s="32"/>
-      <c r="Y40" s="32"/>
-      <c r="Z40" s="32"/>
-      <c r="AA40" s="32"/>
-      <c r="AB40" s="33"/>
-      <c r="AC40" s="33"/>
-      <c r="AD40" s="33"/>
-      <c r="AE40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+      <c r="W40" s="35"/>
+      <c r="X40" s="35"/>
+      <c r="Y40" s="35"/>
+      <c r="Z40" s="35"/>
+      <c r="AA40" s="35"/>
+      <c r="AB40" s="36"/>
+      <c r="AC40" s="36"/>
+      <c r="AD40" s="36"/>
+      <c r="AE40" s="36"/>
     </row>
     <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="31" t="s">
+      <c r="L41" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="31"/>
-      <c r="P41" s="31"/>
-      <c r="Q41" s="31"/>
-      <c r="R41" s="31"/>
-      <c r="W41" s="32"/>
-      <c r="X41" s="32"/>
-      <c r="Y41" s="32"/>
-      <c r="Z41" s="32"/>
-      <c r="AA41" s="32"/>
-      <c r="AB41" s="33"/>
-      <c r="AC41" s="33"/>
-      <c r="AD41" s="33"/>
-      <c r="AE41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="33"/>
+      <c r="W41" s="35"/>
+      <c r="X41" s="35"/>
+      <c r="Y41" s="35"/>
+      <c r="Z41" s="35"/>
+      <c r="AA41" s="35"/>
+      <c r="AB41" s="36"/>
+      <c r="AC41" s="36"/>
+      <c r="AD41" s="36"/>
+      <c r="AE41" s="36"/>
     </row>
     <row r="42" spans="9:37">
       <c r="K42" s="28"/>
-      <c r="L42" s="30" t="s">
+      <c r="L42" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="30"/>
-      <c r="N42" s="30"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
     </row>
     <row r="43" spans="9:37">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 22/07/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95931A9F-79CB-8540-BCDE-8D4D32998354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115D7A00-60D1-394C-80FD-1CEE9DE55E9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -425,6 +425,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -439,15 +448,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="17" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1631,6 +1631,12 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>-36</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>-156</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2858,6 +2864,12 @@
                 </c:pt>
                 <c:pt idx="144">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4473,7 +4485,7 @@
   <dimension ref="A1:GW54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="EW4" sqref="EW4"/>
+      <selection activeCell="EY4" sqref="EY4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4495,32 +4507,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="37" t="s">
+      <c r="Z1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="37"/>
-      <c r="AN1" s="37"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
     </row>
     <row r="2" spans="1:205" ht="16" thickTop="1"/>
     <row r="3" spans="1:205" ht="24.75" customHeight="1">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -5126,12 +5138,12 @@
       </c>
     </row>
     <row r="4" spans="1:205" ht="29.25" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -5576,8 +5588,12 @@
       <c r="EV4" s="7">
         <v>-36</v>
       </c>
-      <c r="EW4" s="7"/>
-      <c r="EX4" s="7"/>
+      <c r="EW4" s="7">
+        <v>-156</v>
+      </c>
+      <c r="EX4" s="7">
+        <v>74</v>
+      </c>
       <c r="EY4" s="7"/>
       <c r="EZ4" s="7"/>
       <c r="FA4" s="7"/>
@@ -5651,75 +5667,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="32" t="s">
+      <c r="L39" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
-      <c r="W39" s="35" t="s">
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="35"/>
+      <c r="W39" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="35"/>
-      <c r="Y39" s="35"/>
-      <c r="Z39" s="35"/>
-      <c r="AA39" s="35"/>
-      <c r="AB39" s="36">
+      <c r="X39" s="30"/>
+      <c r="Y39" s="30"/>
+      <c r="Z39" s="30"/>
+      <c r="AA39" s="30"/>
+      <c r="AB39" s="31">
         <f>SUM(E4:GW4)</f>
-        <v>12404</v>
-      </c>
-      <c r="AC39" s="36"/>
-      <c r="AD39" s="36"/>
-      <c r="AE39" s="36"/>
+        <v>12322</v>
+      </c>
+      <c r="AC39" s="31"/>
+      <c r="AD39" s="31"/>
+      <c r="AE39" s="31"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="33" t="s">
+      <c r="L40" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33"/>
-      <c r="Q40" s="33"/>
-      <c r="W40" s="35"/>
-      <c r="X40" s="35"/>
-      <c r="Y40" s="35"/>
-      <c r="Z40" s="35"/>
-      <c r="AA40" s="35"/>
-      <c r="AB40" s="36"/>
-      <c r="AC40" s="36"/>
-      <c r="AD40" s="36"/>
-      <c r="AE40" s="36"/>
+      <c r="M40" s="36"/>
+      <c r="N40" s="36"/>
+      <c r="O40" s="36"/>
+      <c r="P40" s="36"/>
+      <c r="Q40" s="36"/>
+      <c r="W40" s="30"/>
+      <c r="X40" s="30"/>
+      <c r="Y40" s="30"/>
+      <c r="Z40" s="30"/>
+      <c r="AA40" s="30"/>
+      <c r="AB40" s="31"/>
+      <c r="AC40" s="31"/>
+      <c r="AD40" s="31"/>
+      <c r="AE40" s="31"/>
     </row>
     <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="33" t="s">
+      <c r="L41" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="33"/>
-      <c r="N41" s="33"/>
-      <c r="O41" s="33"/>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="33"/>
-      <c r="R41" s="33"/>
-      <c r="W41" s="35"/>
-      <c r="X41" s="35"/>
-      <c r="Y41" s="35"/>
-      <c r="Z41" s="35"/>
-      <c r="AA41" s="35"/>
-      <c r="AB41" s="36"/>
-      <c r="AC41" s="36"/>
-      <c r="AD41" s="36"/>
-      <c r="AE41" s="36"/>
+      <c r="M41" s="36"/>
+      <c r="N41" s="36"/>
+      <c r="O41" s="36"/>
+      <c r="P41" s="36"/>
+      <c r="Q41" s="36"/>
+      <c r="R41" s="36"/>
+      <c r="W41" s="30"/>
+      <c r="X41" s="30"/>
+      <c r="Y41" s="30"/>
+      <c r="Z41" s="30"/>
+      <c r="AA41" s="30"/>
+      <c r="AB41" s="31"/>
+      <c r="AC41" s="31"/>
+      <c r="AD41" s="31"/>
+      <c r="AE41" s="31"/>
     </row>
     <row r="42" spans="9:37">
       <c r="K42" s="28"/>
-      <c r="L42" s="34" t="s">
+      <c r="L42" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="34"/>
-      <c r="N42" s="34"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37"/>
     </row>
     <row r="43" spans="9:37">
       <c r="I43" s="15"/>
@@ -6100,6 +6116,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="L41:R41"/>
     <mergeCell ref="W39:AA41"/>
     <mergeCell ref="AB39:AE41"/>
     <mergeCell ref="Z1:AN1"/>
@@ -6107,8 +6125,6 @@
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L39:O39"/>
     <mergeCell ref="L40:Q40"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="L41:R41"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:GW4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -6126,7 +6142,7 @@
   <dimension ref="A1:GZ54"/>
   <sheetViews>
     <sheetView zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="EW4" sqref="EW4"/>
+      <selection activeCell="EY4" sqref="EY4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6148,23 +6164,23 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="37" t="s">
+      <c r="Z1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="37"/>
-      <c r="AN1" s="37"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
     </row>
     <row r="2" spans="1:208" ht="16" thickTop="1"/>
     <row r="3" spans="1:208" s="22" customFormat="1" ht="24.75" customHeight="1">
@@ -7238,8 +7254,12 @@
       <c r="EV4" s="21">
         <v>2</v>
       </c>
-      <c r="EW4" s="21"/>
-      <c r="EX4" s="21"/>
+      <c r="EW4" s="21">
+        <v>1</v>
+      </c>
+      <c r="EX4" s="21">
+        <v>18</v>
+      </c>
       <c r="EY4" s="21"/>
       <c r="EZ4" s="21"/>
       <c r="FA4" s="21"/>
@@ -7311,75 +7331,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="32" t="s">
+      <c r="L39" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
-      <c r="W39" s="35" t="s">
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="35"/>
+      <c r="W39" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="35"/>
-      <c r="Y39" s="35"/>
-      <c r="Z39" s="35"/>
-      <c r="AA39" s="35"/>
-      <c r="AB39" s="36">
+      <c r="X39" s="30"/>
+      <c r="Y39" s="30"/>
+      <c r="Z39" s="30"/>
+      <c r="AA39" s="30"/>
+      <c r="AB39" s="31">
         <f>SUM(E4:GZ4)</f>
-        <v>296</v>
-      </c>
-      <c r="AC39" s="36"/>
-      <c r="AD39" s="36"/>
-      <c r="AE39" s="36"/>
+        <v>315</v>
+      </c>
+      <c r="AC39" s="31"/>
+      <c r="AD39" s="31"/>
+      <c r="AE39" s="31"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="33" t="s">
+      <c r="L40" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33"/>
-      <c r="Q40" s="33"/>
-      <c r="W40" s="35"/>
-      <c r="X40" s="35"/>
-      <c r="Y40" s="35"/>
-      <c r="Z40" s="35"/>
-      <c r="AA40" s="35"/>
-      <c r="AB40" s="36"/>
-      <c r="AC40" s="36"/>
-      <c r="AD40" s="36"/>
-      <c r="AE40" s="36"/>
+      <c r="M40" s="36"/>
+      <c r="N40" s="36"/>
+      <c r="O40" s="36"/>
+      <c r="P40" s="36"/>
+      <c r="Q40" s="36"/>
+      <c r="W40" s="30"/>
+      <c r="X40" s="30"/>
+      <c r="Y40" s="30"/>
+      <c r="Z40" s="30"/>
+      <c r="AA40" s="30"/>
+      <c r="AB40" s="31"/>
+      <c r="AC40" s="31"/>
+      <c r="AD40" s="31"/>
+      <c r="AE40" s="31"/>
     </row>
     <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="33" t="s">
+      <c r="L41" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="33"/>
-      <c r="N41" s="33"/>
-      <c r="O41" s="33"/>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="33"/>
-      <c r="R41" s="33"/>
-      <c r="W41" s="35"/>
-      <c r="X41" s="35"/>
-      <c r="Y41" s="35"/>
-      <c r="Z41" s="35"/>
-      <c r="AA41" s="35"/>
-      <c r="AB41" s="36"/>
-      <c r="AC41" s="36"/>
-      <c r="AD41" s="36"/>
-      <c r="AE41" s="36"/>
+      <c r="M41" s="36"/>
+      <c r="N41" s="36"/>
+      <c r="O41" s="36"/>
+      <c r="P41" s="36"/>
+      <c r="Q41" s="36"/>
+      <c r="R41" s="36"/>
+      <c r="W41" s="30"/>
+      <c r="X41" s="30"/>
+      <c r="Y41" s="30"/>
+      <c r="Z41" s="30"/>
+      <c r="AA41" s="30"/>
+      <c r="AB41" s="31"/>
+      <c r="AC41" s="31"/>
+      <c r="AD41" s="31"/>
+      <c r="AE41" s="31"/>
     </row>
     <row r="42" spans="9:37">
       <c r="K42" s="28"/>
-      <c r="L42" s="34" t="s">
+      <c r="L42" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="34"/>
-      <c r="N42" s="34"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37"/>
     </row>
     <row r="43" spans="9:37">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 23/07/20200
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115D7A00-60D1-394C-80FD-1CEE9DE55E9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB44F602-C863-9147-BECC-B7FB59C81338}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -425,6 +425,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -441,12 +447,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1637,6 +1637,9 @@
                 </c:pt>
                 <c:pt idx="149">
                   <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2870,6 +2873,9 @@
                 </c:pt>
                 <c:pt idx="146">
                   <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4485,7 +4491,7 @@
   <dimension ref="A1:GW54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="EY4" sqref="EY4"/>
+      <selection activeCell="EZ4" sqref="EZ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4507,32 +4513,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="32" t="s">
+      <c r="Z1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
+      <c r="AK1" s="34"/>
+      <c r="AL1" s="34"/>
+      <c r="AM1" s="34"/>
+      <c r="AN1" s="34"/>
     </row>
     <row r="2" spans="1:205" ht="16" thickTop="1"/>
     <row r="3" spans="1:205" ht="24.75" customHeight="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -5138,12 +5144,12 @@
       </c>
     </row>
     <row r="4" spans="1:205" ht="29.25" customHeight="1">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -5594,7 +5600,9 @@
       <c r="EX4" s="7">
         <v>74</v>
       </c>
-      <c r="EY4" s="7"/>
+      <c r="EY4" s="7">
+        <v>82</v>
+      </c>
       <c r="EZ4" s="7"/>
       <c r="FA4" s="7"/>
       <c r="FB4" s="7"/>
@@ -5667,75 +5675,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="35" t="s">
+      <c r="L39" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="35"/>
-      <c r="N39" s="35"/>
-      <c r="O39" s="35"/>
-      <c r="W39" s="30" t="s">
+      <c r="M39" s="37"/>
+      <c r="N39" s="37"/>
+      <c r="O39" s="37"/>
+      <c r="W39" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="30"/>
-      <c r="Z39" s="30"/>
-      <c r="AA39" s="30"/>
-      <c r="AB39" s="31">
+      <c r="X39" s="32"/>
+      <c r="Y39" s="32"/>
+      <c r="Z39" s="32"/>
+      <c r="AA39" s="32"/>
+      <c r="AB39" s="33">
         <f>SUM(E4:GW4)</f>
-        <v>12322</v>
-      </c>
-      <c r="AC39" s="31"/>
-      <c r="AD39" s="31"/>
-      <c r="AE39" s="31"/>
+        <v>12404</v>
+      </c>
+      <c r="AC39" s="33"/>
+      <c r="AD39" s="33"/>
+      <c r="AE39" s="33"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="36" t="s">
+      <c r="L40" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="36"/>
-      <c r="N40" s="36"/>
-      <c r="O40" s="36"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="36"/>
-      <c r="W40" s="30"/>
-      <c r="X40" s="30"/>
-      <c r="Y40" s="30"/>
-      <c r="Z40" s="30"/>
-      <c r="AA40" s="30"/>
-      <c r="AB40" s="31"/>
-      <c r="AC40" s="31"/>
-      <c r="AD40" s="31"/>
-      <c r="AE40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="31"/>
+      <c r="W40" s="32"/>
+      <c r="X40" s="32"/>
+      <c r="Y40" s="32"/>
+      <c r="Z40" s="32"/>
+      <c r="AA40" s="32"/>
+      <c r="AB40" s="33"/>
+      <c r="AC40" s="33"/>
+      <c r="AD40" s="33"/>
+      <c r="AE40" s="33"/>
     </row>
     <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="36" t="s">
+      <c r="L41" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="36"/>
-      <c r="N41" s="36"/>
-      <c r="O41" s="36"/>
-      <c r="P41" s="36"/>
-      <c r="Q41" s="36"/>
-      <c r="R41" s="36"/>
-      <c r="W41" s="30"/>
-      <c r="X41" s="30"/>
-      <c r="Y41" s="30"/>
-      <c r="Z41" s="30"/>
-      <c r="AA41" s="30"/>
-      <c r="AB41" s="31"/>
-      <c r="AC41" s="31"/>
-      <c r="AD41" s="31"/>
-      <c r="AE41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="W41" s="32"/>
+      <c r="X41" s="32"/>
+      <c r="Y41" s="32"/>
+      <c r="Z41" s="32"/>
+      <c r="AA41" s="32"/>
+      <c r="AB41" s="33"/>
+      <c r="AC41" s="33"/>
+      <c r="AD41" s="33"/>
+      <c r="AE41" s="33"/>
     </row>
     <row r="42" spans="9:37">
       <c r="K42" s="28"/>
-      <c r="L42" s="37" t="s">
+      <c r="L42" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="37"/>
-      <c r="N42" s="37"/>
+      <c r="M42" s="30"/>
+      <c r="N42" s="30"/>
     </row>
     <row r="43" spans="9:37">
       <c r="I43" s="15"/>
@@ -6116,15 +6124,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="L40:Q40"/>
     <mergeCell ref="L42:N42"/>
     <mergeCell ref="L41:R41"/>
     <mergeCell ref="W39:AA41"/>
     <mergeCell ref="AB39:AE41"/>
     <mergeCell ref="Z1:AN1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L39:O39"/>
-    <mergeCell ref="L40:Q40"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:GW4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -6142,7 +6150,7 @@
   <dimension ref="A1:GZ54"/>
   <sheetViews>
     <sheetView zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="EY4" sqref="EY4"/>
+      <selection activeCell="EZ4" sqref="EZ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6164,23 +6172,23 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="32" t="s">
+      <c r="Z1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
+      <c r="AK1" s="34"/>
+      <c r="AL1" s="34"/>
+      <c r="AM1" s="34"/>
+      <c r="AN1" s="34"/>
     </row>
     <row r="2" spans="1:208" ht="16" thickTop="1"/>
     <row r="3" spans="1:208" s="22" customFormat="1" ht="24.75" customHeight="1">
@@ -7260,7 +7268,9 @@
       <c r="EX4" s="21">
         <v>18</v>
       </c>
-      <c r="EY4" s="21"/>
+      <c r="EY4" s="21">
+        <v>14</v>
+      </c>
       <c r="EZ4" s="21"/>
       <c r="FA4" s="21"/>
       <c r="FB4" s="21"/>
@@ -7331,75 +7341,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="35" t="s">
+      <c r="L39" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="35"/>
-      <c r="N39" s="35"/>
-      <c r="O39" s="35"/>
-      <c r="W39" s="30" t="s">
+      <c r="M39" s="37"/>
+      <c r="N39" s="37"/>
+      <c r="O39" s="37"/>
+      <c r="W39" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="30"/>
-      <c r="Z39" s="30"/>
-      <c r="AA39" s="30"/>
-      <c r="AB39" s="31">
+      <c r="X39" s="32"/>
+      <c r="Y39" s="32"/>
+      <c r="Z39" s="32"/>
+      <c r="AA39" s="32"/>
+      <c r="AB39" s="33">
         <f>SUM(E4:GZ4)</f>
-        <v>315</v>
-      </c>
-      <c r="AC39" s="31"/>
-      <c r="AD39" s="31"/>
-      <c r="AE39" s="31"/>
+        <v>329</v>
+      </c>
+      <c r="AC39" s="33"/>
+      <c r="AD39" s="33"/>
+      <c r="AE39" s="33"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="36" t="s">
+      <c r="L40" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="36"/>
-      <c r="N40" s="36"/>
-      <c r="O40" s="36"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="36"/>
-      <c r="W40" s="30"/>
-      <c r="X40" s="30"/>
-      <c r="Y40" s="30"/>
-      <c r="Z40" s="30"/>
-      <c r="AA40" s="30"/>
-      <c r="AB40" s="31"/>
-      <c r="AC40" s="31"/>
-      <c r="AD40" s="31"/>
-      <c r="AE40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="31"/>
+      <c r="W40" s="32"/>
+      <c r="X40" s="32"/>
+      <c r="Y40" s="32"/>
+      <c r="Z40" s="32"/>
+      <c r="AA40" s="32"/>
+      <c r="AB40" s="33"/>
+      <c r="AC40" s="33"/>
+      <c r="AD40" s="33"/>
+      <c r="AE40" s="33"/>
     </row>
     <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="36" t="s">
+      <c r="L41" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="36"/>
-      <c r="N41" s="36"/>
-      <c r="O41" s="36"/>
-      <c r="P41" s="36"/>
-      <c r="Q41" s="36"/>
-      <c r="R41" s="36"/>
-      <c r="W41" s="30"/>
-      <c r="X41" s="30"/>
-      <c r="Y41" s="30"/>
-      <c r="Z41" s="30"/>
-      <c r="AA41" s="30"/>
-      <c r="AB41" s="31"/>
-      <c r="AC41" s="31"/>
-      <c r="AD41" s="31"/>
-      <c r="AE41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="W41" s="32"/>
+      <c r="X41" s="32"/>
+      <c r="Y41" s="32"/>
+      <c r="Z41" s="32"/>
+      <c r="AA41" s="32"/>
+      <c r="AB41" s="33"/>
+      <c r="AC41" s="33"/>
+      <c r="AD41" s="33"/>
+      <c r="AE41" s="33"/>
     </row>
     <row r="42" spans="9:37">
       <c r="K42" s="28"/>
-      <c r="L42" s="37" t="s">
+      <c r="L42" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="37"/>
-      <c r="N42" s="37"/>
+      <c r="M42" s="30"/>
+      <c r="N42" s="30"/>
     </row>
     <row r="43" spans="9:37">
       <c r="I43" s="15"/>

</xml_diff>

<commit_message>
aggiornamento dati al 27/07/2020
</commit_message>
<xml_diff>
--- a/covid-19.xlsx
+++ b/covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpic24/Documents/covid_19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB44F602-C863-9147-BECC-B7FB59C81338}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9C7ABA-3D20-944A-9BCF-60C540491CAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rtbb7Zfz3RMeVxjpv2hw6lpCwq6xqjYU/FJF6MMvRDu4fQq2rQc241pI9KGE9bG9DeLKX/SQutvpzRKCIqeSIA==" workbookSaltValue="5e6xvbGE1bFbuzE9VyAB5w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{CCFA725D-69DE-48AA-93DE-BFCC1D4EA3B4}"/>
@@ -425,10 +425,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -439,15 +448,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1640,6 +1640,18 @@
                 </c:pt>
                 <c:pt idx="150">
                   <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>-103</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2876,6 +2888,18 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4491,7 +4515,7 @@
   <dimension ref="A1:GW54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="EZ4" sqref="EZ4"/>
+      <selection activeCell="FD4" sqref="FD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4513,32 +4537,32 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="34" t="s">
+      <c r="Z1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
     </row>
     <row r="2" spans="1:205" ht="16" thickTop="1"/>
     <row r="3" spans="1:205" ht="24.75" customHeight="1">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
       <c r="E3" s="4">
         <v>43885</v>
       </c>
@@ -5144,12 +5168,12 @@
       </c>
     </row>
     <row r="4" spans="1:205" ht="29.25" customHeight="1">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="6">
         <v>221</v>
       </c>
@@ -5603,10 +5627,18 @@
       <c r="EY4" s="7">
         <v>82</v>
       </c>
-      <c r="EZ4" s="7"/>
-      <c r="FA4" s="7"/>
-      <c r="FB4" s="7"/>
-      <c r="FC4" s="7"/>
+      <c r="EZ4" s="7">
+        <v>-103</v>
+      </c>
+      <c r="FA4" s="7">
+        <v>141</v>
+      </c>
+      <c r="FB4" s="7">
+        <v>123</v>
+      </c>
+      <c r="FC4" s="7">
+        <v>16</v>
+      </c>
       <c r="FD4" s="7"/>
       <c r="FE4" s="7"/>
       <c r="FF4" s="7"/>
@@ -5675,75 +5707,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="37" t="s">
+      <c r="L39" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="37"/>
-      <c r="N39" s="37"/>
-      <c r="O39" s="37"/>
-      <c r="W39" s="32" t="s">
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
+      <c r="W39" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="32"/>
-      <c r="Y39" s="32"/>
-      <c r="Z39" s="32"/>
-      <c r="AA39" s="32"/>
-      <c r="AB39" s="33">
+      <c r="X39" s="35"/>
+      <c r="Y39" s="35"/>
+      <c r="Z39" s="35"/>
+      <c r="AA39" s="35"/>
+      <c r="AB39" s="36">
         <f>SUM(E4:GW4)</f>
-        <v>12404</v>
-      </c>
-      <c r="AC39" s="33"/>
-      <c r="AD39" s="33"/>
-      <c r="AE39" s="33"/>
+        <v>12581</v>
+      </c>
+      <c r="AC39" s="36"/>
+      <c r="AD39" s="36"/>
+      <c r="AE39" s="36"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="31" t="s">
+      <c r="L40" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="31"/>
-      <c r="N40" s="31"/>
-      <c r="O40" s="31"/>
-      <c r="P40" s="31"/>
-      <c r="Q40" s="31"/>
-      <c r="W40" s="32"/>
-      <c r="X40" s="32"/>
-      <c r="Y40" s="32"/>
-      <c r="Z40" s="32"/>
-      <c r="AA40" s="32"/>
-      <c r="AB40" s="33"/>
-      <c r="AC40" s="33"/>
-      <c r="AD40" s="33"/>
-      <c r="AE40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+      <c r="W40" s="35"/>
+      <c r="X40" s="35"/>
+      <c r="Y40" s="35"/>
+      <c r="Z40" s="35"/>
+      <c r="AA40" s="35"/>
+      <c r="AB40" s="36"/>
+      <c r="AC40" s="36"/>
+      <c r="AD40" s="36"/>
+      <c r="AE40" s="36"/>
     </row>
     <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="31" t="s">
+      <c r="L41" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="31"/>
-      <c r="P41" s="31"/>
-      <c r="Q41" s="31"/>
-      <c r="R41" s="31"/>
-      <c r="W41" s="32"/>
-      <c r="X41" s="32"/>
-      <c r="Y41" s="32"/>
-      <c r="Z41" s="32"/>
-      <c r="AA41" s="32"/>
-      <c r="AB41" s="33"/>
-      <c r="AC41" s="33"/>
-      <c r="AD41" s="33"/>
-      <c r="AE41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="33"/>
+      <c r="W41" s="35"/>
+      <c r="X41" s="35"/>
+      <c r="Y41" s="35"/>
+      <c r="Z41" s="35"/>
+      <c r="AA41" s="35"/>
+      <c r="AB41" s="36"/>
+      <c r="AC41" s="36"/>
+      <c r="AD41" s="36"/>
+      <c r="AE41" s="36"/>
     </row>
     <row r="42" spans="9:37">
       <c r="K42" s="28"/>
-      <c r="L42" s="30" t="s">
+      <c r="L42" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="30"/>
-      <c r="N42" s="30"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
     </row>
     <row r="43" spans="9:37">
       <c r="I43" s="15"/>
@@ -6124,15 +6156,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="W39:AA41"/>
+    <mergeCell ref="AB39:AE41"/>
+    <mergeCell ref="Z1:AN1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L39:O39"/>
     <mergeCell ref="L40:Q40"/>
     <mergeCell ref="L42:N42"/>
     <mergeCell ref="L41:R41"/>
-    <mergeCell ref="W39:AA41"/>
-    <mergeCell ref="AB39:AE41"/>
-    <mergeCell ref="Z1:AN1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:GW4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -6150,7 +6182,7 @@
   <dimension ref="A1:GZ54"/>
   <sheetViews>
     <sheetView zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="EZ4" sqref="EZ4"/>
+      <selection activeCell="FD4" sqref="FD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6172,23 +6204,23 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" s="34" t="s">
+      <c r="Z1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
     </row>
     <row r="2" spans="1:208" ht="16" thickTop="1"/>
     <row r="3" spans="1:208" s="22" customFormat="1" ht="24.75" customHeight="1">
@@ -7271,10 +7303,18 @@
       <c r="EY4" s="21">
         <v>14</v>
       </c>
-      <c r="EZ4" s="21"/>
-      <c r="FA4" s="21"/>
-      <c r="FB4" s="21"/>
-      <c r="FC4" s="21"/>
+      <c r="EZ4" s="21">
+        <v>3</v>
+      </c>
+      <c r="FA4" s="21">
+        <v>9</v>
+      </c>
+      <c r="FB4" s="21">
+        <v>11</v>
+      </c>
+      <c r="FC4" s="21">
+        <v>13</v>
+      </c>
       <c r="FD4" s="21"/>
       <c r="FE4" s="21"/>
       <c r="FF4" s="21"/>
@@ -7341,75 +7381,75 @@
     </row>
     <row r="39" spans="9:37" ht="15" customHeight="1">
       <c r="K39" s="5"/>
-      <c r="L39" s="37" t="s">
+      <c r="L39" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="37"/>
-      <c r="N39" s="37"/>
-      <c r="O39" s="37"/>
-      <c r="W39" s="32" t="s">
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
+      <c r="W39" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="X39" s="32"/>
-      <c r="Y39" s="32"/>
-      <c r="Z39" s="32"/>
-      <c r="AA39" s="32"/>
-      <c r="AB39" s="33">
+      <c r="X39" s="35"/>
+      <c r="Y39" s="35"/>
+      <c r="Z39" s="35"/>
+      <c r="AA39" s="35"/>
+      <c r="AB39" s="36">
         <f>SUM(E4:GZ4)</f>
-        <v>329</v>
-      </c>
-      <c r="AC39" s="33"/>
-      <c r="AD39" s="33"/>
-      <c r="AE39" s="33"/>
+        <v>365</v>
+      </c>
+      <c r="AC39" s="36"/>
+      <c r="AD39" s="36"/>
+      <c r="AE39" s="36"/>
     </row>
     <row r="40" spans="9:37" ht="15" customHeight="1">
       <c r="K40" s="13"/>
-      <c r="L40" s="31" t="s">
+      <c r="L40" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="M40" s="31"/>
-      <c r="N40" s="31"/>
-      <c r="O40" s="31"/>
-      <c r="P40" s="31"/>
-      <c r="Q40" s="31"/>
-      <c r="W40" s="32"/>
-      <c r="X40" s="32"/>
-      <c r="Y40" s="32"/>
-      <c r="Z40" s="32"/>
-      <c r="AA40" s="32"/>
-      <c r="AB40" s="33"/>
-      <c r="AC40" s="33"/>
-      <c r="AD40" s="33"/>
-      <c r="AE40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+      <c r="W40" s="35"/>
+      <c r="X40" s="35"/>
+      <c r="Y40" s="35"/>
+      <c r="Z40" s="35"/>
+      <c r="AA40" s="35"/>
+      <c r="AB40" s="36"/>
+      <c r="AC40" s="36"/>
+      <c r="AD40" s="36"/>
+      <c r="AE40" s="36"/>
     </row>
     <row r="41" spans="9:37">
       <c r="K41" s="11"/>
-      <c r="L41" s="31" t="s">
+      <c r="L41" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="31"/>
-      <c r="P41" s="31"/>
-      <c r="Q41" s="31"/>
-      <c r="R41" s="31"/>
-      <c r="W41" s="32"/>
-      <c r="X41" s="32"/>
-      <c r="Y41" s="32"/>
-      <c r="Z41" s="32"/>
-      <c r="AA41" s="32"/>
-      <c r="AB41" s="33"/>
-      <c r="AC41" s="33"/>
-      <c r="AD41" s="33"/>
-      <c r="AE41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="33"/>
+      <c r="W41" s="35"/>
+      <c r="X41" s="35"/>
+      <c r="Y41" s="35"/>
+      <c r="Z41" s="35"/>
+      <c r="AA41" s="35"/>
+      <c r="AB41" s="36"/>
+      <c r="AC41" s="36"/>
+      <c r="AD41" s="36"/>
+      <c r="AE41" s="36"/>
     </row>
     <row r="42" spans="9:37">
       <c r="K42" s="28"/>
-      <c r="L42" s="30" t="s">
+      <c r="L42" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="30"/>
-      <c r="N42" s="30"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
     </row>
     <row r="43" spans="9:37">
       <c r="I43" s="15"/>

</xml_diff>